<commit_message>
chg: corrected LCC IV CORPS Conops phase 1 + added F-16 presets
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
-    <sheet name="Callsigns" sheetId="2" r:id="rId2"/>
-    <sheet name="Mirage Presets" sheetId="4" r:id="rId3"/>
-    <sheet name="A10 presets" sheetId="5" r:id="rId4"/>
-    <sheet name="Ka-50 presets" sheetId="6" r:id="rId5"/>
-    <sheet name="MI-8 presets" sheetId="7" r:id="rId6"/>
-    <sheet name="F-14 Presets" sheetId="13" r:id="rId7"/>
-    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId8"/>
-    <sheet name="AV-8B Presets" sheetId="8" r:id="rId9"/>
-    <sheet name="AJS-37 Presets" sheetId="9" r:id="rId10"/>
-    <sheet name="AI Callsigns" sheetId="11" r:id="rId11"/>
-    <sheet name="F-16 Presets" sheetId="12" r:id="rId12"/>
+    <sheet name="F-16 Presets" sheetId="12" r:id="rId2"/>
+    <sheet name="Callsigns" sheetId="2" r:id="rId3"/>
+    <sheet name="Mirage Presets" sheetId="4" r:id="rId4"/>
+    <sheet name="A10 presets" sheetId="5" r:id="rId5"/>
+    <sheet name="Ka-50 presets" sheetId="6" r:id="rId6"/>
+    <sheet name="MI-8 presets" sheetId="7" r:id="rId7"/>
+    <sheet name="F-14 Presets" sheetId="13" r:id="rId8"/>
+    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId9"/>
+    <sheet name="AV-8B Presets" sheetId="8" r:id="rId10"/>
+    <sheet name="AJS-37 Presets" sheetId="9" r:id="rId11"/>
+    <sheet name="AI Callsigns" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="826">
   <si>
     <t>AWACS</t>
   </si>
@@ -2209,48 +2209,12 @@
     <t>Internal SEC</t>
   </si>
   <si>
-    <t>143.0</t>
-  </si>
-  <si>
     <t>118.2</t>
   </si>
   <si>
     <t>TWR</t>
   </si>
   <si>
-    <t>119.2</t>
-  </si>
-  <si>
-    <t>Al Ain TWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Al Minhad TWR </t>
-  </si>
-  <si>
-    <t>118.1</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>Bandar Abbas GND</t>
-  </si>
-  <si>
-    <t>Bandar Abbas TWR</t>
-  </si>
-  <si>
-    <t>ARCO tanker</t>
-  </si>
-  <si>
-    <t>Khasab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ras Al Khaimah </t>
-  </si>
-  <si>
-    <t>F-16C presets  (OPUF) V1.0</t>
-  </si>
-  <si>
     <t>COMM 1 (UHF)</t>
   </si>
   <si>
@@ -2537,13 +2501,49 @@
   </si>
   <si>
     <t>LINCOLN CVN 72</t>
+  </si>
+  <si>
+    <t>F-16C presets  (OPAR) V1.0</t>
+  </si>
+  <si>
+    <t>AR601 TEXACO</t>
+  </si>
+  <si>
+    <t>AR701 ARCO1</t>
+  </si>
+  <si>
+    <t>AR702 ARCO2</t>
+  </si>
+  <si>
+    <t>AR703 ARCO3</t>
+  </si>
+  <si>
+    <t>WARRIOR PRI</t>
+  </si>
+  <si>
+    <t>SPARTAN PRI</t>
+  </si>
+  <si>
+    <t>HITMAN PRI</t>
+  </si>
+  <si>
+    <t>WARRIOR SEC</t>
+  </si>
+  <si>
+    <t>SPARTAN SEC</t>
+  </si>
+  <si>
+    <t>HITMAN SEC</t>
+  </si>
+  <si>
+    <t>AWACS VHF Back-up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2694,6 +2694,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="21">
@@ -3241,7 +3247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3441,10 +3447,50 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3455,6 +3501,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3555,70 +3625,15 @@
     <xf numFmtId="0" fontId="16" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3631,6 +3646,58 @@
     </mruColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="66675" y="7572375"/>
+          <a:ext cx="3467100" cy="3419475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3920,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5:AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3971,18 +4038,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="140" t="s">
+      <c r="R3" s="118" t="s">
         <v>292</v>
       </c>
-      <c r="S3" s="140"/>
-      <c r="T3" s="140"/>
-      <c r="Z3" s="99" t="s">
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="Z3" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="100"/>
-      <c r="AB3" s="100"/>
-      <c r="AC3" s="100"/>
-      <c r="AD3" s="101"/>
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
+      <c r="AC3" s="120"/>
+      <c r="AD3" s="121"/>
     </row>
     <row r="4" spans="2:37" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4018,27 +4085,27 @@
       <c r="L4" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="155" t="s">
+      <c r="M4" s="109" t="s">
         <v>31</v>
       </c>
       <c r="N4" s="58" t="s">
         <v>20</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="141" t="s">
-        <v>763</v>
-      </c>
-      <c r="S4" s="142" t="s">
-        <v>764</v>
-      </c>
-      <c r="T4" s="143" t="s">
-        <v>766</v>
-      </c>
-      <c r="V4" s="97" t="s">
+      <c r="R4" s="124" t="s">
+        <v>751</v>
+      </c>
+      <c r="S4" s="101" t="s">
+        <v>752</v>
+      </c>
+      <c r="T4" s="102" t="s">
+        <v>754</v>
+      </c>
+      <c r="V4" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="97"/>
-      <c r="X4" s="97"/>
+      <c r="W4" s="122"/>
+      <c r="X4" s="122"/>
       <c r="Z4" s="92" t="s">
         <v>300</v>
       </c>
@@ -4064,7 +4131,7 @@
       <c r="E5" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="112" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="38" t="s">
@@ -4092,12 +4159,12 @@
         <v>32</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="144"/>
+      <c r="R5" s="125"/>
       <c r="S5" s="31" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>2</v>
@@ -4108,28 +4175,28 @@
       <c r="X5" s="38" t="s">
         <v>494</v>
       </c>
-      <c r="Y5" s="135"/>
+      <c r="Y5" s="97"/>
       <c r="Z5" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="AA5" s="162" t="s">
+      <c r="AA5" s="116" t="s">
         <v>55</v>
       </c>
       <c r="AB5" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="AC5" s="162" t="s">
+      <c r="AC5" s="116" t="s">
         <v>194</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
     </row>
     <row r="6" spans="2:37" ht="16.5" thickBot="1">
       <c r="B6" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="111" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="39" t="s">
@@ -4167,15 +4234,15 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="3" t="s">
-        <v>781</v>
+        <v>769</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="145"/>
-      <c r="S6" s="146" t="s">
-        <v>765</v>
+      <c r="R6" s="126"/>
+      <c r="S6" s="103" t="s">
+        <v>753</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>7</v>
@@ -4184,28 +4251,28 @@
         <v>455</v>
       </c>
       <c r="X6" s="7"/>
-      <c r="Y6" s="135"/>
+      <c r="Y6" s="97"/>
       <c r="Z6" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="AA6" s="162" t="s">
+      <c r="AA6" s="116" t="s">
         <v>267</v>
       </c>
       <c r="AB6" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="AC6" s="162" t="s">
+      <c r="AC6" s="116" t="s">
         <v>70</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
     </row>
     <row r="7" spans="2:37" ht="15.75">
       <c r="B7" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="156" t="s">
+      <c r="C7" s="110" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="53" t="s">
@@ -4246,13 +4313,13 @@
         <v>294</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="141" t="s">
-        <v>769</v>
-      </c>
-      <c r="S7" s="142" t="s">
-        <v>764</v>
-      </c>
-      <c r="T7" s="143" t="s">
+      <c r="R7" s="124" t="s">
+        <v>757</v>
+      </c>
+      <c r="S7" s="101" t="s">
+        <v>752</v>
+      </c>
+      <c r="T7" s="102" t="s">
         <v>543</v>
       </c>
       <c r="V7" s="7" t="s">
@@ -4264,21 +4331,21 @@
       <c r="X7" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="Y7" s="135"/>
+      <c r="Y7" s="97"/>
       <c r="Z7" s="7" t="s">
         <v>624</v>
       </c>
-      <c r="AA7" s="162" t="s">
+      <c r="AA7" s="116" t="s">
         <v>91</v>
       </c>
       <c r="AB7" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="AC7" s="162" t="s">
+      <c r="AC7" s="116" t="s">
         <v>140</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
     </row>
     <row r="8" spans="2:37" ht="15.75">
@@ -4326,9 +4393,9 @@
         <v>295</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="144"/>
+      <c r="R8" s="125"/>
       <c r="S8" s="31" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="T8" s="21" t="s">
         <v>544</v>
@@ -4342,7 +4409,7 @@
       <c r="X8" s="38" t="s">
         <v>499</v>
       </c>
-      <c r="Y8" s="135"/>
+      <c r="Y8" s="97"/>
       <c r="Z8" s="41"/>
       <c r="AA8" s="41"/>
       <c r="AB8" s="41"/>
@@ -4395,9 +4462,9 @@
         <v>296</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="145"/>
-      <c r="S9" s="146" t="s">
-        <v>765</v>
+      <c r="R9" s="126"/>
+      <c r="S9" s="103" t="s">
+        <v>753</v>
       </c>
       <c r="T9" s="25" t="s">
         <v>546</v>
@@ -4411,7 +4478,7 @@
       <c r="X9" s="38" t="s">
         <v>500</v>
       </c>
-      <c r="Y9" s="135"/>
+      <c r="Y9" s="97"/>
       <c r="AD9" s="41"/>
       <c r="AE9" s="41"/>
       <c r="AF9" s="41"/>
@@ -4450,7 +4517,7 @@
       <c r="L10" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="M10" s="156" t="s">
+      <c r="M10" s="110" t="s">
         <v>103</v>
       </c>
       <c r="N10" s="58" t="s">
@@ -4461,9 +4528,9 @@
         <v>297</v>
       </c>
       <c r="Q10" s="3"/>
-      <c r="R10" s="147"/>
+      <c r="R10" s="104"/>
       <c r="S10" s="69"/>
-      <c r="T10" s="148"/>
+      <c r="T10" s="105"/>
       <c r="V10" s="7" t="s">
         <v>11</v>
       </c>
@@ -4473,7 +4540,7 @@
       <c r="X10" s="38" t="s">
         <v>501</v>
       </c>
-      <c r="Y10" s="135"/>
+      <c r="Y10" s="97"/>
       <c r="AD10" s="41"/>
       <c r="AE10" s="41"/>
       <c r="AF10" s="92" t="s">
@@ -4492,7 +4559,7 @@
         <v>313</v>
       </c>
       <c r="AK10" s="92" t="s">
-        <v>824</v>
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15.75">
@@ -4502,7 +4569,7 @@
       <c r="C11" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="111" t="s">
         <v>106</v>
       </c>
       <c r="E11" s="16" t="s">
@@ -4514,7 +4581,7 @@
       <c r="G11" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="156" t="s">
+      <c r="H11" s="110" t="s">
         <v>110</v>
       </c>
       <c r="I11" s="39" t="s">
@@ -4540,14 +4607,14 @@
         <v>13</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="149" t="s">
-        <v>770</v>
-      </c>
-      <c r="S11" s="150" t="s">
-        <v>764</v>
-      </c>
-      <c r="T11" s="151" t="s">
-        <v>771</v>
+      <c r="R11" s="127" t="s">
+        <v>758</v>
+      </c>
+      <c r="S11" s="106" t="s">
+        <v>752</v>
+      </c>
+      <c r="T11" s="107" t="s">
+        <v>759</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>12</v>
@@ -4558,23 +4625,23 @@
       <c r="X11" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="Y11" s="135"/>
-      <c r="Z11" s="137"/>
-      <c r="AA11" s="137"/>
-      <c r="AB11" s="136"/>
-      <c r="AC11" s="136"/>
-      <c r="AD11" s="136"/>
-      <c r="AE11" s="136"/>
-      <c r="AF11" s="139" t="s">
-        <v>825</v>
+      <c r="Y11" s="97"/>
+      <c r="Z11" s="99"/>
+      <c r="AA11" s="99"/>
+      <c r="AB11" s="98"/>
+      <c r="AC11" s="98"/>
+      <c r="AD11" s="98"/>
+      <c r="AE11" s="98"/>
+      <c r="AF11" s="117" t="s">
+        <v>813</v>
       </c>
       <c r="AG11" s="7" t="s">
-        <v>823</v>
+        <v>811</v>
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7" t="s">
-        <v>822</v>
+        <v>810</v>
       </c>
       <c r="AK11" s="7"/>
     </row>
@@ -4606,27 +4673,27 @@
       <c r="J12" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="156" t="s">
+      <c r="K12" s="110" t="s">
         <v>125</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="156" t="s">
+      <c r="M12" s="110" t="s">
         <v>127</v>
       </c>
       <c r="N12" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="O12" s="135"/>
+      <c r="O12" s="97"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="152"/>
-      <c r="S12" s="138" t="s">
-        <v>718</v>
+      <c r="R12" s="128"/>
+      <c r="S12" s="100" t="s">
+        <v>717</v>
       </c>
       <c r="T12" s="21" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V12" s="38" t="s">
         <v>578</v>
@@ -4635,15 +4702,15 @@
         <v>301</v>
       </c>
       <c r="X12" s="7"/>
-      <c r="Y12" s="135"/>
-      <c r="Z12" s="136"/>
-      <c r="AA12" s="136"/>
-      <c r="AB12" s="99" t="s">
-        <v>755</v>
-      </c>
-      <c r="AC12" s="100"/>
-      <c r="AD12" s="101"/>
-      <c r="AF12" s="139"/>
+      <c r="Y12" s="97"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="119" t="s">
+        <v>743</v>
+      </c>
+      <c r="AC12" s="120"/>
+      <c r="AD12" s="121"/>
+      <c r="AF12" s="117"/>
       <c r="AG12" s="7" t="s">
         <v>561</v>
       </c>
@@ -4665,7 +4732,7 @@
       <c r="E13" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="135" t="s">
+      <c r="F13" s="97" t="s">
         <v>132</v>
       </c>
       <c r="G13" s="14" t="s">
@@ -4692,15 +4759,15 @@
       <c r="N13" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="O13" s="135"/>
+      <c r="O13" s="97"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="153"/>
-      <c r="S13" s="154" t="s">
-        <v>765</v>
+      <c r="R13" s="129"/>
+      <c r="S13" s="108" t="s">
+        <v>753</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="V13" s="38" t="s">
         <v>626</v>
@@ -4709,13 +4776,13 @@
         <v>300</v>
       </c>
       <c r="X13" s="7"/>
-      <c r="Y13" s="135"/>
+      <c r="Y13" s="97"/>
       <c r="Z13" s="41"/>
       <c r="AA13" s="41"/>
       <c r="AB13" s="92"/>
       <c r="AC13" s="92"/>
       <c r="AD13" s="92"/>
-      <c r="AF13" s="139"/>
+      <c r="AF13" s="117"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
@@ -4744,7 +4811,7 @@
       <c r="H14" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="I14" s="158" t="s">
+      <c r="I14" s="112" t="s">
         <v>146</v>
       </c>
       <c r="J14" s="14" t="s">
@@ -4767,28 +4834,28 @@
         <v>291</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="141" t="s">
-        <v>773</v>
-      </c>
-      <c r="S14" s="150" t="s">
-        <v>764</v>
-      </c>
-      <c r="T14" s="143" t="s">
-        <v>774</v>
-      </c>
-      <c r="Y14" s="135"/>
+      <c r="R14" s="124" t="s">
+        <v>761</v>
+      </c>
+      <c r="S14" s="106" t="s">
+        <v>752</v>
+      </c>
+      <c r="T14" s="102" t="s">
+        <v>762</v>
+      </c>
+      <c r="Y14" s="97"/>
       <c r="Z14" s="41"/>
       <c r="AA14" s="41"/>
       <c r="AB14" s="7" t="s">
-        <v>747</v>
-      </c>
-      <c r="AC14" s="158" t="s">
+        <v>735</v>
+      </c>
+      <c r="AC14" s="112" t="s">
         <v>110</v>
       </c>
       <c r="AD14" s="38" t="s">
         <v>495</v>
       </c>
-      <c r="AF14" s="139"/>
+      <c r="AF14" s="117"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
@@ -4802,7 +4869,7 @@
       <c r="C15" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="158" t="s">
+      <c r="D15" s="112" t="s">
         <v>153</v>
       </c>
       <c r="E15" s="39" t="s">
@@ -4840,20 +4907,20 @@
         <v>304</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="144"/>
-      <c r="S15" s="138" t="s">
-        <v>718</v>
+      <c r="R15" s="125"/>
+      <c r="S15" s="100" t="s">
+        <v>717</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>775</v>
-      </c>
-      <c r="Y15" s="135"/>
+        <v>763</v>
+      </c>
+      <c r="Y15" s="97"/>
       <c r="Z15" s="41"/>
       <c r="AA15" s="41"/>
       <c r="AB15" s="7" t="s">
-        <v>748</v>
-      </c>
-      <c r="AC15" s="158" t="s">
+        <v>736</v>
+      </c>
+      <c r="AC15" s="112" t="s">
         <v>125</v>
       </c>
       <c r="AD15" s="38" t="s">
@@ -4901,24 +4968,24 @@
         <v>303</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="145"/>
-      <c r="S16" s="154" t="s">
-        <v>765</v>
+      <c r="R16" s="126"/>
+      <c r="S16" s="108" t="s">
+        <v>753</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>776</v>
-      </c>
-      <c r="V16" s="99" t="s">
+        <v>764</v>
+      </c>
+      <c r="V16" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="100"/>
-      <c r="X16" s="100"/>
-      <c r="Y16" s="100"/>
-      <c r="Z16" s="101"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
+      <c r="Y16" s="120"/>
+      <c r="Z16" s="121"/>
       <c r="AB16" s="7" t="s">
-        <v>749</v>
-      </c>
-      <c r="AC16" s="157" t="s">
+        <v>737</v>
+      </c>
+      <c r="AC16" s="111" t="s">
         <v>106</v>
       </c>
       <c r="AD16" s="38" t="s">
@@ -4929,7 +4996,7 @@
       <c r="B17" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="97" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="16" t="s">
@@ -4986,9 +5053,9 @@
         <v>313</v>
       </c>
       <c r="AB17" s="7" t="s">
-        <v>750</v>
-      </c>
-      <c r="AC17" s="158" t="s">
+        <v>738</v>
+      </c>
+      <c r="AC17" s="112" t="s">
         <v>36</v>
       </c>
       <c r="AD17" s="38" t="s">
@@ -5040,12 +5107,12 @@
         <v>308</v>
       </c>
       <c r="Q18" s="3"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="137"/>
-      <c r="T18" s="137"/>
+      <c r="R18" s="99"/>
+      <c r="S18" s="99"/>
+      <c r="T18" s="99"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
-        <v>795</v>
+        <v>783</v>
       </c>
       <c r="W18" s="53" t="s">
         <v>529</v>
@@ -5057,12 +5124,12 @@
         <v>627</v>
       </c>
       <c r="Z18" t="s">
-        <v>791</v>
+        <v>779</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>751</v>
-      </c>
-      <c r="AC18" s="158" t="s">
+        <v>739</v>
+      </c>
+      <c r="AC18" s="112" t="s">
         <v>153</v>
       </c>
       <c r="AD18" s="38" t="s">
@@ -5103,7 +5170,7 @@
       <c r="L19" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="M19" s="155" t="s">
+      <c r="M19" s="109" t="s">
         <v>198</v>
       </c>
       <c r="N19" s="58" t="s">
@@ -5114,29 +5181,29 @@
         <v>311</v>
       </c>
       <c r="Q19" s="3"/>
-      <c r="R19" s="136"/>
-      <c r="S19" s="136"/>
-      <c r="T19" s="136"/>
+      <c r="R19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
       <c r="U19" s="41"/>
       <c r="V19" t="s">
-        <v>796</v>
+        <v>784</v>
       </c>
       <c r="W19" s="53" t="s">
-        <v>813</v>
+        <v>801</v>
       </c>
       <c r="X19" s="53" t="s">
         <v>150</v>
       </c>
       <c r="Y19" t="s">
-        <v>789</v>
+        <v>777</v>
       </c>
       <c r="Z19" t="s">
-        <v>792</v>
+        <v>780</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>752</v>
-      </c>
-      <c r="AC19" s="157" t="s">
+        <v>740</v>
+      </c>
+      <c r="AC19" s="111" t="s">
         <v>240</v>
       </c>
       <c r="AD19" s="38" t="s">
@@ -5188,31 +5255,31 @@
         <v>312</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="97" t="s">
+      <c r="R20" s="122" t="s">
         <v>291</v>
       </c>
-      <c r="S20" s="97"/>
-      <c r="T20" s="97"/>
+      <c r="S20" s="122"/>
+      <c r="T20" s="122"/>
       <c r="U20" s="3"/>
       <c r="V20" t="s">
-        <v>797</v>
+        <v>785</v>
       </c>
       <c r="W20" t="s">
-        <v>811</v>
+        <v>799</v>
       </c>
       <c r="X20" s="53" t="s">
         <v>99</v>
       </c>
       <c r="Y20" t="s">
-        <v>816</v>
+        <v>804</v>
       </c>
       <c r="Z20" t="s">
-        <v>793</v>
+        <v>781</v>
       </c>
       <c r="AB20" s="7" t="s">
-        <v>753</v>
-      </c>
-      <c r="AC20" s="157" t="s">
+        <v>741</v>
+      </c>
+      <c r="AC20" s="111" t="s">
         <v>198</v>
       </c>
       <c r="AD20" s="38" t="s">
@@ -5274,24 +5341,24 @@
       </c>
       <c r="U21" s="41"/>
       <c r="V21" s="3" t="s">
-        <v>798</v>
+        <v>786</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>812</v>
+        <v>800</v>
       </c>
       <c r="X21" s="53" t="s">
         <v>181</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>817</v>
+        <v>805</v>
       </c>
       <c r="Z21" s="41" t="s">
-        <v>794</v>
+        <v>782</v>
       </c>
       <c r="AB21" s="7" t="s">
-        <v>754</v>
-      </c>
-      <c r="AC21" s="157" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC21" s="111" t="s">
         <v>232</v>
       </c>
       <c r="AD21" s="38" t="s">
@@ -5326,7 +5393,7 @@
       <c r="J22" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="K22" s="155" t="s">
+      <c r="K22" s="109" t="s">
         <v>232</v>
       </c>
       <c r="L22" s="14" t="s">
@@ -5351,17 +5418,17 @@
       <c r="T22" t="s">
         <v>493</v>
       </c>
-      <c r="V22" s="99" t="s">
-        <v>788</v>
-      </c>
-      <c r="W22" s="100"/>
-      <c r="X22" s="100"/>
-      <c r="Y22" s="100"/>
-      <c r="Z22" s="101"/>
+      <c r="V22" s="119" t="s">
+        <v>776</v>
+      </c>
+      <c r="W22" s="120"/>
+      <c r="X22" s="120"/>
+      <c r="Y22" s="120"/>
+      <c r="Z22" s="121"/>
       <c r="AB22" s="7" t="s">
-        <v>756</v>
-      </c>
-      <c r="AC22" s="158" t="s">
+        <v>744</v>
+      </c>
+      <c r="AC22" s="112" t="s">
         <v>57</v>
       </c>
       <c r="AD22" s="38" t="s">
@@ -5384,7 +5451,7 @@
       <c r="F23" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="G23" s="155" t="s">
+      <c r="G23" s="109" t="s">
         <v>240</v>
       </c>
       <c r="H23" s="39" t="s">
@@ -5437,9 +5504,9 @@
         <v>313</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="AC23" s="158" t="s">
+        <v>745</v>
+      </c>
+      <c r="AC23" s="112" t="s">
         <v>103</v>
       </c>
       <c r="AD23" s="38" t="s">
@@ -5450,7 +5517,7 @@
       <c r="B24" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="111" t="s">
         <v>248</v>
       </c>
       <c r="D24" s="39" t="s">
@@ -5491,24 +5558,24 @@
         <v>452</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>799</v>
+        <v>787</v>
       </c>
       <c r="W24" s="53" t="s">
-        <v>808</v>
+        <v>796</v>
       </c>
       <c r="X24" s="53" t="s">
         <v>120</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>790</v>
+        <v>778</v>
       </c>
       <c r="Z24" s="41" t="s">
-        <v>803</v>
+        <v>791</v>
       </c>
       <c r="AB24" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="AC24" s="158" t="s">
+        <v>746</v>
+      </c>
+      <c r="AC24" s="112" t="s">
         <v>127</v>
       </c>
       <c r="AD24" s="38" t="s">
@@ -5537,7 +5604,7 @@
       <c r="H25" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="I25" s="135" t="s">
+      <c r="I25" s="97" t="s">
         <v>266</v>
       </c>
       <c r="J25" s="8" t="s">
@@ -5555,37 +5622,37 @@
       <c r="N25" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="O25" s="155"/>
+      <c r="O25" s="109"/>
       <c r="P25" s="3" t="s">
-        <v>782</v>
-      </c>
-      <c r="R25" s="137"/>
-      <c r="S25" s="137"/>
-      <c r="T25" s="137"/>
+        <v>770</v>
+      </c>
+      <c r="R25" s="99"/>
+      <c r="S25" s="99"/>
+      <c r="T25" s="99"/>
       <c r="U25" s="41"/>
       <c r="V25" t="s">
-        <v>800</v>
+        <v>788</v>
       </c>
       <c r="W25" t="s">
-        <v>807</v>
+        <v>795</v>
       </c>
       <c r="X25" s="53" t="s">
         <v>279</v>
       </c>
       <c r="Y25" t="s">
-        <v>814</v>
+        <v>802</v>
       </c>
       <c r="Z25" s="41" t="s">
-        <v>804</v>
+        <v>792</v>
       </c>
       <c r="AB25" s="38" t="s">
-        <v>759</v>
-      </c>
-      <c r="AC25" s="158" t="s">
+        <v>747</v>
+      </c>
+      <c r="AC25" s="112" t="s">
         <v>31</v>
       </c>
       <c r="AD25" s="38" t="s">
-        <v>780</v>
+        <v>768</v>
       </c>
     </row>
     <row r="26" spans="2:30">
@@ -5628,33 +5695,33 @@
       </c>
       <c r="O26" s="52"/>
       <c r="P26" s="3"/>
-      <c r="R26" s="136"/>
-      <c r="S26" s="136"/>
-      <c r="T26" s="136"/>
-      <c r="U26" s="136"/>
+      <c r="R26" s="98"/>
+      <c r="S26" s="98"/>
+      <c r="T26" s="98"/>
+      <c r="U26" s="98"/>
       <c r="V26" t="s">
-        <v>801</v>
+        <v>789</v>
       </c>
       <c r="W26" t="s">
-        <v>809</v>
+        <v>797</v>
       </c>
       <c r="X26" s="53" t="s">
         <v>161</v>
       </c>
       <c r="Y26" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
       <c r="Z26" s="41" t="s">
-        <v>805</v>
+        <v>793</v>
       </c>
       <c r="AB26" s="38" t="s">
-        <v>760</v>
-      </c>
-      <c r="AC26" s="157" t="s">
+        <v>748</v>
+      </c>
+      <c r="AC26" s="111" t="s">
         <v>45</v>
       </c>
       <c r="AD26" s="38" t="s">
-        <v>783</v>
+        <v>771</v>
       </c>
     </row>
     <row r="27" spans="2:30">
@@ -5703,28 +5770,28 @@
       <c r="T27" s="41"/>
       <c r="U27" s="41"/>
       <c r="V27" t="s">
-        <v>802</v>
+        <v>790</v>
       </c>
       <c r="W27" t="s">
-        <v>810</v>
+        <v>798</v>
       </c>
       <c r="X27" s="53" t="s">
         <v>58</v>
       </c>
       <c r="Y27" t="s">
-        <v>818</v>
+        <v>806</v>
       </c>
       <c r="Z27" s="41" t="s">
-        <v>806</v>
+        <v>794</v>
       </c>
       <c r="AB27" s="38" t="s">
-        <v>761</v>
-      </c>
-      <c r="AC27" s="157" t="s">
+        <v>749</v>
+      </c>
+      <c r="AC27" s="111" t="s">
         <v>248</v>
       </c>
       <c r="AD27" s="38" t="s">
-        <v>784</v>
+        <v>772</v>
       </c>
     </row>
     <row r="28" spans="2:30">
@@ -5766,43 +5833,43 @@
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="AB28" s="38" t="s">
-        <v>762</v>
-      </c>
-      <c r="AC28" s="158" t="s">
+        <v>750</v>
+      </c>
+      <c r="AC28" s="112" t="s">
         <v>146</v>
       </c>
       <c r="AD28" s="38" t="s">
-        <v>785</v>
+        <v>773</v>
       </c>
     </row>
     <row r="31" spans="2:30">
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="122" t="s">
         <v>309</v>
       </c>
-      <c r="C31" s="97"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="J31" s="97" t="s">
+      <c r="C31" s="122"/>
+      <c r="D31" s="122"/>
+      <c r="E31" s="122"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="122"/>
+      <c r="J31" s="122" t="s">
         <v>310</v>
       </c>
-      <c r="K31" s="97"/>
-      <c r="L31" s="97"/>
-      <c r="M31" s="97"/>
-      <c r="N31" s="97"/>
-      <c r="O31" s="97"/>
-      <c r="P31" s="97"/>
-      <c r="T31" s="97" t="s">
+      <c r="K31" s="122"/>
+      <c r="L31" s="122"/>
+      <c r="M31" s="122"/>
+      <c r="N31" s="122"/>
+      <c r="O31" s="122"/>
+      <c r="P31" s="122"/>
+      <c r="T31" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="U31" s="97"/>
-      <c r="V31" s="97"/>
-      <c r="W31" s="97"/>
-      <c r="X31" s="97"/>
-      <c r="Y31" s="97"/>
-      <c r="Z31" s="97"/>
+      <c r="U31" s="122"/>
+      <c r="V31" s="122"/>
+      <c r="W31" s="122"/>
+      <c r="X31" s="122"/>
+      <c r="Y31" s="122"/>
+      <c r="Z31" s="122"/>
     </row>
     <row r="32" spans="2:30">
       <c r="B32" s="51" t="s">
@@ -5921,13 +5988,13 @@
       <c r="V33" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W33" s="159" t="s">
+      <c r="W33" s="113" t="s">
         <v>188</v>
       </c>
       <c r="X33" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="Y33" s="160" t="s">
+      <c r="Y33" s="114" t="s">
         <v>258</v>
       </c>
       <c r="Z33" s="7" t="s">
@@ -5986,13 +6053,13 @@
       <c r="V34" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W34" s="159" t="s">
+      <c r="W34" s="113" t="s">
         <v>260</v>
       </c>
       <c r="X34" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="Y34" s="160" t="s">
+      <c r="Y34" s="114" t="s">
         <v>138</v>
       </c>
       <c r="Z34" s="7" t="s">
@@ -6051,13 +6118,13 @@
       <c r="V35" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W35" s="159" t="s">
+      <c r="W35" s="113" t="s">
         <v>238</v>
       </c>
       <c r="X35" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="Y35" s="160" t="s">
+      <c r="Y35" s="114" t="s">
         <v>233</v>
       </c>
       <c r="Z35" s="7" t="s">
@@ -6116,13 +6183,13 @@
       <c r="V36" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W36" s="159" t="s">
+      <c r="W36" s="113" t="s">
         <v>257</v>
       </c>
       <c r="X36" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="Y36" s="160" t="s">
+      <c r="Y36" s="114" t="s">
         <v>245</v>
       </c>
       <c r="Z36" s="7" t="s">
@@ -6181,13 +6248,13 @@
       <c r="V37" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W37" s="159" t="s">
+      <c r="W37" s="113" t="s">
         <v>255</v>
       </c>
       <c r="X37" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="Y37" s="160" t="s">
+      <c r="Y37" s="114" t="s">
         <v>160</v>
       </c>
       <c r="Z37" s="7" t="s">
@@ -6231,13 +6298,13 @@
       <c r="V38" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W38" s="159" t="s">
+      <c r="W38" s="113" t="s">
         <v>210</v>
       </c>
       <c r="X38" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="Y38" s="160" t="s">
+      <c r="Y38" s="114" t="s">
         <v>148</v>
       </c>
       <c r="Z38" s="7" t="s">
@@ -6251,15 +6318,15 @@
       <c r="F39" t="s">
         <v>639</v>
       </c>
-      <c r="J39" s="98" t="s">
+      <c r="J39" s="123" t="s">
         <v>490</v>
       </c>
-      <c r="K39" s="98"/>
-      <c r="L39" s="98"/>
-      <c r="M39" s="98"/>
-      <c r="N39" s="98"/>
-      <c r="O39" s="98"/>
-      <c r="P39" s="98"/>
+      <c r="K39" s="123"/>
+      <c r="L39" s="123"/>
+      <c r="M39" s="123"/>
+      <c r="N39" s="123"/>
+      <c r="O39" s="123"/>
+      <c r="P39" s="123"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -6272,13 +6339,13 @@
       <c r="V39" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W39" s="159" t="s">
+      <c r="W39" s="113" t="s">
         <v>221</v>
       </c>
       <c r="X39" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="Y39" s="160" t="s">
+      <c r="Y39" s="114" t="s">
         <v>218</v>
       </c>
       <c r="Z39" s="7" t="s">
@@ -6304,13 +6371,13 @@
       <c r="V40" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W40" s="159" t="s">
+      <c r="W40" s="113" t="s">
         <v>186</v>
       </c>
       <c r="X40" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="Y40" s="160" t="s">
+      <c r="Y40" s="114" t="s">
         <v>274</v>
       </c>
       <c r="Z40" s="7" t="s">
@@ -6336,13 +6403,13 @@
       <c r="V41" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W41" s="159" t="s">
+      <c r="W41" s="113" t="s">
         <v>171</v>
       </c>
       <c r="X41" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="Y41" s="160" t="s">
+      <c r="Y41" s="114" t="s">
         <v>217</v>
       </c>
       <c r="Z41" s="7" t="s">
@@ -6364,13 +6431,13 @@
       <c r="V42" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="W42" s="159" t="s">
+      <c r="W42" s="113" t="s">
         <v>184</v>
       </c>
       <c r="X42" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="Y42" s="160" t="s">
+      <c r="Y42" s="114" t="s">
         <v>251</v>
       </c>
       <c r="Z42" s="7" t="s">
@@ -6394,13 +6461,13 @@
       <c r="V44" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="W44" s="159" t="s">
+      <c r="W44" s="113" t="s">
         <v>81</v>
       </c>
       <c r="X44" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="Y44" s="160" t="s">
+      <c r="Y44" s="114" t="s">
         <v>142</v>
       </c>
       <c r="Z44" s="7" t="s">
@@ -6413,38 +6480,38 @@
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="W45" s="159" t="s">
+        <v>727</v>
+      </c>
+      <c r="W45" s="113" t="s">
         <v>134</v>
       </c>
       <c r="X45" s="7" t="s">
-        <v>740</v>
-      </c>
-      <c r="Y45" s="160" t="s">
+        <v>728</v>
+      </c>
+      <c r="Y45" s="114" t="s">
         <v>67</v>
       </c>
       <c r="Z45" s="7" t="s">
-        <v>742</v>
+        <v>730</v>
       </c>
     </row>
     <row r="46" spans="2:26">
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
       <c r="V46" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="W46" s="159" t="s">
+        <v>727</v>
+      </c>
+      <c r="W46" s="113" t="s">
         <v>112</v>
       </c>
       <c r="X46" s="7" t="s">
-        <v>741</v>
-      </c>
-      <c r="Y46" s="160" t="s">
+        <v>729</v>
+      </c>
+      <c r="Y46" s="114" t="s">
         <v>202</v>
       </c>
-      <c r="Z46" s="161" t="s">
-        <v>743</v>
+      <c r="Z46" s="115" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="47" spans="2:26">
@@ -6467,104 +6534,104 @@
     </row>
     <row r="49" spans="20:26">
       <c r="T49" s="7" t="s">
-        <v>819</v>
+        <v>807</v>
       </c>
       <c r="U49" s="7"/>
       <c r="V49" s="7" t="s">
-        <v>732</v>
-      </c>
-      <c r="W49" s="159" t="s">
+        <v>720</v>
+      </c>
+      <c r="W49" s="113" t="s">
         <v>97</v>
       </c>
       <c r="X49" s="7" t="s">
-        <v>733</v>
-      </c>
-      <c r="Y49" s="160" t="s">
+        <v>721</v>
+      </c>
+      <c r="Y49" s="114" t="s">
         <v>121</v>
       </c>
       <c r="Z49" s="7" t="s">
-        <v>736</v>
+        <v>724</v>
       </c>
     </row>
     <row r="50" spans="20:26">
       <c r="T50" s="7" t="s">
-        <v>820</v>
+        <v>808</v>
       </c>
       <c r="U50" s="7"/>
       <c r="V50" s="7" t="s">
-        <v>732</v>
-      </c>
-      <c r="W50" s="159" t="s">
+        <v>720</v>
+      </c>
+      <c r="W50" s="113" t="s">
         <v>155</v>
       </c>
       <c r="X50" s="7" t="s">
-        <v>734</v>
-      </c>
-      <c r="Y50" s="160" t="s">
+        <v>722</v>
+      </c>
+      <c r="Y50" s="114" t="s">
         <v>133</v>
       </c>
       <c r="Z50" s="7" t="s">
-        <v>737</v>
+        <v>725</v>
       </c>
     </row>
     <row r="51" spans="20:26">
       <c r="T51" s="7" t="s">
-        <v>821</v>
+        <v>809</v>
       </c>
       <c r="U51" s="7"/>
       <c r="V51" s="7" t="s">
-        <v>732</v>
-      </c>
-      <c r="W51" s="159" t="s">
+        <v>720</v>
+      </c>
+      <c r="W51" s="113" t="s">
         <v>71</v>
       </c>
       <c r="X51" s="7" t="s">
-        <v>735</v>
-      </c>
-      <c r="Y51" s="160" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y51" s="114" t="s">
         <v>147</v>
       </c>
       <c r="Z51" s="7" t="s">
-        <v>738</v>
+        <v>726</v>
       </c>
     </row>
     <row r="52" spans="20:26">
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
       <c r="V52" s="7" t="s">
-        <v>732</v>
-      </c>
-      <c r="W52" s="159" t="s">
+        <v>720</v>
+      </c>
+      <c r="W52" s="113" t="s">
         <v>214</v>
       </c>
       <c r="X52" s="7" t="s">
-        <v>786</v>
-      </c>
-      <c r="Y52" s="160" t="s">
+        <v>774</v>
+      </c>
+      <c r="Y52" s="114" t="s">
         <v>90</v>
       </c>
       <c r="Z52" s="7" t="s">
-        <v>787</v>
+        <v>775</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="AB12:AD12"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AF11:AF14"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="V22:Z22"/>
     <mergeCell ref="V16:Z16"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="AB12:AD12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6573,6 +6640,578 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="150" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="151"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="133" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="133" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="134"/>
+      <c r="F3" s="135"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A4" s="54">
+        <v>1</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>333</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="54">
+        <v>2</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="54">
+        <v>2</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>335</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="54">
+        <v>3</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="D6" s="54">
+        <v>3</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>337</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="54">
+        <v>4</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="D7" s="54">
+        <v>4</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="54">
+        <v>5</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="54">
+        <v>5</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>342</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="54">
+        <v>6</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="D9" s="54">
+        <v>6</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>343</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A10" s="54">
+        <v>7</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>345</v>
+      </c>
+      <c r="D10" s="54">
+        <v>7</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A11" s="54">
+        <v>8</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>347</v>
+      </c>
+      <c r="D11" s="54">
+        <v>8</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A12" s="54">
+        <v>9</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="54">
+        <v>9</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A13" s="54">
+        <v>10</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>351</v>
+      </c>
+      <c r="D13" s="54">
+        <v>10</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A14" s="54">
+        <v>11</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="54">
+        <v>11</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A15" s="54">
+        <v>12</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="54">
+        <v>12</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A16" s="54">
+        <v>13</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="D16" s="54">
+        <v>13</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A17" s="54">
+        <v>14</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>357</v>
+      </c>
+      <c r="D17" s="54">
+        <v>14</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A18" s="54">
+        <v>15</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D18" s="54">
+        <v>15</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A19" s="54">
+        <v>16</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>359</v>
+      </c>
+      <c r="D19" s="54">
+        <v>16</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A20" s="54">
+        <v>17</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="D20" s="54">
+        <v>17</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A21" s="54">
+        <v>18</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>361</v>
+      </c>
+      <c r="D21" s="54">
+        <v>18</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A22" s="54">
+        <v>19</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" s="54">
+        <v>19</v>
+      </c>
+      <c r="E22" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="56" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A23" s="54">
+        <v>20</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>363</v>
+      </c>
+      <c r="D23" s="54">
+        <v>20</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A24" s="54">
+        <v>21</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>364</v>
+      </c>
+      <c r="D24" s="54">
+        <v>21</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A25" s="54">
+        <v>22</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>365</v>
+      </c>
+      <c r="D25" s="54">
+        <v>22</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A26" s="54">
+        <v>23</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>367</v>
+      </c>
+      <c r="D26" s="54">
+        <v>23</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="56" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A27" s="54">
+        <v>24</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>369</v>
+      </c>
+      <c r="D27" s="54">
+        <v>24</v>
+      </c>
+      <c r="E27" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A28" s="54">
+        <v>25</v>
+      </c>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="54">
+        <v>25</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>264</v>
+      </c>
+      <c r="F28" s="56" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A29" s="54">
+        <v>26</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="D29" s="54">
+        <v>26</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -6588,22 +7227,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="152" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="153" t="s">
         <v>374</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -6708,12 +7347,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="125" t="s">
+      <c r="B14" s="153" t="s">
         <v>391</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
+      <c r="C14" s="153"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="153"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -6821,7 +7460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O39"/>
   <sheetViews>
@@ -7820,12 +8459,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7836,43 +8475,46 @@
     <col min="5" max="5" width="3.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="126" t="s">
-        <v>729</v>
-      </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="128"/>
+      <c r="A1" s="154" t="s">
+        <v>814</v>
+      </c>
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="156"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="129"/>
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="131"/>
+      <c r="A2" s="157"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="132" t="s">
-        <v>730</v>
-      </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133" t="s">
-        <v>731</v>
-      </c>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="134"/>
+      <c r="A3" s="160" t="s">
+        <v>718</v>
+      </c>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161" t="s">
+        <v>719</v>
+      </c>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="162"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="81">
@@ -7903,19 +8545,19 @@
         <v>494</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>346</v>
+        <v>2</v>
       </c>
       <c r="E5" s="82">
         <v>2</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>543</v>
+        <v>756</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>723</v>
+        <v>753</v>
       </c>
       <c r="H5" s="83" t="s">
-        <v>539</v>
+        <v>751</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1">
@@ -7923,25 +8565,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C6" s="84" t="s">
-        <v>707</v>
+        <v>499</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>507</v>
+        <v>9</v>
       </c>
       <c r="E6" s="82">
         <v>3</v>
       </c>
       <c r="F6" s="83" t="s">
-        <v>544</v>
+        <v>755</v>
       </c>
       <c r="G6" s="84" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H6" s="83" t="s">
-        <v>721</v>
+        <v>751</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1">
@@ -7949,25 +8591,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C7" s="84" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>508</v>
+        <v>735</v>
       </c>
       <c r="E7" s="82">
         <v>4</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>722</v>
+        <v>760</v>
       </c>
       <c r="G7" s="84" t="s">
-        <v>723</v>
+        <v>753</v>
       </c>
       <c r="H7" s="83" t="s">
-        <v>724</v>
+        <v>758</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" thickBot="1">
@@ -7975,25 +8617,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C8" s="84" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>510</v>
+        <v>736</v>
       </c>
       <c r="E8" s="82">
         <v>5</v>
       </c>
       <c r="F8" s="83" t="s">
+        <v>716</v>
+      </c>
+      <c r="G8" s="84" t="s">
         <v>717</v>
       </c>
-      <c r="G8" s="84" t="s">
-        <v>718</v>
-      </c>
       <c r="H8" s="83" t="s">
-        <v>725</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.75" thickBot="1">
@@ -8001,25 +8643,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C9" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D9" s="91" t="s">
-        <v>511</v>
+        <v>737</v>
       </c>
       <c r="E9" s="82">
         <v>6</v>
       </c>
       <c r="F9" s="83" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>389</v>
+        <v>768</v>
       </c>
       <c r="H9" s="83" t="s">
-        <v>512</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" thickBot="1">
@@ -8027,25 +8669,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="C10" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>513</v>
+        <v>738</v>
       </c>
       <c r="E10" s="82">
         <v>7</v>
       </c>
       <c r="F10" s="83" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G10" s="84" t="s">
-        <v>523</v>
+        <v>771</v>
       </c>
       <c r="H10" s="83" t="s">
-        <v>526</v>
+        <v>748</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" thickBot="1">
@@ -8053,25 +8695,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>514</v>
+        <v>739</v>
       </c>
       <c r="E11" s="82">
         <v>8</v>
       </c>
       <c r="F11" s="83" t="s">
-        <v>267</v>
-      </c>
-      <c r="G11" s="84" t="s">
-        <v>528</v>
+        <v>248</v>
+      </c>
+      <c r="G11" s="165" t="s">
+        <v>772</v>
       </c>
       <c r="H11" s="83" t="s">
-        <v>527</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18.75" thickBot="1">
@@ -8085,17 +8727,19 @@
         <v>515</v>
       </c>
       <c r="D12" s="91" t="s">
-        <v>17</v>
+        <v>740</v>
       </c>
       <c r="E12" s="82">
         <v>9</v>
       </c>
       <c r="F12" s="83" t="s">
-        <v>716</v>
-      </c>
-      <c r="G12" s="84"/>
+        <v>146</v>
+      </c>
+      <c r="G12" s="84" t="s">
+        <v>773</v>
+      </c>
       <c r="H12" s="83" t="s">
-        <v>726</v>
+        <v>750</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18.75" thickBot="1">
@@ -8109,14 +8753,20 @@
         <v>516</v>
       </c>
       <c r="D13" s="91" t="s">
-        <v>517</v>
+        <v>741</v>
       </c>
       <c r="E13" s="82">
         <v>10</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="83"/>
+      <c r="F13" s="83" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="84" t="s">
+        <v>389</v>
+      </c>
+      <c r="H13" s="83" t="s">
+        <v>825</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="18.75" thickBot="1">
       <c r="A14" s="81">
@@ -8129,14 +8779,20 @@
         <v>518</v>
       </c>
       <c r="D14" s="91" t="s">
-        <v>19</v>
+        <v>742</v>
       </c>
       <c r="E14" s="82">
         <v>11</v>
       </c>
-      <c r="F14" s="83"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="83"/>
+      <c r="F14" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="84" t="s">
+        <v>627</v>
+      </c>
+      <c r="H14" s="83" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1">
       <c r="A15" s="81">
@@ -8149,14 +8805,20 @@
         <v>547</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>550</v>
+        <v>744</v>
       </c>
       <c r="E15" s="82">
         <v>12</v>
       </c>
-      <c r="F15" s="83"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="83"/>
+      <c r="F15" s="83" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="165" t="s">
+        <v>777</v>
+      </c>
+      <c r="H15" s="83" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="18.75" thickBot="1">
       <c r="A16" s="81">
@@ -8169,14 +8831,20 @@
         <v>548</v>
       </c>
       <c r="D16" s="91" t="s">
-        <v>551</v>
+        <v>745</v>
       </c>
       <c r="E16" s="82">
         <v>13</v>
       </c>
-      <c r="F16" s="83"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="83"/>
+      <c r="F16" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="84" t="s">
+        <v>804</v>
+      </c>
+      <c r="H16" s="83" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" thickBot="1">
       <c r="A17" s="81">
@@ -8186,131 +8854,159 @@
         <v>127</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>706</v>
+        <v>549</v>
       </c>
       <c r="D17" s="91" t="s">
-        <v>552</v>
+        <v>746</v>
       </c>
       <c r="E17" s="82">
         <v>14</v>
       </c>
-      <c r="F17" s="83"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="83"/>
+      <c r="F17" s="83" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" s="165" t="s">
+        <v>805</v>
+      </c>
+      <c r="H17" s="83" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" thickBot="1">
       <c r="A18" s="81">
         <v>15</v>
       </c>
       <c r="B18" s="83" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="83" t="s">
-        <v>500</v>
-      </c>
-      <c r="D18" s="91" t="s">
-        <v>352</v>
+        <v>194</v>
+      </c>
+      <c r="C18" s="84" t="s">
+        <v>765</v>
+      </c>
+      <c r="D18" s="163" t="s">
+        <v>822</v>
       </c>
       <c r="E18" s="82">
         <v>15</v>
       </c>
-      <c r="F18" s="83"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="83"/>
+      <c r="F18" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="164" t="s">
+        <v>523</v>
+      </c>
+      <c r="H18" s="83" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1">
       <c r="A19" s="81">
         <v>16</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="91"/>
+      <c r="B19" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="84" t="s">
+        <v>766</v>
+      </c>
+      <c r="D19" s="163" t="s">
+        <v>823</v>
+      </c>
       <c r="E19" s="82">
         <v>16</v>
       </c>
-      <c r="F19" s="83"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="83"/>
+      <c r="F19" s="83" t="s">
+        <v>267</v>
+      </c>
+      <c r="G19" s="164" t="s">
+        <v>528</v>
+      </c>
+      <c r="H19" s="83" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1">
       <c r="A20" s="81">
         <v>17</v>
       </c>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="91"/>
+      <c r="B20" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>767</v>
+      </c>
+      <c r="D20" s="163" t="s">
+        <v>824</v>
+      </c>
       <c r="E20" s="82">
         <v>17</v>
       </c>
       <c r="F20" s="83" t="s">
-        <v>619</v>
-      </c>
-      <c r="G20" s="84" t="s">
-        <v>718</v>
+        <v>91</v>
+      </c>
+      <c r="G20" s="165" t="s">
+        <v>625</v>
       </c>
       <c r="H20" s="83" t="s">
-        <v>727</v>
+        <v>821</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1">
       <c r="A21" s="81">
         <v>18</v>
       </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="91"/>
+      <c r="B21" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>500</v>
+      </c>
+      <c r="D21" s="91" t="s">
+        <v>10</v>
+      </c>
       <c r="E21" s="82">
         <v>18</v>
       </c>
-      <c r="F21" s="83" t="s">
-        <v>619</v>
-      </c>
-      <c r="G21" s="84" t="s">
-        <v>718</v>
-      </c>
-      <c r="H21" s="83" t="s">
-        <v>505</v>
-      </c>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="83"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" thickBot="1">
       <c r="A22" s="81">
         <v>19</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="91"/>
+      <c r="B22" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>509</v>
+      </c>
+      <c r="D22" s="91" t="s">
+        <v>8</v>
+      </c>
       <c r="E22" s="82">
         <v>19</v>
       </c>
-      <c r="F22" s="83" t="s">
-        <v>719</v>
-      </c>
-      <c r="G22" s="84" t="s">
-        <v>718</v>
-      </c>
-      <c r="H22" s="83" t="s">
-        <v>720</v>
-      </c>
+      <c r="F22" s="83"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="83"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" thickBot="1">
       <c r="A23" s="81">
         <v>20</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="91"/>
+      <c r="B23" s="83" t="s">
+        <v>558</v>
+      </c>
+      <c r="C23" s="84"/>
+      <c r="D23" s="91" t="s">
+        <v>578</v>
+      </c>
       <c r="E23" s="82">
         <v>20</v>
       </c>
-      <c r="F23" s="83" t="s">
-        <v>717</v>
-      </c>
-      <c r="G23" s="84" t="s">
-        <v>718</v>
-      </c>
-      <c r="H23" s="83" t="s">
-        <v>728</v>
-      </c>
+      <c r="F23" s="83"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="83"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="85"/>
@@ -8322,7 +9018,7 @@
       <c r="G24" s="86"/>
       <c r="H24" s="87"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="85"/>
       <c r="B25" s="86"/>
       <c r="C25" s="86"/>
@@ -8582,7 +9278,7 @@
       <c r="G50" s="86"/>
       <c r="H50" s="87"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" ht="10.5" customHeight="1">
       <c r="A51" s="85"/>
       <c r="B51" s="86"/>
       <c r="C51" s="86"/>
@@ -8592,7 +9288,7 @@
       <c r="G51" s="86"/>
       <c r="H51" s="87"/>
     </row>
-    <row r="52" spans="1:8" ht="24" customHeight="1" thickBot="1">
+    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1">
       <c r="A52" s="88"/>
       <c r="B52" s="89"/>
       <c r="C52" s="89"/>
@@ -8610,10 +9306,11 @@
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P13"/>
   <sheetViews>
@@ -8833,7 +9530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -8850,14 +9547,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="130" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="104"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="132"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -8868,16 +9565,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="133" t="s">
         <v>314</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="105" t="s">
+      <c r="B3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="133" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="107"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="135"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -9130,7 +9827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q39"/>
   <sheetViews>
@@ -9147,28 +9844,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="139" t="s">
         <v>648</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
     </row>
     <row r="2" spans="1:17" ht="15.75">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="136" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="110"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
     </row>
     <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="27"/>
@@ -9468,16 +10165,16 @@
       <c r="Q14" s="41"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="136" t="s">
         <v>320</v>
       </c>
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="110"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="137"/>
+      <c r="E15" s="137"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="138"/>
       <c r="M15" s="41"/>
       <c r="N15" s="41"/>
       <c r="O15" s="41"/>
@@ -9825,16 +10522,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:17" ht="15.75">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="136" t="s">
         <v>321</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="110"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="138"/>
     </row>
     <row r="29" spans="1:17" ht="15.75">
       <c r="A29" s="27"/>
@@ -10130,7 +10827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -10147,12 +10844,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="140" t="s">
         <v>577</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -10341,7 +11038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -10360,28 +11057,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="141" t="s">
         <v>579</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="136" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="110"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -10668,12 +11365,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="136" t="s">
         <v>324</v>
       </c>
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="110"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="138"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -10852,12 +11549,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="108" t="s">
+      <c r="A28" s="136" t="s">
         <v>325</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="138"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -11037,7 +11734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
@@ -11059,40 +11756,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="102" t="s">
-        <v>744</v>
-      </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
+      <c r="A1" s="130" t="s">
+        <v>732</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="132"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="114"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="116"/>
+      <c r="A2" s="142"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="144"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="145" t="s">
         <v>395</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="117" t="s">
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="145" t="s">
         <v>396</v>
       </c>
-      <c r="F3" s="118"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="148"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="76">
@@ -11408,7 +12105,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="77" t="s">
-        <v>746</v>
+        <v>734</v>
       </c>
       <c r="D16" s="79" t="s">
         <v>341</v>
@@ -11434,7 +12131,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="77" t="s">
-        <v>746</v>
+        <v>734</v>
       </c>
       <c r="D17" s="79" t="s">
         <v>341</v>
@@ -11603,7 +12300,7 @@
         <v>21</v>
       </c>
       <c r="F24" s="75" t="s">
-        <v>745</v>
+        <v>733</v>
       </c>
       <c r="G24" s="77" t="s">
         <v>523</v>
@@ -11769,7 +12466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -11791,40 +12488,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="149" t="s">
         <v>536</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="115"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="145" t="s">
         <v>395</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="117" t="s">
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="145" t="s">
         <v>396</v>
       </c>
-      <c r="F3" s="118"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="120"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="148"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="76">
@@ -12335,576 +13032,4 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="122" t="s">
-        <v>329</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="123"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="105" t="s">
-        <v>330</v>
-      </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="105" t="s">
-        <v>331</v>
-      </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="107"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A4" s="54">
-        <v>1</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="56" t="s">
-        <v>332</v>
-      </c>
-      <c r="D4" s="54">
-        <v>1</v>
-      </c>
-      <c r="E4" s="55" t="s">
-        <v>333</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A5" s="54">
-        <v>2</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>334</v>
-      </c>
-      <c r="D5" s="54">
-        <v>2</v>
-      </c>
-      <c r="E5" s="55" t="s">
-        <v>335</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A6" s="54">
-        <v>3</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>216</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" s="54">
-        <v>3</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>337</v>
-      </c>
-      <c r="F6" s="56" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A7" s="54">
-        <v>4</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>339</v>
-      </c>
-      <c r="D7" s="54">
-        <v>4</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>340</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A8" s="54">
-        <v>5</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="56" t="s">
-        <v>341</v>
-      </c>
-      <c r="D8" s="54">
-        <v>5</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>342</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A9" s="54">
-        <v>6</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56" t="s">
-        <v>341</v>
-      </c>
-      <c r="D9" s="54">
-        <v>6</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>343</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="54">
-        <v>7</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="56" t="s">
-        <v>345</v>
-      </c>
-      <c r="D10" s="54">
-        <v>7</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A11" s="54">
-        <v>8</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>347</v>
-      </c>
-      <c r="D11" s="54">
-        <v>8</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A12" s="54">
-        <v>9</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>268</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="D12" s="54">
-        <v>9</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="54">
-        <v>10</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>351</v>
-      </c>
-      <c r="D13" s="54">
-        <v>10</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A14" s="54">
-        <v>11</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>353</v>
-      </c>
-      <c r="D14" s="54">
-        <v>11</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>268</v>
-      </c>
-      <c r="F14" s="56" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A15" s="54">
-        <v>12</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D15" s="54">
-        <v>12</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="56" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A16" s="54">
-        <v>13</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>263</v>
-      </c>
-      <c r="C16" s="56" t="s">
-        <v>356</v>
-      </c>
-      <c r="D16" s="54">
-        <v>13</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="56" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A17" s="54">
-        <v>14</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>215</v>
-      </c>
-      <c r="C17" s="56" t="s">
-        <v>357</v>
-      </c>
-      <c r="D17" s="54">
-        <v>14</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A18" s="54">
-        <v>15</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>358</v>
-      </c>
-      <c r="D18" s="54">
-        <v>15</v>
-      </c>
-      <c r="E18" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="56" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A19" s="54">
-        <v>16</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" s="56" t="s">
-        <v>359</v>
-      </c>
-      <c r="D19" s="54">
-        <v>16</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A20" s="54">
-        <v>17</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="56" t="s">
-        <v>360</v>
-      </c>
-      <c r="D20" s="54">
-        <v>17</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>215</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="54">
-        <v>18</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="56" t="s">
-        <v>361</v>
-      </c>
-      <c r="D21" s="54">
-        <v>18</v>
-      </c>
-      <c r="E21" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="F21" s="56" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A22" s="54">
-        <v>19</v>
-      </c>
-      <c r="B22" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="56" t="s">
-        <v>362</v>
-      </c>
-      <c r="D22" s="54">
-        <v>19</v>
-      </c>
-      <c r="E22" s="55" t="s">
-        <v>155</v>
-      </c>
-      <c r="F22" s="56" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A23" s="54">
-        <v>20</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>363</v>
-      </c>
-      <c r="D23" s="54">
-        <v>20</v>
-      </c>
-      <c r="E23" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" s="56" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A24" s="54">
-        <v>21</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>364</v>
-      </c>
-      <c r="D24" s="54">
-        <v>21</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="56" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A25" s="54">
-        <v>22</v>
-      </c>
-      <c r="B25" s="55" t="s">
-        <v>200</v>
-      </c>
-      <c r="C25" s="56" t="s">
-        <v>365</v>
-      </c>
-      <c r="D25" s="54">
-        <v>22</v>
-      </c>
-      <c r="E25" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="56" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="54">
-        <v>23</v>
-      </c>
-      <c r="B26" s="55" t="s">
-        <v>159</v>
-      </c>
-      <c r="C26" s="56" t="s">
-        <v>367</v>
-      </c>
-      <c r="D26" s="54">
-        <v>23</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>202</v>
-      </c>
-      <c r="F26" s="56" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A27" s="54">
-        <v>24</v>
-      </c>
-      <c r="B27" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="56" t="s">
-        <v>369</v>
-      </c>
-      <c r="D27" s="54">
-        <v>24</v>
-      </c>
-      <c r="E27" s="55" t="s">
-        <v>226</v>
-      </c>
-      <c r="F27" s="56" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A28" s="54">
-        <v>25</v>
-      </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56" t="s">
-        <v>341</v>
-      </c>
-      <c r="D28" s="54">
-        <v>25</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>264</v>
-      </c>
-      <c r="F28" s="56" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A29" s="54">
-        <v>26</v>
-      </c>
-      <c r="B29" s="55" t="s">
-        <v>372</v>
-      </c>
-      <c r="C29" s="56" t="s">
-        <v>296</v>
-      </c>
-      <c r="D29" s="54">
-        <v>26</v>
-      </c>
-      <c r="E29" s="55" t="s">
-        <v>372</v>
-      </c>
-      <c r="F29" s="56" t="s">
-        <v>296</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chg: Added f-16 and Ka-50 presets
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="830">
   <si>
     <t>AWACS</t>
   </si>
@@ -1792,9 +1792,6 @@
     <t>RW internal #6</t>
   </si>
   <si>
-    <t>KA-50 presets OPUF V1.0</t>
-  </si>
-  <si>
     <t>MAGIC AI</t>
   </si>
   <si>
@@ -2537,6 +2534,21 @@
   </si>
   <si>
     <t>AWACS VHF Back-up</t>
+  </si>
+  <si>
+    <t>KA-50 presets OPAR V1.0</t>
+  </si>
+  <si>
+    <t>BLACK 11</t>
+  </si>
+  <si>
+    <t>GREEN 8</t>
+  </si>
+  <si>
+    <t>36.40</t>
+  </si>
+  <si>
+    <t>39.80</t>
   </si>
 </sst>
 </file>
@@ -3487,10 +3499,16 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3500,9 +3518,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3525,6 +3540,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3597,42 +3645,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3987,8 +3999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AK52"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5:AD7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4038,18 +4050,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="118" t="s">
+      <c r="R3" s="132" t="s">
         <v>292</v>
       </c>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="Z3" s="119" t="s">
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
+      <c r="Z3" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="120"/>
-      <c r="AB3" s="120"/>
-      <c r="AC3" s="120"/>
-      <c r="AD3" s="121"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="122"/>
+      <c r="AC3" s="122"/>
+      <c r="AD3" s="123"/>
     </row>
     <row r="4" spans="2:37" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4092,20 +4104,20 @@
         <v>20</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="124" t="s">
+      <c r="R4" s="125" t="s">
+        <v>750</v>
+      </c>
+      <c r="S4" s="101" t="s">
         <v>751</v>
       </c>
-      <c r="S4" s="101" t="s">
-        <v>752</v>
-      </c>
       <c r="T4" s="102" t="s">
-        <v>754</v>
-      </c>
-      <c r="V4" s="122" t="s">
+        <v>753</v>
+      </c>
+      <c r="V4" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="122"/>
-      <c r="X4" s="122"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="120"/>
       <c r="Z4" s="92" t="s">
         <v>300</v>
       </c>
@@ -4143,7 +4155,7 @@
       <c r="I5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="15" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="16" t="s">
@@ -4159,12 +4171,12 @@
         <v>32</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="125"/>
+      <c r="R5" s="126"/>
       <c r="S5" s="31" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>2</v>
@@ -4189,7 +4201,7 @@
         <v>194</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="6" spans="2:37" ht="16.5" thickBot="1">
@@ -4234,15 +4246,15 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="126"/>
+      <c r="R6" s="127"/>
       <c r="S6" s="103" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="T6" s="25" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>7</v>
@@ -4265,7 +4277,7 @@
         <v>70</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="7" spans="2:37" ht="15.75">
@@ -4313,11 +4325,11 @@
         <v>294</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="124" t="s">
-        <v>757</v>
+      <c r="R7" s="125" t="s">
+        <v>756</v>
       </c>
       <c r="S7" s="101" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="T7" s="102" t="s">
         <v>543</v>
@@ -4333,19 +4345,19 @@
       </c>
       <c r="Y7" s="97"/>
       <c r="Z7" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AA7" s="116" t="s">
         <v>91</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AC7" s="116" t="s">
         <v>140</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="8" spans="2:37" ht="15.75">
@@ -4393,9 +4405,9 @@
         <v>295</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="125"/>
+      <c r="R8" s="126"/>
       <c r="S8" s="31" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T8" s="21" t="s">
         <v>544</v>
@@ -4462,9 +4474,9 @@
         <v>296</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="126"/>
+      <c r="R9" s="127"/>
       <c r="S9" s="103" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="T9" s="25" t="s">
         <v>546</v>
@@ -4559,7 +4571,7 @@
         <v>313</v>
       </c>
       <c r="AK10" s="92" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15.75">
@@ -4607,14 +4619,14 @@
         <v>13</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="127" t="s">
+      <c r="R11" s="128" t="s">
+        <v>757</v>
+      </c>
+      <c r="S11" s="106" t="s">
+        <v>751</v>
+      </c>
+      <c r="T11" s="107" t="s">
         <v>758</v>
-      </c>
-      <c r="S11" s="106" t="s">
-        <v>752</v>
-      </c>
-      <c r="T11" s="107" t="s">
-        <v>759</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>12</v>
@@ -4632,16 +4644,16 @@
       <c r="AC11" s="98"/>
       <c r="AD11" s="98"/>
       <c r="AE11" s="98"/>
-      <c r="AF11" s="117" t="s">
-        <v>813</v>
+      <c r="AF11" s="131" t="s">
+        <v>812</v>
       </c>
       <c r="AG11" s="7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="AK11" s="7"/>
     </row>
@@ -4688,15 +4700,15 @@
       <c r="O12" s="97"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="128"/>
+      <c r="R12" s="129"/>
       <c r="S12" s="100" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T12" s="21" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V12" s="38" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="W12" s="68">
         <v>301</v>
@@ -4705,12 +4717,12 @@
       <c r="Y12" s="97"/>
       <c r="Z12" s="98"/>
       <c r="AA12" s="98"/>
-      <c r="AB12" s="119" t="s">
-        <v>743</v>
-      </c>
-      <c r="AC12" s="120"/>
-      <c r="AD12" s="121"/>
-      <c r="AF12" s="117"/>
+      <c r="AB12" s="121" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC12" s="122"/>
+      <c r="AD12" s="123"/>
+      <c r="AF12" s="131"/>
       <c r="AG12" s="7" t="s">
         <v>561</v>
       </c>
@@ -4762,15 +4774,15 @@
       <c r="O13" s="97"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="129"/>
+      <c r="R13" s="130"/>
       <c r="S13" s="108" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="T13" s="25" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="V13" s="38" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W13" s="7">
         <v>300</v>
@@ -4782,7 +4794,7 @@
       <c r="AB13" s="92"/>
       <c r="AC13" s="92"/>
       <c r="AD13" s="92"/>
-      <c r="AF13" s="117"/>
+      <c r="AF13" s="131"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
@@ -4834,20 +4846,20 @@
         <v>291</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="124" t="s">
+      <c r="R14" s="125" t="s">
+        <v>760</v>
+      </c>
+      <c r="S14" s="106" t="s">
+        <v>751</v>
+      </c>
+      <c r="T14" s="102" t="s">
         <v>761</v>
-      </c>
-      <c r="S14" s="106" t="s">
-        <v>752</v>
-      </c>
-      <c r="T14" s="102" t="s">
-        <v>762</v>
       </c>
       <c r="Y14" s="97"/>
       <c r="Z14" s="41"/>
       <c r="AA14" s="41"/>
       <c r="AB14" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="AC14" s="112" t="s">
         <v>110</v>
@@ -4855,7 +4867,7 @@
       <c r="AD14" s="38" t="s">
         <v>495</v>
       </c>
-      <c r="AF14" s="117"/>
+      <c r="AF14" s="131"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
@@ -4907,18 +4919,18 @@
         <v>304</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="125"/>
+      <c r="R15" s="126"/>
       <c r="S15" s="100" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="Y15" s="97"/>
       <c r="Z15" s="41"/>
       <c r="AA15" s="41"/>
       <c r="AB15" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="AC15" s="112" t="s">
         <v>125</v>
@@ -4968,22 +4980,22 @@
         <v>303</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="126"/>
+      <c r="R16" s="127"/>
       <c r="S16" s="108" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="T16" s="25" t="s">
-        <v>764</v>
-      </c>
-      <c r="V16" s="119" t="s">
+        <v>763</v>
+      </c>
+      <c r="V16" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="120"/>
-      <c r="X16" s="120"/>
-      <c r="Y16" s="120"/>
-      <c r="Z16" s="121"/>
+      <c r="W16" s="122"/>
+      <c r="X16" s="122"/>
+      <c r="Y16" s="122"/>
+      <c r="Z16" s="123"/>
       <c r="AB16" s="7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="AC16" s="111" t="s">
         <v>106</v>
@@ -5053,7 +5065,7 @@
         <v>313</v>
       </c>
       <c r="AB17" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="AC17" s="112" t="s">
         <v>36</v>
@@ -5112,7 +5124,7 @@
       <c r="T18" s="99"/>
       <c r="U18" s="41"/>
       <c r="V18" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="W18" s="53" t="s">
         <v>529</v>
@@ -5121,13 +5133,13 @@
         <v>101</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="Z18" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="AB18" s="7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="AC18" s="112" t="s">
         <v>153</v>
@@ -5186,22 +5198,22 @@
       <c r="T19" s="98"/>
       <c r="U19" s="41"/>
       <c r="V19" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="W19" s="53" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="X19" s="53" t="s">
         <v>150</v>
       </c>
       <c r="Y19" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="Z19" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AC19" s="111" t="s">
         <v>240</v>
@@ -5255,29 +5267,29 @@
         <v>312</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="122" t="s">
+      <c r="R20" s="120" t="s">
         <v>291</v>
       </c>
-      <c r="S20" s="122"/>
-      <c r="T20" s="122"/>
+      <c r="S20" s="120"/>
+      <c r="T20" s="120"/>
       <c r="U20" s="3"/>
       <c r="V20" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="W20" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="X20" s="53" t="s">
         <v>99</v>
       </c>
       <c r="Y20" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="Z20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="AB20" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="AC20" s="111" t="s">
         <v>198</v>
@@ -5341,22 +5353,22 @@
       </c>
       <c r="U21" s="41"/>
       <c r="V21" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="X21" s="53" t="s">
         <v>181</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="Z21" s="41" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="AB21" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="AC21" s="111" t="s">
         <v>232</v>
@@ -5418,15 +5430,15 @@
       <c r="T22" t="s">
         <v>493</v>
       </c>
-      <c r="V22" s="119" t="s">
-        <v>776</v>
-      </c>
-      <c r="W22" s="120"/>
-      <c r="X22" s="120"/>
-      <c r="Y22" s="120"/>
-      <c r="Z22" s="121"/>
+      <c r="V22" s="121" t="s">
+        <v>775</v>
+      </c>
+      <c r="W22" s="122"/>
+      <c r="X22" s="122"/>
+      <c r="Y22" s="122"/>
+      <c r="Z22" s="123"/>
       <c r="AB22" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AC22" s="112" t="s">
         <v>57</v>
@@ -5480,13 +5492,13 @@
         <v>400</v>
       </c>
       <c r="R23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="S23" s="9" t="s">
         <v>135</v>
       </c>
       <c r="T23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="V23" s="92" t="s">
         <v>300</v>
@@ -5504,7 +5516,7 @@
         <v>313</v>
       </c>
       <c r="AB23" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="AC23" s="112" t="s">
         <v>103</v>
@@ -5558,22 +5570,22 @@
         <v>452</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="W24" s="53" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="X24" s="53" t="s">
         <v>120</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="Z24" s="41" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="AB24" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AC24" s="112" t="s">
         <v>127</v>
@@ -5624,35 +5636,35 @@
       </c>
       <c r="O25" s="109"/>
       <c r="P25" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="R25" s="99"/>
       <c r="S25" s="99"/>
       <c r="T25" s="99"/>
       <c r="U25" s="41"/>
       <c r="V25" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="X25" s="53" t="s">
         <v>279</v>
       </c>
       <c r="Y25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="Z25" s="41" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="AB25" s="38" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AC25" s="112" t="s">
         <v>31</v>
       </c>
       <c r="AD25" s="38" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="26" spans="2:30">
@@ -5700,28 +5712,28 @@
       <c r="T26" s="98"/>
       <c r="U26" s="98"/>
       <c r="V26" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="W26" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="X26" s="53" t="s">
         <v>161</v>
       </c>
       <c r="Y26" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="Z26" s="41" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="AB26" s="38" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AC26" s="111" t="s">
         <v>45</v>
       </c>
       <c r="AD26" s="38" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="27" spans="2:30">
@@ -5749,7 +5761,7 @@
       <c r="I27" s="65" t="s">
         <v>283</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="15" t="s">
         <v>284</v>
       </c>
       <c r="K27" s="39" t="s">
@@ -5758,7 +5770,7 @@
       <c r="L27" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="15" t="s">
         <v>460</v>
       </c>
       <c r="N27" s="58" t="s">
@@ -5770,28 +5782,28 @@
       <c r="T27" s="41"/>
       <c r="U27" s="41"/>
       <c r="V27" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="W27" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="X27" s="53" t="s">
         <v>58</v>
       </c>
       <c r="Y27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Z27" s="41" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="AB27" s="38" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="AC27" s="111" t="s">
         <v>248</v>
       </c>
       <c r="AD27" s="38" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="28" spans="2:30">
@@ -5833,43 +5845,43 @@
       <c r="T28" s="41"/>
       <c r="U28" s="41"/>
       <c r="AB28" s="38" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AC28" s="112" t="s">
         <v>146</v>
       </c>
       <c r="AD28" s="38" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="31" spans="2:30">
-      <c r="B31" s="122" t="s">
+      <c r="B31" s="120" t="s">
         <v>309</v>
       </c>
-      <c r="C31" s="122"/>
-      <c r="D31" s="122"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="122"/>
-      <c r="G31" s="122"/>
-      <c r="H31" s="122"/>
-      <c r="J31" s="122" t="s">
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="120"/>
+      <c r="G31" s="120"/>
+      <c r="H31" s="120"/>
+      <c r="J31" s="120" t="s">
         <v>310</v>
       </c>
-      <c r="K31" s="122"/>
-      <c r="L31" s="122"/>
-      <c r="M31" s="122"/>
-      <c r="N31" s="122"/>
-      <c r="O31" s="122"/>
-      <c r="P31" s="122"/>
-      <c r="T31" s="122" t="s">
+      <c r="K31" s="120"/>
+      <c r="L31" s="120"/>
+      <c r="M31" s="120"/>
+      <c r="N31" s="120"/>
+      <c r="O31" s="120"/>
+      <c r="P31" s="120"/>
+      <c r="T31" s="120" t="s">
         <v>293</v>
       </c>
-      <c r="U31" s="122"/>
-      <c r="V31" s="122"/>
-      <c r="W31" s="122"/>
-      <c r="X31" s="122"/>
-      <c r="Y31" s="122"/>
-      <c r="Z31" s="122"/>
+      <c r="U31" s="120"/>
+      <c r="V31" s="120"/>
+      <c r="W31" s="120"/>
+      <c r="X31" s="120"/>
+      <c r="Y31" s="120"/>
+      <c r="Z31" s="120"/>
     </row>
     <row r="32" spans="2:30">
       <c r="B32" s="51" t="s">
@@ -5983,7 +5995,7 @@
         <v>423</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="V33" s="7" t="s">
         <v>414</v>
@@ -5998,7 +6010,7 @@
         <v>258</v>
       </c>
       <c r="Z33" s="7" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="34" spans="2:26">
@@ -6048,7 +6060,7 @@
         <v>432</v>
       </c>
       <c r="U34" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="V34" s="7" t="s">
         <v>414</v>
@@ -6063,7 +6075,7 @@
         <v>138</v>
       </c>
       <c r="Z34" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="35" spans="2:26">
@@ -6113,7 +6125,7 @@
         <v>438</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>414</v>
@@ -6128,7 +6140,7 @@
         <v>233</v>
       </c>
       <c r="Z35" s="7" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="36" spans="2:26">
@@ -6136,7 +6148,7 @@
         <v>433</v>
       </c>
       <c r="C36" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D36" t="s">
         <v>464</v>
@@ -6178,7 +6190,7 @@
         <v>442</v>
       </c>
       <c r="U36" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="V36" s="7" t="s">
         <v>414</v>
@@ -6193,7 +6205,7 @@
         <v>245</v>
       </c>
       <c r="Z36" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="37" spans="2:26">
@@ -6201,7 +6213,7 @@
         <v>435</v>
       </c>
       <c r="C37" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D37" t="s">
         <v>464</v>
@@ -6243,7 +6255,7 @@
         <v>446</v>
       </c>
       <c r="U37" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>414</v>
@@ -6258,7 +6270,7 @@
         <v>160</v>
       </c>
       <c r="Z37" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="38" spans="2:26">
@@ -6266,7 +6278,7 @@
         <v>201</v>
       </c>
       <c r="F38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J38" t="s">
         <v>427</v>
@@ -6293,7 +6305,7 @@
         <v>444</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>414</v>
@@ -6308,7 +6320,7 @@
         <v>148</v>
       </c>
       <c r="Z38" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="39" spans="2:26">
@@ -6316,25 +6328,25 @@
         <v>228</v>
       </c>
       <c r="F39" t="s">
-        <v>639</v>
-      </c>
-      <c r="J39" s="123" t="s">
+        <v>638</v>
+      </c>
+      <c r="J39" s="124" t="s">
         <v>490</v>
       </c>
-      <c r="K39" s="123"/>
-      <c r="L39" s="123"/>
-      <c r="M39" s="123"/>
-      <c r="N39" s="123"/>
-      <c r="O39" s="123"/>
-      <c r="P39" s="123"/>
+      <c r="K39" s="124"/>
+      <c r="L39" s="124"/>
+      <c r="M39" s="124"/>
+      <c r="N39" s="124"/>
+      <c r="O39" s="124"/>
+      <c r="P39" s="124"/>
       <c r="S39">
         <v>7</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="V39" s="7" t="s">
         <v>414</v>
@@ -6349,7 +6361,7 @@
         <v>218</v>
       </c>
       <c r="Z39" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="40" spans="2:26">
@@ -6357,16 +6369,22 @@
         <v>253</v>
       </c>
       <c r="F40" t="s">
-        <v>640</v>
+        <v>639</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="N40" t="s">
+        <v>826</v>
       </c>
       <c r="S40">
         <v>8</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>414</v>
@@ -6381,7 +6399,7 @@
         <v>274</v>
       </c>
       <c r="Z40" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="41" spans="2:26">
@@ -6389,16 +6407,22 @@
         <v>252</v>
       </c>
       <c r="F41" t="s">
-        <v>641</v>
+        <v>640</v>
+      </c>
+      <c r="M41" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="N41" t="s">
+        <v>488</v>
       </c>
       <c r="S41">
         <v>9</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="V41" s="7" t="s">
         <v>414</v>
@@ -6413,7 +6437,7 @@
         <v>217</v>
       </c>
       <c r="Z41" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="42" spans="2:26">
@@ -6421,7 +6445,13 @@
         <v>174</v>
       </c>
       <c r="F42" t="s">
-        <v>642</v>
+        <v>641</v>
+      </c>
+      <c r="M42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42" t="s">
+        <v>827</v>
       </c>
       <c r="S42">
         <v>10</v>
@@ -6441,7 +6471,7 @@
         <v>251</v>
       </c>
       <c r="Z42" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="43" spans="2:26">
@@ -6455,63 +6485,63 @@
     </row>
     <row r="44" spans="2:26">
       <c r="T44" s="7" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="U44" s="7"/>
       <c r="V44" s="7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="W44" s="113" t="s">
         <v>81</v>
       </c>
       <c r="X44" s="7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="Y44" s="114" t="s">
         <v>142</v>
       </c>
       <c r="Z44" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="45" spans="2:26">
       <c r="T45" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="W45" s="113" t="s">
         <v>134</v>
       </c>
       <c r="X45" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="Y45" s="114" t="s">
         <v>67</v>
       </c>
       <c r="Z45" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="46" spans="2:26">
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
       <c r="V46" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="W46" s="113" t="s">
         <v>112</v>
       </c>
       <c r="X46" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="Y46" s="114" t="s">
         <v>202</v>
       </c>
       <c r="Z46" s="115" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="47" spans="2:26">
@@ -6534,88 +6564,94 @@
     </row>
     <row r="49" spans="20:26">
       <c r="T49" s="7" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U49" s="7"/>
       <c r="V49" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W49" s="113" t="s">
         <v>97</v>
       </c>
       <c r="X49" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="Y49" s="114" t="s">
         <v>121</v>
       </c>
       <c r="Z49" s="7" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="50" spans="20:26">
       <c r="T50" s="7" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U50" s="7"/>
       <c r="V50" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W50" s="113" t="s">
         <v>155</v>
       </c>
       <c r="X50" s="7" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="Y50" s="114" t="s">
         <v>133</v>
       </c>
       <c r="Z50" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="51" spans="20:26">
       <c r="T51" s="7" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U51" s="7"/>
       <c r="V51" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W51" s="113" t="s">
         <v>71</v>
       </c>
       <c r="X51" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="Y51" s="114" t="s">
         <v>147</v>
       </c>
       <c r="Z51" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="52" spans="20:26">
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
       <c r="V52" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W52" s="113" t="s">
         <v>214</v>
       </c>
       <c r="X52" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="Y52" s="114" t="s">
         <v>90</v>
       </c>
       <c r="Z52" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="V22:Z22"/>
+    <mergeCell ref="V16:Z16"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="T31:Z31"/>
@@ -6626,12 +6662,6 @@
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="R11:R13"/>
     <mergeCell ref="R14:R16"/>
-    <mergeCell ref="AF11:AF14"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="V22:Z22"/>
-    <mergeCell ref="V16:Z16"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="Z3:AD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6658,34 +6688,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="162" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="151"/>
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="145" t="s">
         <v>330</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="133" t="s">
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="145" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="134"/>
-      <c r="F3" s="135"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="147"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7227,22 +7257,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="164" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="165" t="s">
         <v>374</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -7347,12 +7377,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="153" t="s">
+      <c r="B14" s="165" t="s">
         <v>391</v>
       </c>
-      <c r="C14" s="153"/>
-      <c r="D14" s="153"/>
-      <c r="E14" s="153"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="165"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -7477,257 +7507,257 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B1" s="37">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H1" s="37">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N1" s="37">
         <v>1</v>
       </c>
       <c r="O1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B2" s="37">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H2" s="37">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N2" s="37">
         <v>2</v>
       </c>
       <c r="O2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B3" s="37">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H3" s="37">
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N3" s="37">
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B4" s="37">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H4" s="37">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N4" s="37">
         <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B5" s="37">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H5" s="37">
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N5" s="37">
         <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B6" s="37">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H6" s="37">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N6" s="37">
         <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B7" s="37">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H7" s="37">
         <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N7" s="37">
         <v>7</v>
       </c>
       <c r="O7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B8" s="37">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G8" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H8" s="37">
         <v>8</v>
       </c>
       <c r="I8" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M8" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N8" s="37">
         <v>8</v>
       </c>
       <c r="O8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B9" s="37">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G9" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H9" s="37">
         <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="N9" s="74">
         <v>9</v>
@@ -7736,542 +7766,542 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B11" s="37">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H11" s="37">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N11" s="37">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B12" s="37">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G12" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H12" s="37">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N12" s="37">
         <v>2</v>
       </c>
       <c r="O12" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B13" s="37">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G13" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H13" s="37">
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N13" s="37">
         <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B14" s="37">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G14" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H14" s="37">
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N14" s="37">
         <v>4</v>
       </c>
       <c r="O14" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B15" s="37">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G15" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H15" s="37">
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M15" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N15" s="37">
         <v>5</v>
       </c>
       <c r="O15" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B16" s="37">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G16" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H16" s="37">
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M16" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N16" s="37">
         <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B17" s="37">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G17" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H17" s="37">
         <v>7</v>
       </c>
       <c r="I17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N17" s="37">
         <v>7</v>
       </c>
       <c r="O17" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B18" s="37">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G18" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H18" s="37">
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M18" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N18" s="37">
         <v>8</v>
       </c>
       <c r="O18" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B19" s="37">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G19" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H19" s="37">
         <v>9</v>
       </c>
       <c r="I19" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M19" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="N19" s="37">
         <v>9</v>
       </c>
       <c r="O19" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B21" s="37">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G21" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H21" s="37">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M21" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N21" s="37">
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B22" s="37">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G22" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H22" s="37">
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M22" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N22" s="37">
         <v>2</v>
       </c>
       <c r="O22" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B23" s="37">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G23" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H23" s="37">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N23" s="37">
         <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B24" s="37">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G24" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H24" s="37">
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N24" s="37">
         <v>4</v>
       </c>
       <c r="O24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B25" s="37">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G25" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H25" s="37">
         <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="M25" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N25" s="37">
         <v>5</v>
       </c>
       <c r="O25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B26" s="37">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G26" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H26" s="37">
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="M26" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N26" s="37">
         <v>6</v>
       </c>
       <c r="O26" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B27" s="37">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H27" s="37">
         <v>7</v>
       </c>
       <c r="I27" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="M27" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N27" s="37">
         <v>7</v>
       </c>
       <c r="O27" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B28" s="37">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H28" s="37">
         <v>8</v>
       </c>
       <c r="I28" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="M28" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N28" s="37">
         <v>8</v>
       </c>
       <c r="O28" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B29" s="37">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H29" s="74">
         <v>9</v>
       </c>
       <c r="I29" s="2"/>
       <c r="M29" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N29" s="37">
         <v>9</v>
       </c>
       <c r="O29" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B31" s="37">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G31" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H31" s="37">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N31" s="37">
         <v>1</v>
@@ -8279,22 +8309,22 @@
     </row>
     <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B32" s="37">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G32" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H32" s="37">
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N32" s="37">
         <v>2</v>
@@ -8302,22 +8332,22 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B33" s="37">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G33" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H33" s="37">
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N33" s="37">
         <v>3</v>
@@ -8325,22 +8355,22 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B34" s="37">
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G34" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H34" s="37">
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N34" s="37">
         <v>4</v>
@@ -8348,22 +8378,22 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B35" s="37">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G35" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H35" s="37">
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N35" s="37">
         <v>5</v>
@@ -8371,22 +8401,22 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B36" s="37">
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G36" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H36" s="37">
         <v>6</v>
       </c>
       <c r="I36" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N36" s="37">
         <v>6</v>
@@ -8394,22 +8424,22 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B37" s="37">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G37" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H37" s="37">
         <v>7</v>
       </c>
       <c r="I37" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N37" s="37">
         <v>7</v>
@@ -8417,20 +8447,20 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B38" s="74">
         <v>8</v>
       </c>
       <c r="C38" s="2"/>
       <c r="G38" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H38" s="37">
         <v>8</v>
       </c>
       <c r="I38" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="N38" s="37">
         <v>8</v>
@@ -8438,14 +8468,14 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B39" s="74">
         <v>9</v>
       </c>
       <c r="C39" s="2"/>
       <c r="G39" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H39" s="37">
         <v>9</v>
@@ -8463,7 +8493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -8481,40 +8511,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="154" t="s">
-        <v>814</v>
-      </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="156"/>
+      <c r="A1" s="133" t="s">
+        <v>813</v>
+      </c>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="135"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="157"/>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="159"/>
+      <c r="A2" s="136"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
+        <v>717</v>
+      </c>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140" t="s">
         <v>718</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161" t="s">
-        <v>719</v>
-      </c>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="162"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="141"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="81">
@@ -8523,7 +8553,7 @@
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
       <c r="D4" s="91" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E4" s="82">
         <v>1</v>
@@ -8531,7 +8561,7 @@
       <c r="F4" s="83"/>
       <c r="G4" s="84"/>
       <c r="H4" s="83" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.75" thickBot="1">
@@ -8551,13 +8581,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="83" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G5" s="84" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H5" s="83" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1">
@@ -8577,13 +8607,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="83" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G6" s="84" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H6" s="83" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1">
@@ -8597,19 +8627,19 @@
         <v>495</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E7" s="82">
         <v>4</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G7" s="84" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H7" s="83" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18.75" thickBot="1">
@@ -8623,19 +8653,19 @@
         <v>497</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E8" s="82">
         <v>5</v>
       </c>
       <c r="F8" s="83" t="s">
+        <v>715</v>
+      </c>
+      <c r="G8" s="84" t="s">
         <v>716</v>
       </c>
-      <c r="G8" s="84" t="s">
-        <v>717</v>
-      </c>
       <c r="H8" s="83" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.75" thickBot="1">
@@ -8649,7 +8679,7 @@
         <v>496</v>
       </c>
       <c r="D9" s="91" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E9" s="82">
         <v>6</v>
@@ -8658,10 +8688,10 @@
         <v>31</v>
       </c>
       <c r="G9" s="84" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H9" s="83" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" thickBot="1">
@@ -8675,7 +8705,7 @@
         <v>498</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E10" s="82">
         <v>7</v>
@@ -8684,10 +8714,10 @@
         <v>45</v>
       </c>
       <c r="G10" s="84" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H10" s="83" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" thickBot="1">
@@ -8701,7 +8731,7 @@
         <v>501</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E11" s="82">
         <v>8</v>
@@ -8709,11 +8739,11 @@
       <c r="F11" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="G11" s="165" t="s">
-        <v>772</v>
+      <c r="G11" s="119" t="s">
+        <v>771</v>
       </c>
       <c r="H11" s="83" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18.75" thickBot="1">
@@ -8727,7 +8757,7 @@
         <v>515</v>
       </c>
       <c r="D12" s="91" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E12" s="82">
         <v>9</v>
@@ -8736,10 +8766,10 @@
         <v>146</v>
       </c>
       <c r="G12" s="84" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H12" s="83" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18.75" thickBot="1">
@@ -8753,7 +8783,7 @@
         <v>516</v>
       </c>
       <c r="D13" s="91" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E13" s="82">
         <v>10</v>
@@ -8765,7 +8795,7 @@
         <v>389</v>
       </c>
       <c r="H13" s="83" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18.75" thickBot="1">
@@ -8779,7 +8809,7 @@
         <v>518</v>
       </c>
       <c r="D14" s="91" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E14" s="82">
         <v>11</v>
@@ -8788,10 +8818,10 @@
         <v>101</v>
       </c>
       <c r="G14" s="84" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H14" s="83" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1">
@@ -8805,7 +8835,7 @@
         <v>547</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E15" s="82">
         <v>12</v>
@@ -8813,11 +8843,11 @@
       <c r="F15" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="165" t="s">
-        <v>777</v>
+      <c r="G15" s="119" t="s">
+        <v>776</v>
       </c>
       <c r="H15" s="83" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18.75" thickBot="1">
@@ -8831,7 +8861,7 @@
         <v>548</v>
       </c>
       <c r="D16" s="91" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E16" s="82">
         <v>13</v>
@@ -8840,10 +8870,10 @@
         <v>99</v>
       </c>
       <c r="G16" s="84" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H16" s="83" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" thickBot="1">
@@ -8857,7 +8887,7 @@
         <v>549</v>
       </c>
       <c r="D17" s="91" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E17" s="82">
         <v>14</v>
@@ -8865,11 +8895,11 @@
       <c r="F17" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="G17" s="165" t="s">
-        <v>805</v>
+      <c r="G17" s="119" t="s">
+        <v>804</v>
       </c>
       <c r="H17" s="83" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" thickBot="1">
@@ -8880,10 +8910,10 @@
         <v>194</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>765</v>
-      </c>
-      <c r="D18" s="163" t="s">
-        <v>822</v>
+        <v>764</v>
+      </c>
+      <c r="D18" s="117" t="s">
+        <v>821</v>
       </c>
       <c r="E18" s="82">
         <v>15</v>
@@ -8891,11 +8921,11 @@
       <c r="F18" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="164" t="s">
+      <c r="G18" s="118" t="s">
         <v>523</v>
       </c>
       <c r="H18" s="83" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1">
@@ -8906,10 +8936,10 @@
         <v>70</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>766</v>
-      </c>
-      <c r="D19" s="163" t="s">
-        <v>823</v>
+        <v>765</v>
+      </c>
+      <c r="D19" s="117" t="s">
+        <v>822</v>
       </c>
       <c r="E19" s="82">
         <v>16</v>
@@ -8917,11 +8947,11 @@
       <c r="F19" s="83" t="s">
         <v>267</v>
       </c>
-      <c r="G19" s="164" t="s">
+      <c r="G19" s="118" t="s">
         <v>528</v>
       </c>
       <c r="H19" s="83" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1">
@@ -8932,10 +8962,10 @@
         <v>140</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>767</v>
-      </c>
-      <c r="D20" s="163" t="s">
-        <v>824</v>
+        <v>766</v>
+      </c>
+      <c r="D20" s="117" t="s">
+        <v>823</v>
       </c>
       <c r="E20" s="82">
         <v>17</v>
@@ -8943,11 +8973,11 @@
       <c r="F20" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="165" t="s">
-        <v>625</v>
+      <c r="G20" s="119" t="s">
+        <v>624</v>
       </c>
       <c r="H20" s="83" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1">
@@ -8999,7 +9029,7 @@
       </c>
       <c r="C23" s="84"/>
       <c r="D23" s="91" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E23" s="82">
         <v>20</v>
@@ -9494,7 +9524,7 @@
         <v>448</v>
       </c>
       <c r="P10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="11" spans="2:16">
@@ -9502,10 +9532,10 @@
         <v>449</v>
       </c>
       <c r="L11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="12" spans="2:16">
@@ -9513,10 +9543,10 @@
         <v>450</v>
       </c>
       <c r="L12" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P12" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="13" spans="2:16">
@@ -9547,14 +9577,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="142" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="132"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="144"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -9565,16 +9595,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="145" t="s">
         <v>314</v>
       </c>
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="133" t="s">
+      <c r="B3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="145" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="134"/>
-      <c r="F3" s="135"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="147"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -9844,28 +9874,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75">
-      <c r="A1" s="139" t="s">
-        <v>648</v>
-      </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
+      <c r="A1" s="151" t="s">
+        <v>647</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
     </row>
     <row r="2" spans="1:17" ht="15.75">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="148" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="138"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="150"/>
     </row>
     <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="27"/>
@@ -9934,7 +9964,7 @@
         <v>101</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
@@ -10000,13 +10030,13 @@
         <v>15</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G8" s="30" t="s">
         <v>91</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
@@ -10096,17 +10126,17 @@
         <v>9</v>
       </c>
       <c r="B12" s="30" t="s">
+        <v>617</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>618</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>619</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="28">
         <v>19</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>275</v>
@@ -10125,17 +10155,17 @@
         <v>10</v>
       </c>
       <c r="B13" s="30" t="s">
+        <v>619</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>620</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>621</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="28">
         <v>20</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>220</v>
@@ -10165,16 +10195,16 @@
       <c r="Q14" s="41"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="136" t="s">
+      <c r="A15" s="148" t="s">
         <v>320</v>
       </c>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="137"/>
-      <c r="G15" s="137"/>
-      <c r="H15" s="138"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="149"/>
+      <c r="F15" s="149"/>
+      <c r="G15" s="149"/>
+      <c r="H15" s="150"/>
       <c r="M15" s="41"/>
       <c r="N15" s="41"/>
       <c r="O15" s="41"/>
@@ -10472,7 +10502,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C25" s="30">
         <v>301</v>
@@ -10494,7 +10524,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C26" s="30">
         <v>300</v>
@@ -10522,16 +10552,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:17" ht="15.75">
-      <c r="A28" s="136" t="s">
+      <c r="A28" s="148" t="s">
         <v>321</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="138"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="150"/>
     </row>
     <row r="29" spans="1:17" ht="15.75">
       <c r="A29" s="27"/>
@@ -10578,7 +10608,7 @@
         <v>562</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75">
@@ -10598,7 +10628,7 @@
         <v>12</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>457</v>
@@ -10624,7 +10654,7 @@
         <v>13</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>458</v>
@@ -10638,7 +10668,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C33" s="30" t="s">
         <v>197</v>
@@ -10650,7 +10680,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>459</v>
@@ -10664,7 +10694,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>224</v>
@@ -10676,7 +10706,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>281</v>
@@ -10690,19 +10720,19 @@
         <v>6</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>201</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E35" s="28">
         <v>16</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>282</v>
@@ -10716,19 +10746,19 @@
         <v>7</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>228</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E36" s="28">
         <v>17</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>283</v>
@@ -10742,13 +10772,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C37" s="30" t="s">
         <v>253</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E37" s="28">
         <v>18</v>
@@ -10768,13 +10798,13 @@
         <v>9</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>252</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E38" s="28">
         <v>19</v>
@@ -10794,19 +10824,19 @@
         <v>10</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C39" s="30" t="s">
         <v>174</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E39" s="28">
         <v>20</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G39" s="30" t="s">
         <v>164</v>
@@ -10831,8 +10861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10844,12 +10874,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="140" t="s">
-        <v>577</v>
-      </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
+      <c r="A1" s="152" t="s">
+        <v>825</v>
+      </c>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -10975,13 +11005,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="72" t="s">
-        <v>567</v>
+        <v>341</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>132</v>
+        <v>828</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>564</v>
+        <v>826</v>
       </c>
       <c r="E10" s="42"/>
     </row>
@@ -10990,13 +11020,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="72" t="s">
-        <v>568</v>
+        <v>341</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>266</v>
+        <v>829</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>565</v>
+        <v>488</v>
       </c>
       <c r="E11" s="42"/>
     </row>
@@ -11005,13 +11035,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="72" t="s">
-        <v>569</v>
+        <v>341</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>566</v>
+        <v>827</v>
       </c>
       <c r="E12" s="42"/>
     </row>
@@ -11057,28 +11087,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="141" t="s">
-        <v>579</v>
-      </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
+      <c r="A1" s="153" t="s">
+        <v>578</v>
+      </c>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="148" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="138"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="150"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -11111,10 +11141,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>616</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>617</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="28">
@@ -11135,10 +11165,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>617</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>618</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>619</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="28">
@@ -11159,10 +11189,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>619</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>620</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>621</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="28">
@@ -11183,7 +11213,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>39</v>
@@ -11195,13 +11225,13 @@
         <v>14</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>91</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75">
@@ -11209,7 +11239,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>110</v>
@@ -11233,7 +11263,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>125</v>
@@ -11245,7 +11275,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>543</v>
@@ -11269,7 +11299,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>114</v>
@@ -11283,7 +11313,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>38</v>
@@ -11309,7 +11339,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>117</v>
@@ -11365,12 +11395,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="136" t="s">
+      <c r="A15" s="148" t="s">
         <v>324</v>
       </c>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="138"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="150"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -11549,12 +11579,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="136" t="s">
+      <c r="A28" s="148" t="s">
         <v>325</v>
       </c>
-      <c r="B28" s="137"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="138"/>
+      <c r="B28" s="149"/>
+      <c r="C28" s="149"/>
+      <c r="D28" s="150"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -11577,13 +11607,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="31" t="s">
+        <v>585</v>
+      </c>
+      <c r="C30" s="35" t="s">
         <v>586</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="D30" s="31" t="s">
         <v>587</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>588</v>
       </c>
       <c r="E30"/>
     </row>
@@ -11592,13 +11622,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="31" t="s">
+        <v>588</v>
+      </c>
+      <c r="C31" s="35" t="s">
         <v>589</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="D31" s="31" t="s">
         <v>590</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>591</v>
       </c>
       <c r="E31"/>
     </row>
@@ -11607,13 +11637,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="31" t="s">
+        <v>591</v>
+      </c>
+      <c r="C32" s="35" t="s">
         <v>592</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="D32" s="31" t="s">
         <v>593</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>594</v>
       </c>
       <c r="E32"/>
     </row>
@@ -11622,13 +11652,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="31" t="s">
+        <v>594</v>
+      </c>
+      <c r="C33" s="35" t="s">
         <v>595</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="D33" s="31" t="s">
         <v>596</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>597</v>
       </c>
       <c r="E33"/>
     </row>
@@ -11637,13 +11667,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="31" t="s">
+        <v>597</v>
+      </c>
+      <c r="C34" s="35" t="s">
         <v>598</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="D34" s="31" t="s">
         <v>599</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>600</v>
       </c>
       <c r="E34"/>
     </row>
@@ -11652,13 +11682,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="31" t="s">
+        <v>600</v>
+      </c>
+      <c r="C35" s="35" t="s">
         <v>601</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="D35" s="31" t="s">
         <v>602</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>603</v>
       </c>
       <c r="E35"/>
     </row>
@@ -11667,13 +11697,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C36" s="35" t="s">
         <v>604</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="D36" s="31" t="s">
         <v>605</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>606</v>
       </c>
       <c r="E36"/>
     </row>
@@ -11682,13 +11712,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="31" t="s">
+        <v>606</v>
+      </c>
+      <c r="C37" s="35" t="s">
         <v>607</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="D37" s="31" t="s">
         <v>608</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>609</v>
       </c>
       <c r="E37"/>
     </row>
@@ -11697,13 +11727,13 @@
         <v>9</v>
       </c>
       <c r="B38" s="31" t="s">
+        <v>609</v>
+      </c>
+      <c r="C38" s="35" t="s">
         <v>610</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="D38" s="31" t="s">
         <v>611</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>612</v>
       </c>
       <c r="E38"/>
     </row>
@@ -11712,13 +11742,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="31" t="s">
+        <v>612</v>
+      </c>
+      <c r="C39" s="35" t="s">
         <v>613</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="D39" s="31" t="s">
         <v>614</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>615</v>
       </c>
       <c r="E39"/>
     </row>
@@ -11756,40 +11786,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="130" t="s">
-        <v>732</v>
-      </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="132"/>
+      <c r="A1" s="142" t="s">
+        <v>731</v>
+      </c>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="144"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="142"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="144"/>
+      <c r="A2" s="154"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="156"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="157" t="s">
         <v>395</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="145" t="s">
+      <c r="B3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="157" t="s">
         <v>396</v>
       </c>
-      <c r="F3" s="146"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="148"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="76">
@@ -11799,7 +11829,7 @@
         <v>188</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D4" s="78" t="s">
         <v>397</v>
@@ -11823,7 +11853,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D5" s="78" t="s">
         <v>397</v>
@@ -11847,7 +11877,7 @@
         <v>238</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D6" s="78" t="s">
         <v>397</v>
@@ -11871,7 +11901,7 @@
         <v>257</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D7" s="78" t="s">
         <v>397</v>
@@ -11909,7 +11939,7 @@
         <v>106</v>
       </c>
       <c r="G8" s="77" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H8" s="78" t="s">
         <v>507</v>
@@ -12079,7 +12109,7 @@
         <v>254</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D15" s="78" t="s">
         <v>503</v>
@@ -12105,7 +12135,7 @@
         <v>64</v>
       </c>
       <c r="C16" s="77" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D16" s="79" t="s">
         <v>341</v>
@@ -12131,7 +12161,7 @@
         <v>64</v>
       </c>
       <c r="C17" s="77" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D17" s="79" t="s">
         <v>341</v>
@@ -12205,7 +12235,7 @@
         <v>127</v>
       </c>
       <c r="C20" s="77" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D20" s="78" t="s">
         <v>552</v>
@@ -12300,7 +12330,7 @@
         <v>21</v>
       </c>
       <c r="F24" s="75" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G24" s="77" t="s">
         <v>523</v>
@@ -12488,40 +12518,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="161" t="s">
         <v>536</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
+      <c r="A2" s="155"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="157" t="s">
         <v>395</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="145" t="s">
+      <c r="B3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="157" t="s">
         <v>396</v>
       </c>
-      <c r="F3" s="146"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="148"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="76">
@@ -12531,7 +12561,7 @@
         <v>188</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D4" s="78" t="s">
         <v>397</v>
@@ -12555,7 +12585,7 @@
         <v>260</v>
       </c>
       <c r="C5" s="77" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D5" s="78" t="s">
         <v>397</v>
@@ -12579,7 +12609,7 @@
         <v>238</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D6" s="78" t="s">
         <v>397</v>
@@ -12603,7 +12633,7 @@
         <v>257</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D7" s="78" t="s">
         <v>397</v>
@@ -12641,7 +12671,7 @@
         <v>106</v>
       </c>
       <c r="G8" s="77" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H8" s="78" t="s">
         <v>507</v>
@@ -12811,7 +12841,7 @@
         <v>254</v>
       </c>
       <c r="C15" s="77" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D15" s="78" t="s">
         <v>503</v>
@@ -12937,7 +12967,7 @@
         <v>127</v>
       </c>
       <c r="C20" s="77" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D20" s="78" t="s">
         <v>552</v>

</xml_diff>

<commit_message>
chg: Added KA-50 and A-10 with presets
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="811">
   <si>
     <t>AWACS</t>
   </si>
@@ -2486,6 +2486,12 @@
   </si>
   <si>
     <t>A-10C presets  - OPAR v 1.1</t>
+  </si>
+  <si>
+    <t>TUSK</t>
+  </si>
+  <si>
+    <t>UZI</t>
   </si>
 </sst>
 </file>
@@ -3443,10 +3449,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3456,9 +3460,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3481,6 +3482,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3581,7 +3588,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3986,11 +3992,11 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="121" t="s">
+      <c r="R3" s="133" t="s">
         <v>287</v>
       </c>
-      <c r="S3" s="121"/>
-      <c r="T3" s="121"/>
+      <c r="S3" s="133"/>
+      <c r="T3" s="133"/>
       <c r="Z3" s="122" t="s">
         <v>9</v>
       </c>
@@ -4040,7 +4046,7 @@
         <v>15</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="127" t="s">
+      <c r="R4" s="126" t="s">
         <v>708</v>
       </c>
       <c r="S4" s="100" t="s">
@@ -4049,11 +4055,11 @@
       <c r="T4" s="101" t="s">
         <v>711</v>
       </c>
-      <c r="V4" s="125" t="s">
+      <c r="V4" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="125"/>
-      <c r="X4" s="125"/>
+      <c r="W4" s="121"/>
+      <c r="X4" s="121"/>
       <c r="Z4" s="91" t="s">
         <v>295</v>
       </c>
@@ -4107,7 +4113,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="128"/>
+      <c r="R5" s="127"/>
       <c r="S5" s="31" t="s">
         <v>674</v>
       </c>
@@ -4185,7 +4191,7 @@
         <v>726</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="129"/>
+      <c r="R6" s="128"/>
       <c r="S6" s="102" t="s">
         <v>710</v>
       </c>
@@ -4261,7 +4267,7 @@
         <v>289</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="127" t="s">
+      <c r="R7" s="126" t="s">
         <v>714</v>
       </c>
       <c r="S7" s="100" t="s">
@@ -4341,7 +4347,7 @@
         <v>290</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="128"/>
+      <c r="R8" s="127"/>
       <c r="S8" s="31" t="s">
         <v>674</v>
       </c>
@@ -4410,7 +4416,7 @@
         <v>291</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="129"/>
+      <c r="R9" s="128"/>
       <c r="S9" s="102" t="s">
         <v>710</v>
       </c>
@@ -4555,7 +4561,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="130" t="s">
+      <c r="R11" s="129" t="s">
         <v>715</v>
       </c>
       <c r="S11" s="105" t="s">
@@ -4580,7 +4586,7 @@
       <c r="AC11" s="97"/>
       <c r="AD11" s="97"/>
       <c r="AE11" s="97"/>
-      <c r="AF11" s="120" t="s">
+      <c r="AF11" s="132" t="s">
         <v>770</v>
       </c>
       <c r="AG11" s="7" t="s">
@@ -4636,7 +4642,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="131"/>
+      <c r="R12" s="130"/>
       <c r="S12" s="99" t="s">
         <v>674</v>
       </c>
@@ -4658,7 +4664,7 @@
       </c>
       <c r="AC12" s="123"/>
       <c r="AD12" s="124"/>
-      <c r="AF12" s="120"/>
+      <c r="AF12" s="132"/>
       <c r="AG12" s="7" t="s">
         <v>552</v>
       </c>
@@ -4710,7 +4716,7 @@
       <c r="O13" s="96"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="132"/>
+      <c r="R13" s="131"/>
       <c r="S13" s="107" t="s">
         <v>710</v>
       </c>
@@ -4730,7 +4736,7 @@
       <c r="AB13" s="91"/>
       <c r="AC13" s="91"/>
       <c r="AD13" s="91"/>
-      <c r="AF13" s="120"/>
+      <c r="AF13" s="132"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
@@ -4782,7 +4788,7 @@
         <v>286</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="127" t="s">
+      <c r="R14" s="126" t="s">
         <v>718</v>
       </c>
       <c r="S14" s="105" t="s">
@@ -4803,7 +4809,7 @@
       <c r="AD14" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="AF14" s="120"/>
+      <c r="AF14" s="132"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
@@ -4855,7 +4861,7 @@
         <v>299</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="128"/>
+      <c r="R15" s="127"/>
       <c r="S15" s="99" t="s">
         <v>674</v>
       </c>
@@ -4916,7 +4922,7 @@
         <v>298</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="129"/>
+      <c r="R16" s="128"/>
       <c r="S16" s="107" t="s">
         <v>710</v>
       </c>
@@ -5203,11 +5209,11 @@
         <v>307</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="125" t="s">
+      <c r="R20" s="121" t="s">
         <v>286</v>
       </c>
-      <c r="S20" s="125"/>
-      <c r="T20" s="125"/>
+      <c r="S20" s="121"/>
+      <c r="T20" s="121"/>
       <c r="U20" s="3"/>
       <c r="V20" t="s">
         <v>742</v>
@@ -5791,33 +5797,33 @@
       </c>
     </row>
     <row r="31" spans="2:30">
-      <c r="B31" s="125" t="s">
+      <c r="B31" s="121" t="s">
         <v>304</v>
       </c>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="125"/>
-      <c r="H31" s="125"/>
-      <c r="J31" s="125" t="s">
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
+      <c r="G31" s="121"/>
+      <c r="H31" s="121"/>
+      <c r="J31" s="121" t="s">
         <v>305</v>
       </c>
-      <c r="K31" s="125"/>
-      <c r="L31" s="125"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="125"/>
-      <c r="O31" s="125"/>
-      <c r="P31" s="125"/>
-      <c r="T31" s="125" t="s">
+      <c r="K31" s="121"/>
+      <c r="L31" s="121"/>
+      <c r="M31" s="121"/>
+      <c r="N31" s="121"/>
+      <c r="O31" s="121"/>
+      <c r="P31" s="121"/>
+      <c r="T31" s="121" t="s">
         <v>288</v>
       </c>
-      <c r="U31" s="125"/>
-      <c r="V31" s="125"/>
-      <c r="W31" s="125"/>
-      <c r="X31" s="125"/>
-      <c r="Y31" s="125"/>
-      <c r="Z31" s="125"/>
+      <c r="U31" s="121"/>
+      <c r="V31" s="121"/>
+      <c r="W31" s="121"/>
+      <c r="X31" s="121"/>
+      <c r="Y31" s="121"/>
+      <c r="Z31" s="121"/>
     </row>
     <row r="32" spans="2:30">
       <c r="B32" s="51" t="s">
@@ -6266,15 +6272,15 @@
       <c r="F39" t="s">
         <v>627</v>
       </c>
-      <c r="J39" s="126" t="s">
+      <c r="J39" s="125" t="s">
         <v>485</v>
       </c>
-      <c r="K39" s="126"/>
-      <c r="L39" s="126"/>
-      <c r="M39" s="126"/>
-      <c r="N39" s="126"/>
-      <c r="O39" s="126"/>
-      <c r="P39" s="126"/>
+      <c r="K39" s="125"/>
+      <c r="L39" s="125"/>
+      <c r="M39" s="125"/>
+      <c r="N39" s="125"/>
+      <c r="O39" s="125"/>
+      <c r="P39" s="125"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -6582,6 +6588,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="V22:Z22"/>
+    <mergeCell ref="V16:Z16"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="T31:Z31"/>
@@ -6592,12 +6604,6 @@
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="R11:R13"/>
     <mergeCell ref="R14:R16"/>
-    <mergeCell ref="AF11:AF14"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="V22:Z22"/>
-    <mergeCell ref="V16:Z16"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="Z3:AD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6624,34 +6630,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="163" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
+      <c r="A2" s="164"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="164"/>
+      <c r="F2" s="164"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="146" t="s">
         <v>325</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="145" t="s">
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="146" t="s">
         <v>326</v>
       </c>
-      <c r="E3" s="146"/>
-      <c r="F3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="148"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7193,22 +7199,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="165" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="166" t="s">
         <v>369</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -7313,12 +7319,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="166" t="s">
         <v>386</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
-      <c r="E14" s="165"/>
+      <c r="C14" s="166"/>
+      <c r="D14" s="166"/>
+      <c r="E14" s="166"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -7428,15 +7434,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>805</v>
       </c>
@@ -7452,8 +7458,38 @@
       <c r="E1" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H1" t="s">
+        <v>802</v>
+      </c>
+      <c r="I1" t="s">
+        <v>801</v>
+      </c>
+      <c r="J1" t="s">
+        <v>803</v>
+      </c>
+      <c r="K1" t="s">
+        <v>804</v>
+      </c>
+      <c r="M1" t="s">
+        <v>805</v>
+      </c>
+      <c r="N1" t="s">
+        <v>802</v>
+      </c>
+      <c r="O1" t="s">
+        <v>801</v>
+      </c>
+      <c r="P1" t="s">
+        <v>803</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>798</v>
       </c>
@@ -7469,20 +7505,122 @@
       <c r="E2" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="s">
+        <v>809</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>111</v>
+      </c>
+      <c r="J2" t="s">
+        <v>459</v>
+      </c>
+      <c r="K2" t="s">
+        <v>800</v>
+      </c>
+      <c r="M2" t="s">
+        <v>810</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>211</v>
+      </c>
+      <c r="P2" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="C3">
         <v>412</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" t="s">
+        <v>799</v>
+      </c>
+      <c r="E3" t="s">
+        <v>800</v>
+      </c>
+      <c r="I3">
+        <v>112</v>
+      </c>
+      <c r="J3" t="s">
+        <v>459</v>
+      </c>
+      <c r="K3" t="s">
+        <v>800</v>
+      </c>
+      <c r="O3">
+        <v>212</v>
+      </c>
+      <c r="P3" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="C4">
         <v>413</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" t="s">
+        <v>799</v>
+      </c>
+      <c r="E4" t="s">
+        <v>800</v>
+      </c>
+      <c r="I4">
+        <v>113</v>
+      </c>
+      <c r="J4" t="s">
+        <v>459</v>
+      </c>
+      <c r="K4" t="s">
+        <v>800</v>
+      </c>
+      <c r="O4">
+        <v>213</v>
+      </c>
+      <c r="P4" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="C5">
         <v>414</v>
+      </c>
+      <c r="D5" t="s">
+        <v>799</v>
+      </c>
+      <c r="E5" t="s">
+        <v>800</v>
+      </c>
+      <c r="I5">
+        <v>114</v>
+      </c>
+      <c r="J5" t="s">
+        <v>459</v>
+      </c>
+      <c r="K5" t="s">
+        <v>800</v>
+      </c>
+      <c r="O5">
+        <v>214</v>
+      </c>
+      <c r="P5" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -7512,40 +7650,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="134" t="s">
         <v>771</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="135"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="136"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="136"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="138"/>
+      <c r="A2" s="137"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="139"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="140" t="s">
         <v>675</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140" t="s">
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141" t="s">
         <v>676</v>
       </c>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="142"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="80">
@@ -8578,14 +8716,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>323</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="144"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="145"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -8596,16 +8734,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="146" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="146"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="145" t="s">
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="146" t="s">
         <v>310</v>
       </c>
-      <c r="E3" s="146"/>
-      <c r="F3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="148"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -8862,7 +9000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -8875,28 +9013,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="152" t="s">
         <v>808</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="150"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -9171,16 +9309,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="148" t="s">
+      <c r="A15" s="149" t="s">
         <v>315</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="149"/>
-      <c r="F15" s="149"/>
-      <c r="G15" s="149"/>
-      <c r="H15" s="150"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="151"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -9225,7 +9363,7 @@
       <c r="H17" s="30" t="s">
         <v>513</v>
       </c>
-      <c r="K17" s="166"/>
+      <c r="K17" s="120"/>
     </row>
     <row r="18" spans="1:11" ht="15.75">
       <c r="A18" s="28">
@@ -9470,16 +9608,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="149" t="s">
         <v>316</v>
       </c>
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="149"/>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
-      <c r="G28" s="149"/>
-      <c r="H28" s="150"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="151"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -9792,12 +9930,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="153" t="s">
         <v>783</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -10005,28 +10143,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="154" t="s">
         <v>569</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="149" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="150"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -10313,12 +10451,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="148" t="s">
+      <c r="A15" s="149" t="s">
         <v>319</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="149"/>
-      <c r="D15" s="150"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="151"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -10497,12 +10635,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="149" t="s">
         <v>320</v>
       </c>
-      <c r="B28" s="149"/>
-      <c r="C28" s="149"/>
-      <c r="D28" s="150"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="151"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -10704,40 +10842,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>689</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="144"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="145"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="154"/>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="156"/>
+      <c r="A2" s="155"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="158" t="s">
         <v>390</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="157" t="s">
+      <c r="B3" s="159"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="158" t="s">
         <v>391</v>
       </c>
-      <c r="F3" s="158"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="160"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">
@@ -11436,40 +11574,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="162" t="s">
         <v>530</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="155"/>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
+      <c r="A2" s="156"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="158" t="s">
         <v>390</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="157" t="s">
+      <c r="B3" s="159"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="158" t="s">
         <v>391</v>
       </c>
-      <c r="F3" s="158"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="160"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">

</xml_diff>

<commit_message>
insert Carrier CV72 ffrequency
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFE26CA-1836-44C6-96A9-AE0689FE6648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="7320" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="31920" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Forfatter</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="AB12" authorId="0">
+    <comment ref="AB12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -40,7 +41,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="812">
   <si>
     <t>AWACS</t>
   </si>
@@ -2492,13 +2493,16 @@
   </si>
   <si>
     <t>UZI</t>
+  </si>
+  <si>
+    <t>CV72</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3202,7 +3206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3450,7 +3454,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3460,6 +3467,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3482,12 +3492,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3588,6 +3592,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3599,6 +3604,14 @@
       <color rgb="FF891515"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3619,7 +3632,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPr id="2050" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3655,7 +3674,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3697,7 +3716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3729,9 +3748,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3763,6 +3800,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3938,14 +3993,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AK52"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:T16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="16" max="16" width="14.42578125" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -3956,7 +4011,7 @@
     <col min="34" max="34" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:37" ht="15.75" thickBot="1">
+    <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="59">
         <v>1</v>
       </c>
@@ -3992,20 +4047,20 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="133" t="s">
+      <c r="R3" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="S3" s="133"/>
-      <c r="T3" s="133"/>
-      <c r="Z3" s="122" t="s">
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="Z3" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="123"/>
-      <c r="AB3" s="123"/>
-      <c r="AC3" s="123"/>
-      <c r="AD3" s="124"/>
-    </row>
-    <row r="4" spans="2:37" ht="15.75">
+      <c r="AA3" s="124"/>
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="124"/>
+      <c r="AD3" s="125"/>
+    </row>
+    <row r="4" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="57" t="s">
         <v>15</v>
       </c>
@@ -4046,7 +4101,7 @@
         <v>15</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="126" t="s">
+      <c r="R4" s="128" t="s">
         <v>708</v>
       </c>
       <c r="S4" s="100" t="s">
@@ -4055,11 +4110,11 @@
       <c r="T4" s="101" t="s">
         <v>711</v>
       </c>
-      <c r="V4" s="121" t="s">
+      <c r="V4" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="121"/>
-      <c r="X4" s="121"/>
+      <c r="W4" s="126"/>
+      <c r="X4" s="126"/>
       <c r="Z4" s="91" t="s">
         <v>295</v>
       </c>
@@ -4072,7 +4127,7 @@
       </c>
       <c r="AD4" s="91"/>
     </row>
-    <row r="5" spans="2:37" ht="15.75">
+    <row r="5" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="57" t="s">
         <v>27</v>
       </c>
@@ -4113,7 +4168,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="127"/>
+      <c r="R5" s="129"/>
       <c r="S5" s="31" t="s">
         <v>674</v>
       </c>
@@ -4146,7 +4201,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="6" spans="2:37" ht="16.5" thickBot="1">
+    <row r="6" spans="2:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="57" t="s">
         <v>39</v>
       </c>
@@ -4191,7 +4246,7 @@
         <v>726</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="128"/>
+      <c r="R6" s="130"/>
       <c r="S6" s="102" t="s">
         <v>710</v>
       </c>
@@ -4222,7 +4277,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="7" spans="2:37" ht="15.75">
+    <row r="7" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="57" t="s">
         <v>51</v>
       </c>
@@ -4267,7 +4322,7 @@
         <v>289</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="126" t="s">
+      <c r="R7" s="128" t="s">
         <v>714</v>
       </c>
       <c r="S7" s="100" t="s">
@@ -4302,7 +4357,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="8" spans="2:37" ht="15.75">
+    <row r="8" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="57" t="s">
         <v>63</v>
       </c>
@@ -4347,7 +4402,7 @@
         <v>290</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="127"/>
+      <c r="R8" s="129"/>
       <c r="S8" s="31" t="s">
         <v>674</v>
       </c>
@@ -4371,7 +4426,7 @@
       <c r="AE8" s="41"/>
       <c r="AF8" s="41"/>
     </row>
-    <row r="9" spans="2:37" ht="16.5" thickBot="1">
+    <row r="9" spans="2:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="57" t="s">
         <v>75</v>
       </c>
@@ -4416,7 +4471,7 @@
         <v>291</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="128"/>
+      <c r="R9" s="130"/>
       <c r="S9" s="102" t="s">
         <v>710</v>
       </c>
@@ -4437,7 +4492,7 @@
       <c r="AE9" s="41"/>
       <c r="AF9" s="41"/>
     </row>
-    <row r="10" spans="2:37" ht="16.5" thickBot="1">
+    <row r="10" spans="2:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="57" t="s">
         <v>87</v>
       </c>
@@ -4516,7 +4571,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="11" spans="2:37" ht="15.75">
+    <row r="11" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="57" t="s">
         <v>99</v>
       </c>
@@ -4561,7 +4616,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="129" t="s">
+      <c r="R11" s="131" t="s">
         <v>715</v>
       </c>
       <c r="S11" s="105" t="s">
@@ -4586,20 +4641,26 @@
       <c r="AC11" s="97"/>
       <c r="AD11" s="97"/>
       <c r="AE11" s="97"/>
-      <c r="AF11" s="132" t="s">
+      <c r="AF11" s="121" t="s">
         <v>770</v>
       </c>
       <c r="AG11" s="7" t="s">
         <v>768</v>
       </c>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
+      <c r="AH11" s="167">
+        <v>309100</v>
+      </c>
+      <c r="AI11" s="7" t="s">
+        <v>811</v>
+      </c>
       <c r="AJ11" s="7" t="s">
         <v>767</v>
       </c>
-      <c r="AK11" s="7"/>
-    </row>
-    <row r="12" spans="2:37" ht="15.75">
+      <c r="AK11" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="57" t="s">
         <v>111</v>
       </c>
@@ -4642,7 +4703,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="130"/>
+      <c r="R12" s="132"/>
       <c r="S12" s="99" t="s">
         <v>674</v>
       </c>
@@ -4659,12 +4720,12 @@
       <c r="Y12" s="96"/>
       <c r="Z12" s="97"/>
       <c r="AA12" s="97"/>
-      <c r="AB12" s="122" t="s">
+      <c r="AB12" s="123" t="s">
         <v>700</v>
       </c>
-      <c r="AC12" s="123"/>
-      <c r="AD12" s="124"/>
-      <c r="AF12" s="132"/>
+      <c r="AC12" s="124"/>
+      <c r="AD12" s="125"/>
+      <c r="AF12" s="121"/>
       <c r="AG12" s="7" t="s">
         <v>552</v>
       </c>
@@ -4673,7 +4734,7 @@
       <c r="AJ12" s="7"/>
       <c r="AK12" s="7"/>
     </row>
-    <row r="13" spans="2:37" ht="16.5" thickBot="1">
+    <row r="13" spans="2:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="57" t="s">
         <v>123</v>
       </c>
@@ -4716,7 +4777,7 @@
       <c r="O13" s="96"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="131"/>
+      <c r="R13" s="133"/>
       <c r="S13" s="107" t="s">
         <v>710</v>
       </c>
@@ -4736,14 +4797,14 @@
       <c r="AB13" s="91"/>
       <c r="AC13" s="91"/>
       <c r="AD13" s="91"/>
-      <c r="AF13" s="132"/>
+      <c r="AF13" s="121"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
       <c r="AJ13" s="7"/>
       <c r="AK13" s="7"/>
     </row>
-    <row r="14" spans="2:37" ht="15.75">
+    <row r="14" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="57" t="s">
         <v>134</v>
       </c>
@@ -4788,7 +4849,7 @@
         <v>286</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="126" t="s">
+      <c r="R14" s="128" t="s">
         <v>718</v>
       </c>
       <c r="S14" s="105" t="s">
@@ -4809,14 +4870,14 @@
       <c r="AD14" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="AF14" s="132"/>
+      <c r="AF14" s="121"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="7"/>
       <c r="AK14" s="7"/>
     </row>
-    <row r="15" spans="2:37" ht="15.75">
+    <row r="15" spans="2:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="57" t="s">
         <v>146</v>
       </c>
@@ -4861,7 +4922,7 @@
         <v>299</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="127"/>
+      <c r="R15" s="129"/>
       <c r="S15" s="99" t="s">
         <v>674</v>
       </c>
@@ -4881,7 +4942,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="16" spans="2:37" ht="16.5" thickBot="1">
+    <row r="16" spans="2:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="61">
         <v>1</v>
@@ -4922,20 +4983,20 @@
         <v>298</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="128"/>
+      <c r="R16" s="130"/>
       <c r="S16" s="107" t="s">
         <v>710</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="V16" s="122" t="s">
+      <c r="V16" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="123"/>
-      <c r="X16" s="123"/>
-      <c r="Y16" s="123"/>
-      <c r="Z16" s="124"/>
+      <c r="W16" s="124"/>
+      <c r="X16" s="124"/>
+      <c r="Y16" s="124"/>
+      <c r="Z16" s="125"/>
       <c r="AB16" s="7" t="s">
         <v>694</v>
       </c>
@@ -4946,7 +5007,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="17" spans="2:30">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="57" t="s">
         <v>158</v>
       </c>
@@ -5016,7 +5077,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="18" spans="2:30">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="57" t="s">
         <v>170</v>
       </c>
@@ -5090,7 +5151,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="19" spans="2:30">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="57" t="s">
         <v>182</v>
       </c>
@@ -5164,7 +5225,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="20" spans="2:30">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" s="57" t="s">
         <v>194</v>
       </c>
@@ -5209,11 +5270,11 @@
         <v>307</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="121" t="s">
+      <c r="R20" s="126" t="s">
         <v>286</v>
       </c>
-      <c r="S20" s="121"/>
-      <c r="T20" s="121"/>
+      <c r="S20" s="126"/>
+      <c r="T20" s="126"/>
       <c r="U20" s="3"/>
       <c r="V20" t="s">
         <v>742</v>
@@ -5240,7 +5301,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="21" spans="2:30">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="57" t="s">
         <v>206</v>
       </c>
@@ -5319,7 +5380,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="22" spans="2:30">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B22" s="57" t="s">
         <v>218</v>
       </c>
@@ -5372,13 +5433,13 @@
       <c r="T22" t="s">
         <v>488</v>
       </c>
-      <c r="V22" s="122" t="s">
+      <c r="V22" s="123" t="s">
         <v>733</v>
       </c>
-      <c r="W22" s="123"/>
-      <c r="X22" s="123"/>
-      <c r="Y22" s="123"/>
-      <c r="Z22" s="124"/>
+      <c r="W22" s="124"/>
+      <c r="X22" s="124"/>
+      <c r="Y22" s="124"/>
+      <c r="Z22" s="125"/>
       <c r="AB22" s="7" t="s">
         <v>701</v>
       </c>
@@ -5389,7 +5450,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="23" spans="2:30">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="57" t="s">
         <v>230</v>
       </c>
@@ -5467,7 +5528,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="24" spans="2:30">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="57" t="s">
         <v>242</v>
       </c>
@@ -5536,7 +5597,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="25" spans="2:30">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>254</v>
       </c>
@@ -5609,7 +5670,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="26" spans="2:30">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="57" t="s">
         <v>266</v>
       </c>
@@ -5678,7 +5739,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="27" spans="2:30">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27" s="57" t="s">
         <v>275</v>
       </c>
@@ -5748,7 +5809,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="28" spans="2:30">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C28" s="62">
         <v>1</v>
       </c>
@@ -5796,36 +5857,36 @@
         <v>730</v>
       </c>
     </row>
-    <row r="31" spans="2:30">
-      <c r="B31" s="121" t="s">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B31" s="126" t="s">
         <v>304</v>
       </c>
-      <c r="C31" s="121"/>
-      <c r="D31" s="121"/>
-      <c r="E31" s="121"/>
-      <c r="F31" s="121"/>
-      <c r="G31" s="121"/>
-      <c r="H31" s="121"/>
-      <c r="J31" s="121" t="s">
+      <c r="C31" s="126"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="126"/>
+      <c r="J31" s="126" t="s">
         <v>305</v>
       </c>
-      <c r="K31" s="121"/>
-      <c r="L31" s="121"/>
-      <c r="M31" s="121"/>
-      <c r="N31" s="121"/>
-      <c r="O31" s="121"/>
-      <c r="P31" s="121"/>
-      <c r="T31" s="121" t="s">
+      <c r="K31" s="126"/>
+      <c r="L31" s="126"/>
+      <c r="M31" s="126"/>
+      <c r="N31" s="126"/>
+      <c r="O31" s="126"/>
+      <c r="P31" s="126"/>
+      <c r="T31" s="126" t="s">
         <v>288</v>
       </c>
-      <c r="U31" s="121"/>
-      <c r="V31" s="121"/>
-      <c r="W31" s="121"/>
-      <c r="X31" s="121"/>
-      <c r="Y31" s="121"/>
-      <c r="Z31" s="121"/>
-    </row>
-    <row r="32" spans="2:30">
+      <c r="U31" s="126"/>
+      <c r="V31" s="126"/>
+      <c r="W31" s="126"/>
+      <c r="X31" s="126"/>
+      <c r="Y31" s="126"/>
+      <c r="Z31" s="126"/>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B32" s="51" t="s">
         <v>301</v>
       </c>
@@ -5890,7 +5951,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>414</v>
       </c>
@@ -5955,7 +6016,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="34" spans="2:26">
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>401</v>
       </c>
@@ -6020,7 +6081,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="35" spans="2:26">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>419</v>
       </c>
@@ -6085,7 +6146,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="36" spans="2:26">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>428</v>
       </c>
@@ -6150,7 +6211,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="37" spans="2:26">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>430</v>
       </c>
@@ -6215,7 +6276,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="38" spans="2:26">
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E38" s="10" t="s">
         <v>196</v>
       </c>
@@ -6265,22 +6326,22 @@
         <v>655</v>
       </c>
     </row>
-    <row r="39" spans="2:26">
+    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E39" s="10" t="s">
         <v>223</v>
       </c>
       <c r="F39" t="s">
         <v>627</v>
       </c>
-      <c r="J39" s="125" t="s">
+      <c r="J39" s="127" t="s">
         <v>485</v>
       </c>
-      <c r="K39" s="125"/>
-      <c r="L39" s="125"/>
-      <c r="M39" s="125"/>
-      <c r="N39" s="125"/>
-      <c r="O39" s="125"/>
-      <c r="P39" s="125"/>
+      <c r="K39" s="127"/>
+      <c r="L39" s="127"/>
+      <c r="M39" s="127"/>
+      <c r="N39" s="127"/>
+      <c r="O39" s="127"/>
+      <c r="P39" s="127"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -6306,7 +6367,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="40" spans="2:26">
+    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E40" s="10" t="s">
         <v>248</v>
       </c>
@@ -6344,7 +6405,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="41" spans="2:26">
+    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E41" s="10" t="s">
         <v>247</v>
       </c>
@@ -6382,7 +6443,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="42" spans="2:26">
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E42" s="10" t="s">
         <v>169</v>
       </c>
@@ -6416,7 +6477,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="43" spans="2:26">
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
@@ -6425,7 +6486,7 @@
       <c r="Y43" s="7"/>
       <c r="Z43" s="7"/>
     </row>
-    <row r="44" spans="2:26">
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T44" s="7" t="s">
         <v>667</v>
       </c>
@@ -6446,7 +6507,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="45" spans="2:26">
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T45" s="7" t="s">
         <v>649</v>
       </c>
@@ -6467,7 +6528,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="46" spans="2:26">
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
       <c r="V46" s="7" t="s">
@@ -6486,7 +6547,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="47" spans="2:26">
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
@@ -6495,7 +6556,7 @@
       <c r="Y47" s="7"/>
       <c r="Z47" s="7"/>
     </row>
-    <row r="48" spans="2:26">
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
@@ -6504,7 +6565,7 @@
       <c r="Y48" s="7"/>
       <c r="Z48" s="7"/>
     </row>
-    <row r="49" spans="20:26">
+    <row r="49" spans="20:26" x14ac:dyDescent="0.25">
       <c r="T49" s="7" t="s">
         <v>764</v>
       </c>
@@ -6525,7 +6586,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="50" spans="20:26">
+    <row r="50" spans="20:26" x14ac:dyDescent="0.25">
       <c r="T50" s="7" t="s">
         <v>765</v>
       </c>
@@ -6546,7 +6607,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="51" spans="20:26">
+    <row r="51" spans="20:26" x14ac:dyDescent="0.25">
       <c r="T51" s="7" t="s">
         <v>766</v>
       </c>
@@ -6567,7 +6628,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="52" spans="20:26">
+    <row r="52" spans="20:26" x14ac:dyDescent="0.25">
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
       <c r="V52" s="7" t="s">
@@ -6588,12 +6649,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AF11:AF14"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="V22:Z22"/>
-    <mergeCell ref="V16:Z16"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="T31:Z31"/>
@@ -6604,6 +6659,12 @@
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="R11:R13"/>
     <mergeCell ref="R14:R16"/>
+    <mergeCell ref="AF11:AF14"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="V22:Z22"/>
+    <mergeCell ref="V16:Z16"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="Z3:AD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6612,14 +6673,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -6629,7 +6690,7 @@
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="163" t="s">
         <v>324</v>
       </c>
@@ -6639,7 +6700,7 @@
       <c r="E1" s="163"/>
       <c r="F1" s="163"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="164"/>
       <c r="B2" s="164"/>
       <c r="C2" s="164"/>
@@ -6647,7 +6708,7 @@
       <c r="E2" s="164"/>
       <c r="F2" s="164"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="146" t="s">
         <v>325</v>
       </c>
@@ -6659,7 +6720,7 @@
       <c r="E3" s="147"/>
       <c r="F3" s="148"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54">
         <v>1</v>
       </c>
@@ -6679,7 +6740,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54">
         <v>2</v>
       </c>
@@ -6699,7 +6760,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54">
         <v>3</v>
       </c>
@@ -6719,7 +6780,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="54">
         <v>4</v>
       </c>
@@ -6739,7 +6800,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="54">
         <v>5</v>
       </c>
@@ -6757,7 +6818,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="54">
         <v>6</v>
       </c>
@@ -6775,7 +6836,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="54">
         <v>7</v>
       </c>
@@ -6795,7 +6856,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="54">
         <v>8</v>
       </c>
@@ -6815,7 +6876,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="54">
         <v>9</v>
       </c>
@@ -6835,7 +6896,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="54">
         <v>10</v>
       </c>
@@ -6855,7 +6916,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54">
         <v>11</v>
       </c>
@@ -6875,7 +6936,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="54">
         <v>12</v>
       </c>
@@ -6895,7 +6956,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="54">
         <v>13</v>
       </c>
@@ -6915,7 +6976,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="54">
         <v>14</v>
       </c>
@@ -6935,7 +6996,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="54">
         <v>15</v>
       </c>
@@ -6955,7 +7016,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="54">
         <v>16</v>
       </c>
@@ -6975,7 +7036,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="54">
         <v>17</v>
       </c>
@@ -6995,7 +7056,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="54">
         <v>18</v>
       </c>
@@ -7015,7 +7076,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="54">
         <v>19</v>
       </c>
@@ -7035,7 +7096,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="54">
         <v>20</v>
       </c>
@@ -7055,7 +7116,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="54">
         <v>21</v>
       </c>
@@ -7075,7 +7136,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="54">
         <v>22</v>
       </c>
@@ -7095,7 +7156,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="54">
         <v>23</v>
       </c>
@@ -7115,7 +7176,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="54">
         <v>24</v>
       </c>
@@ -7135,7 +7196,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="54">
         <v>25</v>
       </c>
@@ -7153,7 +7214,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="54">
         <v>26</v>
       </c>
@@ -7184,21 +7245,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="165" t="s">
         <v>368</v>
       </c>
@@ -7208,7 +7269,7 @@
       <c r="E1" s="165"/>
       <c r="F1" s="165"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="166" t="s">
         <v>369</v>
       </c>
@@ -7216,7 +7277,7 @@
       <c r="D2" s="166"/>
       <c r="E2" s="166"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="43"/>
       <c r="C3" s="44" t="s">
         <v>313</v>
@@ -7228,7 +7289,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="44" t="s">
         <v>370</v>
       </c>
@@ -7240,7 +7301,7 @@
       </c>
       <c r="E4" s="43"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="44" t="s">
         <v>372</v>
       </c>
@@ -7252,7 +7313,7 @@
       </c>
       <c r="E5" s="43"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="44" t="s">
         <v>374</v>
       </c>
@@ -7264,7 +7325,7 @@
       </c>
       <c r="E6" s="43"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
         <v>376</v>
       </c>
@@ -7278,7 +7339,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="44" t="s">
         <v>379</v>
       </c>
@@ -7292,7 +7353,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="44" t="s">
         <v>382</v>
       </c>
@@ -7306,7 +7367,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="44" t="s">
         <v>385</v>
       </c>
@@ -7318,7 +7379,7 @@
       </c>
       <c r="E10" s="43"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="166" t="s">
         <v>386</v>
       </c>
@@ -7326,7 +7387,7 @@
       <c r="D14" s="166"/>
       <c r="E14" s="166"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="43"/>
       <c r="C15" s="44" t="s">
         <v>313</v>
@@ -7338,7 +7399,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="44" t="s">
         <v>370</v>
       </c>
@@ -7350,7 +7411,7 @@
       </c>
       <c r="E16" s="43"/>
     </row>
-    <row r="17" spans="2:5" ht="18.75">
+    <row r="17" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="44" t="s">
         <v>372</v>
       </c>
@@ -7362,7 +7423,7 @@
       </c>
       <c r="E17" s="43"/>
     </row>
-    <row r="18" spans="2:5" ht="18.75">
+    <row r="18" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="44" t="s">
         <v>374</v>
       </c>
@@ -7374,7 +7435,7 @@
       </c>
       <c r="E18" s="43"/>
     </row>
-    <row r="19" spans="2:5" ht="18.75">
+    <row r="19" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="44" t="s">
         <v>376</v>
       </c>
@@ -7386,7 +7447,7 @@
       </c>
       <c r="E19" s="43"/>
     </row>
-    <row r="20" spans="2:5" ht="18.75">
+    <row r="20" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="44" t="s">
         <v>379</v>
       </c>
@@ -7398,7 +7459,7 @@
       </c>
       <c r="E20" s="43"/>
     </row>
-    <row r="21" spans="2:5" ht="18.75">
+    <row r="21" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="44" t="s">
         <v>382</v>
       </c>
@@ -7410,7 +7471,7 @@
       </c>
       <c r="E21" s="43"/>
     </row>
-    <row r="22" spans="2:5" ht="18.75">
+    <row r="22" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="44" t="s">
         <v>385</v>
       </c>
@@ -7433,16 +7494,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>805</v>
       </c>
@@ -7489,7 +7550,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>798</v>
       </c>
@@ -7536,7 +7597,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>412</v>
       </c>
@@ -7565,7 +7626,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>413</v>
       </c>
@@ -7594,7 +7655,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>414</v>
       </c>
@@ -7629,14 +7690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
@@ -7649,7 +7710,7 @@
     <col min="22" max="22" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="134" t="s">
         <v>771</v>
       </c>
@@ -7661,7 +7722,7 @@
       <c r="G1" s="135"/>
       <c r="H1" s="136"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="137"/>
       <c r="B2" s="138"/>
       <c r="C2" s="138"/>
@@ -7671,7 +7732,7 @@
       <c r="G2" s="138"/>
       <c r="H2" s="139"/>
     </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1">
+    <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="140" t="s">
         <v>675</v>
       </c>
@@ -7685,7 +7746,7 @@
       <c r="G3" s="141"/>
       <c r="H3" s="142"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" thickBot="1">
+    <row r="4" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="80">
         <v>1</v>
       </c>
@@ -7703,7 +7764,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" thickBot="1">
+    <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="80">
         <v>2</v>
       </c>
@@ -7729,7 +7790,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" thickBot="1">
+    <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80">
         <v>3</v>
       </c>
@@ -7755,7 +7816,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+    <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="80">
         <v>4</v>
       </c>
@@ -7781,7 +7842,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" thickBot="1">
+    <row r="8" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80">
         <v>5</v>
       </c>
@@ -7807,7 +7868,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" thickBot="1">
+    <row r="9" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80">
         <v>6</v>
       </c>
@@ -7833,7 +7894,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" thickBot="1">
+    <row r="10" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80">
         <v>7</v>
       </c>
@@ -7859,7 +7920,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" thickBot="1">
+    <row r="11" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80">
         <v>8</v>
       </c>
@@ -7885,7 +7946,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" thickBot="1">
+    <row r="12" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80">
         <v>9</v>
       </c>
@@ -7911,7 +7972,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" thickBot="1">
+    <row r="13" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80">
         <v>10</v>
       </c>
@@ -7937,7 +7998,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+    <row r="14" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="80">
         <v>11</v>
       </c>
@@ -7963,7 +8024,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" thickBot="1">
+    <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="80">
         <v>12</v>
       </c>
@@ -7989,7 +8050,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" thickBot="1">
+    <row r="16" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80">
         <v>13</v>
       </c>
@@ -8015,7 +8076,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" thickBot="1">
+    <row r="17" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="80">
         <v>14</v>
       </c>
@@ -8041,7 +8102,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" thickBot="1">
+    <row r="18" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="80">
         <v>15</v>
       </c>
@@ -8067,7 +8128,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" thickBot="1">
+    <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="80">
         <v>16</v>
       </c>
@@ -8093,7 +8154,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" thickBot="1">
+    <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="80">
         <v>17</v>
       </c>
@@ -8119,7 +8180,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" thickBot="1">
+    <row r="21" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80">
         <v>18</v>
       </c>
@@ -8139,7 +8200,7 @@
       <c r="G21" s="83"/>
       <c r="H21" s="82"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75" thickBot="1">
+    <row r="22" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="80">
         <v>19</v>
       </c>
@@ -8159,7 +8220,7 @@
       <c r="G22" s="83"/>
       <c r="H22" s="82"/>
     </row>
-    <row r="23" spans="1:8" ht="18.75" thickBot="1">
+    <row r="23" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="80">
         <v>20</v>
       </c>
@@ -8177,7 +8238,7 @@
       <c r="G23" s="83"/>
       <c r="H23" s="82"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="84"/>
       <c r="B24" s="85"/>
       <c r="C24" s="85"/>
@@ -8187,7 +8248,7 @@
       <c r="G24" s="85"/>
       <c r="H24" s="86"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="84"/>
       <c r="B25" s="85"/>
       <c r="C25" s="85"/>
@@ -8197,7 +8258,7 @@
       <c r="G25" s="85"/>
       <c r="H25" s="86"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="84"/>
       <c r="B26" s="85"/>
       <c r="C26" s="85"/>
@@ -8207,7 +8268,7 @@
       <c r="G26" s="85"/>
       <c r="H26" s="86"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="84"/>
       <c r="B27" s="85"/>
       <c r="C27" s="85"/>
@@ -8217,7 +8278,7 @@
       <c r="G27" s="85"/>
       <c r="H27" s="86"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="84"/>
       <c r="B28" s="85"/>
       <c r="C28" s="85"/>
@@ -8227,7 +8288,7 @@
       <c r="G28" s="85"/>
       <c r="H28" s="86"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="84"/>
       <c r="B29" s="85"/>
       <c r="C29" s="85"/>
@@ -8237,7 +8298,7 @@
       <c r="G29" s="85"/>
       <c r="H29" s="86"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="84"/>
       <c r="B30" s="85"/>
       <c r="C30" s="85"/>
@@ -8247,7 +8308,7 @@
       <c r="G30" s="85"/>
       <c r="H30" s="86"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="84"/>
       <c r="B31" s="85"/>
       <c r="C31" s="85"/>
@@ -8257,7 +8318,7 @@
       <c r="G31" s="85"/>
       <c r="H31" s="86"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="84"/>
       <c r="B32" s="85"/>
       <c r="C32" s="85"/>
@@ -8267,7 +8328,7 @@
       <c r="G32" s="85"/>
       <c r="H32" s="86"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
       <c r="B33" s="85"/>
       <c r="C33" s="85"/>
@@ -8277,7 +8338,7 @@
       <c r="G33" s="85"/>
       <c r="H33" s="86"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="84"/>
       <c r="B34" s="85"/>
       <c r="C34" s="85"/>
@@ -8287,7 +8348,7 @@
       <c r="G34" s="85"/>
       <c r="H34" s="86"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="84"/>
       <c r="B35" s="85"/>
       <c r="C35" s="85"/>
@@ -8297,7 +8358,7 @@
       <c r="G35" s="85"/>
       <c r="H35" s="86"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="84"/>
       <c r="B36" s="85"/>
       <c r="C36" s="85"/>
@@ -8307,7 +8368,7 @@
       <c r="G36" s="85"/>
       <c r="H36" s="86"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="84"/>
       <c r="B37" s="85"/>
       <c r="C37" s="85"/>
@@ -8317,7 +8378,7 @@
       <c r="G37" s="85"/>
       <c r="H37" s="86"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="84"/>
       <c r="B38" s="85"/>
       <c r="C38" s="85"/>
@@ -8327,7 +8388,7 @@
       <c r="G38" s="85"/>
       <c r="H38" s="86"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="84"/>
       <c r="B39" s="85"/>
       <c r="C39" s="85"/>
@@ -8337,7 +8398,7 @@
       <c r="G39" s="85"/>
       <c r="H39" s="86"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="84"/>
       <c r="B40" s="85"/>
       <c r="C40" s="85"/>
@@ -8347,7 +8408,7 @@
       <c r="G40" s="85"/>
       <c r="H40" s="86"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="84"/>
       <c r="B41" s="85"/>
       <c r="C41" s="85"/>
@@ -8357,7 +8418,7 @@
       <c r="G41" s="85"/>
       <c r="H41" s="86"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="84"/>
       <c r="B42" s="85"/>
       <c r="C42" s="85"/>
@@ -8367,7 +8428,7 @@
       <c r="G42" s="85"/>
       <c r="H42" s="86"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="84"/>
       <c r="B43" s="85"/>
       <c r="C43" s="85"/>
@@ -8377,7 +8438,7 @@
       <c r="G43" s="85"/>
       <c r="H43" s="86"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="84"/>
       <c r="B44" s="85"/>
       <c r="C44" s="85"/>
@@ -8387,7 +8448,7 @@
       <c r="G44" s="85"/>
       <c r="H44" s="86"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="84"/>
       <c r="B45" s="85"/>
       <c r="C45" s="85"/>
@@ -8397,7 +8458,7 @@
       <c r="G45" s="85"/>
       <c r="H45" s="86"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="84"/>
       <c r="B46" s="85"/>
       <c r="C46" s="85"/>
@@ -8407,7 +8468,7 @@
       <c r="G46" s="85"/>
       <c r="H46" s="86"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="84"/>
       <c r="B47" s="85"/>
       <c r="C47" s="85"/>
@@ -8417,7 +8478,7 @@
       <c r="G47" s="85"/>
       <c r="H47" s="86"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="84"/>
       <c r="B48" s="85"/>
       <c r="C48" s="85"/>
@@ -8427,7 +8488,7 @@
       <c r="G48" s="85"/>
       <c r="H48" s="86"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="84"/>
       <c r="B49" s="85"/>
       <c r="C49" s="85"/>
@@ -8437,7 +8498,7 @@
       <c r="G49" s="85"/>
       <c r="H49" s="86"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="84"/>
       <c r="B50" s="85"/>
       <c r="C50" s="85"/>
@@ -8447,7 +8508,7 @@
       <c r="G50" s="85"/>
       <c r="H50" s="86"/>
     </row>
-    <row r="51" spans="1:8" ht="10.5" customHeight="1">
+    <row r="51" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="84"/>
       <c r="B51" s="85"/>
       <c r="C51" s="85"/>
@@ -8457,7 +8518,7 @@
       <c r="G51" s="85"/>
       <c r="H51" s="86"/>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1">
+    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="87"/>
       <c r="B52" s="88"/>
       <c r="C52" s="88"/>
@@ -8480,16 +8541,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:P13"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4:P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>396</v>
       </c>
@@ -8512,7 +8573,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>401</v>
       </c>
@@ -8544,7 +8605,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>410</v>
       </c>
@@ -8573,7 +8634,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>419</v>
       </c>
@@ -8602,7 +8663,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>428</v>
       </c>
@@ -8622,7 +8683,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>434</v>
       </c>
@@ -8636,7 +8697,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>438</v>
       </c>
@@ -8650,7 +8711,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>442</v>
       </c>
@@ -8658,7 +8719,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>443</v>
       </c>
@@ -8666,7 +8727,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>444</v>
       </c>
@@ -8677,7 +8738,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
         <v>445</v>
       </c>
@@ -8688,7 +8749,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>446</v>
       </c>
@@ -8700,14 +8761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -8715,7 +8776,7 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="143" t="s">
         <v>323</v>
       </c>
@@ -8725,7 +8786,7 @@
       <c r="E1" s="144"/>
       <c r="F1" s="145"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -8733,7 +8794,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="146" t="s">
         <v>309</v>
       </c>
@@ -8745,7 +8806,7 @@
       <c r="E3" s="147"/>
       <c r="F3" s="148"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>1</v>
       </c>
@@ -8757,7 +8818,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>2</v>
       </c>
@@ -8769,7 +8830,7 @@
       <c r="E5" s="40"/>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -8781,7 +8842,7 @@
       <c r="E6" s="48"/>
       <c r="F6" s="47"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>4</v>
       </c>
@@ -8793,7 +8854,7 @@
       <c r="E7" s="40"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>5</v>
       </c>
@@ -8805,7 +8866,7 @@
       <c r="E8" s="40"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>6</v>
       </c>
@@ -8817,7 +8878,7 @@
       <c r="E9" s="40"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>7</v>
       </c>
@@ -8829,7 +8890,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>8</v>
       </c>
@@ -8841,7 +8902,7 @@
       <c r="E11" s="40"/>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>9</v>
       </c>
@@ -8853,7 +8914,7 @@
       <c r="E12" s="40"/>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>10</v>
       </c>
@@ -8865,7 +8926,7 @@
       <c r="E13" s="40"/>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>11</v>
       </c>
@@ -8877,7 +8938,7 @@
       <c r="E14" s="40"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>12</v>
       </c>
@@ -8889,7 +8950,7 @@
       <c r="E15" s="40"/>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>13</v>
       </c>
@@ -8901,7 +8962,7 @@
       <c r="E16" s="40"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>14</v>
       </c>
@@ -8913,7 +8974,7 @@
       <c r="E17" s="40"/>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>15</v>
       </c>
@@ -8925,7 +8986,7 @@
       <c r="E18" s="40"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>16</v>
       </c>
@@ -8937,7 +8998,7 @@
       <c r="E19" s="40"/>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>17</v>
       </c>
@@ -8949,7 +9010,7 @@
       <c r="E20" s="40"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>18</v>
       </c>
@@ -8961,7 +9022,7 @@
       <c r="E21" s="40"/>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>19</v>
       </c>
@@ -8973,7 +9034,7 @@
       <c r="E22" s="40"/>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>20</v>
       </c>
@@ -8997,14 +9058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -9012,7 +9073,7 @@
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="152" t="s">
         <v>808</v>
       </c>
@@ -9024,7 +9085,7 @@
       <c r="G1" s="152"/>
       <c r="H1" s="152"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="149" t="s">
         <v>312</v>
       </c>
@@ -9036,7 +9097,7 @@
       <c r="G2" s="150"/>
       <c r="H2" s="151"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="B3" s="28" t="s">
         <v>313</v>
@@ -9058,7 +9119,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>1</v>
       </c>
@@ -9082,7 +9143,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>2</v>
       </c>
@@ -9106,7 +9167,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>3</v>
       </c>
@@ -9130,7 +9191,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>4</v>
       </c>
@@ -9154,7 +9215,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>5</v>
       </c>
@@ -9178,7 +9239,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>6</v>
       </c>
@@ -9202,7 +9263,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>7</v>
       </c>
@@ -9228,7 +9289,7 @@
       <c r="J10" s="41"/>
       <c r="K10" s="41"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>8</v>
       </c>
@@ -9254,7 +9315,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="41"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>9</v>
       </c>
@@ -9276,7 +9337,7 @@
       </c>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>10</v>
       </c>
@@ -9298,7 +9359,7 @@
       </c>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -9308,7 +9369,7 @@
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="149" t="s">
         <v>315</v>
       </c>
@@ -9320,7 +9381,7 @@
       <c r="G15" s="150"/>
       <c r="H15" s="151"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
       <c r="B16" s="28" t="s">
         <v>313</v>
@@ -9342,7 +9403,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75">
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>1</v>
       </c>
@@ -9365,7 +9426,7 @@
       </c>
       <c r="K17" s="120"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75">
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>2</v>
       </c>
@@ -9391,7 +9452,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>3</v>
       </c>
@@ -9417,7 +9478,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75">
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
         <v>4</v>
       </c>
@@ -9443,7 +9504,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75">
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <v>5</v>
       </c>
@@ -9469,7 +9530,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75">
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <v>6</v>
       </c>
@@ -9495,7 +9556,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75">
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>7</v>
       </c>
@@ -9521,7 +9582,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75">
+    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <v>8</v>
       </c>
@@ -9547,7 +9608,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75">
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <v>9</v>
       </c>
@@ -9573,7 +9634,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75">
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="28">
         <v>10</v>
       </c>
@@ -9597,7 +9658,7 @@
       </c>
       <c r="H26" s="30"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75">
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -9607,7 +9668,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75">
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="149" t="s">
         <v>316</v>
       </c>
@@ -9619,7 +9680,7 @@
       <c r="G28" s="150"/>
       <c r="H28" s="151"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75">
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="28" t="s">
         <v>313</v>
@@ -9641,7 +9702,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75">
+    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>1</v>
       </c>
@@ -9667,7 +9728,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75">
+    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>2</v>
       </c>
@@ -9693,7 +9754,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75">
+    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="28">
         <v>3</v>
       </c>
@@ -9719,7 +9780,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75">
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>4</v>
       </c>
@@ -9745,7 +9806,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75">
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <v>5</v>
       </c>
@@ -9771,7 +9832,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75">
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>6</v>
       </c>
@@ -9797,7 +9858,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75">
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="28">
         <v>7</v>
       </c>
@@ -9823,7 +9884,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75">
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>8</v>
       </c>
@@ -9849,7 +9910,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75">
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="28">
         <v>9</v>
       </c>
@@ -9875,7 +9936,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75">
+    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <v>10</v>
       </c>
@@ -9914,14 +9975,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
@@ -9929,7 +9990,7 @@
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5">
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="153" t="s">
         <v>783</v>
       </c>
@@ -9938,7 +9999,7 @@
       <c r="D1" s="153"/>
       <c r="E1" s="42"/>
     </row>
-    <row r="2" spans="1:5" ht="28.5">
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="70"/>
       <c r="B2" s="71" t="s">
         <v>313</v>
@@ -9951,7 +10012,7 @@
       </c>
       <c r="E2" s="42"/>
     </row>
-    <row r="3" spans="1:5" ht="28.5">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="71">
         <v>1</v>
       </c>
@@ -9966,7 +10027,7 @@
       </c>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" ht="28.5">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="71">
         <v>2</v>
       </c>
@@ -9981,7 +10042,7 @@
       </c>
       <c r="E4" s="42"/>
     </row>
-    <row r="5" spans="1:5" ht="28.5">
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="71">
         <v>3</v>
       </c>
@@ -9996,7 +10057,7 @@
       </c>
       <c r="E5" s="42"/>
     </row>
-    <row r="6" spans="1:5" ht="28.5">
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="71">
         <v>4</v>
       </c>
@@ -10011,7 +10072,7 @@
       </c>
       <c r="E6" s="42"/>
     </row>
-    <row r="7" spans="1:5" ht="28.5">
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="71">
         <v>5</v>
       </c>
@@ -10026,7 +10087,7 @@
       </c>
       <c r="E7" s="42"/>
     </row>
-    <row r="8" spans="1:5" ht="28.5">
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="71">
         <v>6</v>
       </c>
@@ -10041,7 +10102,7 @@
       </c>
       <c r="E8" s="42"/>
     </row>
-    <row r="9" spans="1:5" ht="28.5">
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="71">
         <v>7</v>
       </c>
@@ -10056,7 +10117,7 @@
       </c>
       <c r="E9" s="42"/>
     </row>
-    <row r="10" spans="1:5" ht="28.5">
+    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="71">
         <v>8</v>
       </c>
@@ -10071,7 +10132,7 @@
       </c>
       <c r="E10" s="42"/>
     </row>
-    <row r="11" spans="1:5" ht="28.5">
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="71">
         <v>9</v>
       </c>
@@ -10086,7 +10147,7 @@
       </c>
       <c r="E11" s="42"/>
     </row>
-    <row r="12" spans="1:5" ht="28.5">
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="71">
         <v>10</v>
       </c>
@@ -10101,14 +10162,14 @@
       </c>
       <c r="E12" s="42"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75">
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="42"/>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -10125,14 +10186,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
@@ -10142,7 +10203,7 @@
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="154" t="s">
         <v>569</v>
       </c>
@@ -10154,7 +10215,7 @@
       <c r="G1" s="154"/>
       <c r="H1" s="154"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="149" t="s">
         <v>317</v>
       </c>
@@ -10166,7 +10227,7 @@
       <c r="G2" s="150"/>
       <c r="H2" s="151"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>318</v>
       </c>
@@ -10192,7 +10253,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>1</v>
       </c>
@@ -10216,7 +10277,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>2</v>
       </c>
@@ -10240,7 +10301,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>3</v>
       </c>
@@ -10264,7 +10325,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>4</v>
       </c>
@@ -10290,7 +10351,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>5</v>
       </c>
@@ -10314,7 +10375,7 @@
       </c>
       <c r="H8" s="30"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>6</v>
       </c>
@@ -10338,7 +10399,7 @@
       </c>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>7</v>
       </c>
@@ -10364,7 +10425,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>8</v>
       </c>
@@ -10390,7 +10451,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>9</v>
       </c>
@@ -10416,7 +10477,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>10</v>
       </c>
@@ -10440,7 +10501,7 @@
       </c>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -10450,7 +10511,7 @@
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="149" t="s">
         <v>319</v>
       </c>
@@ -10459,7 +10520,7 @@
       <c r="D15" s="151"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>318</v>
       </c>
@@ -10474,7 +10535,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:8" ht="18.75">
+    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>1</v>
       </c>
@@ -10489,7 +10550,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:8" ht="18.75">
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>2</v>
       </c>
@@ -10504,7 +10565,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:8" ht="18.75">
+    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>3</v>
       </c>
@@ -10519,7 +10580,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:8" ht="18.75">
+    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>4</v>
       </c>
@@ -10534,7 +10595,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:8" ht="18.75">
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>5</v>
       </c>
@@ -10549,7 +10610,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:8" ht="18.75">
+    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>6</v>
       </c>
@@ -10564,7 +10625,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:8" ht="18.75">
+    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="28">
         <v>7</v>
       </c>
@@ -10579,7 +10640,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:8" ht="18.75">
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="28">
         <v>8</v>
       </c>
@@ -10594,7 +10655,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:8" ht="18.75">
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="28">
         <v>9</v>
       </c>
@@ -10609,7 +10670,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:8" ht="18.75">
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="28">
         <v>10</v>
       </c>
@@ -10624,7 +10685,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -10634,7 +10695,7 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="149" t="s">
         <v>320</v>
       </c>
@@ -10643,7 +10704,7 @@
       <c r="D28" s="151"/>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>318</v>
       </c>
@@ -10658,7 +10719,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>1</v>
       </c>
@@ -10673,7 +10734,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>2</v>
       </c>
@@ -10688,7 +10749,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="28">
         <v>3</v>
       </c>
@@ -10703,7 +10764,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75">
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>4</v>
       </c>
@@ -10718,7 +10779,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75">
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <v>5</v>
       </c>
@@ -10733,7 +10794,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75">
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>6</v>
       </c>
@@ -10748,7 +10809,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="28">
         <v>7</v>
       </c>
@@ -10763,7 +10824,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75">
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>8</v>
       </c>
@@ -10778,7 +10839,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75">
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="28">
         <v>9</v>
       </c>
@@ -10793,7 +10854,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75">
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <v>10</v>
       </c>
@@ -10821,14 +10882,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -10841,7 +10902,7 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="143" t="s">
         <v>689</v>
       </c>
@@ -10853,7 +10914,7 @@
       <c r="G1" s="144"/>
       <c r="H1" s="145"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="155"/>
       <c r="B2" s="156"/>
       <c r="C2" s="156"/>
@@ -10863,7 +10924,7 @@
       <c r="G2" s="156"/>
       <c r="H2" s="157"/>
     </row>
-    <row r="3" spans="1:8" ht="23.25">
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="158" t="s">
         <v>390</v>
       </c>
@@ -10877,7 +10938,7 @@
       <c r="G3" s="160"/>
       <c r="H3" s="161"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" thickBot="1">
+    <row r="4" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="75">
         <v>1</v>
       </c>
@@ -10901,7 +10962,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" thickBot="1">
+    <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="75">
         <v>2</v>
       </c>
@@ -10925,7 +10986,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" thickBot="1">
+    <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75">
         <v>3</v>
       </c>
@@ -10949,7 +11010,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+    <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="75">
         <v>4</v>
       </c>
@@ -10975,7 +11036,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" thickBot="1">
+    <row r="8" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="75">
         <v>5</v>
       </c>
@@ -11001,7 +11062,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" thickBot="1">
+    <row r="9" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="75">
         <v>6</v>
       </c>
@@ -11027,7 +11088,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" thickBot="1">
+    <row r="10" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="75">
         <v>7</v>
       </c>
@@ -11053,7 +11114,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" thickBot="1">
+    <row r="11" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="75">
         <v>8</v>
       </c>
@@ -11079,7 +11140,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" thickBot="1">
+    <row r="12" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="75">
         <v>9</v>
       </c>
@@ -11105,7 +11166,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" thickBot="1">
+    <row r="13" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="75">
         <v>10</v>
       </c>
@@ -11131,7 +11192,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+    <row r="14" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="75">
         <v>11</v>
       </c>
@@ -11157,7 +11218,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" thickBot="1">
+    <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="75">
         <v>12</v>
       </c>
@@ -11183,7 +11244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" thickBot="1">
+    <row r="16" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75">
         <v>13</v>
       </c>
@@ -11209,7 +11270,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" thickBot="1">
+    <row r="17" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="75">
         <v>14</v>
       </c>
@@ -11235,7 +11296,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" thickBot="1">
+    <row r="18" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="75">
         <v>15</v>
       </c>
@@ -11259,7 +11320,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" thickBot="1">
+    <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="75">
         <v>16</v>
       </c>
@@ -11283,7 +11344,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" thickBot="1">
+    <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="75">
         <v>17</v>
       </c>
@@ -11307,7 +11368,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" thickBot="1">
+    <row r="21" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="75">
         <v>18</v>
       </c>
@@ -11329,7 +11390,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18.75" thickBot="1">
+    <row r="22" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="75">
         <v>19</v>
       </c>
@@ -11355,7 +11416,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.75" thickBot="1">
+    <row r="23" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="75">
         <v>20</v>
       </c>
@@ -11377,7 +11438,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75" thickBot="1">
+    <row r="24" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="92"/>
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
@@ -11395,7 +11456,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" thickBot="1">
+    <row r="25" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92"/>
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
@@ -11413,7 +11474,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" thickBot="1">
+    <row r="26" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="92"/>
       <c r="B26" s="93"/>
       <c r="C26" s="93"/>
@@ -11429,7 +11490,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" thickBot="1">
+    <row r="27" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="92"/>
       <c r="B27" s="93"/>
       <c r="C27" s="93"/>
@@ -11445,7 +11506,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.75" thickBot="1">
+    <row r="28" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="92"/>
       <c r="B28" s="93"/>
       <c r="C28" s="93"/>
@@ -11461,7 +11522,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="18.75" thickBot="1">
+    <row r="29" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="92"/>
       <c r="B29" s="93"/>
       <c r="C29" s="93"/>
@@ -11477,7 +11538,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="18.75" thickBot="1">
+    <row r="30" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="92"/>
       <c r="B30" s="93"/>
       <c r="C30" s="93"/>
@@ -11493,7 +11554,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="18.75" thickBot="1">
+    <row r="31" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="92"/>
       <c r="B31" s="93"/>
       <c r="C31" s="93"/>
@@ -11509,7 +11570,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18.75" thickBot="1">
+    <row r="32" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="92"/>
       <c r="B32" s="93"/>
       <c r="C32" s="93"/>
@@ -11525,7 +11586,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="18.75" thickBot="1">
+    <row r="33" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="94"/>
       <c r="B33" s="95"/>
       <c r="C33" s="95"/>
@@ -11553,14 +11614,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -11573,7 +11634,7 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="162" t="s">
         <v>530</v>
       </c>
@@ -11585,7 +11646,7 @@
       <c r="G1" s="162"/>
       <c r="H1" s="162"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="156"/>
       <c r="B2" s="156"/>
       <c r="C2" s="156"/>
@@ -11595,7 +11656,7 @@
       <c r="G2" s="156"/>
       <c r="H2" s="156"/>
     </row>
-    <row r="3" spans="1:8" ht="23.25">
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="158" t="s">
         <v>390</v>
       </c>
@@ -11609,7 +11670,7 @@
       <c r="G3" s="160"/>
       <c r="H3" s="161"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" thickBot="1">
+    <row r="4" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="75">
         <v>1</v>
       </c>
@@ -11633,7 +11694,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" thickBot="1">
+    <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="75">
         <v>2</v>
       </c>
@@ -11657,7 +11718,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" thickBot="1">
+    <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="75">
         <v>3</v>
       </c>
@@ -11681,7 +11742,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+    <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="75">
         <v>4</v>
       </c>
@@ -11707,7 +11768,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" thickBot="1">
+    <row r="8" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="75">
         <v>5</v>
       </c>
@@ -11733,7 +11794,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" thickBot="1">
+    <row r="9" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="75">
         <v>6</v>
       </c>
@@ -11759,7 +11820,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" thickBot="1">
+    <row r="10" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="75">
         <v>7</v>
       </c>
@@ -11785,7 +11846,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" thickBot="1">
+    <row r="11" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="75">
         <v>8</v>
       </c>
@@ -11811,7 +11872,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" thickBot="1">
+    <row r="12" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="75">
         <v>9</v>
       </c>
@@ -11837,7 +11898,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" thickBot="1">
+    <row r="13" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="75">
         <v>10</v>
       </c>
@@ -11863,7 +11924,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+    <row r="14" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="75">
         <v>11</v>
       </c>
@@ -11889,7 +11950,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" thickBot="1">
+    <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="75">
         <v>12</v>
       </c>
@@ -11915,7 +11976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" thickBot="1">
+    <row r="16" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75">
         <v>13</v>
       </c>
@@ -11941,7 +12002,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" thickBot="1">
+    <row r="17" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="75">
         <v>14</v>
       </c>
@@ -11967,7 +12028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" thickBot="1">
+    <row r="18" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="75">
         <v>15</v>
       </c>
@@ -11991,7 +12052,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" thickBot="1">
+    <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="75">
         <v>16</v>
       </c>
@@ -12015,7 +12076,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" thickBot="1">
+    <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="75">
         <v>17</v>
       </c>
@@ -12039,7 +12100,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" thickBot="1">
+    <row r="21" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="75">
         <v>18</v>
       </c>
@@ -12061,7 +12122,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18.75" thickBot="1">
+    <row r="22" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="75">
         <v>19</v>
       </c>
@@ -12087,7 +12148,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.75" thickBot="1">
+    <row r="23" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="75">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
chg: Added SPINS (Early version)
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -3194,7 +3194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3446,12 +3446,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3460,10 +3454,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3475,6 +3481,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3483,21 +3492,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3640,7 +3634,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4074,8 +4068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:T16"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4084,7 +4078,7 @@
     <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.140625" customWidth="1"/>
-    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
     <col min="32" max="32" width="16" customWidth="1"/>
     <col min="33" max="33" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="18.28515625" customWidth="1"/>
@@ -4126,18 +4120,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="140" t="s">
+      <c r="R3" s="128" t="s">
         <v>284</v>
       </c>
-      <c r="S3" s="140"/>
-      <c r="T3" s="140"/>
-      <c r="AA3" s="123" t="s">
+      <c r="S3" s="128"/>
+      <c r="T3" s="128"/>
+      <c r="AA3" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="124"/>
-      <c r="AC3" s="124"/>
-      <c r="AD3" s="124"/>
-      <c r="AE3" s="125"/>
+      <c r="AB3" s="131"/>
+      <c r="AC3" s="131"/>
+      <c r="AD3" s="131"/>
+      <c r="AE3" s="132"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4189,12 +4183,12 @@
       <c r="T4" s="101" t="s">
         <v>690</v>
       </c>
-      <c r="V4" s="131" t="s">
+      <c r="V4" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="131"/>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="131"/>
+      <c r="W4" s="129"/>
+      <c r="X4" s="129"/>
+      <c r="Y4" s="129"/>
       <c r="AA4" s="91" t="s">
         <v>292</v>
       </c>
@@ -4264,7 +4258,7 @@
       <c r="X5" s="38" t="s">
         <v>486</v>
       </c>
-      <c r="Y5" s="127"/>
+      <c r="Y5" s="123"/>
       <c r="AA5" s="7" t="s">
         <v>515</v>
       </c>
@@ -4340,7 +4334,7 @@
         <v>447</v>
       </c>
       <c r="X6" s="7"/>
-      <c r="Y6" s="127"/>
+      <c r="Y6" s="123"/>
       <c r="AA6" s="7" t="s">
         <v>516</v>
       </c>
@@ -4420,7 +4414,7 @@
       <c r="X7" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="Y7" s="127"/>
+      <c r="Y7" s="123"/>
       <c r="AA7" s="7" t="s">
         <v>594</v>
       </c>
@@ -4498,7 +4492,7 @@
       <c r="X8" s="38" t="s">
         <v>491</v>
       </c>
-      <c r="Y8" s="127"/>
+      <c r="Y8" s="123"/>
       <c r="Z8" s="41"/>
       <c r="AA8" s="41"/>
       <c r="AB8" s="41"/>
@@ -4567,7 +4561,7 @@
       <c r="X9" s="38" t="s">
         <v>492</v>
       </c>
-      <c r="Y9" s="127"/>
+      <c r="Y9" s="123"/>
       <c r="AD9" s="41"/>
       <c r="AE9" s="41"/>
       <c r="AF9" s="41"/>
@@ -4629,7 +4623,7 @@
       <c r="X10" s="38" t="s">
         <v>493</v>
       </c>
-      <c r="Y10" s="127"/>
+      <c r="Y10" s="123"/>
       <c r="AD10" s="41"/>
       <c r="AE10" s="41"/>
     </row>
@@ -4678,7 +4672,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="136" t="s">
+      <c r="R11" s="137" t="s">
         <v>694</v>
       </c>
       <c r="S11" s="105" t="s">
@@ -4751,7 +4745,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="137"/>
+      <c r="R12" s="138"/>
       <c r="S12" s="99" t="s">
         <v>653</v>
       </c>
@@ -4816,7 +4810,7 @@
       <c r="O13" s="96"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="138"/>
+      <c r="R13" s="139"/>
       <c r="S13" s="107" t="s">
         <v>689</v>
       </c>
@@ -4837,11 +4831,11 @@
         <v>501</v>
       </c>
       <c r="AA13" s="41"/>
-      <c r="AD13" s="141" t="s">
+      <c r="AD13" s="130" t="s">
         <v>679</v>
       </c>
-      <c r="AE13" s="142"/>
-      <c r="AF13" s="143"/>
+      <c r="AE13" s="131"/>
+      <c r="AF13" s="132"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5034,15 +5028,15 @@
       <c r="T16" s="25" t="s">
         <v>700</v>
       </c>
-      <c r="V16" s="131" t="s">
+      <c r="V16" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="131"/>
-      <c r="X16" s="131"/>
-      <c r="Y16" s="131"/>
-      <c r="Z16" s="131"/>
-      <c r="AA16" s="131"/>
-      <c r="AB16" s="131"/>
+      <c r="W16" s="129"/>
+      <c r="X16" s="129"/>
+      <c r="Y16" s="129"/>
+      <c r="Z16" s="129"/>
+      <c r="AA16" s="129"/>
+      <c r="AB16" s="129"/>
       <c r="AD16" s="7" t="s">
         <v>672</v>
       </c>
@@ -5181,10 +5175,10 @@
       <c r="V18" s="39" t="s">
         <v>719</v>
       </c>
-      <c r="W18" s="126" t="s">
+      <c r="W18" s="39" t="s">
         <v>520</v>
       </c>
-      <c r="X18" s="126" t="s">
+      <c r="X18" s="39" t="s">
         <v>93</v>
       </c>
       <c r="Y18" s="39" t="s">
@@ -5261,10 +5255,10 @@
       <c r="V19" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="W19" s="126" t="s">
+      <c r="W19" s="39" t="s">
         <v>737</v>
       </c>
-      <c r="X19" s="126" t="s">
+      <c r="X19" s="39" t="s">
         <v>142</v>
       </c>
       <c r="Y19" s="7" t="s">
@@ -5334,19 +5328,19 @@
         <v>304</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="131" t="s">
+      <c r="R20" s="129" t="s">
         <v>283</v>
       </c>
-      <c r="S20" s="131"/>
-      <c r="T20" s="131"/>
+      <c r="S20" s="129"/>
+      <c r="T20" s="129"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>721</v>
       </c>
-      <c r="W20" s="7" t="s">
+      <c r="W20" s="38" t="s">
         <v>735</v>
       </c>
-      <c r="X20" s="126" t="s">
+      <c r="X20" s="39" t="s">
         <v>91</v>
       </c>
       <c r="Y20" s="7" t="s">
@@ -5431,7 +5425,7 @@
       <c r="W21" s="39" t="s">
         <v>736</v>
       </c>
-      <c r="X21" s="126" t="s">
+      <c r="X21" s="39" t="s">
         <v>173</v>
       </c>
       <c r="Y21" s="39" t="s">
@@ -5509,15 +5503,15 @@
       <c r="T22" t="s">
         <v>485</v>
       </c>
-      <c r="V22" s="141" t="s">
+      <c r="V22" s="130" t="s">
         <v>712</v>
       </c>
-      <c r="W22" s="142"/>
-      <c r="X22" s="142"/>
-      <c r="Y22" s="142"/>
-      <c r="Z22" s="142"/>
-      <c r="AA22" s="142"/>
-      <c r="AB22" s="143"/>
+      <c r="W22" s="131"/>
+      <c r="X22" s="131"/>
+      <c r="Y22" s="131"/>
+      <c r="Z22" s="131"/>
+      <c r="AA22" s="131"/>
+      <c r="AB22" s="132"/>
       <c r="AD22" s="7" t="s">
         <v>678</v>
       </c>
@@ -5659,10 +5653,10 @@
       <c r="V24" s="39" t="s">
         <v>723</v>
       </c>
-      <c r="W24" s="126" t="s">
+      <c r="W24" s="39" t="s">
         <v>732</v>
       </c>
-      <c r="X24" s="126" t="s">
+      <c r="X24" s="39" t="s">
         <v>112</v>
       </c>
       <c r="Y24" s="39" t="s">
@@ -5738,10 +5732,10 @@
       <c r="V25" s="7" t="s">
         <v>724</v>
       </c>
-      <c r="W25" s="7" t="s">
+      <c r="W25" s="38" t="s">
         <v>731</v>
       </c>
-      <c r="X25" s="126" t="s">
+      <c r="X25" s="39" t="s">
         <v>271</v>
       </c>
       <c r="Y25" s="7" t="s">
@@ -5813,10 +5807,10 @@
       <c r="V26" s="7" t="s">
         <v>725</v>
       </c>
-      <c r="W26" s="7" t="s">
+      <c r="W26" s="38" t="s">
         <v>733</v>
       </c>
-      <c r="X26" s="126" t="s">
+      <c r="X26" s="39" t="s">
         <v>153</v>
       </c>
       <c r="Y26" s="7" t="s">
@@ -5889,10 +5883,10 @@
       <c r="V27" s="7" t="s">
         <v>726</v>
       </c>
-      <c r="W27" s="7" t="s">
+      <c r="W27" s="38" t="s">
         <v>734</v>
       </c>
-      <c r="X27" s="126" t="s">
+      <c r="X27" s="39" t="s">
         <v>50</v>
       </c>
       <c r="Y27" s="7" t="s">
@@ -5977,33 +5971,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="131" t="s">
+      <c r="B31" s="129" t="s">
         <v>301</v>
       </c>
-      <c r="C31" s="131"/>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="131"/>
-      <c r="H31" s="131"/>
-      <c r="J31" s="131" t="s">
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="129"/>
+      <c r="H31" s="129"/>
+      <c r="J31" s="129" t="s">
         <v>302</v>
       </c>
-      <c r="K31" s="131"/>
-      <c r="L31" s="131"/>
-      <c r="M31" s="131"/>
-      <c r="N31" s="131"/>
-      <c r="O31" s="131"/>
-      <c r="P31" s="131"/>
-      <c r="T31" s="131" t="s">
+      <c r="K31" s="129"/>
+      <c r="L31" s="129"/>
+      <c r="M31" s="129"/>
+      <c r="N31" s="129"/>
+      <c r="O31" s="129"/>
+      <c r="P31" s="129"/>
+      <c r="T31" s="129" t="s">
         <v>285</v>
       </c>
-      <c r="U31" s="131"/>
-      <c r="V31" s="131"/>
-      <c r="W31" s="131"/>
-      <c r="X31" s="131"/>
-      <c r="Y31" s="131"/>
-      <c r="Z31" s="131"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="129"/>
+      <c r="X31" s="129"/>
+      <c r="Y31" s="129"/>
+      <c r="Z31" s="129"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6282,7 +6276,7 @@
       <c r="Z35" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="AD35" s="139" t="s">
+      <c r="AD35" s="127" t="s">
         <v>749</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6365,7 +6359,7 @@
       <c r="Z36" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="AD36" s="139"/>
+      <c r="AD36" s="127"/>
       <c r="AE36" s="7" t="s">
         <v>549</v>
       </c>
@@ -6438,7 +6432,7 @@
       <c r="Z37" s="7" t="s">
         <v>619</v>
       </c>
-      <c r="AD37" s="139"/>
+      <c r="AD37" s="127"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -6494,7 +6488,7 @@
       <c r="Z38" s="7" t="s">
         <v>634</v>
       </c>
-      <c r="AD38" s="139"/>
+      <c r="AD38" s="127"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -6508,15 +6502,15 @@
       <c r="F39" t="s">
         <v>606</v>
       </c>
-      <c r="J39" s="132" t="s">
+      <c r="J39" s="136" t="s">
         <v>482</v>
       </c>
-      <c r="K39" s="132"/>
-      <c r="L39" s="132"/>
-      <c r="M39" s="132"/>
-      <c r="N39" s="132"/>
-      <c r="O39" s="132"/>
-      <c r="P39" s="132"/>
+      <c r="K39" s="136"/>
+      <c r="L39" s="136"/>
+      <c r="M39" s="136"/>
+      <c r="N39" s="136"/>
+      <c r="O39" s="136"/>
+      <c r="P39" s="136"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -6823,7 +6817,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -6832,13 +6833,7 @@
     <mergeCell ref="V22:AB22"/>
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
+    <mergeCell ref="AA3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6865,34 +6860,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="169" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="174"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
+      <c r="A2" s="170"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="152" t="s">
         <v>322</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="156" t="s">
+      <c r="B3" s="153"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="152" t="s">
         <v>323</v>
       </c>
-      <c r="E3" s="157"/>
-      <c r="F3" s="158"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="154"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7434,22 +7429,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="171" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="172" t="s">
         <v>366</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -7554,12 +7549,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="176" t="s">
+      <c r="B14" s="172" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="176"/>
-      <c r="D14" s="176"/>
-      <c r="E14" s="176"/>
+      <c r="C14" s="172"/>
+      <c r="D14" s="172"/>
+      <c r="E14" s="172"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -7671,7 +7666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -7945,40 +7940,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="140" t="s">
         <v>750</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="146"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="142"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="147"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="149"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="150" t="s">
+      <c r="A3" s="146" t="s">
         <v>654</v>
       </c>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151" t="s">
+      <c r="B3" s="147"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147" t="s">
         <v>655</v>
       </c>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="152"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="148"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="80">
@@ -9011,14 +9006,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="149" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="155"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="151"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -9029,16 +9024,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="152" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="156" t="s">
+      <c r="B3" s="153"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="152" t="s">
         <v>307</v>
       </c>
-      <c r="E3" s="157"/>
-      <c r="F3" s="158"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="154"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -9308,28 +9303,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="158" t="s">
         <v>787</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="155" t="s">
         <v>309</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -9604,16 +9599,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="155" t="s">
         <v>312</v>
       </c>
-      <c r="B15" s="160"/>
-      <c r="C15" s="160"/>
-      <c r="D15" s="160"/>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="161"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="156"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="157"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -9903,16 +9898,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="159" t="s">
+      <c r="A28" s="155" t="s">
         <v>313</v>
       </c>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
-      <c r="G28" s="160"/>
-      <c r="H28" s="161"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="157"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -10225,12 +10220,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="159" t="s">
         <v>762</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -10438,28 +10433,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="160" t="s">
         <v>802</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="155" t="s">
         <v>314</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -10690,7 +10685,7 @@
       <c r="A12" s="28">
         <v>9</v>
       </c>
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="126" t="s">
         <v>801</v>
       </c>
       <c r="C12" s="30" t="str">
@@ -10750,12 +10745,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="155" t="s">
         <v>316</v>
       </c>
-      <c r="B15" s="160"/>
-      <c r="C15" s="160"/>
-      <c r="D15" s="161"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="157"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -10783,11 +10778,11 @@
       <c r="C17" s="46" t="s">
         <v>550</v>
       </c>
-      <c r="D17" s="128" t="s">
+      <c r="D17" s="124" t="s">
         <v>562</v>
       </c>
       <c r="E17"/>
-      <c r="F17" s="129"/>
+      <c r="F17" s="125"/>
     </row>
     <row r="18" spans="1:8" ht="18.75">
       <c r="A18" s="28">
@@ -10905,7 +10900,7 @@
         <f>[1]Frequencies!V6</f>
         <v>Air Request Net</v>
       </c>
-      <c r="C26" s="128" t="str">
+      <c r="C26" s="124" t="str">
         <f>[1]Frequencies!W6</f>
         <v>21.00</v>
       </c>
@@ -10923,12 +10918,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="159" t="s">
+      <c r="A28" s="155" t="s">
         <v>317</v>
       </c>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="161"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="157"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -11130,40 +11125,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="149" t="s">
         <v>668</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="155"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="151"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="167"/>
+      <c r="A2" s="161"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="163"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="164" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="170"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="168" t="s">
+      <c r="B3" s="165"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="164" t="s">
         <v>388</v>
       </c>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="171"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">
@@ -11862,40 +11857,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="168" t="s">
         <v>527</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="166"/>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="164" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="170"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="168" t="s">
+      <c r="B3" s="165"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="164" t="s">
         <v>388</v>
       </c>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="171"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">

</xml_diff>

<commit_message>
chg: Updated communications master list with bort and callsigns for client aircrafts
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="882">
   <si>
     <t>AWACS</t>
   </si>
@@ -2705,6 +2705,9 @@
   </si>
   <si>
     <t>F/A-18C presets OPAR V1.0</t>
+  </si>
+  <si>
+    <t>COLT</t>
   </si>
 </sst>
 </file>
@@ -2883,7 +2886,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3007,6 +3010,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3626,7 +3635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3886,21 +3895,124 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3910,21 +4022,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4009,6 +4106,75 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4021,163 +4187,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="21" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="21" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="21" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="21" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4220,7 +4230,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4654,7 +4664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AA33" sqref="AA33"/>
     </sheetView>
   </sheetViews>
@@ -4706,18 +4716,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="136" t="s">
+      <c r="R3" s="158" t="s">
         <v>284</v>
       </c>
-      <c r="S3" s="136"/>
-      <c r="T3" s="136"/>
-      <c r="AA3" s="137" t="s">
+      <c r="S3" s="158"/>
+      <c r="T3" s="158"/>
+      <c r="AA3" s="160" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="138"/>
-      <c r="AC3" s="138"/>
-      <c r="AD3" s="138"/>
-      <c r="AE3" s="139"/>
+      <c r="AB3" s="161"/>
+      <c r="AC3" s="161"/>
+      <c r="AD3" s="161"/>
+      <c r="AE3" s="162"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4760,7 +4770,7 @@
         <v>12</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="129" t="s">
+      <c r="R4" s="163" t="s">
         <v>686</v>
       </c>
       <c r="S4" s="100" t="s">
@@ -4769,12 +4779,12 @@
       <c r="T4" s="101" t="s">
         <v>689</v>
       </c>
-      <c r="V4" s="127" t="s">
+      <c r="V4" s="159" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="127"/>
-      <c r="X4" s="127"/>
-      <c r="Y4" s="127"/>
+      <c r="W4" s="159"/>
+      <c r="X4" s="159"/>
+      <c r="Y4" s="159"/>
       <c r="AA4" s="91" t="s">
         <v>292</v>
       </c>
@@ -4828,7 +4838,7 @@
         <v>24</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="130"/>
+      <c r="R5" s="164"/>
       <c r="S5" s="31" t="s">
         <v>652</v>
       </c>
@@ -4906,7 +4916,7 @@
         <v>704</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="131"/>
+      <c r="R6" s="165"/>
       <c r="S6" s="102" t="s">
         <v>688</v>
       </c>
@@ -4982,7 +4992,7 @@
         <v>286</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="129" t="s">
+      <c r="R7" s="163" t="s">
         <v>692</v>
       </c>
       <c r="S7" s="100" t="s">
@@ -5062,7 +5072,7 @@
         <v>287</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="130"/>
+      <c r="R8" s="164"/>
       <c r="S8" s="31" t="s">
         <v>652</v>
       </c>
@@ -5131,7 +5141,7 @@
         <v>288</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="131"/>
+      <c r="R9" s="165"/>
       <c r="S9" s="102" t="s">
         <v>688</v>
       </c>
@@ -5258,7 +5268,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="132" t="s">
+      <c r="R11" s="167" t="s">
         <v>693</v>
       </c>
       <c r="S11" s="105" t="s">
@@ -5331,7 +5341,7 @@
       <c r="O12" s="96"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="133"/>
+      <c r="R12" s="168"/>
       <c r="S12" s="99" t="s">
         <v>652</v>
       </c>
@@ -5396,7 +5406,7 @@
       <c r="O13" s="96"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="134"/>
+      <c r="R13" s="169"/>
       <c r="S13" s="107" t="s">
         <v>688</v>
       </c>
@@ -5417,11 +5427,11 @@
         <v>501</v>
       </c>
       <c r="AA13" s="41"/>
-      <c r="AD13" s="137" t="s">
+      <c r="AD13" s="160" t="s">
         <v>678</v>
       </c>
-      <c r="AE13" s="138"/>
-      <c r="AF13" s="139"/>
+      <c r="AE13" s="161"/>
+      <c r="AF13" s="162"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5468,7 +5478,7 @@
         <v>283</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="129" t="s">
+      <c r="R14" s="163" t="s">
         <v>696</v>
       </c>
       <c r="S14" s="105" t="s">
@@ -5546,7 +5556,7 @@
         <v>296</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="130"/>
+      <c r="R15" s="164"/>
       <c r="S15" s="99" t="s">
         <v>652</v>
       </c>
@@ -5607,22 +5617,22 @@
         <v>295</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="131"/>
+      <c r="R16" s="165"/>
       <c r="S16" s="107" t="s">
         <v>688</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>699</v>
       </c>
-      <c r="V16" s="127" t="s">
+      <c r="V16" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="127"/>
-      <c r="X16" s="127"/>
-      <c r="Y16" s="127"/>
-      <c r="Z16" s="127"/>
-      <c r="AA16" s="127"/>
-      <c r="AB16" s="127"/>
+      <c r="W16" s="159"/>
+      <c r="X16" s="159"/>
+      <c r="Y16" s="159"/>
+      <c r="Z16" s="159"/>
+      <c r="AA16" s="159"/>
+      <c r="AB16" s="159"/>
       <c r="AD16" s="7" t="s">
         <v>671</v>
       </c>
@@ -5914,11 +5924,11 @@
         <v>304</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="127" t="s">
+      <c r="R20" s="159" t="s">
         <v>283</v>
       </c>
-      <c r="S20" s="127"/>
-      <c r="T20" s="127"/>
+      <c r="S20" s="159"/>
+      <c r="T20" s="159"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>720</v>
@@ -6089,15 +6099,15 @@
       <c r="T22" t="s">
         <v>485</v>
       </c>
-      <c r="V22" s="137" t="s">
+      <c r="V22" s="160" t="s">
         <v>711</v>
       </c>
-      <c r="W22" s="138"/>
-      <c r="X22" s="138"/>
-      <c r="Y22" s="138"/>
-      <c r="Z22" s="138"/>
-      <c r="AA22" s="138"/>
-      <c r="AB22" s="139"/>
+      <c r="W22" s="161"/>
+      <c r="X22" s="161"/>
+      <c r="Y22" s="161"/>
+      <c r="Z22" s="161"/>
+      <c r="AA22" s="161"/>
+      <c r="AB22" s="162"/>
       <c r="AD22" s="7" t="s">
         <v>677</v>
       </c>
@@ -6557,33 +6567,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="127" t="s">
+      <c r="B31" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="C31" s="127"/>
-      <c r="D31" s="127"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
-      <c r="G31" s="127"/>
-      <c r="H31" s="127"/>
-      <c r="J31" s="127" t="s">
+      <c r="C31" s="159"/>
+      <c r="D31" s="159"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="159"/>
+      <c r="J31" s="159" t="s">
         <v>302</v>
       </c>
-      <c r="K31" s="127"/>
-      <c r="L31" s="127"/>
-      <c r="M31" s="127"/>
-      <c r="N31" s="127"/>
-      <c r="O31" s="127"/>
-      <c r="P31" s="127"/>
-      <c r="T31" s="127" t="s">
+      <c r="K31" s="159"/>
+      <c r="L31" s="159"/>
+      <c r="M31" s="159"/>
+      <c r="N31" s="159"/>
+      <c r="O31" s="159"/>
+      <c r="P31" s="159"/>
+      <c r="T31" s="159" t="s">
         <v>285</v>
       </c>
-      <c r="U31" s="127"/>
-      <c r="V31" s="127"/>
-      <c r="W31" s="127"/>
-      <c r="X31" s="127"/>
-      <c r="Y31" s="127"/>
-      <c r="Z31" s="127"/>
+      <c r="U31" s="159"/>
+      <c r="V31" s="159"/>
+      <c r="W31" s="159"/>
+      <c r="X31" s="159"/>
+      <c r="Y31" s="159"/>
+      <c r="Z31" s="159"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6862,7 +6872,7 @@
       <c r="Z35" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="AD35" s="135" t="s">
+      <c r="AD35" s="157" t="s">
         <v>748</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6945,7 +6955,7 @@
       <c r="Z36" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="AD36" s="135"/>
+      <c r="AD36" s="157"/>
       <c r="AE36" s="7" t="s">
         <v>548</v>
       </c>
@@ -7018,7 +7028,7 @@
       <c r="Z37" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="AD37" s="135"/>
+      <c r="AD37" s="157"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7074,7 +7084,7 @@
       <c r="Z38" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="AD38" s="135"/>
+      <c r="AD38" s="157"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7088,15 +7098,15 @@
       <c r="F39" t="s">
         <v>605</v>
       </c>
-      <c r="J39" s="128" t="s">
+      <c r="J39" s="166" t="s">
         <v>482</v>
       </c>
-      <c r="K39" s="128"/>
-      <c r="L39" s="128"/>
-      <c r="M39" s="128"/>
-      <c r="N39" s="128"/>
-      <c r="O39" s="128"/>
-      <c r="P39" s="128"/>
+      <c r="K39" s="166"/>
+      <c r="L39" s="166"/>
+      <c r="M39" s="166"/>
+      <c r="N39" s="166"/>
+      <c r="O39" s="166"/>
+      <c r="P39" s="166"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7404,6 +7414,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7413,13 +7430,6 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7446,34 +7456,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="221" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="169"/>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
+      <c r="A2" s="222"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="182" t="s">
         <v>322</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="152" t="s">
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="182" t="s">
         <v>323</v>
       </c>
-      <c r="E3" s="153"/>
-      <c r="F3" s="154"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="184"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -8015,22 +8025,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="223" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="224" t="s">
         <v>366</v>
       </c>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -8135,12 +8145,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="224" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="171"/>
-      <c r="E14" s="171"/>
+      <c r="C14" s="224"/>
+      <c r="D14" s="224"/>
+      <c r="E14" s="224"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -8250,10 +8260,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W31"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8262,312 +8272,982 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" t="s">
+      <c r="A1" s="225" t="s">
         <v>783</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="225" t="s">
         <v>779</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="225" t="s">
         <v>782</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="225" t="s">
         <v>783</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="225" t="s">
         <v>779</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="225" t="s">
         <v>782</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="225" t="s">
         <v>783</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="225" t="s">
         <v>779</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="225" t="s">
         <v>782</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="225" t="s">
         <v>783</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="225" t="s">
         <v>779</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="225" t="s">
         <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>776</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>411</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="7" t="s">
         <v>787</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
         <v>111</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="7" t="s">
         <v>788</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="7">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="7">
         <v>211</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="7" t="s">
         <v>803</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="7">
         <v>1</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="7">
         <v>611</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="7" t="s">
         <v>802</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="7" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="C3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7">
         <v>412</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="I3">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7">
         <v>112</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="O3">
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7">
         <v>212</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="U3">
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7">
         <v>612</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="7" t="s">
         <v>802</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="7" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="C4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7">
         <v>413</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="I4">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7">
         <v>113</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="O4">
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7">
         <v>213</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="U4">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7">
         <v>613</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="7" t="s">
         <v>802</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="7" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="C5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7">
         <v>414</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="I5">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7">
         <v>114</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="O5">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7">
         <v>214</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="U5">
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7">
         <v>614</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="7" t="s">
         <v>802</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="7" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+    <row r="6" spans="1:23">
+      <c r="A6" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>421</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7">
+        <v>121</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+      <c r="O6" s="7">
+        <v>221</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7">
+        <v>422</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7">
+        <v>122</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7">
+        <v>222</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
+        <v>423</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7">
+        <v>123</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7">
+        <v>223</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7">
+        <v>424</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7">
+        <v>124</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7">
+        <v>224</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7">
+        <v>431</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="H10" s="7">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7">
+        <v>131</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="N10" s="7">
+        <v>3</v>
+      </c>
+      <c r="O10" s="7">
+        <v>231</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
+        <v>432</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7">
+        <v>132</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7">
+        <v>232</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7">
+        <v>433</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7">
+        <v>133</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7">
+        <v>233</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7">
+        <v>434</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7">
+        <v>134</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7">
+        <v>234</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
+        <v>441</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="H14" s="7">
+        <v>4</v>
+      </c>
+      <c r="I14" s="7">
+        <v>141</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7">
+        <v>442</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7">
+        <v>142</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7">
+        <v>443</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7">
+        <v>143</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7">
+        <v>444</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7">
+        <v>144</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="G18" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="H18" s="7">
+        <v>5</v>
+      </c>
+      <c r="I18" s="7">
+        <v>151</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7">
+        <v>152</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7">
+        <v>153</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <v>154</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="225" t="s">
         <v>783</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="225" t="s">
         <v>780</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="225" t="s">
         <v>779</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="225" t="s">
         <v>781</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="225" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+      <c r="G27" s="225" t="s">
+        <v>783</v>
+      </c>
+      <c r="H27" s="225" t="s">
+        <v>780</v>
+      </c>
+      <c r="I27" s="225" t="s">
+        <v>779</v>
+      </c>
+      <c r="J27" s="225" t="s">
+        <v>781</v>
+      </c>
+      <c r="K27" s="225" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="7" t="s">
         <v>804</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>311</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>805</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="7" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="C29">
+      <c r="G28" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="H28" s="7">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7">
+        <v>611</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7">
         <v>312</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>805</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="7" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="C30">
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7">
+        <v>612</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7">
         <v>313</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>805</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="7" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="C31">
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7">
+        <v>613</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7">
         <v>314</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7" t="s">
         <v>805</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="7" t="s">
+        <v>806</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7">
+        <v>614</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>321</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7">
+        <v>322</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7">
+        <v>323</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7">
+        <v>324</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="B36" s="7">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7">
+        <v>331</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7">
+        <v>332</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7">
+        <v>333</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7">
+        <v>334</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>805</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>806</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8593,40 +9273,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="170" t="s">
         <v>749</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="142"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="172"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="145"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="175"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="176" t="s">
         <v>653</v>
       </c>
-      <c r="B3" s="147"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147" t="s">
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177" t="s">
         <v>654</v>
       </c>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="148"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="178"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="80">
@@ -9659,14 +10339,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="179" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="151"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="181"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -9677,16 +10357,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="182" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="154"/>
-      <c r="D3" s="152" t="s">
+      <c r="B3" s="183"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="182" t="s">
         <v>307</v>
       </c>
-      <c r="E3" s="153"/>
-      <c r="F3" s="154"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="184"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -9956,28 +10636,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="188" t="s">
         <v>786</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="185" t="s">
         <v>309</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="157"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="187"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -10252,16 +10932,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="185" t="s">
         <v>312</v>
       </c>
-      <c r="B15" s="156"/>
-      <c r="C15" s="156"/>
-      <c r="D15" s="156"/>
-      <c r="E15" s="156"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="156"/>
-      <c r="H15" s="157"/>
+      <c r="B15" s="186"/>
+      <c r="C15" s="186"/>
+      <c r="D15" s="186"/>
+      <c r="E15" s="186"/>
+      <c r="F15" s="186"/>
+      <c r="G15" s="186"/>
+      <c r="H15" s="187"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -10551,16 +11231,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="185" t="s">
         <v>313</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
-      <c r="H28" s="157"/>
+      <c r="B28" s="186"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="187"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -10873,12 +11553,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="189" t="s">
         <v>761</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -11086,28 +11766,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="190" t="s">
         <v>801</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="190"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="185" t="s">
         <v>314</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="157"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="187"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -11398,12 +12078,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="185" t="s">
         <v>316</v>
       </c>
-      <c r="B15" s="156"/>
-      <c r="C15" s="156"/>
-      <c r="D15" s="157"/>
+      <c r="B15" s="186"/>
+      <c r="C15" s="186"/>
+      <c r="D15" s="187"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -11571,12 +12251,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="185" t="s">
         <v>317</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="157"/>
+      <c r="B28" s="186"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="187"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -11778,40 +12458,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="179" t="s">
         <v>667</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="151"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="181"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="161"/>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="163"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
+      <c r="H2" s="193"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="194" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="164" t="s">
+      <c r="B3" s="195"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="194" t="s">
         <v>388</v>
       </c>
-      <c r="F3" s="165"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="167"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="197"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">
@@ -12492,7 +13172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -12510,889 +13190,918 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="215" t="s">
         <v>880</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
+      <c r="G1" s="215"/>
+      <c r="H1" s="215"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="173"/>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
+      <c r="A2" s="216"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="217" t="s">
         <v>387</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="174" t="s">
+      <c r="B3" s="218"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="217" t="s">
         <v>388</v>
       </c>
-      <c r="F3" s="175"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="177"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="219"/>
+      <c r="H3" s="220"/>
     </row>
     <row r="4" spans="1:8" ht="18">
-      <c r="A4" s="178">
+      <c r="A4" s="127">
         <v>1</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="129" t="s">
         <v>487</v>
       </c>
-      <c r="D4" s="181" t="s">
+      <c r="D4" s="130" t="s">
         <v>670</v>
       </c>
-      <c r="E4" s="182">
+      <c r="E4" s="131">
         <v>1</v>
       </c>
-      <c r="F4" s="183" t="s">
+      <c r="F4" s="132" t="s">
         <v>807</v>
       </c>
-      <c r="G4" s="184" t="s">
+      <c r="G4" s="133" t="s">
         <v>808</v>
       </c>
-      <c r="H4" s="185" t="s">
+      <c r="H4" s="134" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
-      <c r="A5" s="186">
+      <c r="A5" s="135">
         <v>2</v>
       </c>
-      <c r="B5" s="187" t="s">
+      <c r="B5" s="136" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="137" t="s">
         <v>489</v>
       </c>
-      <c r="D5" s="189" t="s">
+      <c r="D5" s="138" t="s">
         <v>671</v>
       </c>
-      <c r="E5" s="190">
+      <c r="E5" s="139">
         <v>2</v>
       </c>
-      <c r="F5" s="191" t="s">
+      <c r="F5" s="140" t="s">
         <v>810</v>
       </c>
-      <c r="G5" s="192" t="s">
+      <c r="G5" s="141" t="s">
         <v>808</v>
       </c>
-      <c r="H5" s="193" t="s">
+      <c r="H5" s="142" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
-      <c r="A6" s="190">
+      <c r="A6" s="139">
         <v>3</v>
       </c>
-      <c r="B6" s="191" t="s">
+      <c r="B6" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="192" t="s">
+      <c r="C6" s="141" t="s">
         <v>488</v>
       </c>
-      <c r="D6" s="194" t="s">
+      <c r="D6" s="143" t="s">
         <v>672</v>
       </c>
-      <c r="E6" s="186">
+      <c r="E6" s="135">
         <v>3</v>
       </c>
-      <c r="F6" s="187" t="s">
+      <c r="F6" s="136" t="s">
         <v>812</v>
       </c>
-      <c r="G6" s="188" t="s">
+      <c r="G6" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="H6" s="195" t="s">
+      <c r="H6" s="144" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
-      <c r="A7" s="186">
+      <c r="A7" s="135">
         <v>4</v>
       </c>
-      <c r="B7" s="187" t="s">
+      <c r="B7" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="137" t="s">
         <v>490</v>
       </c>
-      <c r="D7" s="189" t="s">
+      <c r="D7" s="138" t="s">
         <v>673</v>
       </c>
-      <c r="E7" s="190">
+      <c r="E7" s="139">
         <v>4</v>
       </c>
-      <c r="F7" s="191" t="s">
+      <c r="F7" s="140" t="s">
         <v>814</v>
       </c>
-      <c r="G7" s="192" t="s">
+      <c r="G7" s="141" t="s">
         <v>808</v>
       </c>
-      <c r="H7" s="193" t="s">
+      <c r="H7" s="142" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
-      <c r="A8" s="190">
+      <c r="A8" s="139">
         <v>5</v>
       </c>
-      <c r="B8" s="191" t="s">
+      <c r="B8" s="140" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="192" t="s">
+      <c r="C8" s="141" t="s">
         <v>493</v>
       </c>
-      <c r="D8" s="194" t="s">
+      <c r="D8" s="143" t="s">
         <v>674</v>
       </c>
-      <c r="E8" s="186">
+      <c r="E8" s="135">
         <v>5</v>
       </c>
-      <c r="F8" s="187" t="s">
+      <c r="F8" s="136" t="s">
         <v>816</v>
       </c>
-      <c r="G8" s="188" t="s">
+      <c r="G8" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="H8" s="195" t="s">
+      <c r="H8" s="144" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
-      <c r="A9" s="186">
+      <c r="A9" s="135">
         <v>6</v>
       </c>
-      <c r="B9" s="187" t="s">
+      <c r="B9" s="136" t="s">
         <v>232</v>
       </c>
-      <c r="C9" s="188" t="s">
+      <c r="C9" s="137" t="s">
         <v>507</v>
       </c>
-      <c r="D9" s="189" t="s">
+      <c r="D9" s="138" t="s">
         <v>675</v>
       </c>
-      <c r="E9" s="190">
+      <c r="E9" s="139">
         <v>6</v>
       </c>
-      <c r="F9" s="191" t="s">
+      <c r="F9" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="192" t="s">
+      <c r="G9" s="141" t="s">
         <v>514</v>
       </c>
-      <c r="H9" s="193" t="s">
+      <c r="H9" s="142" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
-      <c r="A10" s="190">
+      <c r="A10" s="139">
         <v>7</v>
       </c>
-      <c r="B10" s="191" t="s">
+      <c r="B10" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="192" t="s">
+      <c r="C10" s="141" t="s">
         <v>508</v>
       </c>
-      <c r="D10" s="194" t="s">
+      <c r="D10" s="143" t="s">
         <v>676</v>
       </c>
-      <c r="E10" s="186">
+      <c r="E10" s="135">
         <v>7</v>
       </c>
-      <c r="F10" s="187" t="s">
+      <c r="F10" s="136" t="s">
         <v>259</v>
       </c>
-      <c r="G10" s="188" t="s">
+      <c r="G10" s="137" t="s">
         <v>519</v>
       </c>
-      <c r="H10" s="195" t="s">
+      <c r="H10" s="144" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
-      <c r="A11" s="186">
+      <c r="A11" s="135">
         <v>8</v>
       </c>
-      <c r="B11" s="187" t="s">
+      <c r="B11" s="136" t="s">
         <v>224</v>
       </c>
-      <c r="C11" s="188" t="s">
+      <c r="C11" s="137" t="s">
         <v>510</v>
       </c>
-      <c r="D11" s="189" t="s">
+      <c r="D11" s="138" t="s">
         <v>677</v>
       </c>
-      <c r="E11" s="190">
+      <c r="E11" s="139">
         <v>8</v>
       </c>
-      <c r="F11" s="191" t="s">
+      <c r="F11" s="140" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="192" t="s">
+      <c r="G11" s="141" t="s">
         <v>594</v>
       </c>
-      <c r="H11" s="193" t="s">
+      <c r="H11" s="142" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
-      <c r="A12" s="190">
+      <c r="A12" s="139">
         <v>9</v>
       </c>
-      <c r="B12" s="191" t="s">
+      <c r="B12" s="140" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="192" t="s">
+      <c r="C12" s="141" t="s">
         <v>534</v>
       </c>
-      <c r="D12" s="194" t="s">
+      <c r="D12" s="143" t="s">
         <v>679</v>
       </c>
-      <c r="E12" s="186">
+      <c r="E12" s="135">
         <v>9</v>
       </c>
-      <c r="F12" s="187" t="s">
+      <c r="F12" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="188" t="s">
+      <c r="G12" s="137" t="s">
         <v>486</v>
       </c>
-      <c r="H12" s="195" t="s">
+      <c r="H12" s="144" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
-      <c r="A13" s="186">
+      <c r="A13" s="135">
         <v>10</v>
       </c>
-      <c r="B13" s="187" t="s">
+      <c r="B13" s="136" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="188" t="s">
+      <c r="C13" s="137" t="s">
         <v>535</v>
       </c>
-      <c r="D13" s="189" t="s">
+      <c r="D13" s="138" t="s">
         <v>680</v>
       </c>
-      <c r="E13" s="190">
+      <c r="E13" s="139">
         <v>10</v>
       </c>
-      <c r="F13" s="191" t="s">
+      <c r="F13" s="140" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="192" t="s">
+      <c r="G13" s="141" t="s">
         <v>491</v>
       </c>
-      <c r="H13" s="193" t="s">
+      <c r="H13" s="142" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
-      <c r="A14" s="190">
+      <c r="A14" s="139">
         <v>11</v>
       </c>
-      <c r="B14" s="191" t="s">
+      <c r="B14" s="140" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="141" t="s">
         <v>536</v>
       </c>
-      <c r="D14" s="194" t="s">
+      <c r="D14" s="143" t="s">
         <v>681</v>
       </c>
-      <c r="E14" s="186">
+      <c r="E14" s="135">
         <v>11</v>
       </c>
-      <c r="F14" s="187" t="s">
+      <c r="F14" s="136" t="s">
         <v>820</v>
       </c>
-      <c r="G14" s="188" t="s">
+      <c r="G14" s="137" t="s">
         <v>821</v>
       </c>
-      <c r="H14" s="195" t="s">
+      <c r="H14" s="144" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
-      <c r="A15" s="186">
+      <c r="A15" s="135">
         <v>12</v>
       </c>
-      <c r="B15" s="187" t="s">
+      <c r="B15" s="136" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="188" t="s">
+      <c r="C15" s="137" t="s">
         <v>703</v>
       </c>
-      <c r="D15" s="189" t="s">
+      <c r="D15" s="138" t="s">
         <v>682</v>
       </c>
-      <c r="E15" s="190">
+      <c r="E15" s="139">
         <v>12</v>
       </c>
-      <c r="F15" s="191" t="s">
+      <c r="F15" s="140" t="s">
         <v>207</v>
       </c>
-      <c r="G15" s="192" t="s">
+      <c r="G15" s="141" t="s">
         <v>823</v>
       </c>
-      <c r="H15" s="193" t="s">
+      <c r="H15" s="142" t="s">
         <v>824</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
-      <c r="A16" s="190">
+      <c r="A16" s="139">
         <v>13</v>
       </c>
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="192" t="s">
+      <c r="C16" s="141" t="s">
         <v>706</v>
       </c>
-      <c r="D16" s="194" t="s">
+      <c r="D16" s="143" t="s">
         <v>683</v>
       </c>
-      <c r="E16" s="186">
+      <c r="E16" s="135">
         <v>13</v>
       </c>
-      <c r="F16" s="187" t="s">
+      <c r="F16" s="136" t="s">
         <v>825</v>
       </c>
-      <c r="G16" s="188"/>
-      <c r="H16" s="195" t="s">
+      <c r="G16" s="137"/>
+      <c r="H16" s="144" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
-      <c r="A17" s="186">
+      <c r="A17" s="135">
         <v>14</v>
       </c>
-      <c r="B17" s="187" t="s">
+      <c r="B17" s="136" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="188" t="s">
+      <c r="C17" s="137" t="s">
         <v>707</v>
       </c>
-      <c r="D17" s="189" t="s">
+      <c r="D17" s="138" t="s">
         <v>684</v>
       </c>
-      <c r="E17" s="190">
+      <c r="E17" s="139">
         <v>14</v>
       </c>
-      <c r="F17" s="191" t="s">
+      <c r="F17" s="140" t="s">
         <v>827</v>
       </c>
-      <c r="G17" s="192"/>
-      <c r="H17" s="193" t="s">
+      <c r="G17" s="141"/>
+      <c r="H17" s="142" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18">
-      <c r="A18" s="190">
+      <c r="A18" s="139">
         <v>15</v>
       </c>
-      <c r="B18" s="191" t="s">
+      <c r="B18" s="140" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="192" t="s">
+      <c r="C18" s="141" t="s">
         <v>708</v>
       </c>
-      <c r="D18" s="194" t="s">
+      <c r="D18" s="143" t="s">
         <v>685</v>
       </c>
-      <c r="E18" s="186">
+      <c r="E18" s="135">
         <v>15</v>
       </c>
-      <c r="F18" s="187" t="s">
+      <c r="F18" s="136" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="188" t="s">
+      <c r="G18" s="137" t="s">
         <v>713</v>
       </c>
-      <c r="H18" s="195" t="s">
+      <c r="H18" s="144" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18">
-      <c r="A19" s="186">
+      <c r="A19" s="135">
         <v>16</v>
       </c>
-      <c r="B19" s="187" t="s">
+      <c r="B19" s="136" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="188" t="s">
+      <c r="C19" s="137" t="s">
         <v>700</v>
       </c>
-      <c r="D19" s="196" t="s">
+      <c r="D19" s="145" t="s">
         <v>829</v>
       </c>
-      <c r="E19" s="190">
+      <c r="E19" s="139">
         <v>16</v>
       </c>
-      <c r="F19" s="191" t="s">
+      <c r="F19" s="140" t="s">
         <v>271</v>
       </c>
-      <c r="G19" s="192" t="s">
+      <c r="G19" s="141" t="s">
         <v>737</v>
       </c>
-      <c r="H19" s="193" t="s">
+      <c r="H19" s="142" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
-      <c r="A20" s="190">
+      <c r="A20" s="139">
         <v>17</v>
       </c>
-      <c r="B20" s="191" t="s">
+      <c r="B20" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="192" t="s">
+      <c r="C20" s="141" t="s">
         <v>701</v>
       </c>
-      <c r="D20" s="197" t="s">
+      <c r="D20" s="146" t="s">
         <v>830</v>
       </c>
-      <c r="E20" s="186">
+      <c r="E20" s="135">
         <v>17</v>
       </c>
-      <c r="F20" s="187" t="s">
+      <c r="F20" s="136" t="s">
         <v>153</v>
       </c>
-      <c r="G20" s="188" t="s">
+      <c r="G20" s="137" t="s">
         <v>738</v>
       </c>
-      <c r="H20" s="195" t="s">
+      <c r="H20" s="144" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18">
-      <c r="A21" s="186">
+      <c r="A21" s="135">
         <v>18</v>
       </c>
-      <c r="B21" s="187" t="s">
+      <c r="B21" s="136" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="188" t="s">
+      <c r="C21" s="137" t="s">
         <v>702</v>
       </c>
-      <c r="D21" s="196" t="s">
+      <c r="D21" s="145" t="s">
         <v>831</v>
       </c>
-      <c r="E21" s="190">
+      <c r="E21" s="139">
         <v>18</v>
       </c>
-      <c r="F21" s="191" t="s">
+      <c r="F21" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="192" t="s">
+      <c r="G21" s="141" t="s">
         <v>741</v>
       </c>
-      <c r="H21" s="193" t="s">
+      <c r="H21" s="142" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18">
-      <c r="A22" s="190">
+      <c r="A22" s="139">
         <v>19</v>
       </c>
-      <c r="B22" s="191" t="s">
+      <c r="B22" s="140" t="s">
         <v>832</v>
       </c>
-      <c r="C22" s="192" t="s">
+      <c r="C22" s="141" t="s">
         <v>808</v>
       </c>
-      <c r="D22" s="194" t="s">
+      <c r="D22" s="143" t="s">
         <v>790</v>
       </c>
-      <c r="E22" s="186">
+      <c r="E22" s="135">
         <v>19</v>
       </c>
-      <c r="F22" s="187" t="s">
+      <c r="F22" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="188" t="s">
+      <c r="G22" s="137" t="s">
         <v>492</v>
       </c>
-      <c r="H22" s="195" t="s">
+      <c r="H22" s="144" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A23" s="198">
+      <c r="A23" s="147">
         <v>20</v>
       </c>
-      <c r="B23" s="199" t="s">
+      <c r="B23" s="148" t="s">
         <v>834</v>
       </c>
-      <c r="C23" s="200" t="s">
+      <c r="C23" s="149" t="s">
         <v>808</v>
       </c>
-      <c r="D23" s="201" t="s">
+      <c r="D23" s="150" t="s">
         <v>792</v>
       </c>
-      <c r="E23" s="202">
+      <c r="E23" s="151">
         <v>20</v>
       </c>
-      <c r="F23" s="203" t="s">
+      <c r="F23" s="152" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="204" t="s">
+      <c r="G23" s="153" t="s">
         <v>501</v>
       </c>
-      <c r="H23" s="205" t="s">
+      <c r="H23" s="154" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A24" s="206"/>
-      <c r="B24" s="206"/>
-      <c r="C24" s="206"/>
-      <c r="D24" s="206"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
+      <c r="A24" s="155"/>
+      <c r="B24" s="155"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="155"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="155"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="174" t="s">
+      <c r="A25" s="217" t="s">
         <v>836</v>
       </c>
-      <c r="B25" s="175"/>
-      <c r="C25" s="176"/>
-      <c r="D25" s="177"/>
-      <c r="E25" s="174" t="s">
+      <c r="B25" s="218"/>
+      <c r="C25" s="219"/>
+      <c r="D25" s="220"/>
+      <c r="E25" s="217" t="s">
         <v>837</v>
       </c>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="177"/>
+      <c r="F25" s="218"/>
+      <c r="G25" s="219"/>
+      <c r="H25" s="220"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A26" s="182" t="s">
+      <c r="A26" s="131" t="s">
         <v>838</v>
       </c>
-      <c r="B26" s="207" t="s">
+      <c r="B26" s="204" t="s">
         <v>839</v>
       </c>
-      <c r="C26" s="208"/>
-      <c r="D26" s="209"/>
-      <c r="E26" s="178" t="s">
+      <c r="C26" s="205"/>
+      <c r="D26" s="206"/>
+      <c r="E26" s="127" t="s">
         <v>840</v>
       </c>
-      <c r="F26" s="210" t="s">
+      <c r="F26" s="212" t="s">
         <v>841</v>
       </c>
-      <c r="G26" s="211"/>
-      <c r="H26" s="212" t="s">
+      <c r="G26" s="213"/>
+      <c r="H26" s="214" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A27" s="190" t="s">
+      <c r="A27" s="139" t="s">
         <v>842</v>
       </c>
-      <c r="B27" s="213" t="s">
+      <c r="B27" s="207" t="s">
         <v>843</v>
       </c>
-      <c r="C27" s="214"/>
-      <c r="D27" s="215" t="s">
+      <c r="C27" s="208"/>
+      <c r="D27" s="210" t="s">
         <v>671</v>
       </c>
-      <c r="E27" s="182" t="s">
+      <c r="E27" s="131" t="s">
         <v>844</v>
       </c>
-      <c r="F27" s="207" t="s">
+      <c r="F27" s="204" t="s">
         <v>845</v>
       </c>
-      <c r="G27" s="208"/>
-      <c r="H27" s="216" t="s">
+      <c r="G27" s="205"/>
+      <c r="H27" s="211" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A28" s="182" t="s">
+      <c r="A28" s="131" t="s">
         <v>846</v>
       </c>
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="204" t="s">
         <v>847</v>
       </c>
-      <c r="C28" s="208"/>
-      <c r="D28" s="209" t="s">
+      <c r="C28" s="205"/>
+      <c r="D28" s="206" t="s">
         <v>672</v>
       </c>
-      <c r="E28" s="190" t="s">
+      <c r="E28" s="139" t="s">
         <v>848</v>
       </c>
-      <c r="F28" s="213" t="s">
+      <c r="F28" s="207" t="s">
         <v>849</v>
       </c>
-      <c r="G28" s="214"/>
-      <c r="H28" s="217" t="s">
+      <c r="G28" s="208"/>
+      <c r="H28" s="209" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A29" s="190" t="s">
+      <c r="A29" s="139" t="s">
         <v>850</v>
       </c>
-      <c r="B29" s="213" t="s">
+      <c r="B29" s="207" t="s">
         <v>851</v>
       </c>
-      <c r="C29" s="214"/>
-      <c r="D29" s="215" t="s">
+      <c r="C29" s="208"/>
+      <c r="D29" s="210" t="s">
         <v>673</v>
       </c>
-      <c r="E29" s="182" t="s">
+      <c r="E29" s="131" t="s">
         <v>852</v>
       </c>
-      <c r="F29" s="207" t="s">
+      <c r="F29" s="204" t="s">
         <v>853</v>
       </c>
-      <c r="G29" s="208"/>
-      <c r="H29" s="216" t="s">
+      <c r="G29" s="205"/>
+      <c r="H29" s="211" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A30" s="182" t="s">
+      <c r="A30" s="131" t="s">
         <v>854</v>
       </c>
-      <c r="B30" s="207" t="s">
+      <c r="B30" s="204" t="s">
         <v>855</v>
       </c>
-      <c r="C30" s="208"/>
-      <c r="D30" s="209" t="s">
+      <c r="C30" s="205"/>
+      <c r="D30" s="206" t="s">
         <v>674</v>
       </c>
-      <c r="E30" s="190" t="s">
+      <c r="E30" s="139" t="s">
         <v>856</v>
       </c>
-      <c r="F30" s="213" t="s">
+      <c r="F30" s="207" t="s">
         <v>857</v>
       </c>
-      <c r="G30" s="214"/>
-      <c r="H30" s="217" t="s">
+      <c r="G30" s="208"/>
+      <c r="H30" s="209" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A31" s="190" t="s">
+      <c r="A31" s="139" t="s">
         <v>858</v>
       </c>
-      <c r="B31" s="213" t="s">
+      <c r="B31" s="207" t="s">
         <v>859</v>
       </c>
-      <c r="C31" s="214"/>
-      <c r="D31" s="215" t="s">
+      <c r="C31" s="208"/>
+      <c r="D31" s="210" t="s">
         <v>675</v>
       </c>
-      <c r="E31" s="182" t="s">
+      <c r="E31" s="131" t="s">
         <v>860</v>
       </c>
-      <c r="F31" s="207" t="s">
+      <c r="F31" s="204" t="s">
         <v>861</v>
       </c>
-      <c r="G31" s="208"/>
-      <c r="H31" s="216" t="s">
+      <c r="G31" s="205"/>
+      <c r="H31" s="211" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A32" s="182" t="s">
+      <c r="A32" s="131" t="s">
         <v>862</v>
       </c>
-      <c r="B32" s="207" t="s">
+      <c r="B32" s="204" t="s">
         <v>863</v>
       </c>
-      <c r="C32" s="208"/>
-      <c r="D32" s="209" t="s">
+      <c r="C32" s="205"/>
+      <c r="D32" s="206" t="s">
         <v>676</v>
       </c>
-      <c r="E32" s="190"/>
-      <c r="F32" s="213"/>
-      <c r="G32" s="214"/>
-      <c r="H32" s="217" t="s">
+      <c r="E32" s="139"/>
+      <c r="F32" s="207"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="209" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A33" s="190" t="s">
+      <c r="A33" s="139" t="s">
         <v>864</v>
       </c>
-      <c r="B33" s="213" t="s">
+      <c r="B33" s="207" t="s">
         <v>865</v>
       </c>
-      <c r="C33" s="214"/>
-      <c r="D33" s="215" t="s">
+      <c r="C33" s="208"/>
+      <c r="D33" s="210" t="s">
         <v>670</v>
       </c>
-      <c r="E33" s="182"/>
-      <c r="F33" s="207"/>
-      <c r="G33" s="208"/>
-      <c r="H33" s="216" t="s">
+      <c r="E33" s="131"/>
+      <c r="F33" s="204"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="211" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A34" s="182" t="s">
+      <c r="A34" s="131" t="s">
         <v>866</v>
       </c>
-      <c r="B34" s="207" t="s">
+      <c r="B34" s="204" t="s">
         <v>867</v>
       </c>
-      <c r="C34" s="208"/>
-      <c r="D34" s="209" t="s">
+      <c r="C34" s="205"/>
+      <c r="D34" s="206" t="s">
         <v>671</v>
       </c>
-      <c r="E34" s="190"/>
-      <c r="F34" s="213"/>
-      <c r="G34" s="214"/>
-      <c r="H34" s="217" t="s">
+      <c r="E34" s="139"/>
+      <c r="F34" s="207"/>
+      <c r="G34" s="208"/>
+      <c r="H34" s="209" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A35" s="190" t="s">
+      <c r="A35" s="139" t="s">
         <v>868</v>
       </c>
-      <c r="B35" s="213" t="s">
+      <c r="B35" s="207" t="s">
         <v>869</v>
       </c>
-      <c r="C35" s="214"/>
-      <c r="D35" s="215" t="s">
+      <c r="C35" s="208"/>
+      <c r="D35" s="210" t="s">
         <v>672</v>
       </c>
-      <c r="E35" s="182"/>
-      <c r="F35" s="207"/>
-      <c r="G35" s="208"/>
-      <c r="H35" s="216" t="s">
+      <c r="E35" s="131"/>
+      <c r="F35" s="204"/>
+      <c r="G35" s="205"/>
+      <c r="H35" s="211" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A36" s="182" t="s">
+      <c r="A36" s="131" t="s">
         <v>870</v>
       </c>
-      <c r="B36" s="207" t="s">
+      <c r="B36" s="204" t="s">
         <v>871</v>
       </c>
-      <c r="C36" s="208"/>
-      <c r="D36" s="209" t="s">
+      <c r="C36" s="205"/>
+      <c r="D36" s="206" t="s">
         <v>673</v>
       </c>
-      <c r="E36" s="190"/>
-      <c r="F36" s="213"/>
-      <c r="G36" s="214"/>
-      <c r="H36" s="217" t="s">
+      <c r="E36" s="139"/>
+      <c r="F36" s="207"/>
+      <c r="G36" s="208"/>
+      <c r="H36" s="209" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A37" s="190" t="s">
+      <c r="A37" s="139" t="s">
         <v>872</v>
       </c>
-      <c r="B37" s="213" t="s">
+      <c r="B37" s="207" t="s">
         <v>873</v>
       </c>
-      <c r="C37" s="214"/>
-      <c r="D37" s="215" t="s">
+      <c r="C37" s="208"/>
+      <c r="D37" s="210" t="s">
         <v>674</v>
       </c>
-      <c r="E37" s="182"/>
-      <c r="F37" s="207"/>
-      <c r="G37" s="208"/>
-      <c r="H37" s="216" t="s">
+      <c r="E37" s="131"/>
+      <c r="F37" s="204"/>
+      <c r="G37" s="205"/>
+      <c r="H37" s="211" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A38" s="182" t="s">
+      <c r="A38" s="131" t="s">
         <v>874</v>
       </c>
-      <c r="B38" s="207" t="s">
+      <c r="B38" s="204" t="s">
         <v>875</v>
       </c>
-      <c r="C38" s="208"/>
-      <c r="D38" s="209" t="s">
+      <c r="C38" s="205"/>
+      <c r="D38" s="206" t="s">
         <v>675</v>
       </c>
-      <c r="E38" s="190"/>
-      <c r="F38" s="213"/>
-      <c r="G38" s="214"/>
-      <c r="H38" s="217" t="s">
+      <c r="E38" s="139"/>
+      <c r="F38" s="207"/>
+      <c r="G38" s="208"/>
+      <c r="H38" s="209" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A39" s="190" t="s">
+      <c r="A39" s="139" t="s">
         <v>876</v>
       </c>
-      <c r="B39" s="213" t="s">
+      <c r="B39" s="207" t="s">
         <v>877</v>
       </c>
-      <c r="C39" s="214"/>
-      <c r="D39" s="215" t="s">
+      <c r="C39" s="208"/>
+      <c r="D39" s="210" t="s">
         <v>676</v>
       </c>
-      <c r="E39" s="182"/>
-      <c r="F39" s="207"/>
-      <c r="G39" s="208"/>
-      <c r="H39" s="216" t="s">
+      <c r="E39" s="131"/>
+      <c r="F39" s="204"/>
+      <c r="G39" s="205"/>
+      <c r="H39" s="211" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A40" s="182" t="s">
+      <c r="A40" s="131" t="s">
         <v>878</v>
       </c>
-      <c r="B40" s="207" t="s">
+      <c r="B40" s="204" t="s">
         <v>877</v>
       </c>
-      <c r="C40" s="208"/>
-      <c r="D40" s="209" t="s">
+      <c r="C40" s="205"/>
+      <c r="D40" s="206" t="s">
         <v>676</v>
       </c>
-      <c r="E40" s="190"/>
-      <c r="F40" s="213"/>
-      <c r="G40" s="214"/>
-      <c r="H40" s="217"/>
+      <c r="E40" s="139"/>
+      <c r="F40" s="207"/>
+      <c r="G40" s="208"/>
+      <c r="H40" s="209"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A41" s="202" t="s">
+      <c r="A41" s="151" t="s">
         <v>879</v>
       </c>
-      <c r="B41" s="218" t="s">
+      <c r="B41" s="198" t="s">
         <v>877</v>
       </c>
-      <c r="C41" s="219"/>
-      <c r="D41" s="220" t="s">
+      <c r="C41" s="199"/>
+      <c r="D41" s="200" t="s">
         <v>676</v>
       </c>
-      <c r="E41" s="221"/>
-      <c r="F41" s="222"/>
-      <c r="G41" s="223"/>
-      <c r="H41" s="224"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="201"/>
+      <c r="G41" s="202"/>
+      <c r="H41" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -13401,35 +14110,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added WIP VID Intrep D+2
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="7"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="847">
   <si>
     <t>AWACS</t>
   </si>
@@ -2600,6 +2600,9 @@
   </si>
   <si>
     <t>Ramat David TWR</t>
+  </si>
+  <si>
+    <t>DODGE  QRA</t>
   </si>
 </sst>
 </file>
@@ -3873,21 +3876,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3897,21 +3918,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3996,6 +4002,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4014,57 +4071,6 @@
     <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4076,9 +4082,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4122,7 +4125,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4608,18 +4611,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="166" t="s">
+      <c r="R3" s="159" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="166"/>
-      <c r="T3" s="166"/>
-      <c r="AA3" s="167" t="s">
+      <c r="S3" s="159"/>
+      <c r="T3" s="159"/>
+      <c r="AA3" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="168"/>
-      <c r="AC3" s="168"/>
-      <c r="AD3" s="168"/>
-      <c r="AE3" s="169"/>
+      <c r="AB3" s="162"/>
+      <c r="AC3" s="162"/>
+      <c r="AD3" s="162"/>
+      <c r="AE3" s="163"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4662,7 +4665,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="159" t="s">
+      <c r="R4" s="164" t="s">
         <v>644</v>
       </c>
       <c r="S4" s="99" t="s">
@@ -4671,12 +4674,12 @@
       <c r="T4" s="100" t="s">
         <v>647</v>
       </c>
-      <c r="V4" s="157" t="s">
+      <c r="V4" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="157"/>
-      <c r="X4" s="157"/>
-      <c r="Y4" s="157"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
       <c r="AA4" s="90" t="s">
         <v>290</v>
       </c>
@@ -4730,7 +4733,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="160"/>
+      <c r="R5" s="165"/>
       <c r="S5" s="31" t="s">
         <v>613</v>
       </c>
@@ -4808,7 +4811,7 @@
         <v>662</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="161"/>
+      <c r="R6" s="166"/>
       <c r="S6" s="101" t="s">
         <v>646</v>
       </c>
@@ -4884,7 +4887,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="159" t="s">
+      <c r="R7" s="164" t="s">
         <v>650</v>
       </c>
       <c r="S7" s="99" t="s">
@@ -4964,7 +4967,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="160"/>
+      <c r="R8" s="165"/>
       <c r="S8" s="31" t="s">
         <v>613</v>
       </c>
@@ -5033,7 +5036,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="161"/>
+      <c r="R9" s="166"/>
       <c r="S9" s="101" t="s">
         <v>646</v>
       </c>
@@ -5160,7 +5163,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="162" t="s">
+      <c r="R11" s="168" t="s">
         <v>651</v>
       </c>
       <c r="S11" s="104" t="s">
@@ -5233,7 +5236,7 @@
       <c r="O12" s="95"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="163"/>
+      <c r="R12" s="169"/>
       <c r="S12" s="98" t="s">
         <v>613</v>
       </c>
@@ -5298,7 +5301,7 @@
       <c r="O13" s="95"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="164"/>
+      <c r="R13" s="170"/>
       <c r="S13" s="106" t="s">
         <v>646</v>
       </c>
@@ -5319,11 +5322,11 @@
         <v>501</v>
       </c>
       <c r="AA13" s="41"/>
-      <c r="AD13" s="167" t="s">
+      <c r="AD13" s="161" t="s">
         <v>636</v>
       </c>
-      <c r="AE13" s="168"/>
-      <c r="AF13" s="169"/>
+      <c r="AE13" s="162"/>
+      <c r="AF13" s="163"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5370,7 +5373,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="159" t="s">
+      <c r="R14" s="164" t="s">
         <v>654</v>
       </c>
       <c r="S14" s="104" t="s">
@@ -5448,7 +5451,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="160"/>
+      <c r="R15" s="165"/>
       <c r="S15" s="98" t="s">
         <v>613</v>
       </c>
@@ -5509,22 +5512,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="161"/>
+      <c r="R16" s="166"/>
       <c r="S16" s="106" t="s">
         <v>646</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>657</v>
       </c>
-      <c r="V16" s="157" t="s">
+      <c r="V16" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="157"/>
-      <c r="X16" s="157"/>
-      <c r="Y16" s="157"/>
-      <c r="Z16" s="157"/>
-      <c r="AA16" s="157"/>
-      <c r="AB16" s="157"/>
+      <c r="W16" s="160"/>
+      <c r="X16" s="160"/>
+      <c r="Y16" s="160"/>
+      <c r="Z16" s="160"/>
+      <c r="AA16" s="160"/>
+      <c r="AB16" s="160"/>
       <c r="AD16" s="7" t="s">
         <v>629</v>
       </c>
@@ -5816,11 +5819,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="157" t="s">
+      <c r="R20" s="160" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="157"/>
-      <c r="T20" s="157"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>678</v>
@@ -5991,15 +5994,15 @@
       <c r="T22" t="s">
         <v>483</v>
       </c>
-      <c r="V22" s="167" t="s">
+      <c r="V22" s="161" t="s">
         <v>669</v>
       </c>
-      <c r="W22" s="168"/>
-      <c r="X22" s="168"/>
-      <c r="Y22" s="168"/>
-      <c r="Z22" s="168"/>
-      <c r="AA22" s="168"/>
-      <c r="AB22" s="169"/>
+      <c r="W22" s="162"/>
+      <c r="X22" s="162"/>
+      <c r="Y22" s="162"/>
+      <c r="Z22" s="162"/>
+      <c r="AA22" s="162"/>
+      <c r="AB22" s="163"/>
       <c r="AD22" s="7" t="s">
         <v>635</v>
       </c>
@@ -6459,33 +6462,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="157" t="s">
+      <c r="B31" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="157"/>
-      <c r="H31" s="157"/>
-      <c r="J31" s="157" t="s">
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="J31" s="160" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="157"/>
-      <c r="L31" s="157"/>
-      <c r="M31" s="157"/>
-      <c r="N31" s="157"/>
-      <c r="O31" s="157"/>
-      <c r="P31" s="157"/>
-      <c r="T31" s="157" t="s">
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+      <c r="T31" s="160" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="157"/>
-      <c r="V31" s="157"/>
-      <c r="W31" s="157"/>
-      <c r="X31" s="157"/>
-      <c r="Y31" s="157"/>
-      <c r="Z31" s="157"/>
+      <c r="U31" s="160"/>
+      <c r="V31" s="160"/>
+      <c r="W31" s="160"/>
+      <c r="X31" s="160"/>
+      <c r="Y31" s="160"/>
+      <c r="Z31" s="160"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6764,7 +6767,7 @@
       <c r="Z35" s="7" t="s">
         <v>584</v>
       </c>
-      <c r="AD35" s="165" t="s">
+      <c r="AD35" s="158" t="s">
         <v>706</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6847,7 +6850,7 @@
       <c r="Z36" s="7" t="s">
         <v>585</v>
       </c>
-      <c r="AD36" s="165"/>
+      <c r="AD36" s="158"/>
       <c r="AE36" s="7" t="s">
         <v>516</v>
       </c>
@@ -6920,7 +6923,7 @@
       <c r="Z37" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="AD37" s="165"/>
+      <c r="AD37" s="158"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -6976,7 +6979,7 @@
       <c r="Z38" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="AD38" s="165"/>
+      <c r="AD38" s="158"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -6990,15 +6993,15 @@
       <c r="F39" t="s">
         <v>573</v>
       </c>
-      <c r="J39" s="158" t="s">
+      <c r="J39" s="167" t="s">
         <v>480</v>
       </c>
-      <c r="K39" s="158"/>
-      <c r="L39" s="158"/>
-      <c r="M39" s="158"/>
-      <c r="N39" s="158"/>
-      <c r="O39" s="158"/>
-      <c r="P39" s="158"/>
+      <c r="K39" s="167"/>
+      <c r="L39" s="167"/>
+      <c r="M39" s="167"/>
+      <c r="N39" s="167"/>
+      <c r="O39" s="167"/>
+      <c r="P39" s="167"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7306,6 +7309,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7315,13 +7325,6 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7348,34 +7351,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="221" t="s">
+      <c r="A1" s="222" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="222"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="A2" s="223"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="183" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="182" t="s">
+      <c r="B3" s="184"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="183" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7917,22 +7920,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="224" t="s">
         <v>363</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="225" t="s">
         <v>364</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -8037,12 +8040,12 @@
       <c r="E10" s="43"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
-      <c r="B14" s="224" t="s">
+      <c r="B14" s="225" t="s">
         <v>381</v>
       </c>
-      <c r="C14" s="224"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="224"/>
+      <c r="C14" s="225"/>
+      <c r="D14" s="225"/>
+      <c r="E14" s="225"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="B15" s="43"/>
@@ -8154,8 +8157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8834,6 +8837,21 @@
       </c>
     </row>
     <row r="18" spans="1:11">
+      <c r="A18" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="B18" s="7">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>451</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>736</v>
+      </c>
       <c r="G18" s="7" t="s">
         <v>745</v>
       </c>
@@ -8851,6 +8869,17 @@
       </c>
     </row>
     <row r="19" spans="1:11">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7">
+        <v>452</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>736</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7">
@@ -8864,6 +8893,17 @@
       </c>
     </row>
     <row r="20" spans="1:11">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7">
+        <v>453</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>736</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7">
@@ -8877,6 +8917,17 @@
       </c>
     </row>
     <row r="21" spans="1:11">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7">
+        <v>454</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>736</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7">
@@ -9041,8 +9092,23 @@
       <c r="E32" s="7" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="H32" s="7">
+        <v>2</v>
+      </c>
+      <c r="I32" s="7">
+        <v>621</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7">
@@ -9054,8 +9120,19 @@
       <c r="E33" s="7" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7">
+        <v>622</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7">
@@ -9067,8 +9144,19 @@
       <c r="E34" s="7" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7">
+        <v>623</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7">
@@ -9080,8 +9168,19 @@
       <c r="E35" s="7" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7">
+        <v>624</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="7" t="s">
         <v>762</v>
       </c>
@@ -9098,7 +9197,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:11">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7">
@@ -9111,7 +9210,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:11">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7">
@@ -9124,7 +9223,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:11">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7">
@@ -9165,40 +9264,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="171" t="s">
         <v>707</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="172"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="173"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="175"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="176"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="177" t="s">
         <v>614</v>
       </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177" t="s">
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178" t="s">
         <v>615</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="179"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="79">
@@ -10231,14 +10330,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="182"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -10249,16 +10348,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="183" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="182" t="s">
+      <c r="B3" s="184"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="183" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -10528,28 +10627,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="189" t="s">
         <v>744</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="189"/>
+      <c r="H1" s="189"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="186" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -10824,16 +10923,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="186" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="186"/>
-      <c r="C15" s="186"/>
-      <c r="D15" s="186"/>
-      <c r="E15" s="186"/>
-      <c r="F15" s="186"/>
-      <c r="G15" s="186"/>
-      <c r="H15" s="187"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="187"/>
+      <c r="E15" s="187"/>
+      <c r="F15" s="187"/>
+      <c r="G15" s="187"/>
+      <c r="H15" s="188"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -11123,16 +11222,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="186" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="186"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="186"/>
-      <c r="E28" s="186"/>
-      <c r="F28" s="186"/>
-      <c r="G28" s="186"/>
-      <c r="H28" s="187"/>
+      <c r="B28" s="187"/>
+      <c r="C28" s="187"/>
+      <c r="D28" s="187"/>
+      <c r="E28" s="187"/>
+      <c r="F28" s="187"/>
+      <c r="G28" s="187"/>
+      <c r="H28" s="188"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -11445,12 +11544,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="190" t="s">
         <v>719</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -11658,28 +11757,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="191" t="s">
         <v>759</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="186" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -11970,12 +12069,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="186" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="186"/>
-      <c r="C15" s="186"/>
-      <c r="D15" s="187"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="188"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -12143,12 +12242,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="186" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="186"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="187"/>
+      <c r="B28" s="187"/>
+      <c r="C28" s="187"/>
+      <c r="D28" s="188"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -12332,7 +12431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
@@ -12352,40 +12451,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>840</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="182"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="191"/>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="193"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="194"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="195" t="s">
         <v>385</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="194" t="s">
+      <c r="B3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="195" t="s">
         <v>386</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="197"/>
+      <c r="F3" s="196"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="198"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="75">
@@ -12476,7 +12575,7 @@
       <c r="F7" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="225" t="s">
+      <c r="G7" s="157" t="s">
         <v>489</v>
       </c>
       <c r="H7" s="76" t="s">
@@ -12799,7 +12898,7 @@
       <c r="C20" s="76" t="s">
         <v>658</v>
       </c>
-      <c r="D20" s="225" t="s">
+      <c r="D20" s="157" t="s">
         <v>842</v>
       </c>
       <c r="E20" s="75">
@@ -12825,7 +12924,7 @@
       <c r="C21" s="76" t="s">
         <v>659</v>
       </c>
-      <c r="D21" s="225" t="s">
+      <c r="D21" s="157" t="s">
         <v>843</v>
       </c>
       <c r="E21" s="75">
@@ -12849,7 +12948,7 @@
       <c r="C22" s="76" t="s">
         <v>660</v>
       </c>
-      <c r="D22" s="225" t="s">
+      <c r="D22" s="157" t="s">
         <v>844</v>
       </c>
       <c r="E22" s="75">
@@ -13078,40 +13177,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="216" t="s">
         <v>838</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
+      <c r="A2" s="217"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="218" t="s">
         <v>385</v>
       </c>
-      <c r="B3" s="201"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="200" t="s">
+      <c r="B3" s="219"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="218" t="s">
         <v>386</v>
       </c>
-      <c r="F3" s="201"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="203"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="221"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="126">
@@ -13640,36 +13739,36 @@
       <c r="H24" s="154"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="200" t="s">
+      <c r="A25" s="218" t="s">
         <v>794</v>
       </c>
-      <c r="B25" s="201"/>
-      <c r="C25" s="202"/>
-      <c r="D25" s="203"/>
-      <c r="E25" s="200" t="s">
+      <c r="B25" s="219"/>
+      <c r="C25" s="220"/>
+      <c r="D25" s="221"/>
+      <c r="E25" s="218" t="s">
         <v>795</v>
       </c>
-      <c r="F25" s="201"/>
-      <c r="G25" s="202"/>
-      <c r="H25" s="203"/>
+      <c r="F25" s="219"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="221"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="130" t="s">
         <v>796</v>
       </c>
-      <c r="B26" s="204" t="s">
+      <c r="B26" s="205" t="s">
         <v>797</v>
       </c>
-      <c r="C26" s="205"/>
-      <c r="D26" s="206"/>
+      <c r="C26" s="206"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="126" t="s">
         <v>798</v>
       </c>
-      <c r="F26" s="207" t="s">
+      <c r="F26" s="213" t="s">
         <v>799</v>
       </c>
-      <c r="G26" s="208"/>
-      <c r="H26" s="209" t="s">
+      <c r="G26" s="214"/>
+      <c r="H26" s="215" t="s">
         <v>767</v>
       </c>
     </row>
@@ -13677,21 +13776,21 @@
       <c r="A27" s="138" t="s">
         <v>800</v>
       </c>
-      <c r="B27" s="210" t="s">
+      <c r="B27" s="208" t="s">
         <v>801</v>
       </c>
-      <c r="C27" s="211"/>
-      <c r="D27" s="212" t="s">
+      <c r="C27" s="209"/>
+      <c r="D27" s="211" t="s">
         <v>629</v>
       </c>
       <c r="E27" s="130" t="s">
         <v>802</v>
       </c>
-      <c r="F27" s="204" t="s">
+      <c r="F27" s="205" t="s">
         <v>803</v>
       </c>
-      <c r="G27" s="205"/>
-      <c r="H27" s="213" t="s">
+      <c r="G27" s="206"/>
+      <c r="H27" s="212" t="s">
         <v>769</v>
       </c>
     </row>
@@ -13699,21 +13798,21 @@
       <c r="A28" s="130" t="s">
         <v>804</v>
       </c>
-      <c r="B28" s="204" t="s">
+      <c r="B28" s="205" t="s">
         <v>805</v>
       </c>
-      <c r="C28" s="205"/>
-      <c r="D28" s="206" t="s">
+      <c r="C28" s="206"/>
+      <c r="D28" s="207" t="s">
         <v>630</v>
       </c>
       <c r="E28" s="138" t="s">
         <v>806</v>
       </c>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="208" t="s">
         <v>807</v>
       </c>
-      <c r="G28" s="211"/>
-      <c r="H28" s="214" t="s">
+      <c r="G28" s="209"/>
+      <c r="H28" s="210" t="s">
         <v>771</v>
       </c>
     </row>
@@ -13721,21 +13820,21 @@
       <c r="A29" s="138" t="s">
         <v>808</v>
       </c>
-      <c r="B29" s="210" t="s">
+      <c r="B29" s="208" t="s">
         <v>809</v>
       </c>
-      <c r="C29" s="211"/>
-      <c r="D29" s="212" t="s">
+      <c r="C29" s="209"/>
+      <c r="D29" s="211" t="s">
         <v>631</v>
       </c>
       <c r="E29" s="130" t="s">
         <v>810</v>
       </c>
-      <c r="F29" s="204" t="s">
+      <c r="F29" s="205" t="s">
         <v>811</v>
       </c>
-      <c r="G29" s="205"/>
-      <c r="H29" s="213" t="s">
+      <c r="G29" s="206"/>
+      <c r="H29" s="212" t="s">
         <v>773</v>
       </c>
     </row>
@@ -13743,21 +13842,21 @@
       <c r="A30" s="130" t="s">
         <v>812</v>
       </c>
-      <c r="B30" s="204" t="s">
+      <c r="B30" s="205" t="s">
         <v>813</v>
       </c>
-      <c r="C30" s="205"/>
-      <c r="D30" s="206" t="s">
+      <c r="C30" s="206"/>
+      <c r="D30" s="207" t="s">
         <v>632</v>
       </c>
       <c r="E30" s="138" t="s">
         <v>814</v>
       </c>
-      <c r="F30" s="210" t="s">
+      <c r="F30" s="208" t="s">
         <v>815</v>
       </c>
-      <c r="G30" s="211"/>
-      <c r="H30" s="214" t="s">
+      <c r="G30" s="209"/>
+      <c r="H30" s="210" t="s">
         <v>775</v>
       </c>
     </row>
@@ -13765,21 +13864,21 @@
       <c r="A31" s="138" t="s">
         <v>816</v>
       </c>
-      <c r="B31" s="210" t="s">
+      <c r="B31" s="208" t="s">
         <v>817</v>
       </c>
-      <c r="C31" s="211"/>
-      <c r="D31" s="212" t="s">
+      <c r="C31" s="209"/>
+      <c r="D31" s="211" t="s">
         <v>633</v>
       </c>
       <c r="E31" s="130" t="s">
         <v>818</v>
       </c>
-      <c r="F31" s="204" t="s">
+      <c r="F31" s="205" t="s">
         <v>819</v>
       </c>
-      <c r="G31" s="205"/>
-      <c r="H31" s="213" t="s">
+      <c r="G31" s="206"/>
+      <c r="H31" s="212" t="s">
         <v>499</v>
       </c>
     </row>
@@ -13787,17 +13886,17 @@
       <c r="A32" s="130" t="s">
         <v>820</v>
       </c>
-      <c r="B32" s="204" t="s">
+      <c r="B32" s="205" t="s">
         <v>821</v>
       </c>
-      <c r="C32" s="205"/>
-      <c r="D32" s="206" t="s">
+      <c r="C32" s="206"/>
+      <c r="D32" s="207" t="s">
         <v>634</v>
       </c>
       <c r="E32" s="138"/>
-      <c r="F32" s="210"/>
-      <c r="G32" s="211"/>
-      <c r="H32" s="214" t="s">
+      <c r="F32" s="208"/>
+      <c r="G32" s="209"/>
+      <c r="H32" s="210" t="s">
         <v>500</v>
       </c>
     </row>
@@ -13805,17 +13904,17 @@
       <c r="A33" s="138" t="s">
         <v>822</v>
       </c>
-      <c r="B33" s="210" t="s">
+      <c r="B33" s="208" t="s">
         <v>823</v>
       </c>
-      <c r="C33" s="211"/>
-      <c r="D33" s="212" t="s">
+      <c r="C33" s="209"/>
+      <c r="D33" s="211" t="s">
         <v>628</v>
       </c>
       <c r="E33" s="130"/>
-      <c r="F33" s="204"/>
-      <c r="G33" s="205"/>
-      <c r="H33" s="213" t="s">
+      <c r="F33" s="205"/>
+      <c r="G33" s="206"/>
+      <c r="H33" s="212" t="s">
         <v>767</v>
       </c>
     </row>
@@ -13823,17 +13922,17 @@
       <c r="A34" s="130" t="s">
         <v>824</v>
       </c>
-      <c r="B34" s="204" t="s">
+      <c r="B34" s="205" t="s">
         <v>825</v>
       </c>
-      <c r="C34" s="205"/>
-      <c r="D34" s="206" t="s">
+      <c r="C34" s="206"/>
+      <c r="D34" s="207" t="s">
         <v>629</v>
       </c>
       <c r="E34" s="138"/>
-      <c r="F34" s="210"/>
-      <c r="G34" s="211"/>
-      <c r="H34" s="214" t="s">
+      <c r="F34" s="208"/>
+      <c r="G34" s="209"/>
+      <c r="H34" s="210" t="s">
         <v>769</v>
       </c>
     </row>
@@ -13841,17 +13940,17 @@
       <c r="A35" s="138" t="s">
         <v>826</v>
       </c>
-      <c r="B35" s="210" t="s">
+      <c r="B35" s="208" t="s">
         <v>827</v>
       </c>
-      <c r="C35" s="211"/>
-      <c r="D35" s="212" t="s">
+      <c r="C35" s="209"/>
+      <c r="D35" s="211" t="s">
         <v>630</v>
       </c>
       <c r="E35" s="130"/>
-      <c r="F35" s="204"/>
-      <c r="G35" s="205"/>
-      <c r="H35" s="213" t="s">
+      <c r="F35" s="205"/>
+      <c r="G35" s="206"/>
+      <c r="H35" s="212" t="s">
         <v>771</v>
       </c>
     </row>
@@ -13859,17 +13958,17 @@
       <c r="A36" s="130" t="s">
         <v>828</v>
       </c>
-      <c r="B36" s="204" t="s">
+      <c r="B36" s="205" t="s">
         <v>829</v>
       </c>
-      <c r="C36" s="205"/>
-      <c r="D36" s="206" t="s">
+      <c r="C36" s="206"/>
+      <c r="D36" s="207" t="s">
         <v>631</v>
       </c>
       <c r="E36" s="138"/>
-      <c r="F36" s="210"/>
-      <c r="G36" s="211"/>
-      <c r="H36" s="214" t="s">
+      <c r="F36" s="208"/>
+      <c r="G36" s="209"/>
+      <c r="H36" s="210" t="s">
         <v>773</v>
       </c>
     </row>
@@ -13877,17 +13976,17 @@
       <c r="A37" s="138" t="s">
         <v>830</v>
       </c>
-      <c r="B37" s="210" t="s">
+      <c r="B37" s="208" t="s">
         <v>831</v>
       </c>
-      <c r="C37" s="211"/>
-      <c r="D37" s="212" t="s">
+      <c r="C37" s="209"/>
+      <c r="D37" s="211" t="s">
         <v>632</v>
       </c>
       <c r="E37" s="130"/>
-      <c r="F37" s="204"/>
-      <c r="G37" s="205"/>
-      <c r="H37" s="213" t="s">
+      <c r="F37" s="205"/>
+      <c r="G37" s="206"/>
+      <c r="H37" s="212" t="s">
         <v>775</v>
       </c>
     </row>
@@ -13895,17 +13994,17 @@
       <c r="A38" s="130" t="s">
         <v>832</v>
       </c>
-      <c r="B38" s="204" t="s">
+      <c r="B38" s="205" t="s">
         <v>833</v>
       </c>
-      <c r="C38" s="205"/>
-      <c r="D38" s="206" t="s">
+      <c r="C38" s="206"/>
+      <c r="D38" s="207" t="s">
         <v>633</v>
       </c>
       <c r="E38" s="138"/>
-      <c r="F38" s="210"/>
-      <c r="G38" s="211"/>
-      <c r="H38" s="214" t="s">
+      <c r="F38" s="208"/>
+      <c r="G38" s="209"/>
+      <c r="H38" s="210" t="s">
         <v>499</v>
       </c>
     </row>
@@ -13913,17 +14012,17 @@
       <c r="A39" s="138" t="s">
         <v>834</v>
       </c>
-      <c r="B39" s="210" t="s">
+      <c r="B39" s="208" t="s">
         <v>835</v>
       </c>
-      <c r="C39" s="211"/>
-      <c r="D39" s="212" t="s">
+      <c r="C39" s="209"/>
+      <c r="D39" s="211" t="s">
         <v>634</v>
       </c>
       <c r="E39" s="130"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="205"/>
-      <c r="H39" s="213" t="s">
+      <c r="F39" s="205"/>
+      <c r="G39" s="206"/>
+      <c r="H39" s="212" t="s">
         <v>500</v>
       </c>
     </row>
@@ -13931,36 +14030,65 @@
       <c r="A40" s="130" t="s">
         <v>836</v>
       </c>
-      <c r="B40" s="204" t="s">
+      <c r="B40" s="205" t="s">
         <v>835</v>
       </c>
-      <c r="C40" s="205"/>
-      <c r="D40" s="206" t="s">
+      <c r="C40" s="206"/>
+      <c r="D40" s="207" t="s">
         <v>634</v>
       </c>
       <c r="E40" s="138"/>
-      <c r="F40" s="210"/>
-      <c r="G40" s="211"/>
-      <c r="H40" s="214"/>
+      <c r="F40" s="208"/>
+      <c r="G40" s="209"/>
+      <c r="H40" s="210"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="150" t="s">
         <v>837</v>
       </c>
-      <c r="B41" s="215" t="s">
+      <c r="B41" s="199" t="s">
         <v>835</v>
       </c>
-      <c r="C41" s="216"/>
-      <c r="D41" s="217" t="s">
+      <c r="C41" s="200"/>
+      <c r="D41" s="201" t="s">
         <v>634</v>
       </c>
       <c r="E41" s="155"/>
-      <c r="F41" s="218"/>
-      <c r="G41" s="219"/>
-      <c r="H41" s="220"/>
+      <c r="F41" s="202"/>
+      <c r="G41" s="203"/>
+      <c r="H41" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -13969,35 +14097,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added A-10C II to AC overview
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="854">
   <si>
     <t>AWACS</t>
   </si>
@@ -3905,21 +3905,39 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3929,21 +3947,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4028,6 +4031,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4046,57 +4100,6 @@
     <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4108,9 +4111,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4154,7 +4154,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4692,18 +4692,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="166" t="s">
+      <c r="R3" s="159" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="166"/>
-      <c r="T3" s="166"/>
-      <c r="AA3" s="167" t="s">
+      <c r="S3" s="159"/>
+      <c r="T3" s="159"/>
+      <c r="AA3" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="168"/>
-      <c r="AC3" s="168"/>
-      <c r="AD3" s="168"/>
-      <c r="AE3" s="169"/>
+      <c r="AB3" s="162"/>
+      <c r="AC3" s="162"/>
+      <c r="AD3" s="162"/>
+      <c r="AE3" s="163"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4746,7 +4746,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="159" t="s">
+      <c r="R4" s="164" t="s">
         <v>639</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -4755,12 +4755,12 @@
       <c r="T4" s="99" t="s">
         <v>642</v>
       </c>
-      <c r="V4" s="157" t="s">
+      <c r="V4" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="157"/>
-      <c r="X4" s="157"/>
-      <c r="Y4" s="157"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="160"/>
+      <c r="R5" s="165"/>
       <c r="S5" s="31" t="s">
         <v>608</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>657</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="161"/>
+      <c r="R6" s="166"/>
       <c r="S6" s="100" t="s">
         <v>641</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="159" t="s">
+      <c r="R7" s="164" t="s">
         <v>645</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5048,7 +5048,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="160"/>
+      <c r="R8" s="165"/>
       <c r="S8" s="31" t="s">
         <v>608</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="161"/>
+      <c r="R9" s="166"/>
       <c r="S9" s="100" t="s">
         <v>641</v>
       </c>
@@ -5163,7 +5163,7 @@
       <c r="I10" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="225" t="s">
+      <c r="J10" s="157" t="s">
         <v>90</v>
       </c>
       <c r="K10" s="53" t="s">
@@ -5221,7 +5221,7 @@
       <c r="H11" s="107" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="225" t="s">
+      <c r="I11" s="157" t="s">
         <v>101</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -5244,7 +5244,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="162" t="s">
+      <c r="R11" s="168" t="s">
         <v>646</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5317,7 +5317,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="163"/>
+      <c r="R12" s="169"/>
       <c r="S12" s="97" t="s">
         <v>608</v>
       </c>
@@ -5367,7 +5367,7 @@
       <c r="J13" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="K13" s="225" t="s">
+      <c r="K13" s="157" t="s">
         <v>126</v>
       </c>
       <c r="L13" s="39" t="s">
@@ -5382,7 +5382,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="164"/>
+      <c r="R13" s="170"/>
       <c r="S13" s="105" t="s">
         <v>641</v>
       </c>
@@ -5403,11 +5403,11 @@
         <v>501</v>
       </c>
       <c r="AA13" s="41"/>
-      <c r="AD13" s="167" t="s">
+      <c r="AD13" s="161" t="s">
         <v>631</v>
       </c>
-      <c r="AE13" s="168"/>
-      <c r="AF13" s="169"/>
+      <c r="AE13" s="162"/>
+      <c r="AF13" s="163"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5454,7 +5454,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="159" t="s">
+      <c r="R14" s="164" t="s">
         <v>649</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5532,7 +5532,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="160"/>
+      <c r="R15" s="165"/>
       <c r="S15" s="97" t="s">
         <v>608</v>
       </c>
@@ -5593,22 +5593,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="161"/>
+      <c r="R16" s="166"/>
       <c r="S16" s="105" t="s">
         <v>641</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>652</v>
       </c>
-      <c r="V16" s="157" t="s">
+      <c r="V16" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="157"/>
-      <c r="X16" s="157"/>
-      <c r="Y16" s="157"/>
-      <c r="Z16" s="157"/>
-      <c r="AA16" s="157"/>
-      <c r="AB16" s="157"/>
+      <c r="W16" s="160"/>
+      <c r="X16" s="160"/>
+      <c r="Y16" s="160"/>
+      <c r="Z16" s="160"/>
+      <c r="AA16" s="160"/>
+      <c r="AB16" s="160"/>
       <c r="AD16" s="7" t="s">
         <v>624</v>
       </c>
@@ -5900,11 +5900,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="157" t="s">
+      <c r="R20" s="160" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="157"/>
-      <c r="T20" s="157"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>673</v>
@@ -6075,15 +6075,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="167" t="s">
+      <c r="V22" s="161" t="s">
         <v>664</v>
       </c>
-      <c r="W22" s="168"/>
-      <c r="X22" s="168"/>
-      <c r="Y22" s="168"/>
-      <c r="Z22" s="168"/>
-      <c r="AA22" s="168"/>
-      <c r="AB22" s="169"/>
+      <c r="W22" s="162"/>
+      <c r="X22" s="162"/>
+      <c r="Y22" s="162"/>
+      <c r="Z22" s="162"/>
+      <c r="AA22" s="162"/>
+      <c r="AB22" s="163"/>
       <c r="AD22" s="7" t="s">
         <v>630</v>
       </c>
@@ -6218,7 +6218,7 @@
       <c r="N24" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="O24" s="225"/>
+      <c r="O24" s="157"/>
       <c r="P24" s="3" t="s">
         <v>437</v>
       </c>
@@ -6543,33 +6543,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="157" t="s">
+      <c r="B31" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="157"/>
-      <c r="D31" s="157"/>
-      <c r="E31" s="157"/>
-      <c r="F31" s="157"/>
-      <c r="G31" s="157"/>
-      <c r="H31" s="157"/>
-      <c r="J31" s="157" t="s">
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="J31" s="160" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="157"/>
-      <c r="L31" s="157"/>
-      <c r="M31" s="157"/>
-      <c r="N31" s="157"/>
-      <c r="O31" s="157"/>
-      <c r="P31" s="157"/>
-      <c r="T31" s="157" t="s">
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+      <c r="T31" s="160" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="157"/>
-      <c r="V31" s="157"/>
-      <c r="W31" s="157"/>
-      <c r="X31" s="157"/>
-      <c r="Y31" s="157"/>
-      <c r="Z31" s="157"/>
+      <c r="U31" s="160"/>
+      <c r="V31" s="160"/>
+      <c r="W31" s="160"/>
+      <c r="X31" s="160"/>
+      <c r="Y31" s="160"/>
+      <c r="Z31" s="160"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6848,7 +6848,7 @@
       <c r="Z35" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD35" s="165" t="s">
+      <c r="AD35" s="158" t="s">
         <v>701</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6931,7 +6931,7 @@
       <c r="Z36" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD36" s="165"/>
+      <c r="AD36" s="158"/>
       <c r="AE36" s="7" t="s">
         <v>511</v>
       </c>
@@ -7004,7 +7004,7 @@
       <c r="Z37" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="AD37" s="165"/>
+      <c r="AD37" s="158"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7060,7 +7060,7 @@
       <c r="Z38" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="AD38" s="165"/>
+      <c r="AD38" s="158"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7074,15 +7074,15 @@
       <c r="F39" t="s">
         <v>568</v>
       </c>
-      <c r="J39" s="158" t="s">
+      <c r="J39" s="167" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="158"/>
-      <c r="L39" s="158"/>
-      <c r="M39" s="158"/>
-      <c r="N39" s="158"/>
-      <c r="O39" s="158"/>
-      <c r="P39" s="158"/>
+      <c r="K39" s="167"/>
+      <c r="L39" s="167"/>
+      <c r="M39" s="167"/>
+      <c r="N39" s="167"/>
+      <c r="O39" s="167"/>
+      <c r="P39" s="167"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7301,7 +7301,7 @@
       <c r="D48" t="s">
         <v>437</v>
       </c>
-      <c r="E48" s="225" t="s">
+      <c r="E48" s="157" t="s">
         <v>101</v>
       </c>
       <c r="F48" t="s">
@@ -7316,7 +7316,7 @@
       <c r="Z48" s="7"/>
     </row>
     <row r="49" spans="5:26">
-      <c r="E49" s="225" t="s">
+      <c r="E49" s="157" t="s">
         <v>90</v>
       </c>
       <c r="F49" t="s">
@@ -7343,7 +7343,7 @@
       </c>
     </row>
     <row r="50" spans="5:26">
-      <c r="E50" s="225" t="s">
+      <c r="E50" s="157" t="s">
         <v>126</v>
       </c>
       <c r="F50" t="s">
@@ -7411,6 +7411,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7420,13 +7427,6 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7453,34 +7453,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="221" t="s">
+      <c r="A1" s="222" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="221"/>
-      <c r="C1" s="221"/>
-      <c r="D1" s="221"/>
-      <c r="E1" s="221"/>
-      <c r="F1" s="221"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="222"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="A2" s="223"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="183" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="182" t="s">
+      <c r="B3" s="184"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="183" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7837,14 +7837,14 @@
       <c r="F21" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="N21" s="223" t="s">
+      <c r="N21" s="224" t="s">
         <v>842</v>
       </c>
-      <c r="O21" s="223"/>
-      <c r="P21" s="223"/>
-      <c r="Q21" s="223"/>
-      <c r="R21" s="223"/>
-      <c r="S21" s="223"/>
+      <c r="O21" s="224"/>
+      <c r="P21" s="224"/>
+      <c r="Q21" s="224"/>
+      <c r="R21" s="224"/>
+      <c r="S21" s="224"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1">
       <c r="A22" s="54">
@@ -7865,12 +7865,12 @@
       <c r="F22" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="O22" s="224" t="s">
+      <c r="O22" s="225" t="s">
         <v>363</v>
       </c>
-      <c r="P22" s="224"/>
-      <c r="Q22" s="224"/>
-      <c r="R22" s="224"/>
+      <c r="P22" s="225"/>
+      <c r="Q22" s="225"/>
+      <c r="R22" s="225"/>
     </row>
     <row r="23" spans="1:19" ht="19.5" thickBot="1">
       <c r="A23" s="54">
@@ -8114,7 +8114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -8127,22 +8127,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="224" t="s">
         <v>842</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="224" t="s">
+      <c r="B2" s="225" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -8263,10 +8263,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8920,7 +8920,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:11">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7">
@@ -8944,7 +8944,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:11">
       <c r="A18" s="7" t="s">
         <v>841</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:11">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7">
@@ -9000,7 +9000,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:11">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7">
@@ -9024,7 +9024,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:11">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7">
@@ -9048,338 +9048,562 @@
         <v>646</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="155" t="s">
-        <v>736</v>
-      </c>
-      <c r="B27" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="C27" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="D27" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="E27" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="G27" s="155" t="s">
-        <v>736</v>
-      </c>
-      <c r="H27" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="I27" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="J27" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="K27" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="M27" s="155" t="s">
-        <v>736</v>
-      </c>
-      <c r="N27" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="O27" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="P27" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="Q27" s="155" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1</v>
-      </c>
-      <c r="C28" s="7">
-        <v>311</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="H28" s="7">
-        <v>1</v>
-      </c>
+    <row r="22" spans="1:11">
+      <c r="G22" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="H22" s="7">
+        <v>6</v>
+      </c>
+      <c r="I22" s="7">
+        <v>161</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7">
+        <v>162</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7">
+        <v>163</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7">
+        <v>164</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="G26" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="H26" s="7">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7">
+        <v>171</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7">
+        <v>172</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="7">
-        <v>611</v>
+        <v>173</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>849</v>
-      </c>
-      <c r="N28" s="7">
-        <v>1</v>
-      </c>
-      <c r="O28" s="7">
-        <v>711</v>
-      </c>
-      <c r="P28" s="7" t="s">
-        <v>848</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7">
-        <v>312</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>759</v>
-      </c>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7">
-        <v>612</v>
+        <v>174</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="O29">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7">
-        <v>313</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="G30" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="H30" s="7">
+        <v>8</v>
+      </c>
       <c r="I30" s="7">
-        <v>613</v>
+        <v>181</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="O30">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7">
-        <v>314</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>759</v>
-      </c>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7">
-        <v>614</v>
+        <v>182</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="O31">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="B32" s="7">
-        <v>2</v>
-      </c>
-      <c r="C32" s="7">
-        <v>321</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="H32" s="7">
-        <v>2</v>
-      </c>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="7">
-        <v>621</v>
+        <v>183</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7">
-        <v>322</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>759</v>
-      </c>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7">
-        <v>622</v>
+        <v>184</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7">
-        <v>323</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>759</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+        <v>731</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="G34" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="H34" s="7">
+        <v>9</v>
+      </c>
       <c r="I34" s="7">
-        <v>623</v>
+        <v>191</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>602</v>
+        <v>449</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7">
-        <v>324</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>759</v>
-      </c>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7">
+        <v>192</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7">
+        <v>193</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7">
+        <v>194</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="155" t="s">
+        <v>736</v>
+      </c>
+      <c r="B39" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="C39" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="D39" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="E39" s="155" t="s">
+        <v>735</v>
+      </c>
+      <c r="G39" s="155" t="s">
+        <v>736</v>
+      </c>
+      <c r="H39" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="I39" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="J39" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="K39" s="155" t="s">
+        <v>735</v>
+      </c>
+      <c r="M39" s="155" t="s">
+        <v>736</v>
+      </c>
+      <c r="N39" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="O39" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="P39" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q39" s="155" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
+        <v>311</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1</v>
+      </c>
+      <c r="I40" s="7">
+        <v>611</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="N40" s="7">
+        <v>1</v>
+      </c>
+      <c r="O40" s="7">
+        <v>711</v>
+      </c>
+      <c r="P40" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7">
+        <v>312</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7">
+        <v>612</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="O41">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7">
+        <v>313</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7">
+        <v>613</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="O42">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7">
+        <v>314</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7">
+        <v>614</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="O43">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="B44" s="7">
+        <v>2</v>
+      </c>
+      <c r="C44" s="7">
+        <v>321</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="H44" s="7">
+        <v>2</v>
+      </c>
+      <c r="I44" s="7">
+        <v>621</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7">
+        <v>322</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7">
+        <v>622</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7">
+        <v>323</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7">
+        <v>623</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7">
+        <v>324</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7">
         <v>624</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="J47" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="K47" s="7" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="7" t="s">
+    <row r="48" spans="1:17">
+      <c r="A48" s="7" t="s">
         <v>757</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B48" s="7">
         <v>3</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C48" s="7">
         <v>331</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7">
+    <row r="49" spans="1:5">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7">
         <v>332</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7">
+    <row r="50" spans="1:5">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7">
         <v>333</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D50" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7">
+    <row r="51" spans="1:5">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7">
         <v>334</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>759</v>
       </c>
     </row>
@@ -9411,40 +9635,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="171" t="s">
         <v>702</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="172"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="173"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="173"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="175"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="176"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="177" t="s">
         <v>609</v>
       </c>
-      <c r="B3" s="177"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177" t="s">
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178" t="s">
         <v>610</v>
       </c>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="179"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="78">
@@ -10477,14 +10701,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="182"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -10495,16 +10719,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="183" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="182" t="s">
+      <c r="B3" s="184"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="183" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -10774,28 +10998,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="189" t="s">
         <v>739</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="189"/>
+      <c r="H1" s="189"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="186" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -11070,16 +11294,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="186" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="186"/>
-      <c r="C15" s="186"/>
-      <c r="D15" s="186"/>
-      <c r="E15" s="186"/>
-      <c r="F15" s="186"/>
-      <c r="G15" s="186"/>
-      <c r="H15" s="187"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="187"/>
+      <c r="E15" s="187"/>
+      <c r="F15" s="187"/>
+      <c r="G15" s="187"/>
+      <c r="H15" s="188"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -11369,16 +11593,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="186" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="186"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="186"/>
-      <c r="E28" s="186"/>
-      <c r="F28" s="186"/>
-      <c r="G28" s="186"/>
-      <c r="H28" s="187"/>
+      <c r="B28" s="187"/>
+      <c r="C28" s="187"/>
+      <c r="D28" s="187"/>
+      <c r="E28" s="187"/>
+      <c r="F28" s="187"/>
+      <c r="G28" s="187"/>
+      <c r="H28" s="188"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -11691,12 +11915,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="190" t="s">
         <v>714</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -11904,28 +12128,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="191" t="s">
         <v>754</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
+      <c r="F1" s="191"/>
+      <c r="G1" s="191"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="186" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -12216,12 +12440,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="186" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="186"/>
-      <c r="C15" s="186"/>
-      <c r="D15" s="187"/>
+      <c r="B15" s="187"/>
+      <c r="C15" s="187"/>
+      <c r="D15" s="188"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -12389,12 +12613,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="185" t="s">
+      <c r="A28" s="186" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="186"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="187"/>
+      <c r="B28" s="187"/>
+      <c r="C28" s="187"/>
+      <c r="D28" s="188"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -12598,40 +12822,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>835</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="182"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="191"/>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
-      <c r="H2" s="193"/>
+      <c r="A2" s="192"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="194"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="195" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="194" t="s">
+      <c r="B3" s="196"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="195" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="197"/>
+      <c r="F3" s="196"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="198"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="74">
@@ -13324,40 +13548,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="216" t="s">
         <v>833</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="199"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
+      <c r="A2" s="217"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="218" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="201"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="200" t="s">
+      <c r="B3" s="219"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="218" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="201"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="203"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="221"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -13886,36 +14110,36 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="200" t="s">
+      <c r="A25" s="218" t="s">
         <v>789</v>
       </c>
-      <c r="B25" s="201"/>
-      <c r="C25" s="202"/>
-      <c r="D25" s="203"/>
-      <c r="E25" s="200" t="s">
+      <c r="B25" s="219"/>
+      <c r="C25" s="220"/>
+      <c r="D25" s="221"/>
+      <c r="E25" s="218" t="s">
         <v>790</v>
       </c>
-      <c r="F25" s="201"/>
-      <c r="G25" s="202"/>
-      <c r="H25" s="203"/>
+      <c r="F25" s="219"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="221"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
         <v>791</v>
       </c>
-      <c r="B26" s="204" t="s">
+      <c r="B26" s="205" t="s">
         <v>792</v>
       </c>
-      <c r="C26" s="205"/>
-      <c r="D26" s="206"/>
+      <c r="C26" s="206"/>
+      <c r="D26" s="207"/>
       <c r="E26" s="125" t="s">
         <v>793</v>
       </c>
-      <c r="F26" s="207" t="s">
+      <c r="F26" s="213" t="s">
         <v>794</v>
       </c>
-      <c r="G26" s="208"/>
-      <c r="H26" s="209" t="s">
+      <c r="G26" s="214"/>
+      <c r="H26" s="215" t="s">
         <v>762</v>
       </c>
     </row>
@@ -13923,21 +14147,21 @@
       <c r="A27" s="137" t="s">
         <v>795</v>
       </c>
-      <c r="B27" s="210" t="s">
+      <c r="B27" s="208" t="s">
         <v>796</v>
       </c>
-      <c r="C27" s="211"/>
-      <c r="D27" s="212" t="s">
+      <c r="C27" s="209"/>
+      <c r="D27" s="211" t="s">
         <v>624</v>
       </c>
       <c r="E27" s="129" t="s">
         <v>797</v>
       </c>
-      <c r="F27" s="204" t="s">
+      <c r="F27" s="205" t="s">
         <v>798</v>
       </c>
-      <c r="G27" s="205"/>
-      <c r="H27" s="213" t="s">
+      <c r="G27" s="206"/>
+      <c r="H27" s="212" t="s">
         <v>764</v>
       </c>
     </row>
@@ -13945,21 +14169,21 @@
       <c r="A28" s="129" t="s">
         <v>799</v>
       </c>
-      <c r="B28" s="204" t="s">
+      <c r="B28" s="205" t="s">
         <v>800</v>
       </c>
-      <c r="C28" s="205"/>
-      <c r="D28" s="206" t="s">
+      <c r="C28" s="206"/>
+      <c r="D28" s="207" t="s">
         <v>625</v>
       </c>
       <c r="E28" s="137" t="s">
         <v>801</v>
       </c>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="208" t="s">
         <v>802</v>
       </c>
-      <c r="G28" s="211"/>
-      <c r="H28" s="214" t="s">
+      <c r="G28" s="209"/>
+      <c r="H28" s="210" t="s">
         <v>766</v>
       </c>
     </row>
@@ -13967,21 +14191,21 @@
       <c r="A29" s="137" t="s">
         <v>803</v>
       </c>
-      <c r="B29" s="210" t="s">
+      <c r="B29" s="208" t="s">
         <v>804</v>
       </c>
-      <c r="C29" s="211"/>
-      <c r="D29" s="212" t="s">
+      <c r="C29" s="209"/>
+      <c r="D29" s="211" t="s">
         <v>626</v>
       </c>
       <c r="E29" s="129" t="s">
         <v>805</v>
       </c>
-      <c r="F29" s="204" t="s">
+      <c r="F29" s="205" t="s">
         <v>806</v>
       </c>
-      <c r="G29" s="205"/>
-      <c r="H29" s="213" t="s">
+      <c r="G29" s="206"/>
+      <c r="H29" s="212" t="s">
         <v>768</v>
       </c>
     </row>
@@ -13989,21 +14213,21 @@
       <c r="A30" s="129" t="s">
         <v>807</v>
       </c>
-      <c r="B30" s="204" t="s">
+      <c r="B30" s="205" t="s">
         <v>808</v>
       </c>
-      <c r="C30" s="205"/>
-      <c r="D30" s="206" t="s">
+      <c r="C30" s="206"/>
+      <c r="D30" s="207" t="s">
         <v>627</v>
       </c>
       <c r="E30" s="137" t="s">
         <v>809</v>
       </c>
-      <c r="F30" s="210" t="s">
+      <c r="F30" s="208" t="s">
         <v>810</v>
       </c>
-      <c r="G30" s="211"/>
-      <c r="H30" s="214" t="s">
+      <c r="G30" s="209"/>
+      <c r="H30" s="210" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14011,21 +14235,21 @@
       <c r="A31" s="137" t="s">
         <v>811</v>
       </c>
-      <c r="B31" s="210" t="s">
+      <c r="B31" s="208" t="s">
         <v>812</v>
       </c>
-      <c r="C31" s="211"/>
-      <c r="D31" s="212" t="s">
+      <c r="C31" s="209"/>
+      <c r="D31" s="211" t="s">
         <v>628</v>
       </c>
       <c r="E31" s="129" t="s">
         <v>813</v>
       </c>
-      <c r="F31" s="204" t="s">
+      <c r="F31" s="205" t="s">
         <v>814</v>
       </c>
-      <c r="G31" s="205"/>
-      <c r="H31" s="213" t="s">
+      <c r="G31" s="206"/>
+      <c r="H31" s="212" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14033,17 +14257,17 @@
       <c r="A32" s="129" t="s">
         <v>815</v>
       </c>
-      <c r="B32" s="204" t="s">
+      <c r="B32" s="205" t="s">
         <v>816</v>
       </c>
-      <c r="C32" s="205"/>
-      <c r="D32" s="206" t="s">
+      <c r="C32" s="206"/>
+      <c r="D32" s="207" t="s">
         <v>629</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="210"/>
-      <c r="G32" s="211"/>
-      <c r="H32" s="214" t="s">
+      <c r="F32" s="208"/>
+      <c r="G32" s="209"/>
+      <c r="H32" s="210" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14051,17 +14275,17 @@
       <c r="A33" s="137" t="s">
         <v>817</v>
       </c>
-      <c r="B33" s="210" t="s">
+      <c r="B33" s="208" t="s">
         <v>818</v>
       </c>
-      <c r="C33" s="211"/>
-      <c r="D33" s="212" t="s">
+      <c r="C33" s="209"/>
+      <c r="D33" s="211" t="s">
         <v>623</v>
       </c>
       <c r="E33" s="129"/>
-      <c r="F33" s="204"/>
-      <c r="G33" s="205"/>
-      <c r="H33" s="213" t="s">
+      <c r="F33" s="205"/>
+      <c r="G33" s="206"/>
+      <c r="H33" s="212" t="s">
         <v>762</v>
       </c>
     </row>
@@ -14069,17 +14293,17 @@
       <c r="A34" s="129" t="s">
         <v>819</v>
       </c>
-      <c r="B34" s="204" t="s">
+      <c r="B34" s="205" t="s">
         <v>820</v>
       </c>
-      <c r="C34" s="205"/>
-      <c r="D34" s="206" t="s">
+      <c r="C34" s="206"/>
+      <c r="D34" s="207" t="s">
         <v>624</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="210"/>
-      <c r="G34" s="211"/>
-      <c r="H34" s="214" t="s">
+      <c r="F34" s="208"/>
+      <c r="G34" s="209"/>
+      <c r="H34" s="210" t="s">
         <v>764</v>
       </c>
     </row>
@@ -14087,17 +14311,17 @@
       <c r="A35" s="137" t="s">
         <v>821</v>
       </c>
-      <c r="B35" s="210" t="s">
+      <c r="B35" s="208" t="s">
         <v>822</v>
       </c>
-      <c r="C35" s="211"/>
-      <c r="D35" s="212" t="s">
+      <c r="C35" s="209"/>
+      <c r="D35" s="211" t="s">
         <v>625</v>
       </c>
       <c r="E35" s="129"/>
-      <c r="F35" s="204"/>
-      <c r="G35" s="205"/>
-      <c r="H35" s="213" t="s">
+      <c r="F35" s="205"/>
+      <c r="G35" s="206"/>
+      <c r="H35" s="212" t="s">
         <v>766</v>
       </c>
     </row>
@@ -14105,17 +14329,17 @@
       <c r="A36" s="129" t="s">
         <v>823</v>
       </c>
-      <c r="B36" s="204" t="s">
+      <c r="B36" s="205" t="s">
         <v>824</v>
       </c>
-      <c r="C36" s="205"/>
-      <c r="D36" s="206" t="s">
+      <c r="C36" s="206"/>
+      <c r="D36" s="207" t="s">
         <v>626</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="210"/>
-      <c r="G36" s="211"/>
-      <c r="H36" s="214" t="s">
+      <c r="F36" s="208"/>
+      <c r="G36" s="209"/>
+      <c r="H36" s="210" t="s">
         <v>768</v>
       </c>
     </row>
@@ -14123,17 +14347,17 @@
       <c r="A37" s="137" t="s">
         <v>825</v>
       </c>
-      <c r="B37" s="210" t="s">
+      <c r="B37" s="208" t="s">
         <v>826</v>
       </c>
-      <c r="C37" s="211"/>
-      <c r="D37" s="212" t="s">
+      <c r="C37" s="209"/>
+      <c r="D37" s="211" t="s">
         <v>627</v>
       </c>
       <c r="E37" s="129"/>
-      <c r="F37" s="204"/>
-      <c r="G37" s="205"/>
-      <c r="H37" s="213" t="s">
+      <c r="F37" s="205"/>
+      <c r="G37" s="206"/>
+      <c r="H37" s="212" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14141,17 +14365,17 @@
       <c r="A38" s="129" t="s">
         <v>827</v>
       </c>
-      <c r="B38" s="204" t="s">
+      <c r="B38" s="205" t="s">
         <v>828</v>
       </c>
-      <c r="C38" s="205"/>
-      <c r="D38" s="206" t="s">
+      <c r="C38" s="206"/>
+      <c r="D38" s="207" t="s">
         <v>628</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="210"/>
-      <c r="G38" s="211"/>
-      <c r="H38" s="214" t="s">
+      <c r="F38" s="208"/>
+      <c r="G38" s="209"/>
+      <c r="H38" s="210" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14159,17 +14383,17 @@
       <c r="A39" s="137" t="s">
         <v>829</v>
       </c>
-      <c r="B39" s="210" t="s">
+      <c r="B39" s="208" t="s">
         <v>830</v>
       </c>
-      <c r="C39" s="211"/>
-      <c r="D39" s="212" t="s">
+      <c r="C39" s="209"/>
+      <c r="D39" s="211" t="s">
         <v>629</v>
       </c>
       <c r="E39" s="129"/>
-      <c r="F39" s="204"/>
-      <c r="G39" s="205"/>
-      <c r="H39" s="213" t="s">
+      <c r="F39" s="205"/>
+      <c r="G39" s="206"/>
+      <c r="H39" s="212" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14177,36 +14401,65 @@
       <c r="A40" s="129" t="s">
         <v>831</v>
       </c>
-      <c r="B40" s="204" t="s">
+      <c r="B40" s="205" t="s">
         <v>830</v>
       </c>
-      <c r="C40" s="205"/>
-      <c r="D40" s="206" t="s">
+      <c r="C40" s="206"/>
+      <c r="D40" s="207" t="s">
         <v>629</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="210"/>
-      <c r="G40" s="211"/>
-      <c r="H40" s="214"/>
+      <c r="F40" s="208"/>
+      <c r="G40" s="209"/>
+      <c r="H40" s="210"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>832</v>
       </c>
-      <c r="B41" s="215" t="s">
+      <c r="B41" s="199" t="s">
         <v>830</v>
       </c>
-      <c r="C41" s="216"/>
-      <c r="D41" s="217" t="s">
+      <c r="C41" s="200"/>
+      <c r="D41" s="201" t="s">
         <v>629</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="218"/>
-      <c r="G41" s="219"/>
-      <c r="H41" s="220"/>
+      <c r="F41" s="202"/>
+      <c r="G41" s="203"/>
+      <c r="H41" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -14215,35 +14468,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Updated Airspace Control Plan
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="857">
   <si>
     <t>AWACS</t>
   </si>
@@ -2624,6 +2624,15 @@
   </si>
   <si>
     <t>118.75</t>
+  </si>
+  <si>
+    <t>FARP LONDON</t>
+  </si>
+  <si>
+    <t>AEW502</t>
+  </si>
+  <si>
+    <t>AEW501</t>
   </si>
 </sst>
 </file>
@@ -4640,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49:F49"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5337,7 +5346,9 @@
       <c r="Z12" s="38">
         <v>502</v>
       </c>
-      <c r="AA12" s="95"/>
+      <c r="AA12" s="95" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="13" spans="2:32" ht="16.5" thickBot="1">
       <c r="B13" s="57" t="s">
@@ -5402,7 +5413,9 @@
       <c r="Z13" s="38">
         <v>501</v>
       </c>
-      <c r="AA13" s="41"/>
+      <c r="AA13" s="41" t="s">
+        <v>856</v>
+      </c>
       <c r="AD13" s="161" t="s">
         <v>631</v>
       </c>
@@ -8265,12 +8278,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8871,6 +8885,21 @@
       <c r="K14" s="7" t="s">
         <v>646</v>
       </c>
+      <c r="M14" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="N14" s="7">
+        <v>4</v>
+      </c>
+      <c r="O14" s="7">
+        <v>241</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="7"/>
@@ -8895,6 +8924,17 @@
       <c r="K15" s="7" t="s">
         <v>646</v>
       </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7">
+        <v>242</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="7"/>
@@ -8919,8 +8959,19 @@
       <c r="K16" s="7" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7">
+        <v>243</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7">
@@ -8943,8 +8994,19 @@
       <c r="K17" s="7" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7">
+        <v>244</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="7" t="s">
         <v>841</v>
       </c>
@@ -8976,7 +9038,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:17">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7">
@@ -9000,7 +9062,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:17">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7">
@@ -9024,7 +9086,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:17">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7">
@@ -9048,7 +9110,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:17">
       <c r="G22" s="7" t="s">
         <v>740</v>
       </c>
@@ -9065,7 +9127,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:17">
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7">
@@ -9078,7 +9140,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:17">
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7">
@@ -9091,7 +9153,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:17">
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7">
@@ -9104,7 +9166,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:17">
       <c r="G26" s="7" t="s">
         <v>740</v>
       </c>
@@ -9121,7 +9183,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:17">
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7">
@@ -9134,7 +9196,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:17">
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7">
@@ -9147,7 +9209,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:17">
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7">
@@ -9160,7 +9222,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:17">
       <c r="G30" s="7" t="s">
         <v>740</v>
       </c>
@@ -9177,7 +9239,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:17">
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7">
@@ -9190,7 +9252,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:17">
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7">

</xml_diff>

<commit_message>
Chg: Updates for MSN 6
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="859">
   <si>
     <t>AWACS</t>
   </si>
@@ -2633,6 +2633,12 @@
   </si>
   <si>
     <t>AEW501</t>
+  </si>
+  <si>
+    <t>DALLAS</t>
+  </si>
+  <si>
+    <t>ORANGE 11</t>
   </si>
 </sst>
 </file>
@@ -3917,21 +3923,36 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3941,21 +3962,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4040,6 +4046,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4057,57 +4114,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4163,7 +4169,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4649,8 +4655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AI52"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4701,18 +4707,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="167" t="s">
+      <c r="R3" s="159" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="167"/>
-      <c r="T3" s="167"/>
-      <c r="AA3" s="168" t="s">
+      <c r="S3" s="159"/>
+      <c r="T3" s="159"/>
+      <c r="AA3" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="169"/>
-      <c r="AC3" s="169"/>
-      <c r="AD3" s="169"/>
-      <c r="AE3" s="170"/>
+      <c r="AB3" s="162"/>
+      <c r="AC3" s="162"/>
+      <c r="AD3" s="162"/>
+      <c r="AE3" s="163"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4755,7 +4761,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="160" t="s">
+      <c r="R4" s="164" t="s">
         <v>639</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -4764,12 +4770,12 @@
       <c r="T4" s="99" t="s">
         <v>642</v>
       </c>
-      <c r="V4" s="158" t="s">
+      <c r="V4" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="158"/>
-      <c r="X4" s="158"/>
-      <c r="Y4" s="158"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="161"/>
+      <c r="R5" s="165"/>
       <c r="S5" s="31" t="s">
         <v>608</v>
       </c>
@@ -4901,7 +4907,7 @@
         <v>657</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="162"/>
+      <c r="R6" s="166"/>
       <c r="S6" s="100" t="s">
         <v>641</v>
       </c>
@@ -4977,7 +4983,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="160" t="s">
+      <c r="R7" s="164" t="s">
         <v>645</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5046,7 +5052,7 @@
       <c r="L8" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="9" t="s">
         <v>69</v>
       </c>
       <c r="N8" s="58" t="s">
@@ -5057,7 +5063,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="161"/>
+      <c r="R8" s="165"/>
       <c r="S8" s="31" t="s">
         <v>608</v>
       </c>
@@ -5126,7 +5132,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="162"/>
+      <c r="R9" s="166"/>
       <c r="S9" s="100" t="s">
         <v>641</v>
       </c>
@@ -5253,7 +5259,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="163" t="s">
+      <c r="R11" s="168" t="s">
         <v>646</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5326,7 +5332,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="164"/>
+      <c r="R12" s="169"/>
       <c r="S12" s="97" t="s">
         <v>608</v>
       </c>
@@ -5393,7 +5399,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="165"/>
+      <c r="R13" s="170"/>
       <c r="S13" s="105" t="s">
         <v>641</v>
       </c>
@@ -5416,11 +5422,11 @@
       <c r="AA13" s="41" t="s">
         <v>856</v>
       </c>
-      <c r="AD13" s="168" t="s">
+      <c r="AD13" s="161" t="s">
         <v>631</v>
       </c>
-      <c r="AE13" s="169"/>
-      <c r="AF13" s="170"/>
+      <c r="AE13" s="162"/>
+      <c r="AF13" s="163"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5467,7 +5473,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="160" t="s">
+      <c r="R14" s="164" t="s">
         <v>649</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5545,7 +5551,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="161"/>
+      <c r="R15" s="165"/>
       <c r="S15" s="97" t="s">
         <v>608</v>
       </c>
@@ -5606,22 +5612,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="162"/>
+      <c r="R16" s="166"/>
       <c r="S16" s="105" t="s">
         <v>641</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>652</v>
       </c>
-      <c r="V16" s="158" t="s">
+      <c r="V16" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="158"/>
-      <c r="X16" s="158"/>
-      <c r="Y16" s="158"/>
-      <c r="Z16" s="158"/>
-      <c r="AA16" s="158"/>
-      <c r="AB16" s="158"/>
+      <c r="W16" s="160"/>
+      <c r="X16" s="160"/>
+      <c r="Y16" s="160"/>
+      <c r="Z16" s="160"/>
+      <c r="AA16" s="160"/>
+      <c r="AB16" s="160"/>
       <c r="AD16" s="7" t="s">
         <v>624</v>
       </c>
@@ -5913,11 +5919,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="158" t="s">
+      <c r="R20" s="160" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="158"/>
-      <c r="T20" s="158"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>673</v>
@@ -6088,15 +6094,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="168" t="s">
+      <c r="V22" s="161" t="s">
         <v>664</v>
       </c>
-      <c r="W22" s="169"/>
-      <c r="X22" s="169"/>
-      <c r="Y22" s="169"/>
-      <c r="Z22" s="169"/>
-      <c r="AA22" s="169"/>
-      <c r="AB22" s="170"/>
+      <c r="W22" s="162"/>
+      <c r="X22" s="162"/>
+      <c r="Y22" s="162"/>
+      <c r="Z22" s="162"/>
+      <c r="AA22" s="162"/>
+      <c r="AB22" s="163"/>
       <c r="AD22" s="7" t="s">
         <v>630</v>
       </c>
@@ -6234,6 +6240,15 @@
       <c r="O24" s="157"/>
       <c r="P24" s="3" t="s">
         <v>437</v>
+      </c>
+      <c r="R24" t="s">
+        <v>857</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="T24" t="s">
+        <v>858</v>
       </c>
       <c r="V24" s="39" t="s">
         <v>675</v>
@@ -6556,33 +6571,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="158" t="s">
+      <c r="B31" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="158"/>
-      <c r="D31" s="158"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="J31" s="158" t="s">
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="J31" s="160" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="158"/>
-      <c r="L31" s="158"/>
-      <c r="M31" s="158"/>
-      <c r="N31" s="158"/>
-      <c r="O31" s="158"/>
-      <c r="P31" s="158"/>
-      <c r="T31" s="158" t="s">
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+      <c r="T31" s="160" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="158"/>
-      <c r="V31" s="158"/>
-      <c r="W31" s="158"/>
-      <c r="X31" s="158"/>
-      <c r="Y31" s="158"/>
-      <c r="Z31" s="158"/>
+      <c r="U31" s="160"/>
+      <c r="V31" s="160"/>
+      <c r="W31" s="160"/>
+      <c r="X31" s="160"/>
+      <c r="Y31" s="160"/>
+      <c r="Z31" s="160"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6861,7 +6876,7 @@
       <c r="Z35" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD35" s="166" t="s">
+      <c r="AD35" s="158" t="s">
         <v>701</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6944,7 +6959,7 @@
       <c r="Z36" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD36" s="166"/>
+      <c r="AD36" s="158"/>
       <c r="AE36" s="7" t="s">
         <v>511</v>
       </c>
@@ -7017,7 +7032,7 @@
       <c r="Z37" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="AD37" s="166"/>
+      <c r="AD37" s="158"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7073,7 +7088,7 @@
       <c r="Z38" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="AD38" s="166"/>
+      <c r="AD38" s="158"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7087,15 +7102,15 @@
       <c r="F39" t="s">
         <v>568</v>
       </c>
-      <c r="J39" s="159" t="s">
+      <c r="J39" s="167" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="159"/>
-      <c r="L39" s="159"/>
-      <c r="M39" s="159"/>
-      <c r="N39" s="159"/>
-      <c r="O39" s="159"/>
-      <c r="P39" s="159"/>
+      <c r="K39" s="167"/>
+      <c r="L39" s="167"/>
+      <c r="M39" s="167"/>
+      <c r="N39" s="167"/>
+      <c r="O39" s="167"/>
+      <c r="P39" s="167"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7424,6 +7439,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7433,13 +7455,6 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8278,7 +8293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -13714,40 +13729,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="216" t="s">
         <v>833</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="200"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
+      <c r="A2" s="217"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="201" t="s">
+      <c r="A3" s="218" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="201" t="s">
+      <c r="B3" s="219"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="218" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="202"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="204"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="221"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -14276,18 +14291,18 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="218" t="s">
         <v>789</v>
       </c>
-      <c r="B25" s="202"/>
-      <c r="C25" s="203"/>
-      <c r="D25" s="204"/>
-      <c r="E25" s="201" t="s">
+      <c r="B25" s="219"/>
+      <c r="C25" s="220"/>
+      <c r="D25" s="221"/>
+      <c r="E25" s="218" t="s">
         <v>790</v>
       </c>
-      <c r="F25" s="202"/>
-      <c r="G25" s="203"/>
-      <c r="H25" s="204"/>
+      <c r="F25" s="219"/>
+      <c r="G25" s="220"/>
+      <c r="H25" s="221"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
@@ -14301,11 +14316,11 @@
       <c r="E26" s="125" t="s">
         <v>793</v>
       </c>
-      <c r="F26" s="208" t="s">
+      <c r="F26" s="213" t="s">
         <v>794</v>
       </c>
-      <c r="G26" s="209"/>
-      <c r="H26" s="210" t="s">
+      <c r="G26" s="214"/>
+      <c r="H26" s="215" t="s">
         <v>762</v>
       </c>
     </row>
@@ -14313,11 +14328,11 @@
       <c r="A27" s="137" t="s">
         <v>795</v>
       </c>
-      <c r="B27" s="211" t="s">
+      <c r="B27" s="208" t="s">
         <v>796</v>
       </c>
-      <c r="C27" s="212"/>
-      <c r="D27" s="213" t="s">
+      <c r="C27" s="209"/>
+      <c r="D27" s="211" t="s">
         <v>624</v>
       </c>
       <c r="E27" s="129" t="s">
@@ -14327,7 +14342,7 @@
         <v>798</v>
       </c>
       <c r="G27" s="206"/>
-      <c r="H27" s="214" t="s">
+      <c r="H27" s="212" t="s">
         <v>764</v>
       </c>
     </row>
@@ -14345,11 +14360,11 @@
       <c r="E28" s="137" t="s">
         <v>801</v>
       </c>
-      <c r="F28" s="211" t="s">
+      <c r="F28" s="208" t="s">
         <v>802</v>
       </c>
-      <c r="G28" s="212"/>
-      <c r="H28" s="215" t="s">
+      <c r="G28" s="209"/>
+      <c r="H28" s="210" t="s">
         <v>766</v>
       </c>
     </row>
@@ -14357,11 +14372,11 @@
       <c r="A29" s="137" t="s">
         <v>803</v>
       </c>
-      <c r="B29" s="211" t="s">
+      <c r="B29" s="208" t="s">
         <v>804</v>
       </c>
-      <c r="C29" s="212"/>
-      <c r="D29" s="213" t="s">
+      <c r="C29" s="209"/>
+      <c r="D29" s="211" t="s">
         <v>626</v>
       </c>
       <c r="E29" s="129" t="s">
@@ -14371,7 +14386,7 @@
         <v>806</v>
       </c>
       <c r="G29" s="206"/>
-      <c r="H29" s="214" t="s">
+      <c r="H29" s="212" t="s">
         <v>768</v>
       </c>
     </row>
@@ -14389,11 +14404,11 @@
       <c r="E30" s="137" t="s">
         <v>809</v>
       </c>
-      <c r="F30" s="211" t="s">
+      <c r="F30" s="208" t="s">
         <v>810</v>
       </c>
-      <c r="G30" s="212"/>
-      <c r="H30" s="215" t="s">
+      <c r="G30" s="209"/>
+      <c r="H30" s="210" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14401,11 +14416,11 @@
       <c r="A31" s="137" t="s">
         <v>811</v>
       </c>
-      <c r="B31" s="211" t="s">
+      <c r="B31" s="208" t="s">
         <v>812</v>
       </c>
-      <c r="C31" s="212"/>
-      <c r="D31" s="213" t="s">
+      <c r="C31" s="209"/>
+      <c r="D31" s="211" t="s">
         <v>628</v>
       </c>
       <c r="E31" s="129" t="s">
@@ -14415,7 +14430,7 @@
         <v>814</v>
       </c>
       <c r="G31" s="206"/>
-      <c r="H31" s="214" t="s">
+      <c r="H31" s="212" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14431,9 +14446,9 @@
         <v>629</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="211"/>
-      <c r="G32" s="212"/>
-      <c r="H32" s="215" t="s">
+      <c r="F32" s="208"/>
+      <c r="G32" s="209"/>
+      <c r="H32" s="210" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14441,17 +14456,17 @@
       <c r="A33" s="137" t="s">
         <v>817</v>
       </c>
-      <c r="B33" s="211" t="s">
+      <c r="B33" s="208" t="s">
         <v>818</v>
       </c>
-      <c r="C33" s="212"/>
-      <c r="D33" s="213" t="s">
+      <c r="C33" s="209"/>
+      <c r="D33" s="211" t="s">
         <v>623</v>
       </c>
       <c r="E33" s="129"/>
       <c r="F33" s="205"/>
       <c r="G33" s="206"/>
-      <c r="H33" s="214" t="s">
+      <c r="H33" s="212" t="s">
         <v>762</v>
       </c>
     </row>
@@ -14467,9 +14482,9 @@
         <v>624</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="211"/>
-      <c r="G34" s="212"/>
-      <c r="H34" s="215" t="s">
+      <c r="F34" s="208"/>
+      <c r="G34" s="209"/>
+      <c r="H34" s="210" t="s">
         <v>764</v>
       </c>
     </row>
@@ -14477,17 +14492,17 @@
       <c r="A35" s="137" t="s">
         <v>821</v>
       </c>
-      <c r="B35" s="211" t="s">
+      <c r="B35" s="208" t="s">
         <v>822</v>
       </c>
-      <c r="C35" s="212"/>
-      <c r="D35" s="213" t="s">
+      <c r="C35" s="209"/>
+      <c r="D35" s="211" t="s">
         <v>625</v>
       </c>
       <c r="E35" s="129"/>
       <c r="F35" s="205"/>
       <c r="G35" s="206"/>
-      <c r="H35" s="214" t="s">
+      <c r="H35" s="212" t="s">
         <v>766</v>
       </c>
     </row>
@@ -14503,9 +14518,9 @@
         <v>626</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="211"/>
-      <c r="G36" s="212"/>
-      <c r="H36" s="215" t="s">
+      <c r="F36" s="208"/>
+      <c r="G36" s="209"/>
+      <c r="H36" s="210" t="s">
         <v>768</v>
       </c>
     </row>
@@ -14513,17 +14528,17 @@
       <c r="A37" s="137" t="s">
         <v>825</v>
       </c>
-      <c r="B37" s="211" t="s">
+      <c r="B37" s="208" t="s">
         <v>826</v>
       </c>
-      <c r="C37" s="212"/>
-      <c r="D37" s="213" t="s">
+      <c r="C37" s="209"/>
+      <c r="D37" s="211" t="s">
         <v>627</v>
       </c>
       <c r="E37" s="129"/>
       <c r="F37" s="205"/>
       <c r="G37" s="206"/>
-      <c r="H37" s="214" t="s">
+      <c r="H37" s="212" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14539,9 +14554,9 @@
         <v>628</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="211"/>
-      <c r="G38" s="212"/>
-      <c r="H38" s="215" t="s">
+      <c r="F38" s="208"/>
+      <c r="G38" s="209"/>
+      <c r="H38" s="210" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14549,17 +14564,17 @@
       <c r="A39" s="137" t="s">
         <v>829</v>
       </c>
-      <c r="B39" s="211" t="s">
+      <c r="B39" s="208" t="s">
         <v>830</v>
       </c>
-      <c r="C39" s="212"/>
-      <c r="D39" s="213" t="s">
+      <c r="C39" s="209"/>
+      <c r="D39" s="211" t="s">
         <v>629</v>
       </c>
       <c r="E39" s="129"/>
       <c r="F39" s="205"/>
       <c r="G39" s="206"/>
-      <c r="H39" s="214" t="s">
+      <c r="H39" s="212" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14575,28 +14590,57 @@
         <v>629</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="211"/>
-      <c r="G40" s="212"/>
-      <c r="H40" s="215"/>
+      <c r="F40" s="208"/>
+      <c r="G40" s="209"/>
+      <c r="H40" s="210"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>832</v>
       </c>
-      <c r="B41" s="216" t="s">
+      <c r="B41" s="199" t="s">
         <v>830</v>
       </c>
-      <c r="C41" s="217"/>
-      <c r="D41" s="218" t="s">
+      <c r="C41" s="200"/>
+      <c r="D41" s="201" t="s">
         <v>629</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="219"/>
-      <c r="G41" s="220"/>
-      <c r="H41" s="221"/>
+      <c r="F41" s="202"/>
+      <c r="G41" s="203"/>
+      <c r="H41" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -14605,35 +14649,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: WIP D&G D+12, WIP VID INTREP D+11
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="861">
   <si>
     <t>AWACS</t>
   </si>
@@ -2639,6 +2639,12 @@
   </si>
   <si>
     <t>ORANGE 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLT </t>
+  </si>
+  <si>
+    <t>CVN-73</t>
   </si>
 </sst>
 </file>
@@ -3572,7 +3578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3923,15 +3929,36 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3941,27 +3968,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4046,6 +4052,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4064,57 +4121,6 @@
     <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4127,6 +4133,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4169,7 +4176,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4655,7 +4662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AI52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
@@ -4707,18 +4714,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="159" t="s">
+      <c r="R3" s="167" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="159"/>
-      <c r="T3" s="159"/>
-      <c r="AA3" s="161" t="s">
+      <c r="S3" s="167"/>
+      <c r="T3" s="167"/>
+      <c r="AA3" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="162"/>
-      <c r="AC3" s="162"/>
-      <c r="AD3" s="162"/>
-      <c r="AE3" s="163"/>
+      <c r="AB3" s="169"/>
+      <c r="AC3" s="169"/>
+      <c r="AD3" s="169"/>
+      <c r="AE3" s="170"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4761,7 +4768,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="164" t="s">
+      <c r="R4" s="160" t="s">
         <v>639</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -4770,12 +4777,12 @@
       <c r="T4" s="99" t="s">
         <v>642</v>
       </c>
-      <c r="V4" s="160" t="s">
+      <c r="V4" s="158" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="160"/>
+      <c r="W4" s="158"/>
+      <c r="X4" s="158"/>
+      <c r="Y4" s="158"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -4829,7 +4836,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="165"/>
+      <c r="R5" s="161"/>
       <c r="S5" s="31" t="s">
         <v>608</v>
       </c>
@@ -4907,7 +4914,7 @@
         <v>657</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="166"/>
+      <c r="R6" s="162"/>
       <c r="S6" s="100" t="s">
         <v>641</v>
       </c>
@@ -4983,7 +4990,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="164" t="s">
+      <c r="R7" s="160" t="s">
         <v>645</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5063,7 +5070,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="165"/>
+      <c r="R8" s="161"/>
       <c r="S8" s="31" t="s">
         <v>608</v>
       </c>
@@ -5132,7 +5139,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="166"/>
+      <c r="R9" s="162"/>
       <c r="S9" s="100" t="s">
         <v>641</v>
       </c>
@@ -5259,7 +5266,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="168" t="s">
+      <c r="R11" s="163" t="s">
         <v>646</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5332,7 +5339,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="169"/>
+      <c r="R12" s="164"/>
       <c r="S12" s="97" t="s">
         <v>608</v>
       </c>
@@ -5399,7 +5406,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="170"/>
+      <c r="R13" s="165"/>
       <c r="S13" s="105" t="s">
         <v>641</v>
       </c>
@@ -5422,11 +5429,11 @@
       <c r="AA13" s="41" t="s">
         <v>856</v>
       </c>
-      <c r="AD13" s="161" t="s">
+      <c r="AD13" s="168" t="s">
         <v>631</v>
       </c>
-      <c r="AE13" s="162"/>
-      <c r="AF13" s="163"/>
+      <c r="AE13" s="169"/>
+      <c r="AF13" s="170"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5473,7 +5480,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="164" t="s">
+      <c r="R14" s="160" t="s">
         <v>649</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5551,7 +5558,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="165"/>
+      <c r="R15" s="161"/>
       <c r="S15" s="97" t="s">
         <v>608</v>
       </c>
@@ -5612,22 +5619,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="166"/>
+      <c r="R16" s="162"/>
       <c r="S16" s="105" t="s">
         <v>641</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>652</v>
       </c>
-      <c r="V16" s="160" t="s">
+      <c r="V16" s="158" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="160"/>
-      <c r="X16" s="160"/>
-      <c r="Y16" s="160"/>
-      <c r="Z16" s="160"/>
-      <c r="AA16" s="160"/>
-      <c r="AB16" s="160"/>
+      <c r="W16" s="158"/>
+      <c r="X16" s="158"/>
+      <c r="Y16" s="158"/>
+      <c r="Z16" s="158"/>
+      <c r="AA16" s="158"/>
+      <c r="AB16" s="158"/>
       <c r="AD16" s="7" t="s">
         <v>624</v>
       </c>
@@ -5919,11 +5926,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="160" t="s">
+      <c r="R20" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="160"/>
-      <c r="T20" s="160"/>
+      <c r="S20" s="158"/>
+      <c r="T20" s="158"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>673</v>
@@ -6094,15 +6101,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="161" t="s">
+      <c r="V22" s="168" t="s">
         <v>664</v>
       </c>
-      <c r="W22" s="162"/>
-      <c r="X22" s="162"/>
-      <c r="Y22" s="162"/>
-      <c r="Z22" s="162"/>
-      <c r="AA22" s="162"/>
-      <c r="AB22" s="163"/>
+      <c r="W22" s="169"/>
+      <c r="X22" s="169"/>
+      <c r="Y22" s="169"/>
+      <c r="Z22" s="169"/>
+      <c r="AA22" s="169"/>
+      <c r="AB22" s="170"/>
       <c r="AD22" s="7" t="s">
         <v>630</v>
       </c>
@@ -6571,33 +6578,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="160" t="s">
+      <c r="B31" s="158" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="160"/>
-      <c r="D31" s="160"/>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
-      <c r="G31" s="160"/>
-      <c r="H31" s="160"/>
-      <c r="J31" s="160" t="s">
+      <c r="C31" s="158"/>
+      <c r="D31" s="158"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="158"/>
+      <c r="H31" s="158"/>
+      <c r="J31" s="158" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="160"/>
-      <c r="L31" s="160"/>
-      <c r="M31" s="160"/>
-      <c r="N31" s="160"/>
-      <c r="O31" s="160"/>
-      <c r="P31" s="160"/>
-      <c r="T31" s="160" t="s">
+      <c r="K31" s="158"/>
+      <c r="L31" s="158"/>
+      <c r="M31" s="158"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="158"/>
+      <c r="T31" s="158" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="160"/>
-      <c r="V31" s="160"/>
-      <c r="W31" s="160"/>
-      <c r="X31" s="160"/>
-      <c r="Y31" s="160"/>
-      <c r="Z31" s="160"/>
+      <c r="U31" s="158"/>
+      <c r="V31" s="158"/>
+      <c r="W31" s="158"/>
+      <c r="X31" s="158"/>
+      <c r="Y31" s="158"/>
+      <c r="Z31" s="158"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6876,7 +6883,7 @@
       <c r="Z35" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD35" s="158" t="s">
+      <c r="AD35" s="166" t="s">
         <v>701</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6959,7 +6966,7 @@
       <c r="Z36" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD36" s="158"/>
+      <c r="AD36" s="166"/>
       <c r="AE36" s="7" t="s">
         <v>511</v>
       </c>
@@ -7032,7 +7039,7 @@
       <c r="Z37" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="AD37" s="158"/>
+      <c r="AD37" s="166"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7088,7 +7095,7 @@
       <c r="Z38" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="AD38" s="158"/>
+      <c r="AD38" s="166"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7102,15 +7109,15 @@
       <c r="F39" t="s">
         <v>568</v>
       </c>
-      <c r="J39" s="167" t="s">
+      <c r="J39" s="159" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="167"/>
-      <c r="L39" s="167"/>
-      <c r="M39" s="167"/>
-      <c r="N39" s="167"/>
-      <c r="O39" s="167"/>
-      <c r="P39" s="167"/>
+      <c r="K39" s="159"/>
+      <c r="L39" s="159"/>
+      <c r="M39" s="159"/>
+      <c r="N39" s="159"/>
+      <c r="O39" s="159"/>
+      <c r="P39" s="159"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7439,13 +7446,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7455,6 +7455,13 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8291,10 +8298,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9693,7 +9700,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:11">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7">
@@ -9706,7 +9713,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:11">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7">
@@ -9718,8 +9725,23 @@
       <c r="E50" s="7" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" t="s">
+        <v>859</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>631</v>
+      </c>
+      <c r="J50" t="s">
+        <v>602</v>
+      </c>
+      <c r="K50" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7">
@@ -9731,8 +9753,20 @@
       <c r="E51" s="7" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="G51" t="s">
+        <v>859</v>
+      </c>
+      <c r="I51">
+        <v>632</v>
+      </c>
+      <c r="J51" t="s">
+        <v>602</v>
+      </c>
+      <c r="K51" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="7" t="s">
         <v>757</v>
       </c>
@@ -9748,8 +9782,20 @@
       <c r="E52" s="7" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="G52" t="s">
+        <v>859</v>
+      </c>
+      <c r="I52">
+        <v>633</v>
+      </c>
+      <c r="J52" t="s">
+        <v>602</v>
+      </c>
+      <c r="K52" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7">
@@ -9761,8 +9807,20 @@
       <c r="E53" s="7" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="G53" t="s">
+        <v>859</v>
+      </c>
+      <c r="I53">
+        <v>634</v>
+      </c>
+      <c r="J53" t="s">
+        <v>602</v>
+      </c>
+      <c r="K53" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7">
@@ -9775,7 +9833,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:11">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7">
@@ -9786,6 +9844,67 @@
       </c>
       <c r="E55" s="7" t="s">
         <v>759</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="C56" s="226"/>
+      <c r="D56" s="226"/>
+      <c r="E56" s="226"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>757</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" s="226">
+        <v>351</v>
+      </c>
+      <c r="D57" s="226" t="s">
+        <v>758</v>
+      </c>
+      <c r="E57" s="226" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" t="s">
+        <v>757</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+      <c r="C61" s="226">
+        <v>361</v>
+      </c>
+      <c r="D61" s="226" t="s">
+        <v>758</v>
+      </c>
+      <c r="E61" s="226" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>757</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65" s="226">
+        <v>351</v>
+      </c>
+      <c r="D65" s="226" t="s">
+        <v>758</v>
+      </c>
+      <c r="E65" s="226" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="C66">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -13729,40 +13848,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="199" t="s">
         <v>833</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="217"/>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
+      <c r="A2" s="200"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="201" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="221"/>
-      <c r="E3" s="218" t="s">
+      <c r="B3" s="202"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="201" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="219"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="221"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="203"/>
+      <c r="H3" s="204"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -14291,18 +14410,18 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="218" t="s">
+      <c r="A25" s="201" t="s">
         <v>789</v>
       </c>
-      <c r="B25" s="219"/>
-      <c r="C25" s="220"/>
-      <c r="D25" s="221"/>
-      <c r="E25" s="218" t="s">
+      <c r="B25" s="202"/>
+      <c r="C25" s="203"/>
+      <c r="D25" s="204"/>
+      <c r="E25" s="201" t="s">
         <v>790</v>
       </c>
-      <c r="F25" s="219"/>
-      <c r="G25" s="220"/>
-      <c r="H25" s="221"/>
+      <c r="F25" s="202"/>
+      <c r="G25" s="203"/>
+      <c r="H25" s="204"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
@@ -14316,11 +14435,11 @@
       <c r="E26" s="125" t="s">
         <v>793</v>
       </c>
-      <c r="F26" s="213" t="s">
+      <c r="F26" s="208" t="s">
         <v>794</v>
       </c>
-      <c r="G26" s="214"/>
-      <c r="H26" s="215" t="s">
+      <c r="G26" s="209"/>
+      <c r="H26" s="210" t="s">
         <v>762</v>
       </c>
     </row>
@@ -14328,11 +14447,11 @@
       <c r="A27" s="137" t="s">
         <v>795</v>
       </c>
-      <c r="B27" s="208" t="s">
+      <c r="B27" s="211" t="s">
         <v>796</v>
       </c>
-      <c r="C27" s="209"/>
-      <c r="D27" s="211" t="s">
+      <c r="C27" s="212"/>
+      <c r="D27" s="213" t="s">
         <v>624</v>
       </c>
       <c r="E27" s="129" t="s">
@@ -14342,7 +14461,7 @@
         <v>798</v>
       </c>
       <c r="G27" s="206"/>
-      <c r="H27" s="212" t="s">
+      <c r="H27" s="214" t="s">
         <v>764</v>
       </c>
     </row>
@@ -14360,11 +14479,11 @@
       <c r="E28" s="137" t="s">
         <v>801</v>
       </c>
-      <c r="F28" s="208" t="s">
+      <c r="F28" s="211" t="s">
         <v>802</v>
       </c>
-      <c r="G28" s="209"/>
-      <c r="H28" s="210" t="s">
+      <c r="G28" s="212"/>
+      <c r="H28" s="215" t="s">
         <v>766</v>
       </c>
     </row>
@@ -14372,11 +14491,11 @@
       <c r="A29" s="137" t="s">
         <v>803</v>
       </c>
-      <c r="B29" s="208" t="s">
+      <c r="B29" s="211" t="s">
         <v>804</v>
       </c>
-      <c r="C29" s="209"/>
-      <c r="D29" s="211" t="s">
+      <c r="C29" s="212"/>
+      <c r="D29" s="213" t="s">
         <v>626</v>
       </c>
       <c r="E29" s="129" t="s">
@@ -14386,7 +14505,7 @@
         <v>806</v>
       </c>
       <c r="G29" s="206"/>
-      <c r="H29" s="212" t="s">
+      <c r="H29" s="214" t="s">
         <v>768</v>
       </c>
     </row>
@@ -14404,11 +14523,11 @@
       <c r="E30" s="137" t="s">
         <v>809</v>
       </c>
-      <c r="F30" s="208" t="s">
+      <c r="F30" s="211" t="s">
         <v>810</v>
       </c>
-      <c r="G30" s="209"/>
-      <c r="H30" s="210" t="s">
+      <c r="G30" s="212"/>
+      <c r="H30" s="215" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14416,11 +14535,11 @@
       <c r="A31" s="137" t="s">
         <v>811</v>
       </c>
-      <c r="B31" s="208" t="s">
+      <c r="B31" s="211" t="s">
         <v>812</v>
       </c>
-      <c r="C31" s="209"/>
-      <c r="D31" s="211" t="s">
+      <c r="C31" s="212"/>
+      <c r="D31" s="213" t="s">
         <v>628</v>
       </c>
       <c r="E31" s="129" t="s">
@@ -14430,7 +14549,7 @@
         <v>814</v>
       </c>
       <c r="G31" s="206"/>
-      <c r="H31" s="212" t="s">
+      <c r="H31" s="214" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14446,9 +14565,9 @@
         <v>629</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="208"/>
-      <c r="G32" s="209"/>
-      <c r="H32" s="210" t="s">
+      <c r="F32" s="211"/>
+      <c r="G32" s="212"/>
+      <c r="H32" s="215" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14456,17 +14575,17 @@
       <c r="A33" s="137" t="s">
         <v>817</v>
       </c>
-      <c r="B33" s="208" t="s">
+      <c r="B33" s="211" t="s">
         <v>818</v>
       </c>
-      <c r="C33" s="209"/>
-      <c r="D33" s="211" t="s">
+      <c r="C33" s="212"/>
+      <c r="D33" s="213" t="s">
         <v>623</v>
       </c>
       <c r="E33" s="129"/>
       <c r="F33" s="205"/>
       <c r="G33" s="206"/>
-      <c r="H33" s="212" t="s">
+      <c r="H33" s="214" t="s">
         <v>762</v>
       </c>
     </row>
@@ -14482,9 +14601,9 @@
         <v>624</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="208"/>
-      <c r="G34" s="209"/>
-      <c r="H34" s="210" t="s">
+      <c r="F34" s="211"/>
+      <c r="G34" s="212"/>
+      <c r="H34" s="215" t="s">
         <v>764</v>
       </c>
     </row>
@@ -14492,17 +14611,17 @@
       <c r="A35" s="137" t="s">
         <v>821</v>
       </c>
-      <c r="B35" s="208" t="s">
+      <c r="B35" s="211" t="s">
         <v>822</v>
       </c>
-      <c r="C35" s="209"/>
-      <c r="D35" s="211" t="s">
+      <c r="C35" s="212"/>
+      <c r="D35" s="213" t="s">
         <v>625</v>
       </c>
       <c r="E35" s="129"/>
       <c r="F35" s="205"/>
       <c r="G35" s="206"/>
-      <c r="H35" s="212" t="s">
+      <c r="H35" s="214" t="s">
         <v>766</v>
       </c>
     </row>
@@ -14518,9 +14637,9 @@
         <v>626</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="208"/>
-      <c r="G36" s="209"/>
-      <c r="H36" s="210" t="s">
+      <c r="F36" s="211"/>
+      <c r="G36" s="212"/>
+      <c r="H36" s="215" t="s">
         <v>768</v>
       </c>
     </row>
@@ -14528,17 +14647,17 @@
       <c r="A37" s="137" t="s">
         <v>825</v>
       </c>
-      <c r="B37" s="208" t="s">
+      <c r="B37" s="211" t="s">
         <v>826</v>
       </c>
-      <c r="C37" s="209"/>
-      <c r="D37" s="211" t="s">
+      <c r="C37" s="212"/>
+      <c r="D37" s="213" t="s">
         <v>627</v>
       </c>
       <c r="E37" s="129"/>
       <c r="F37" s="205"/>
       <c r="G37" s="206"/>
-      <c r="H37" s="212" t="s">
+      <c r="H37" s="214" t="s">
         <v>770</v>
       </c>
     </row>
@@ -14554,9 +14673,9 @@
         <v>628</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="208"/>
-      <c r="G38" s="209"/>
-      <c r="H38" s="210" t="s">
+      <c r="F38" s="211"/>
+      <c r="G38" s="212"/>
+      <c r="H38" s="215" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14564,17 +14683,17 @@
       <c r="A39" s="137" t="s">
         <v>829</v>
       </c>
-      <c r="B39" s="208" t="s">
+      <c r="B39" s="211" t="s">
         <v>830</v>
       </c>
-      <c r="C39" s="209"/>
-      <c r="D39" s="211" t="s">
+      <c r="C39" s="212"/>
+      <c r="D39" s="213" t="s">
         <v>629</v>
       </c>
       <c r="E39" s="129"/>
       <c r="F39" s="205"/>
       <c r="G39" s="206"/>
-      <c r="H39" s="212" t="s">
+      <c r="H39" s="214" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14590,57 +14709,28 @@
         <v>629</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="208"/>
-      <c r="G40" s="209"/>
-      <c r="H40" s="210"/>
+      <c r="F40" s="211"/>
+      <c r="G40" s="212"/>
+      <c r="H40" s="215"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>832</v>
       </c>
-      <c r="B41" s="199" t="s">
+      <c r="B41" s="216" t="s">
         <v>830</v>
       </c>
-      <c r="C41" s="200"/>
-      <c r="D41" s="201" t="s">
+      <c r="C41" s="217"/>
+      <c r="D41" s="218" t="s">
         <v>629</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="202"/>
-      <c r="G41" s="203"/>
-      <c r="H41" s="204"/>
+      <c r="F41" s="219"/>
+      <c r="G41" s="220"/>
+      <c r="H41" s="221"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -14649,6 +14739,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added AH64 presets
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="AV-8B Presets" sheetId="8" r:id="rId10"/>
     <sheet name="AJS-37 Presets" sheetId="9" r:id="rId11"/>
     <sheet name="AIRCRAFTS" sheetId="14" r:id="rId12"/>
+    <sheet name="AH64 PResets" sheetId="16" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="885">
   <si>
     <t>AWACS</t>
   </si>
@@ -2648,13 +2649,85 @@
   </si>
   <si>
     <t>309.80</t>
+  </si>
+  <si>
+    <t>AH-64D presets  (OPAR) V1.0</t>
+  </si>
+  <si>
+    <t>VHF</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>SLATE 1</t>
+  </si>
+  <si>
+    <t>OLIVE 11</t>
+  </si>
+  <si>
+    <t>SLATE 2</t>
+  </si>
+  <si>
+    <t>SLATE 3</t>
+  </si>
+  <si>
+    <t>SLATE 4</t>
+  </si>
+  <si>
+    <t>SLATE 5</t>
+  </si>
+  <si>
+    <t>SLATE 6</t>
+  </si>
+  <si>
+    <t>SLATE 7</t>
+  </si>
+  <si>
+    <t>SLATE 8</t>
+  </si>
+  <si>
+    <t>SLATE 9</t>
+  </si>
+  <si>
+    <t>SLATE 10</t>
+  </si>
+  <si>
+    <t>RW COMMON</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #1</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #2</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #3</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #4</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #5</t>
+  </si>
+  <si>
+    <t>RW INTERNAL #6</t>
+  </si>
+  <si>
+    <t>AH-64D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2825,6 +2898,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="24">
     <fill>
@@ -2966,7 +3072,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -3577,11 +3683,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3936,15 +4068,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3954,27 +4107,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4059,6 +4191,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4077,57 +4260,6 @@
     <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4140,6 +4272,82 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4182,7 +4390,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4666,10 +4874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:AJ52"/>
+  <dimension ref="B3:AJ57"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC44" sqref="AC44"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4720,18 +4928,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="161" t="s">
+      <c r="R3" s="169" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="161"/>
-      <c r="T3" s="161"/>
-      <c r="AA3" s="163" t="s">
+      <c r="S3" s="169"/>
+      <c r="T3" s="169"/>
+      <c r="AA3" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="164"/>
-      <c r="AC3" s="164"/>
-      <c r="AD3" s="164"/>
-      <c r="AE3" s="165"/>
+      <c r="AB3" s="171"/>
+      <c r="AC3" s="171"/>
+      <c r="AD3" s="171"/>
+      <c r="AE3" s="172"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4774,7 +4982,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="166" t="s">
+      <c r="R4" s="162" t="s">
         <v>638</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -4783,12 +4991,12 @@
       <c r="T4" s="99" t="s">
         <v>641</v>
       </c>
-      <c r="V4" s="162" t="s">
+      <c r="V4" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
-      <c r="Y4" s="162"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -4842,7 +5050,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="167"/>
+      <c r="R5" s="163"/>
       <c r="S5" s="31" t="s">
         <v>607</v>
       </c>
@@ -4920,7 +5128,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="168"/>
+      <c r="R6" s="164"/>
       <c r="S6" s="100" t="s">
         <v>640</v>
       </c>
@@ -4996,7 +5204,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="166" t="s">
+      <c r="R7" s="162" t="s">
         <v>644</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5076,7 +5284,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="167"/>
+      <c r="R8" s="163"/>
       <c r="S8" s="31" t="s">
         <v>607</v>
       </c>
@@ -5145,7 +5353,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="168"/>
+      <c r="R9" s="164"/>
       <c r="S9" s="100" t="s">
         <v>640</v>
       </c>
@@ -5272,7 +5480,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="170" t="s">
+      <c r="R11" s="165" t="s">
         <v>645</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5345,7 +5553,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="171"/>
+      <c r="R12" s="166"/>
       <c r="S12" s="97" t="s">
         <v>607</v>
       </c>
@@ -5412,7 +5620,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="172"/>
+      <c r="R13" s="167"/>
       <c r="S13" s="105" t="s">
         <v>640</v>
       </c>
@@ -5435,11 +5643,11 @@
       <c r="AA13" s="41" t="s">
         <v>855</v>
       </c>
-      <c r="AD13" s="163" t="s">
+      <c r="AD13" s="170" t="s">
         <v>630</v>
       </c>
-      <c r="AE13" s="164"/>
-      <c r="AF13" s="165"/>
+      <c r="AE13" s="171"/>
+      <c r="AF13" s="172"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5486,7 +5694,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="166" t="s">
+      <c r="R14" s="162" t="s">
         <v>648</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5564,7 +5772,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="167"/>
+      <c r="R15" s="163"/>
       <c r="S15" s="97" t="s">
         <v>607</v>
       </c>
@@ -5625,22 +5833,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="168"/>
+      <c r="R16" s="164"/>
       <c r="S16" s="105" t="s">
         <v>640</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="V16" s="162" t="s">
+      <c r="V16" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="162"/>
-      <c r="X16" s="162"/>
-      <c r="Y16" s="162"/>
-      <c r="Z16" s="162"/>
-      <c r="AA16" s="162"/>
-      <c r="AB16" s="162"/>
+      <c r="W16" s="160"/>
+      <c r="X16" s="160"/>
+      <c r="Y16" s="160"/>
+      <c r="Z16" s="160"/>
+      <c r="AA16" s="160"/>
+      <c r="AB16" s="160"/>
       <c r="AD16" s="7" t="s">
         <v>623</v>
       </c>
@@ -5932,11 +6140,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="162" t="s">
+      <c r="R20" s="160" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="162"/>
-      <c r="T20" s="162"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>672</v>
@@ -6107,15 +6315,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="163" t="s">
+      <c r="V22" s="170" t="s">
         <v>663</v>
       </c>
-      <c r="W22" s="164"/>
-      <c r="X22" s="164"/>
-      <c r="Y22" s="164"/>
-      <c r="Z22" s="164"/>
-      <c r="AA22" s="164"/>
-      <c r="AB22" s="165"/>
+      <c r="W22" s="171"/>
+      <c r="X22" s="171"/>
+      <c r="Y22" s="171"/>
+      <c r="Z22" s="171"/>
+      <c r="AA22" s="171"/>
+      <c r="AB22" s="172"/>
       <c r="AD22" s="7" t="s">
         <v>629</v>
       </c>
@@ -6584,33 +6792,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="162" t="s">
+      <c r="B31" s="160" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="162"/>
-      <c r="D31" s="162"/>
-      <c r="E31" s="162"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="162"/>
-      <c r="H31" s="162"/>
-      <c r="J31" s="162" t="s">
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="J31" s="160" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="162"/>
-      <c r="L31" s="162"/>
-      <c r="M31" s="162"/>
-      <c r="N31" s="162"/>
-      <c r="O31" s="162"/>
-      <c r="P31" s="162"/>
-      <c r="T31" s="162" t="s">
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+      <c r="T31" s="160" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="162"/>
-      <c r="V31" s="162"/>
-      <c r="W31" s="162"/>
-      <c r="X31" s="162"/>
-      <c r="Y31" s="162"/>
-      <c r="Z31" s="162"/>
+      <c r="U31" s="160"/>
+      <c r="V31" s="160"/>
+      <c r="W31" s="160"/>
+      <c r="X31" s="160"/>
+      <c r="Y31" s="160"/>
+      <c r="Z31" s="160"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -6892,7 +7100,7 @@
       <c r="Z35" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AD35" s="160" t="s">
+      <c r="AD35" s="168" t="s">
         <v>700</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -6978,7 +7186,7 @@
       <c r="Z36" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD36" s="160"/>
+      <c r="AD36" s="168"/>
       <c r="AE36" s="7"/>
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
@@ -7050,7 +7258,7 @@
       <c r="Z37" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD37" s="160"/>
+      <c r="AD37" s="168"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7107,7 +7315,7 @@
       <c r="Z38" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="AD38" s="160"/>
+      <c r="AD38" s="168"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7122,15 +7330,15 @@
       <c r="F39" t="s">
         <v>567</v>
       </c>
-      <c r="J39" s="169" t="s">
+      <c r="J39" s="161" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="169"/>
-      <c r="L39" s="169"/>
-      <c r="M39" s="169"/>
-      <c r="N39" s="169"/>
-      <c r="O39" s="169"/>
-      <c r="P39" s="169"/>
+      <c r="K39" s="161"/>
+      <c r="L39" s="161"/>
+      <c r="M39" s="161"/>
+      <c r="N39" s="161"/>
+      <c r="O39" s="161"/>
+      <c r="P39" s="161"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7355,6 +7563,15 @@
       <c r="F48" t="s">
         <v>842</v>
       </c>
+      <c r="J48" t="s">
+        <v>884</v>
+      </c>
+      <c r="L48" s="253">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M48" t="s">
+        <v>866</v>
+      </c>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
@@ -7370,6 +7587,15 @@
       <c r="F49" t="s">
         <v>843</v>
       </c>
+      <c r="J49" t="s">
+        <v>884</v>
+      </c>
+      <c r="L49" s="253">
+        <v>65.7</v>
+      </c>
+      <c r="M49" t="s">
+        <v>868</v>
+      </c>
       <c r="T49" s="7" t="s">
         <v>694</v>
       </c>
@@ -7397,6 +7623,15 @@
       <c r="F50" t="s">
         <v>844</v>
       </c>
+      <c r="J50" t="s">
+        <v>884</v>
+      </c>
+      <c r="L50" s="253">
+        <v>65.8</v>
+      </c>
+      <c r="M50" t="s">
+        <v>869</v>
+      </c>
       <c r="T50" s="7" t="s">
         <v>695</v>
       </c>
@@ -7418,6 +7653,15 @@
       </c>
     </row>
     <row r="51" spans="5:26">
+      <c r="J51" t="s">
+        <v>884</v>
+      </c>
+      <c r="L51" s="253">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="M51" t="s">
+        <v>870</v>
+      </c>
       <c r="T51" s="7" t="s">
         <v>696</v>
       </c>
@@ -7439,6 +7683,15 @@
       </c>
     </row>
     <row r="52" spans="5:26">
+      <c r="J52" t="s">
+        <v>884</v>
+      </c>
+      <c r="L52" s="253">
+        <v>66</v>
+      </c>
+      <c r="M52" t="s">
+        <v>871</v>
+      </c>
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
       <c r="V52" s="7" t="s">
@@ -7457,15 +7710,63 @@
         <v>662</v>
       </c>
     </row>
+    <row r="53" spans="5:26">
+      <c r="J53" t="s">
+        <v>884</v>
+      </c>
+      <c r="L53" s="253">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M53" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="54" spans="5:26">
+      <c r="J54" t="s">
+        <v>884</v>
+      </c>
+      <c r="L54" s="253">
+        <v>66.2</v>
+      </c>
+      <c r="M54" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="55" spans="5:26">
+      <c r="J55" t="s">
+        <v>884</v>
+      </c>
+      <c r="L55" s="253">
+        <v>66.300000000000097</v>
+      </c>
+      <c r="M55" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="56" spans="5:26">
+      <c r="J56" t="s">
+        <v>884</v>
+      </c>
+      <c r="L56" s="253">
+        <v>66.400000000000105</v>
+      </c>
+      <c r="M56" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="57" spans="5:26">
+      <c r="J57" t="s">
+        <v>884</v>
+      </c>
+      <c r="L57" s="253">
+        <v>66.500000000000099</v>
+      </c>
+      <c r="M57" t="s">
+        <v>876</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7475,6 +7776,13 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8313,7 +8621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
@@ -9923,6 +10231,962 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="228" t="s">
+        <v>862</v>
+      </c>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="230"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="231"/>
+      <c r="H2" s="231"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25">
+      <c r="A3" s="232" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="233"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233" t="s">
+        <v>863</v>
+      </c>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="234"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A4" s="239">
+        <v>1</v>
+      </c>
+      <c r="B4" s="240" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="235" t="s">
+        <v>479</v>
+      </c>
+      <c r="D4" s="237" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="81">
+        <v>1</v>
+      </c>
+      <c r="F4" s="240">
+        <v>129.6</v>
+      </c>
+      <c r="G4" s="236" t="s">
+        <v>640</v>
+      </c>
+      <c r="H4" s="237" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A5" s="239">
+        <v>2</v>
+      </c>
+      <c r="B5" s="240" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="237" t="s">
+        <v>484</v>
+      </c>
+      <c r="D5" s="250" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="81">
+        <v>2</v>
+      </c>
+      <c r="F5" s="240">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="G5" s="236" t="s">
+        <v>607</v>
+      </c>
+      <c r="H5" s="237" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A6" s="239">
+        <v>3</v>
+      </c>
+      <c r="B6" s="240" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="235" t="s">
+        <v>480</v>
+      </c>
+      <c r="D6" s="237" t="s">
+        <v>622</v>
+      </c>
+      <c r="E6" s="81">
+        <v>3</v>
+      </c>
+      <c r="F6" s="240">
+        <v>118.4</v>
+      </c>
+      <c r="G6" s="236" t="s">
+        <v>640</v>
+      </c>
+      <c r="H6" s="237" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A7" s="239">
+        <v>4</v>
+      </c>
+      <c r="B7" s="240" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="235" t="s">
+        <v>482</v>
+      </c>
+      <c r="D7" s="237" t="s">
+        <v>623</v>
+      </c>
+      <c r="E7" s="81">
+        <v>4</v>
+      </c>
+      <c r="F7" s="240">
+        <v>118.2</v>
+      </c>
+      <c r="G7" s="236" t="s">
+        <v>607</v>
+      </c>
+      <c r="H7" s="237" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A8" s="239">
+        <v>5</v>
+      </c>
+      <c r="B8" s="240" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="235" t="s">
+        <v>481</v>
+      </c>
+      <c r="D8" s="237" t="s">
+        <v>624</v>
+      </c>
+      <c r="E8" s="81">
+        <v>5</v>
+      </c>
+      <c r="F8" s="240" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="236" t="s">
+        <v>655</v>
+      </c>
+      <c r="H8" s="237" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A9" s="239">
+        <v>6</v>
+      </c>
+      <c r="B9" s="240" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="235" t="s">
+        <v>483</v>
+      </c>
+      <c r="D9" s="237" t="s">
+        <v>625</v>
+      </c>
+      <c r="E9" s="81">
+        <v>6</v>
+      </c>
+      <c r="F9" s="240" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="236" t="s">
+        <v>658</v>
+      </c>
+      <c r="H9" s="237" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A10" s="239">
+        <v>7</v>
+      </c>
+      <c r="B10" s="240" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="235" t="s">
+        <v>486</v>
+      </c>
+      <c r="D10" s="237" t="s">
+        <v>626</v>
+      </c>
+      <c r="E10" s="81">
+        <v>7</v>
+      </c>
+      <c r="F10" s="240" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" s="236" t="s">
+        <v>659</v>
+      </c>
+      <c r="H10" s="237" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A11" s="239">
+        <v>8</v>
+      </c>
+      <c r="B11" s="240" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="235" t="s">
+        <v>488</v>
+      </c>
+      <c r="D11" s="237" t="s">
+        <v>627</v>
+      </c>
+      <c r="E11" s="81">
+        <v>8</v>
+      </c>
+      <c r="F11" s="240" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="236" t="s">
+        <v>660</v>
+      </c>
+      <c r="H11" s="237" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A12" s="239">
+        <v>9</v>
+      </c>
+      <c r="B12" s="240" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="235" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="237" t="s">
+        <v>628</v>
+      </c>
+      <c r="E12" s="81">
+        <v>9</v>
+      </c>
+      <c r="F12" s="240" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="236" t="s">
+        <v>378</v>
+      </c>
+      <c r="H12" s="250" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A13" s="239">
+        <v>10</v>
+      </c>
+      <c r="B13" s="240" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="235" t="s">
+        <v>490</v>
+      </c>
+      <c r="D13" s="237" t="s">
+        <v>629</v>
+      </c>
+      <c r="E13" s="81">
+        <v>10</v>
+      </c>
+      <c r="F13" s="240" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="236" t="s">
+        <v>491</v>
+      </c>
+      <c r="H13" s="238" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A14" s="239">
+        <v>11</v>
+      </c>
+      <c r="B14" s="240" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="235" t="s">
+        <v>506</v>
+      </c>
+      <c r="D14" s="237" t="s">
+        <v>631</v>
+      </c>
+      <c r="E14" s="81">
+        <v>11</v>
+      </c>
+      <c r="F14" s="240" t="s">
+        <v>257</v>
+      </c>
+      <c r="G14" s="236" t="s">
+        <v>496</v>
+      </c>
+      <c r="H14" s="238" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A15" s="239">
+        <v>12</v>
+      </c>
+      <c r="B15" s="240" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="235" t="s">
+        <v>507</v>
+      </c>
+      <c r="D15" s="237" t="s">
+        <v>632</v>
+      </c>
+      <c r="E15" s="81">
+        <v>12</v>
+      </c>
+      <c r="F15" s="240" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="236" t="s">
+        <v>556</v>
+      </c>
+      <c r="H15" s="237" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A16" s="239">
+        <v>13</v>
+      </c>
+      <c r="B16" s="240" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="235" t="s">
+        <v>508</v>
+      </c>
+      <c r="D16" s="237" t="s">
+        <v>633</v>
+      </c>
+      <c r="E16" s="81">
+        <v>13</v>
+      </c>
+      <c r="F16" s="240"/>
+      <c r="G16" s="235"/>
+      <c r="H16" s="235"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A17" s="239">
+        <v>14</v>
+      </c>
+      <c r="B17" s="240" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="235" t="s">
+        <v>652</v>
+      </c>
+      <c r="D17" s="237" t="s">
+        <v>709</v>
+      </c>
+      <c r="E17" s="81">
+        <v>14</v>
+      </c>
+      <c r="F17" s="240"/>
+      <c r="G17" s="235"/>
+      <c r="H17" s="235"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A18" s="239">
+        <v>15</v>
+      </c>
+      <c r="B18" s="240" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="235" t="s">
+        <v>653</v>
+      </c>
+      <c r="D18" s="237" t="s">
+        <v>710</v>
+      </c>
+      <c r="E18" s="81">
+        <v>15</v>
+      </c>
+      <c r="F18" s="240"/>
+      <c r="G18" s="235"/>
+      <c r="H18" s="235"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A19" s="239">
+        <v>16</v>
+      </c>
+      <c r="B19" s="240" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="235" t="s">
+        <v>654</v>
+      </c>
+      <c r="D19" s="237" t="s">
+        <v>711</v>
+      </c>
+      <c r="E19" s="81">
+        <v>16</v>
+      </c>
+      <c r="F19" s="240"/>
+      <c r="G19" s="235"/>
+      <c r="H19" s="235"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A20" s="239">
+        <v>17</v>
+      </c>
+      <c r="B20" s="240" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="235" t="s">
+        <v>485</v>
+      </c>
+      <c r="D20" s="237" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="81">
+        <v>17</v>
+      </c>
+      <c r="F20" s="240"/>
+      <c r="G20" s="235"/>
+      <c r="H20" s="235"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A21" s="239">
+        <v>18</v>
+      </c>
+      <c r="B21" s="240" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="235" t="s">
+        <v>487</v>
+      </c>
+      <c r="D21" s="237" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="81">
+        <v>18</v>
+      </c>
+      <c r="F21" s="240"/>
+      <c r="G21" s="235"/>
+      <c r="H21" s="235"/>
+    </row>
+    <row r="22" spans="1:8" ht="19.5">
+      <c r="A22" s="241" t="s">
+        <v>864</v>
+      </c>
+      <c r="B22" s="242"/>
+      <c r="C22" s="242"/>
+      <c r="D22" s="242"/>
+      <c r="E22" s="241" t="s">
+        <v>865</v>
+      </c>
+      <c r="F22" s="242"/>
+      <c r="G22" s="242"/>
+      <c r="H22" s="242"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A23" s="239">
+        <v>1</v>
+      </c>
+      <c r="B23" s="243">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="C23" s="244" t="s">
+        <v>866</v>
+      </c>
+      <c r="D23" s="244" t="s">
+        <v>866</v>
+      </c>
+      <c r="E23" s="239">
+        <v>1</v>
+      </c>
+      <c r="F23" s="243">
+        <v>21</v>
+      </c>
+      <c r="G23" s="244" t="s">
+        <v>867</v>
+      </c>
+      <c r="H23" s="251" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A24" s="239">
+        <v>2</v>
+      </c>
+      <c r="B24" s="245">
+        <v>65.7</v>
+      </c>
+      <c r="C24" s="246" t="s">
+        <v>868</v>
+      </c>
+      <c r="D24" s="246" t="s">
+        <v>868</v>
+      </c>
+      <c r="E24" s="239">
+        <v>2</v>
+      </c>
+      <c r="F24" s="245"/>
+      <c r="G24" s="246"/>
+      <c r="H24" s="246"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A25" s="239">
+        <v>3</v>
+      </c>
+      <c r="B25" s="245">
+        <v>65.8</v>
+      </c>
+      <c r="C25" s="246" t="s">
+        <v>869</v>
+      </c>
+      <c r="D25" s="246" t="s">
+        <v>869</v>
+      </c>
+      <c r="E25" s="239">
+        <v>3</v>
+      </c>
+      <c r="F25" s="245"/>
+      <c r="G25" s="246"/>
+      <c r="H25" s="246"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A26" s="239">
+        <v>4</v>
+      </c>
+      <c r="B26" s="245">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="C26" s="246" t="s">
+        <v>870</v>
+      </c>
+      <c r="D26" s="246" t="s">
+        <v>870</v>
+      </c>
+      <c r="E26" s="239">
+        <v>4</v>
+      </c>
+      <c r="F26" s="245"/>
+      <c r="G26" s="246"/>
+      <c r="H26" s="246"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A27" s="239">
+        <v>5</v>
+      </c>
+      <c r="B27" s="245">
+        <v>66</v>
+      </c>
+      <c r="C27" s="246" t="s">
+        <v>871</v>
+      </c>
+      <c r="D27" s="246" t="s">
+        <v>871</v>
+      </c>
+      <c r="E27" s="239">
+        <v>5</v>
+      </c>
+      <c r="F27" s="245"/>
+      <c r="G27" s="246"/>
+      <c r="H27" s="246"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A28" s="239">
+        <v>6</v>
+      </c>
+      <c r="B28" s="245">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="C28" s="246" t="s">
+        <v>872</v>
+      </c>
+      <c r="D28" s="246" t="s">
+        <v>872</v>
+      </c>
+      <c r="E28" s="239">
+        <v>6</v>
+      </c>
+      <c r="F28" s="245"/>
+      <c r="G28" s="246"/>
+      <c r="H28" s="246"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A29" s="239">
+        <v>7</v>
+      </c>
+      <c r="B29" s="245">
+        <v>66.2</v>
+      </c>
+      <c r="C29" s="246" t="s">
+        <v>873</v>
+      </c>
+      <c r="D29" s="246" t="s">
+        <v>873</v>
+      </c>
+      <c r="E29" s="239">
+        <v>7</v>
+      </c>
+      <c r="F29" s="245"/>
+      <c r="G29" s="246"/>
+      <c r="H29" s="246"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A30" s="239">
+        <v>8</v>
+      </c>
+      <c r="B30" s="245">
+        <v>66.300000000000097</v>
+      </c>
+      <c r="C30" s="246" t="s">
+        <v>874</v>
+      </c>
+      <c r="D30" s="246" t="s">
+        <v>874</v>
+      </c>
+      <c r="E30" s="239">
+        <v>8</v>
+      </c>
+      <c r="F30" s="245"/>
+      <c r="G30" s="246"/>
+      <c r="H30" s="246"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A31" s="239">
+        <v>9</v>
+      </c>
+      <c r="B31" s="245">
+        <v>66.400000000000105</v>
+      </c>
+      <c r="C31" s="247" t="s">
+        <v>875</v>
+      </c>
+      <c r="D31" s="247" t="s">
+        <v>875</v>
+      </c>
+      <c r="E31" s="239">
+        <v>9</v>
+      </c>
+      <c r="F31" s="245"/>
+      <c r="G31" s="247"/>
+      <c r="H31" s="247"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A32" s="239">
+        <v>10</v>
+      </c>
+      <c r="B32" s="245">
+        <v>66.500000000000099</v>
+      </c>
+      <c r="C32" s="247" t="s">
+        <v>876</v>
+      </c>
+      <c r="D32" s="247" t="s">
+        <v>876</v>
+      </c>
+      <c r="E32" s="239">
+        <v>10</v>
+      </c>
+      <c r="F32" s="245"/>
+      <c r="G32" s="247"/>
+      <c r="H32" s="247"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A33" s="239">
+        <v>11</v>
+      </c>
+      <c r="B33" s="248">
+        <v>35.6</v>
+      </c>
+      <c r="C33" s="249" t="s">
+        <v>523</v>
+      </c>
+      <c r="D33" s="252" t="s">
+        <v>877</v>
+      </c>
+      <c r="E33" s="239">
+        <v>11</v>
+      </c>
+      <c r="F33" s="248"/>
+      <c r="G33" s="249"/>
+      <c r="H33" s="247"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A34" s="239">
+        <v>12</v>
+      </c>
+      <c r="B34" s="248" t="s">
+        <v>442</v>
+      </c>
+      <c r="C34" s="249" t="s">
+        <v>463</v>
+      </c>
+      <c r="D34" s="252" t="s">
+        <v>878</v>
+      </c>
+      <c r="E34" s="239">
+        <v>12</v>
+      </c>
+      <c r="F34" s="248"/>
+      <c r="G34" s="249"/>
+      <c r="H34" s="247"/>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A35" s="239">
+        <v>13</v>
+      </c>
+      <c r="B35" s="248" t="s">
+        <v>443</v>
+      </c>
+      <c r="C35" s="249" t="s">
+        <v>466</v>
+      </c>
+      <c r="D35" s="252" t="s">
+        <v>879</v>
+      </c>
+      <c r="E35" s="239">
+        <v>13</v>
+      </c>
+      <c r="F35" s="248"/>
+      <c r="G35" s="249"/>
+      <c r="H35" s="247"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A36" s="239">
+        <v>14</v>
+      </c>
+      <c r="B36" s="248" t="s">
+        <v>444</v>
+      </c>
+      <c r="C36" s="249" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="252" t="s">
+        <v>880</v>
+      </c>
+      <c r="E36" s="239">
+        <v>14</v>
+      </c>
+      <c r="F36" s="248"/>
+      <c r="G36" s="249"/>
+      <c r="H36" s="247"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A37" s="239">
+        <v>15</v>
+      </c>
+      <c r="B37" s="248" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="249" t="s">
+        <v>469</v>
+      </c>
+      <c r="D37" s="252" t="s">
+        <v>881</v>
+      </c>
+      <c r="E37" s="239">
+        <v>15</v>
+      </c>
+      <c r="F37" s="248"/>
+      <c r="G37" s="249"/>
+      <c r="H37" s="247"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A38" s="239">
+        <v>16</v>
+      </c>
+      <c r="B38" s="248" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="249" t="s">
+        <v>471</v>
+      </c>
+      <c r="D38" s="252" t="s">
+        <v>882</v>
+      </c>
+      <c r="E38" s="239">
+        <v>16</v>
+      </c>
+      <c r="F38" s="248"/>
+      <c r="G38" s="249"/>
+      <c r="H38" s="247"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A39" s="239">
+        <v>17</v>
+      </c>
+      <c r="B39" s="248" t="s">
+        <v>273</v>
+      </c>
+      <c r="C39" s="249" t="s">
+        <v>473</v>
+      </c>
+      <c r="D39" s="252" t="s">
+        <v>883</v>
+      </c>
+      <c r="E39" s="239">
+        <v>17</v>
+      </c>
+      <c r="F39" s="248"/>
+      <c r="G39" s="249"/>
+      <c r="H39" s="247"/>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A40" s="239">
+        <v>18</v>
+      </c>
+      <c r="B40" s="248">
+        <v>36.4</v>
+      </c>
+      <c r="C40" s="249" t="s">
+        <v>714</v>
+      </c>
+      <c r="D40" s="247"/>
+      <c r="E40" s="239">
+        <v>18</v>
+      </c>
+      <c r="F40" s="248"/>
+      <c r="G40" s="249"/>
+      <c r="H40" s="247"/>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A41" s="239">
+        <v>19</v>
+      </c>
+      <c r="B41" s="248">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C41" s="249" t="s">
+        <v>473</v>
+      </c>
+      <c r="D41" s="247"/>
+      <c r="E41" s="239">
+        <v>19</v>
+      </c>
+      <c r="F41" s="248"/>
+      <c r="G41" s="249"/>
+      <c r="H41" s="247"/>
+    </row>
+    <row r="42" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A42" s="239">
+        <v>20</v>
+      </c>
+      <c r="B42" s="248">
+        <v>32.25</v>
+      </c>
+      <c r="C42" s="249" t="s">
+        <v>715</v>
+      </c>
+      <c r="D42" s="247"/>
+      <c r="E42" s="239">
+        <v>20</v>
+      </c>
+      <c r="F42" s="248"/>
+      <c r="G42" s="249"/>
+      <c r="H42" s="247"/>
+    </row>
+    <row r="43" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A43" s="248"/>
+      <c r="B43" s="248"/>
+      <c r="C43" s="248"/>
+      <c r="D43" s="248"/>
+      <c r="E43" s="248"/>
+      <c r="F43" s="248"/>
+      <c r="G43" s="248"/>
+      <c r="H43" s="248"/>
+    </row>
+    <row r="44" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A44" s="248"/>
+      <c r="B44" s="248"/>
+      <c r="C44" s="248"/>
+      <c r="D44" s="248"/>
+      <c r="E44" s="248"/>
+      <c r="F44" s="248"/>
+      <c r="G44" s="248"/>
+      <c r="H44" s="248"/>
+    </row>
+    <row r="45" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A45" s="248"/>
+      <c r="B45" s="248"/>
+      <c r="C45" s="248"/>
+      <c r="D45" s="248"/>
+      <c r="E45" s="248"/>
+      <c r="F45" s="248"/>
+      <c r="G45" s="248"/>
+      <c r="H45" s="248"/>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A46" s="248"/>
+      <c r="B46" s="248"/>
+      <c r="C46" s="248"/>
+      <c r="D46" s="248"/>
+      <c r="E46" s="248"/>
+      <c r="F46" s="248"/>
+      <c r="G46" s="248"/>
+      <c r="H46" s="248"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="A1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13115,8 +14379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -13843,8 +15107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -13861,40 +15125,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="201" t="s">
         <v>832</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="219"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
+      <c r="A2" s="202"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="220" t="s">
+      <c r="A3" s="203" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="221"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="223"/>
-      <c r="E3" s="220" t="s">
+      <c r="B3" s="204"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="203" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="221"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="223"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="205"/>
+      <c r="H3" s="206"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -14423,18 +15687,18 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="220" t="s">
+      <c r="A25" s="203" t="s">
         <v>788</v>
       </c>
-      <c r="B25" s="221"/>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223"/>
-      <c r="E25" s="220" t="s">
+      <c r="B25" s="204"/>
+      <c r="C25" s="205"/>
+      <c r="D25" s="206"/>
+      <c r="E25" s="203" t="s">
         <v>789</v>
       </c>
-      <c r="F25" s="221"/>
-      <c r="G25" s="222"/>
-      <c r="H25" s="223"/>
+      <c r="F25" s="204"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="206"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
@@ -14448,11 +15712,11 @@
       <c r="E26" s="125" t="s">
         <v>792</v>
       </c>
-      <c r="F26" s="215" t="s">
+      <c r="F26" s="210" t="s">
         <v>793</v>
       </c>
-      <c r="G26" s="216"/>
-      <c r="H26" s="217" t="s">
+      <c r="G26" s="211"/>
+      <c r="H26" s="212" t="s">
         <v>761</v>
       </c>
     </row>
@@ -14460,11 +15724,11 @@
       <c r="A27" s="137" t="s">
         <v>794</v>
       </c>
-      <c r="B27" s="210" t="s">
+      <c r="B27" s="213" t="s">
         <v>795</v>
       </c>
-      <c r="C27" s="211"/>
-      <c r="D27" s="213" t="s">
+      <c r="C27" s="214"/>
+      <c r="D27" s="215" t="s">
         <v>623</v>
       </c>
       <c r="E27" s="129" t="s">
@@ -14474,7 +15738,7 @@
         <v>797</v>
       </c>
       <c r="G27" s="208"/>
-      <c r="H27" s="214" t="s">
+      <c r="H27" s="216" t="s">
         <v>763</v>
       </c>
     </row>
@@ -14492,11 +15756,11 @@
       <c r="E28" s="137" t="s">
         <v>800</v>
       </c>
-      <c r="F28" s="210" t="s">
+      <c r="F28" s="213" t="s">
         <v>801</v>
       </c>
-      <c r="G28" s="211"/>
-      <c r="H28" s="212" t="s">
+      <c r="G28" s="214"/>
+      <c r="H28" s="217" t="s">
         <v>765</v>
       </c>
     </row>
@@ -14504,11 +15768,11 @@
       <c r="A29" s="137" t="s">
         <v>802</v>
       </c>
-      <c r="B29" s="210" t="s">
+      <c r="B29" s="213" t="s">
         <v>803</v>
       </c>
-      <c r="C29" s="211"/>
-      <c r="D29" s="213" t="s">
+      <c r="C29" s="214"/>
+      <c r="D29" s="215" t="s">
         <v>625</v>
       </c>
       <c r="E29" s="129" t="s">
@@ -14518,7 +15782,7 @@
         <v>805</v>
       </c>
       <c r="G29" s="208"/>
-      <c r="H29" s="214" t="s">
+      <c r="H29" s="216" t="s">
         <v>767</v>
       </c>
     </row>
@@ -14536,11 +15800,11 @@
       <c r="E30" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="F30" s="210" t="s">
+      <c r="F30" s="213" t="s">
         <v>809</v>
       </c>
-      <c r="G30" s="211"/>
-      <c r="H30" s="212" t="s">
+      <c r="G30" s="214"/>
+      <c r="H30" s="217" t="s">
         <v>769</v>
       </c>
     </row>
@@ -14548,11 +15812,11 @@
       <c r="A31" s="137" t="s">
         <v>810</v>
       </c>
-      <c r="B31" s="210" t="s">
+      <c r="B31" s="213" t="s">
         <v>811</v>
       </c>
-      <c r="C31" s="211"/>
-      <c r="D31" s="213" t="s">
+      <c r="C31" s="214"/>
+      <c r="D31" s="215" t="s">
         <v>627</v>
       </c>
       <c r="E31" s="129" t="s">
@@ -14562,7 +15826,7 @@
         <v>813</v>
       </c>
       <c r="G31" s="208"/>
-      <c r="H31" s="214" t="s">
+      <c r="H31" s="216" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14578,9 +15842,9 @@
         <v>628</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="210"/>
-      <c r="G32" s="211"/>
-      <c r="H32" s="212" t="s">
+      <c r="F32" s="213"/>
+      <c r="G32" s="214"/>
+      <c r="H32" s="217" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14588,17 +15852,17 @@
       <c r="A33" s="137" t="s">
         <v>816</v>
       </c>
-      <c r="B33" s="210" t="s">
+      <c r="B33" s="213" t="s">
         <v>817</v>
       </c>
-      <c r="C33" s="211"/>
-      <c r="D33" s="213" t="s">
+      <c r="C33" s="214"/>
+      <c r="D33" s="215" t="s">
         <v>622</v>
       </c>
       <c r="E33" s="129"/>
       <c r="F33" s="207"/>
       <c r="G33" s="208"/>
-      <c r="H33" s="214" t="s">
+      <c r="H33" s="216" t="s">
         <v>761</v>
       </c>
     </row>
@@ -14614,9 +15878,9 @@
         <v>623</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="210"/>
-      <c r="G34" s="211"/>
-      <c r="H34" s="212" t="s">
+      <c r="F34" s="213"/>
+      <c r="G34" s="214"/>
+      <c r="H34" s="217" t="s">
         <v>763</v>
       </c>
     </row>
@@ -14624,17 +15888,17 @@
       <c r="A35" s="137" t="s">
         <v>820</v>
       </c>
-      <c r="B35" s="210" t="s">
+      <c r="B35" s="213" t="s">
         <v>821</v>
       </c>
-      <c r="C35" s="211"/>
-      <c r="D35" s="213" t="s">
+      <c r="C35" s="214"/>
+      <c r="D35" s="215" t="s">
         <v>624</v>
       </c>
       <c r="E35" s="129"/>
       <c r="F35" s="207"/>
       <c r="G35" s="208"/>
-      <c r="H35" s="214" t="s">
+      <c r="H35" s="216" t="s">
         <v>765</v>
       </c>
     </row>
@@ -14650,9 +15914,9 @@
         <v>625</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="210"/>
-      <c r="G36" s="211"/>
-      <c r="H36" s="212" t="s">
+      <c r="F36" s="213"/>
+      <c r="G36" s="214"/>
+      <c r="H36" s="217" t="s">
         <v>767</v>
       </c>
     </row>
@@ -14660,17 +15924,17 @@
       <c r="A37" s="137" t="s">
         <v>824</v>
       </c>
-      <c r="B37" s="210" t="s">
+      <c r="B37" s="213" t="s">
         <v>825</v>
       </c>
-      <c r="C37" s="211"/>
-      <c r="D37" s="213" t="s">
+      <c r="C37" s="214"/>
+      <c r="D37" s="215" t="s">
         <v>626</v>
       </c>
       <c r="E37" s="129"/>
       <c r="F37" s="207"/>
       <c r="G37" s="208"/>
-      <c r="H37" s="214" t="s">
+      <c r="H37" s="216" t="s">
         <v>769</v>
       </c>
     </row>
@@ -14686,9 +15950,9 @@
         <v>627</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="210"/>
-      <c r="G38" s="211"/>
-      <c r="H38" s="212" t="s">
+      <c r="F38" s="213"/>
+      <c r="G38" s="214"/>
+      <c r="H38" s="217" t="s">
         <v>494</v>
       </c>
     </row>
@@ -14696,17 +15960,17 @@
       <c r="A39" s="137" t="s">
         <v>828</v>
       </c>
-      <c r="B39" s="210" t="s">
+      <c r="B39" s="213" t="s">
         <v>829</v>
       </c>
-      <c r="C39" s="211"/>
-      <c r="D39" s="213" t="s">
+      <c r="C39" s="214"/>
+      <c r="D39" s="215" t="s">
         <v>628</v>
       </c>
       <c r="E39" s="129"/>
       <c r="F39" s="207"/>
       <c r="G39" s="208"/>
-      <c r="H39" s="214" t="s">
+      <c r="H39" s="216" t="s">
         <v>495</v>
       </c>
     </row>
@@ -14722,57 +15986,28 @@
         <v>628</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="210"/>
-      <c r="G40" s="211"/>
-      <c r="H40" s="212"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="214"/>
+      <c r="H40" s="217"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>831</v>
       </c>
-      <c r="B41" s="201" t="s">
+      <c r="B41" s="218" t="s">
         <v>829</v>
       </c>
-      <c r="C41" s="202"/>
-      <c r="D41" s="203" t="s">
+      <c r="C41" s="219"/>
+      <c r="D41" s="220" t="s">
         <v>628</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="204"/>
-      <c r="G41" s="205"/>
-      <c r="H41" s="206"/>
+      <c r="F41" s="221"/>
+      <c r="G41" s="222"/>
+      <c r="H41" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -14781,6 +16016,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Changes to callsign list
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="890">
   <si>
     <t>AWACS</t>
   </si>
@@ -2249,9 +2249,6 @@
     <t>Haifa TWR</t>
   </si>
   <si>
-    <t xml:space="preserve">DODGE </t>
-  </si>
-  <si>
     <t>F-16</t>
   </si>
   <si>
@@ -2285,9 +2282,6 @@
     <t>TUSK</t>
   </si>
   <si>
-    <t>UZI</t>
-  </si>
-  <si>
     <t>CV72</t>
   </si>
   <si>
@@ -2585,9 +2579,6 @@
     <t>Ramat David TWR</t>
   </si>
   <si>
-    <t>DODGE  QRA</t>
-  </si>
-  <si>
     <t>AJS-37 Viggen presets OPAR v1.0</t>
   </si>
   <si>
@@ -2624,9 +2615,6 @@
     <t>118.75</t>
   </si>
   <si>
-    <t>FARP LONDON</t>
-  </si>
-  <si>
     <t>AEW502</t>
   </si>
   <si>
@@ -2718,6 +2706,33 @@
   </si>
   <si>
     <t>AH-64D</t>
+  </si>
+  <si>
+    <t>VENOM</t>
+  </si>
+  <si>
+    <t>LOBO</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>RATTLER</t>
+  </si>
+  <si>
+    <t>HAWG</t>
+  </si>
+  <si>
+    <t>BOAR</t>
+  </si>
+  <si>
+    <t>PIG</t>
+  </si>
+  <si>
+    <t>SNAKE</t>
+  </si>
+  <si>
+    <t>HORNET</t>
   </si>
 </sst>
 </file>
@@ -3713,7 +3728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4117,15 +4132,36 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4135,27 +4171,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4240,6 +4255,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4258,57 +4324,6 @@
     <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4348,6 +4363,7 @@
     <xf numFmtId="0" fontId="25" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4390,7 +4406,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4876,7 +4892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AJ57"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
@@ -4928,18 +4944,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="178" t="s">
+      <c r="R3" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="178"/>
-      <c r="T3" s="178"/>
-      <c r="AA3" s="180" t="s">
+      <c r="S3" s="186"/>
+      <c r="T3" s="186"/>
+      <c r="AA3" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="181"/>
-      <c r="AC3" s="181"/>
-      <c r="AD3" s="181"/>
-      <c r="AE3" s="182"/>
+      <c r="AB3" s="188"/>
+      <c r="AC3" s="188"/>
+      <c r="AD3" s="188"/>
+      <c r="AE3" s="189"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -4982,7 +4998,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="183" t="s">
+      <c r="R4" s="179" t="s">
         <v>638</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -4991,12 +5007,12 @@
       <c r="T4" s="99" t="s">
         <v>641</v>
       </c>
-      <c r="V4" s="179" t="s">
+      <c r="V4" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="179"/>
-      <c r="X4" s="179"/>
-      <c r="Y4" s="179"/>
+      <c r="W4" s="177"/>
+      <c r="X4" s="177"/>
+      <c r="Y4" s="177"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -5050,7 +5066,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="184"/>
+      <c r="R5" s="180"/>
       <c r="S5" s="31" t="s">
         <v>607</v>
       </c>
@@ -5128,7 +5144,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="185"/>
+      <c r="R6" s="181"/>
       <c r="S6" s="100" t="s">
         <v>640</v>
       </c>
@@ -5204,7 +5220,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="183" t="s">
+      <c r="R7" s="179" t="s">
         <v>644</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5284,7 +5300,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="184"/>
+      <c r="R8" s="180"/>
       <c r="S8" s="31" t="s">
         <v>607</v>
       </c>
@@ -5353,7 +5369,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="185"/>
+      <c r="R9" s="181"/>
       <c r="S9" s="100" t="s">
         <v>640</v>
       </c>
@@ -5480,7 +5496,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="187" t="s">
+      <c r="R11" s="182" t="s">
         <v>645</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5499,10 +5515,10 @@
         <v>378</v>
       </c>
       <c r="Y11" s="119" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="Z11" s="119" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="AA11" s="96"/>
       <c r="AB11" s="95"/>
@@ -5553,7 +5569,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="188"/>
+      <c r="R12" s="183"/>
       <c r="S12" s="97" t="s">
         <v>607</v>
       </c>
@@ -5561,7 +5577,7 @@
         <v>606</v>
       </c>
       <c r="V12" s="38" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="W12" s="67">
         <v>301</v>
@@ -5574,7 +5590,7 @@
         <v>502</v>
       </c>
       <c r="AA12" s="95" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="13" spans="2:32" ht="16.5" thickBot="1">
@@ -5620,7 +5636,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="189"/>
+      <c r="R13" s="184"/>
       <c r="S13" s="105" t="s">
         <v>640</v>
       </c>
@@ -5628,7 +5644,7 @@
         <v>647</v>
       </c>
       <c r="V13" s="38" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="W13" s="7">
         <v>300</v>
@@ -5641,13 +5657,13 @@
         <v>501</v>
       </c>
       <c r="AA13" s="41" t="s">
-        <v>855</v>
-      </c>
-      <c r="AD13" s="180" t="s">
+        <v>851</v>
+      </c>
+      <c r="AD13" s="187" t="s">
         <v>630</v>
       </c>
-      <c r="AE13" s="181"/>
-      <c r="AF13" s="182"/>
+      <c r="AE13" s="188"/>
+      <c r="AF13" s="189"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5694,7 +5710,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="183" t="s">
+      <c r="R14" s="179" t="s">
         <v>648</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5704,7 +5720,7 @@
         <v>649</v>
       </c>
       <c r="V14" s="38" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="W14" s="7">
         <v>302</v>
@@ -5772,7 +5788,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="184"/>
+      <c r="R15" s="180"/>
       <c r="S15" s="97" t="s">
         <v>607</v>
       </c>
@@ -5833,22 +5849,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="185"/>
+      <c r="R16" s="181"/>
       <c r="S16" s="105" t="s">
         <v>640</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="V16" s="179" t="s">
+      <c r="V16" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="179"/>
-      <c r="X16" s="179"/>
-      <c r="Y16" s="179"/>
-      <c r="Z16" s="179"/>
-      <c r="AA16" s="179"/>
-      <c r="AB16" s="179"/>
+      <c r="W16" s="177"/>
+      <c r="X16" s="177"/>
+      <c r="Y16" s="177"/>
+      <c r="Z16" s="177"/>
+      <c r="AA16" s="177"/>
+      <c r="AB16" s="177"/>
       <c r="AD16" s="7" t="s">
         <v>623</v>
       </c>
@@ -5920,10 +5936,10 @@
         <v>303</v>
       </c>
       <c r="AA17" s="119" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="AB17" s="119" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>624</v>
@@ -6140,11 +6156,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="179" t="s">
+      <c r="R20" s="177" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="179"/>
-      <c r="T20" s="179"/>
+      <c r="S20" s="177"/>
+      <c r="T20" s="177"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>672</v>
@@ -6315,15 +6331,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="180" t="s">
+      <c r="V22" s="187" t="s">
         <v>663</v>
       </c>
-      <c r="W22" s="181"/>
-      <c r="X22" s="181"/>
-      <c r="Y22" s="181"/>
-      <c r="Z22" s="181"/>
-      <c r="AA22" s="181"/>
-      <c r="AB22" s="182"/>
+      <c r="W22" s="188"/>
+      <c r="X22" s="188"/>
+      <c r="Y22" s="188"/>
+      <c r="Z22" s="188"/>
+      <c r="AA22" s="188"/>
+      <c r="AB22" s="189"/>
       <c r="AD22" s="7" t="s">
         <v>629</v>
       </c>
@@ -6403,10 +6419,10 @@
         <v>303</v>
       </c>
       <c r="AA23" s="119" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="AB23" s="119" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="AD23" s="7" t="s">
         <v>631</v>
@@ -6463,13 +6479,13 @@
         <v>437</v>
       </c>
       <c r="R24" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="S24" s="9" t="s">
         <v>69</v>
       </c>
       <c r="T24" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="V24" s="39" t="s">
         <v>674</v>
@@ -6792,33 +6808,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="179" t="s">
+      <c r="B31" s="177" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="179"/>
-      <c r="D31" s="179"/>
-      <c r="E31" s="179"/>
-      <c r="F31" s="179"/>
-      <c r="G31" s="179"/>
-      <c r="H31" s="179"/>
-      <c r="J31" s="179" t="s">
+      <c r="C31" s="177"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="177"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="177"/>
+      <c r="H31" s="177"/>
+      <c r="J31" s="177" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="179"/>
-      <c r="L31" s="179"/>
-      <c r="M31" s="179"/>
-      <c r="N31" s="179"/>
-      <c r="O31" s="179"/>
-      <c r="P31" s="179"/>
-      <c r="T31" s="179" t="s">
+      <c r="K31" s="177"/>
+      <c r="L31" s="177"/>
+      <c r="M31" s="177"/>
+      <c r="N31" s="177"/>
+      <c r="O31" s="177"/>
+      <c r="P31" s="177"/>
+      <c r="T31" s="177" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="179"/>
-      <c r="V31" s="179"/>
-      <c r="W31" s="179"/>
-      <c r="X31" s="179"/>
-      <c r="Y31" s="179"/>
-      <c r="Z31" s="179"/>
+      <c r="U31" s="177"/>
+      <c r="V31" s="177"/>
+      <c r="W31" s="177"/>
+      <c r="X31" s="177"/>
+      <c r="Y31" s="177"/>
+      <c r="Z31" s="177"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -7033,7 +7049,7 @@
         <v>699</v>
       </c>
       <c r="AJ34" s="158" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="35" spans="2:36">
@@ -7100,7 +7116,7 @@
       <c r="Z35" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AD35" s="177" t="s">
+      <c r="AD35" s="185" t="s">
         <v>700</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -7110,7 +7126,7 @@
         <v>309100</v>
       </c>
       <c r="AG35" s="7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="AH35" s="7" t="s">
         <v>697</v>
@@ -7119,7 +7135,7 @@
         <v>12</v>
       </c>
       <c r="AJ35" s="38" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="36" spans="2:36">
@@ -7186,7 +7202,7 @@
       <c r="Z36" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD36" s="177"/>
+      <c r="AD36" s="185"/>
       <c r="AE36" s="7"/>
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
@@ -7258,7 +7274,7 @@
       <c r="Z37" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD37" s="177"/>
+      <c r="AD37" s="185"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7315,7 +7331,7 @@
       <c r="Z38" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="AD38" s="177"/>
+      <c r="AD38" s="185"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7330,15 +7346,15 @@
       <c r="F39" t="s">
         <v>567</v>
       </c>
-      <c r="J39" s="186" t="s">
+      <c r="J39" s="178" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="186"/>
-      <c r="L39" s="186"/>
-      <c r="M39" s="186"/>
-      <c r="N39" s="186"/>
-      <c r="O39" s="186"/>
-      <c r="P39" s="186"/>
+      <c r="K39" s="178"/>
+      <c r="L39" s="178"/>
+      <c r="M39" s="178"/>
+      <c r="N39" s="178"/>
+      <c r="O39" s="178"/>
+      <c r="P39" s="178"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7561,16 +7577,16 @@
         <v>101</v>
       </c>
       <c r="F48" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="J48" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L48" s="176">
         <v>65.599999999999994</v>
       </c>
       <c r="M48" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
@@ -7585,16 +7601,16 @@
         <v>90</v>
       </c>
       <c r="F49" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="J49" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L49" s="176">
         <v>65.7</v>
       </c>
       <c r="M49" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="T49" s="7" t="s">
         <v>694</v>
@@ -7621,16 +7637,16 @@
         <v>126</v>
       </c>
       <c r="F50" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="J50" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L50" s="176">
         <v>65.8</v>
       </c>
       <c r="M50" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="T50" s="7" t="s">
         <v>695</v>
@@ -7654,13 +7670,13 @@
     </row>
     <row r="51" spans="5:26">
       <c r="J51" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L51" s="176">
         <v>65.900000000000006</v>
       </c>
       <c r="M51" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="T51" s="7" t="s">
         <v>696</v>
@@ -7684,13 +7700,13 @@
     </row>
     <row r="52" spans="5:26">
       <c r="J52" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L52" s="176">
         <v>66</v>
       </c>
       <c r="M52" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
@@ -7712,68 +7728,61 @@
     </row>
     <row r="53" spans="5:26">
       <c r="J53" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L53" s="176">
         <v>66.099999999999994</v>
       </c>
       <c r="M53" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="54" spans="5:26">
       <c r="J54" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L54" s="176">
         <v>66.2</v>
       </c>
       <c r="M54" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="55" spans="5:26">
       <c r="J55" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L55" s="176">
         <v>66.300000000000097</v>
       </c>
       <c r="M55" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="56" spans="5:26">
       <c r="J56" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L56" s="176">
         <v>66.400000000000105</v>
       </c>
       <c r="M56" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="57" spans="5:26">
       <c r="J57" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="L57" s="176">
         <v>66.500000000000099</v>
       </c>
       <c r="M57" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7783,6 +7792,13 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8194,7 +8210,7 @@
         <v>348</v>
       </c>
       <c r="N21" s="243" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="O21" s="243"/>
       <c r="P21" s="243"/>
@@ -8439,7 +8455,7 @@
         <v>126</v>
       </c>
       <c r="R29" s="43" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="18.75">
@@ -8484,7 +8500,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="243" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="B1" s="243"/>
       <c r="C1" s="243"/>
@@ -8535,7 +8551,7 @@
         <v>101</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75">
@@ -8546,7 +8562,7 @@
         <v>635</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="E6" s="43" t="s">
         <v>658</v>
@@ -8560,7 +8576,7 @@
         <v>634</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="E7" s="43" t="s">
         <v>655</v>
@@ -8574,7 +8590,7 @@
         <v>633</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>508</v>
@@ -8588,7 +8604,7 @@
         <v>382</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>375</v>
@@ -8619,10 +8635,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W66"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8633,64 +8649,64 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="155" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B1" s="155" t="s">
+        <v>731</v>
+      </c>
+      <c r="C1" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="D1" s="155" t="s">
         <v>732</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="E1" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="G1" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="H1" s="155" t="s">
         <v>731</v>
       </c>
-      <c r="D1" s="155" t="s">
+      <c r="I1" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="J1" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="K1" s="155" t="s">
         <v>733</v>
       </c>
-      <c r="E1" s="155" t="s">
+      <c r="M1" s="155" t="s">
         <v>734</v>
       </c>
-      <c r="G1" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="H1" s="155" t="s">
+      <c r="N1" s="155" t="s">
+        <v>731</v>
+      </c>
+      <c r="O1" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="P1" s="155" t="s">
         <v>732</v>
       </c>
-      <c r="I1" s="155" t="s">
+      <c r="Q1" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="S1" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="T1" s="155" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="155" t="s">
+      <c r="U1" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="V1" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="W1" s="155" t="s">
         <v>733</v>
-      </c>
-      <c r="K1" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="M1" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="N1" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="O1" s="155" t="s">
-        <v>731</v>
-      </c>
-      <c r="P1" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q1" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="S1" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="T1" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="U1" s="155" t="s">
-        <v>731</v>
-      </c>
-      <c r="V1" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="W1" s="155" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -8704,13 +8720,13 @@
         <v>411</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>730</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>739</v>
+        <v>885</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -8722,10 +8738,10 @@
         <v>449</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>740</v>
+        <v>753</v>
       </c>
       <c r="N2" s="7">
         <v>1</v>
@@ -8737,35 +8753,37 @@
         <v>387</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>755</v>
-      </c>
-      <c r="T2" s="7">
+        <v>729</v>
+      </c>
+      <c r="S2" s="66" t="s">
+        <v>753</v>
+      </c>
+      <c r="T2" s="66">
         <v>1</v>
       </c>
-      <c r="U2" s="7">
+      <c r="U2" s="66">
         <v>611</v>
       </c>
-      <c r="V2" s="7" t="s">
-        <v>754</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>730</v>
+      <c r="V2" s="66" t="s">
+        <v>752</v>
+      </c>
+      <c r="W2" s="66" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
       <c r="C3" s="7">
         <v>412</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -8776,7 +8794,7 @@
         <v>449</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -8787,31 +8805,33 @@
         <v>387</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7">
+        <v>729</v>
+      </c>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66">
         <v>612</v>
       </c>
-      <c r="V3" s="7" t="s">
-        <v>754</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>730</v>
+      <c r="V3" s="66" t="s">
+        <v>752</v>
+      </c>
+      <c r="W3" s="66" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
       <c r="C4" s="7">
         <v>413</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -8822,7 +8842,7 @@
         <v>449</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -8833,31 +8853,33 @@
         <v>387</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7">
+        <v>729</v>
+      </c>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66">
         <v>613</v>
       </c>
-      <c r="V4" s="7" t="s">
-        <v>754</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>730</v>
+      <c r="V4" s="66" t="s">
+        <v>752</v>
+      </c>
+      <c r="W4" s="66" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
       <c r="C5" s="7">
         <v>414</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -8868,7 +8890,7 @@
         <v>449</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -8879,23 +8901,23 @@
         <v>387</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7">
+        <v>729</v>
+      </c>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66">
         <v>614</v>
       </c>
-      <c r="V5" s="7" t="s">
-        <v>754</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>730</v>
+      <c r="V5" s="66" t="s">
+        <v>752</v>
+      </c>
+      <c r="W5" s="66" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="7" t="s">
-        <v>728</v>
+        <v>881</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
@@ -8904,13 +8926,13 @@
         <v>421</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>730</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>739</v>
+        <v>886</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
@@ -8922,10 +8944,10 @@
         <v>449</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>740</v>
+        <v>753</v>
       </c>
       <c r="N6" s="7">
         <v>2</v>
@@ -8937,20 +8959,22 @@
         <v>387</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
       <c r="C7" s="7">
         <v>422</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -8961,7 +8985,7 @@
         <v>449</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -8972,20 +8996,22 @@
         <v>387</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
       <c r="C8" s="7">
         <v>423</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -8996,7 +9022,7 @@
         <v>449</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -9007,20 +9033,22 @@
         <v>387</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
       <c r="C9" s="7">
         <v>424</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -9031,7 +9059,7 @@
         <v>449</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -9042,12 +9070,12 @@
         <v>387</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
-        <v>728</v>
+        <v>882</v>
       </c>
       <c r="B10" s="7">
         <v>3</v>
@@ -9056,13 +9084,13 @@
         <v>431</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>730</v>
-      </c>
       <c r="G10" s="7" t="s">
-        <v>739</v>
+        <v>887</v>
       </c>
       <c r="H10" s="7">
         <v>3</v>
@@ -9074,35 +9102,27 @@
         <v>449</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>740</v>
-      </c>
-      <c r="N10" s="7">
-        <v>3</v>
-      </c>
-      <c r="O10" s="7">
-        <v>231</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>645</v>
-      </c>
+        <v>729</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="7">
+        <v>3</v>
+      </c>
       <c r="C11" s="7">
         <v>432</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -9113,31 +9133,27 @@
         <v>449</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="7">
-        <v>232</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7">
+        <v>3</v>
+      </c>
       <c r="C12" s="7">
         <v>433</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -9148,31 +9164,27 @@
         <v>449</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7">
-        <v>233</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>3</v>
+      </c>
       <c r="C13" s="7">
         <v>434</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -9183,23 +9195,17 @@
         <v>449</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="7">
-        <v>234</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="7" t="s">
-        <v>728</v>
+        <v>414</v>
       </c>
       <c r="B14" s="7">
         <v>4</v>
@@ -9208,13 +9214,13 @@
         <v>441</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>645</v>
-      </c>
       <c r="G14" s="7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="H14" s="7">
         <v>4</v>
@@ -9226,35 +9232,27 @@
         <v>449</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>645</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>740</v>
-      </c>
-      <c r="N14" s="7">
-        <v>4</v>
-      </c>
-      <c r="O14" s="7">
-        <v>241</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q14" s="7" t="s">
-        <v>853</v>
-      </c>
+        <v>729</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7">
+        <v>4</v>
+      </c>
       <c r="C15" s="7">
         <v>442</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>645</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -9265,31 +9263,27 @@
         <v>449</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>645</v>
+        <v>729</v>
       </c>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="O15" s="7">
-        <v>242</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>853</v>
-      </c>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
       <c r="C16" s="7">
         <v>443</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>645</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -9300,31 +9294,27 @@
         <v>449</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>645</v>
+        <v>729</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="7">
-        <v>243</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q16" s="7" t="s">
-        <v>853</v>
-      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7">
+        <v>4</v>
+      </c>
       <c r="C17" s="7">
         <v>444</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>645</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -9335,23 +9325,17 @@
         <v>449</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>645</v>
+        <v>729</v>
       </c>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="7">
-        <v>244</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>853</v>
-      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="7" t="s">
-        <v>840</v>
+        <v>883</v>
       </c>
       <c r="B18" s="7">
         <v>5</v>
@@ -9360,102 +9344,80 @@
         <v>451</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="H18" s="7">
-        <v>5</v>
-      </c>
-      <c r="I18" s="7">
-        <v>151</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="7">
+        <v>5</v>
+      </c>
       <c r="C19" s="7">
         <v>452</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="7">
-        <v>152</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
       <c r="C20" s="7">
         <v>453</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="7">
-        <v>153</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="7">
+        <v>5</v>
+      </c>
       <c r="C21" s="7">
         <v>454</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="7">
-        <v>154</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="7" t="s">
-        <v>696</v>
+        <v>884</v>
       </c>
       <c r="B22" s="7">
         <v>6</v>
@@ -9464,317 +9426,251 @@
         <v>461</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="H22" s="7">
-        <v>6</v>
-      </c>
-      <c r="I22" s="7">
-        <v>161</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="7">
+        <v>6</v>
+      </c>
       <c r="C23" s="7">
         <v>462</v>
       </c>
       <c r="D23" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="7">
-        <v>162</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7">
+        <v>6</v>
+      </c>
       <c r="C24" s="7">
         <v>463</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7">
-        <v>163</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7">
+        <v>6</v>
+      </c>
       <c r="C25" s="7">
         <v>464</v>
       </c>
       <c r="D25" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="7">
-        <v>164</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="G26" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="H26" s="7">
-        <v>7</v>
-      </c>
-      <c r="I26" s="7">
-        <v>171</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:17">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="7">
-        <v>172</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:17">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="7">
-        <v>173</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7">
-        <v>174</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="G29" s="254"/>
+      <c r="H29" s="254"/>
+      <c r="I29" s="254"/>
+      <c r="J29" s="254"/>
+      <c r="K29" s="254"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="G30" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="H30" s="7">
-        <v>8</v>
-      </c>
-      <c r="I30" s="7">
-        <v>181</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7">
-        <v>182</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7">
-        <v>183</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
     </row>
     <row r="33" spans="1:17">
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7">
-        <v>184</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>730</v>
-      </c>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="G34" s="7" t="s">
-        <v>739</v>
-      </c>
-      <c r="H34" s="7">
-        <v>9</v>
-      </c>
-      <c r="I34" s="7">
-        <v>191</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7">
-        <v>192</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7">
-        <v>193</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7">
-        <v>194</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>645</v>
-      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="155" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B39" s="155" t="s">
+        <v>731</v>
+      </c>
+      <c r="C39" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="D39" s="155" t="s">
         <v>732</v>
       </c>
-      <c r="C39" s="155" t="s">
+      <c r="E39" s="155" t="s">
+        <v>733</v>
+      </c>
+      <c r="G39" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="H39" s="155" t="s">
         <v>731</v>
       </c>
-      <c r="D39" s="155" t="s">
+      <c r="I39" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="J39" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="K39" s="155" t="s">
         <v>733</v>
       </c>
-      <c r="E39" s="155" t="s">
+      <c r="M39" s="155" t="s">
         <v>734</v>
       </c>
-      <c r="G39" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="H39" s="155" t="s">
+      <c r="N39" s="155" t="s">
+        <v>731</v>
+      </c>
+      <c r="O39" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="P39" s="155" t="s">
         <v>732</v>
       </c>
-      <c r="I39" s="155" t="s">
-        <v>731</v>
-      </c>
-      <c r="J39" s="155" t="s">
+      <c r="Q39" s="155" t="s">
         <v>733</v>
-      </c>
-      <c r="K39" s="155" t="s">
-        <v>734</v>
-      </c>
-      <c r="M39" s="155" t="s">
-        <v>735</v>
-      </c>
-      <c r="N39" s="155" t="s">
-        <v>732</v>
-      </c>
-      <c r="O39" s="155" t="s">
-        <v>731</v>
-      </c>
-      <c r="P39" s="155" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q39" s="155" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="7" t="s">
-        <v>756</v>
+        <v>888</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
@@ -9783,13 +9679,13 @@
         <v>311</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="H40" s="7">
         <v>1</v>
@@ -9801,21 +9697,21 @@
         <v>601</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>848</v>
-      </c>
-      <c r="N40" s="7">
+        <v>729</v>
+      </c>
+      <c r="M40" s="66" t="s">
+        <v>845</v>
+      </c>
+      <c r="N40" s="66">
         <v>1</v>
       </c>
-      <c r="O40" s="7">
+      <c r="O40" s="66">
         <v>711</v>
       </c>
-      <c r="P40" s="7" t="s">
-        <v>847</v>
-      </c>
-      <c r="Q40" s="7" t="s">
+      <c r="P40" s="66" t="s">
+        <v>844</v>
+      </c>
+      <c r="Q40" s="66" t="s">
         <v>638</v>
       </c>
     </row>
@@ -9826,10 +9722,10 @@
         <v>312</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -9840,11 +9736,15 @@
         <v>601</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="O41">
+        <v>729</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2">
         <v>712</v>
       </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="7"/>
@@ -9853,10 +9753,10 @@
         <v>313</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
@@ -9867,11 +9767,15 @@
         <v>601</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="O42">
+        <v>729</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2">
         <v>713</v>
       </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="7"/>
@@ -9880,10 +9784,10 @@
         <v>314</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -9894,15 +9798,19 @@
         <v>601</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="O43">
+        <v>729</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2">
         <v>714</v>
       </c>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="7" t="s">
-        <v>756</v>
+        <v>889</v>
       </c>
       <c r="B44" s="7">
         <v>2</v>
@@ -9911,13 +9819,13 @@
         <v>321</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>833</v>
+        <v>754</v>
       </c>
       <c r="H44" s="7">
         <v>2</v>
@@ -9929,7 +9837,7 @@
         <v>601</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -9939,10 +9847,10 @@
         <v>322</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
@@ -9953,7 +9861,7 @@
         <v>601</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -9963,10 +9871,10 @@
         <v>323</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -9977,7 +9885,7 @@
         <v>601</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -9987,10 +9895,10 @@
         <v>324</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>758</v>
+        <v>729</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -10000,171 +9908,180 @@
       <c r="J47" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="K47" s="7" t="s">
-        <v>758</v>
+      <c r="K47" s="254" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="66" t="s">
+        <v>754</v>
+      </c>
+      <c r="B48" s="66">
+        <v>3</v>
+      </c>
+      <c r="C48" s="66">
+        <v>331</v>
+      </c>
+      <c r="D48" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E48" s="66" t="s">
         <v>756</v>
       </c>
-      <c r="B48" s="7">
+      <c r="K48" s="18"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="66"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66">
+        <v>332</v>
+      </c>
+      <c r="D49" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E49" s="66" t="s">
+        <v>756</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="66"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="66">
+        <v>333</v>
+      </c>
+      <c r="D50" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E50" s="66" t="s">
+        <v>756</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="H50" s="2">
         <v>3</v>
       </c>
-      <c r="C48" s="7">
-        <v>331</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7">
-        <v>332</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7">
-        <v>333</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="G50" t="s">
-        <v>858</v>
-      </c>
-      <c r="H50">
-        <v>3</v>
-      </c>
-      <c r="I50">
+      <c r="I50" s="2">
         <v>631</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="K50" t="s">
-        <v>859</v>
+      <c r="K50" s="2" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7">
+      <c r="A51" s="66"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66">
         <v>334</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="G51" t="s">
-        <v>858</v>
-      </c>
-      <c r="I51">
+      <c r="D51" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E51" s="66" t="s">
+        <v>756</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2">
         <v>632</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="K51" t="s">
-        <v>859</v>
+      <c r="K51" s="2" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="66" t="s">
+        <v>754</v>
+      </c>
+      <c r="B52" s="66">
+        <v>4</v>
+      </c>
+      <c r="C52" s="66">
+        <v>341</v>
+      </c>
+      <c r="D52" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E52" s="66" t="s">
         <v>756</v>
       </c>
-      <c r="B52" s="7">
-        <v>4</v>
-      </c>
-      <c r="C52" s="7">
-        <v>341</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="G52" t="s">
-        <v>858</v>
-      </c>
-      <c r="I52">
+      <c r="G52" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2">
         <v>633</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="K52" t="s">
-        <v>859</v>
+      <c r="K52" s="2" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7">
+      <c r="A53" s="66"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="66">
         <v>342</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>758</v>
-      </c>
-      <c r="G53" t="s">
-        <v>858</v>
-      </c>
-      <c r="I53">
+      <c r="D53" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E53" s="66" t="s">
+        <v>756</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2">
         <v>634</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="K53" t="s">
-        <v>859</v>
+      <c r="K53" s="2" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7">
+      <c r="A54" s="66"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="66">
         <v>343</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>758</v>
+      <c r="D54" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E54" s="66" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7">
+      <c r="A55" s="66"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="66">
         <v>344</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>757</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>758</v>
+      <c r="D55" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E55" s="66" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -10173,60 +10090,19 @@
       <c r="E56" s="159"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" t="s">
-        <v>756</v>
-      </c>
-      <c r="B57">
-        <v>5</v>
-      </c>
-      <c r="C57" s="159">
-        <v>351</v>
-      </c>
-      <c r="D57" s="159" t="s">
-        <v>757</v>
-      </c>
-      <c r="E57" s="159" t="s">
-        <v>859</v>
-      </c>
+      <c r="C57" s="159"/>
+      <c r="D57" s="159"/>
+      <c r="E57" s="159"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" t="s">
-        <v>756</v>
-      </c>
-      <c r="B61">
-        <v>6</v>
-      </c>
-      <c r="C61" s="159">
-        <v>361</v>
-      </c>
-      <c r="D61" s="159" t="s">
-        <v>757</v>
-      </c>
-      <c r="E61" s="159" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>756</v>
-      </c>
-      <c r="B65">
-        <v>7</v>
-      </c>
-      <c r="C65" s="159">
-        <v>351</v>
-      </c>
-      <c r="D65" s="159" t="s">
-        <v>757</v>
-      </c>
-      <c r="E65" s="159" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="C66">
-        <v>371</v>
-      </c>
+      <c r="C61" s="159"/>
+      <c r="D61" s="159"/>
+      <c r="E61" s="159"/>
+    </row>
+    <row r="65" spans="3:5">
+      <c r="C65" s="159"/>
+      <c r="D65" s="159"/>
+      <c r="E65" s="159"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -10257,7 +10133,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="250" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B1" s="251"/>
       <c r="C1" s="251"/>
@@ -10285,7 +10161,7 @@
       <c r="C3" s="246"/>
       <c r="D3" s="246"/>
       <c r="E3" s="246" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F3" s="246"/>
       <c r="G3" s="246"/>
@@ -10725,13 +10601,13 @@
     </row>
     <row r="22" spans="1:8" ht="19.5">
       <c r="A22" s="248" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="B22" s="249"/>
       <c r="C22" s="249"/>
       <c r="D22" s="249"/>
       <c r="E22" s="248" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="F22" s="249"/>
       <c r="G22" s="249"/>
@@ -10745,10 +10621,10 @@
         <v>65.599999999999994</v>
       </c>
       <c r="C23" s="167" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="D23" s="167" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="E23" s="164">
         <v>1</v>
@@ -10757,7 +10633,7 @@
         <v>21</v>
       </c>
       <c r="G23" s="167" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="H23" s="174" t="s">
         <v>3</v>
@@ -10771,10 +10647,10 @@
         <v>65.7</v>
       </c>
       <c r="C24" s="169" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D24" s="169" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="E24" s="164">
         <v>2</v>
@@ -10791,10 +10667,10 @@
         <v>65.8</v>
       </c>
       <c r="C25" s="169" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="D25" s="169" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="E25" s="164">
         <v>3</v>
@@ -10811,10 +10687,10 @@
         <v>65.900000000000006</v>
       </c>
       <c r="C26" s="169" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="D26" s="169" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="E26" s="164">
         <v>4</v>
@@ -10831,10 +10707,10 @@
         <v>66</v>
       </c>
       <c r="C27" s="169" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D27" s="169" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="E27" s="164">
         <v>5</v>
@@ -10851,10 +10727,10 @@
         <v>66.099999999999994</v>
       </c>
       <c r="C28" s="169" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D28" s="169" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="E28" s="164">
         <v>6</v>
@@ -10871,10 +10747,10 @@
         <v>66.2</v>
       </c>
       <c r="C29" s="169" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="D29" s="169" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="E29" s="164">
         <v>7</v>
@@ -10891,10 +10767,10 @@
         <v>66.300000000000097</v>
       </c>
       <c r="C30" s="169" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="D30" s="169" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="E30" s="164">
         <v>8</v>
@@ -10911,10 +10787,10 @@
         <v>66.400000000000105</v>
       </c>
       <c r="C31" s="170" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D31" s="170" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="E31" s="164">
         <v>9</v>
@@ -10931,10 +10807,10 @@
         <v>66.500000000000099</v>
       </c>
       <c r="C32" s="170" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D32" s="170" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="E32" s="164">
         <v>10</v>
@@ -10954,7 +10830,7 @@
         <v>523</v>
       </c>
       <c r="D33" s="175" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="E33" s="164">
         <v>11</v>
@@ -10974,7 +10850,7 @@
         <v>463</v>
       </c>
       <c r="D34" s="175" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="E34" s="164">
         <v>12</v>
@@ -10994,7 +10870,7 @@
         <v>466</v>
       </c>
       <c r="D35" s="175" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="E35" s="164">
         <v>13</v>
@@ -11014,7 +10890,7 @@
         <v>467</v>
       </c>
       <c r="D36" s="175" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="E36" s="164">
         <v>14</v>
@@ -11034,7 +10910,7 @@
         <v>469</v>
       </c>
       <c r="D37" s="175" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="E37" s="164">
         <v>15</v>
@@ -11054,7 +10930,7 @@
         <v>471</v>
       </c>
       <c r="D38" s="175" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="E38" s="164">
         <v>16</v>
@@ -11074,7 +10950,7 @@
         <v>473</v>
       </c>
       <c r="D39" s="175" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="E39" s="164">
         <v>17</v>
@@ -12576,7 +12452,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="208" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B1" s="208"/>
       <c r="C1" s="208"/>
@@ -12831,7 +12707,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="117" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>503</v>
@@ -12853,7 +12729,7 @@
         <v>20</v>
       </c>
       <c r="F13" s="117" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>649</v>
@@ -13690,7 +13566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -13706,7 +13582,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="210" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B1" s="210"/>
       <c r="C1" s="210"/>
@@ -13794,7 +13670,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G5" s="30" t="str">
         <f>[1]Frequencies!T14</f>
@@ -13807,7 +13683,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C6" s="30" t="str">
         <f>[1]Frequencies!T4</f>
@@ -13883,7 +13759,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C9" s="30" t="str">
         <f>[1]Frequencies!T7</f>
@@ -13908,7 +13784,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C10" s="30" t="str">
         <f>[1]Frequencies!T12</f>
@@ -13933,7 +13809,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C11" s="30" t="str">
         <f>[1]Frequencies!T16</f>
@@ -13958,7 +13834,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="124" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C12" s="30" t="str">
         <f>[1]Frequencies!T11</f>
@@ -14379,7 +14255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -14400,7 +14276,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="199" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B1" s="200"/>
       <c r="C1" s="200"/>
@@ -14773,7 +14649,7 @@
       </c>
       <c r="C17" s="75"/>
       <c r="D17" s="75" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E17" s="74">
         <v>14</v>
@@ -14797,7 +14673,7 @@
       </c>
       <c r="C18" s="75"/>
       <c r="D18" s="75" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E18" s="74">
         <v>15</v>
@@ -14821,7 +14697,7 @@
       </c>
       <c r="C19" s="75"/>
       <c r="D19" s="75" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E19" s="74">
         <v>16</v>
@@ -14847,7 +14723,7 @@
         <v>652</v>
       </c>
       <c r="D20" s="156" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E20" s="74">
         <v>17</v>
@@ -14873,7 +14749,7 @@
         <v>653</v>
       </c>
       <c r="D21" s="156" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E21" s="74">
         <v>18</v>
@@ -14897,7 +14773,7 @@
         <v>654</v>
       </c>
       <c r="D22" s="156" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="E22" s="74">
         <v>19</v>
@@ -14915,21 +14791,21 @@
         <v>20</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C23" s="73"/>
       <c r="D23" s="73" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E23" s="74">
         <v>20</v>
       </c>
       <c r="F23" s="73" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="G23" s="73"/>
       <c r="H23" s="73" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18.75" thickBot="1">
@@ -14977,7 +14853,7 @@
       </c>
       <c r="G26" s="73"/>
       <c r="H26" s="75" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
@@ -15057,7 +14933,7 @@
       </c>
       <c r="G31" s="73"/>
       <c r="H31" s="73" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
@@ -15073,7 +14949,7 @@
       </c>
       <c r="G32" s="73"/>
       <c r="H32" s="73" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18.75" thickBot="1">
@@ -15089,7 +14965,7 @@
       </c>
       <c r="G33" s="73"/>
       <c r="H33" s="75" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -15107,7 +14983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -15125,40 +15001,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="235" t="s">
-        <v>832</v>
-      </c>
-      <c r="B1" s="235"/>
-      <c r="C1" s="235"/>
-      <c r="D1" s="235"/>
-      <c r="E1" s="235"/>
-      <c r="F1" s="235"/>
-      <c r="G1" s="235"/>
-      <c r="H1" s="235"/>
+      <c r="A1" s="218" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="236"/>
-      <c r="B2" s="236"/>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
+      <c r="A2" s="219"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="237" t="s">
+      <c r="A3" s="220" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="238"/>
-      <c r="C3" s="239"/>
-      <c r="D3" s="240"/>
-      <c r="E3" s="237" t="s">
+      <c r="B3" s="221"/>
+      <c r="C3" s="222"/>
+      <c r="D3" s="223"/>
+      <c r="E3" s="220" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="238"/>
-      <c r="G3" s="239"/>
-      <c r="H3" s="240"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="223"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -15177,13 +15053,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="130" t="s">
+        <v>757</v>
+      </c>
+      <c r="G4" s="131" t="s">
+        <v>758</v>
+      </c>
+      <c r="H4" s="132" t="s">
         <v>759</v>
-      </c>
-      <c r="G4" s="131" t="s">
-        <v>760</v>
-      </c>
-      <c r="H4" s="132" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -15203,13 +15079,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="138" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G5" s="139" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H5" s="140" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
@@ -15229,13 +15105,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="134" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="G6" s="135" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H6" s="142" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
@@ -15255,13 +15131,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="138" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G7" s="139" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H7" s="140" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -15281,13 +15157,13 @@
         <v>5</v>
       </c>
       <c r="F8" s="134" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="G8" s="135" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H8" s="142" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
@@ -15365,7 +15241,7 @@
         <v>556</v>
       </c>
       <c r="H11" s="140" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
@@ -15417,7 +15293,7 @@
         <v>484</v>
       </c>
       <c r="H13" s="140" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -15437,13 +15313,13 @@
         <v>11</v>
       </c>
       <c r="F14" s="134" t="s">
+        <v>770</v>
+      </c>
+      <c r="G14" s="135" t="s">
+        <v>771</v>
+      </c>
+      <c r="H14" s="142" t="s">
         <v>772</v>
-      </c>
-      <c r="G14" s="135" t="s">
-        <v>773</v>
-      </c>
-      <c r="H14" s="142" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
@@ -15466,10 +15342,10 @@
         <v>205</v>
       </c>
       <c r="G15" s="139" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="H15" s="140" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
@@ -15489,11 +15365,11 @@
         <v>13</v>
       </c>
       <c r="F16" s="134" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G16" s="135"/>
       <c r="H16" s="142" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -15513,11 +15389,11 @@
         <v>14</v>
       </c>
       <c r="F17" s="138" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G17" s="139"/>
       <c r="H17" s="140" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18">
@@ -15557,7 +15433,7 @@
         <v>652</v>
       </c>
       <c r="D19" s="143" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E19" s="137">
         <v>16</v>
@@ -15583,7 +15459,7 @@
         <v>653</v>
       </c>
       <c r="D20" s="144" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E20" s="133">
         <v>17</v>
@@ -15609,7 +15485,7 @@
         <v>654</v>
       </c>
       <c r="D21" s="143" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E21" s="137">
         <v>18</v>
@@ -15629,13 +15505,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="138" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C22" s="139" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D22" s="141" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E22" s="133">
         <v>19</v>
@@ -15647,7 +15523,7 @@
         <v>485</v>
       </c>
       <c r="H22" s="142" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" thickBot="1">
@@ -15655,13 +15531,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="146" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C23" s="147" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D23" s="148" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E23" s="149">
         <v>20</v>
@@ -15673,7 +15549,7 @@
         <v>487</v>
       </c>
       <c r="H23" s="152" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1">
@@ -15687,356 +15563,327 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="237" t="s">
-        <v>788</v>
-      </c>
-      <c r="B25" s="238"/>
-      <c r="C25" s="239"/>
-      <c r="D25" s="240"/>
-      <c r="E25" s="237" t="s">
-        <v>789</v>
-      </c>
-      <c r="F25" s="238"/>
-      <c r="G25" s="239"/>
-      <c r="H25" s="240"/>
+      <c r="A25" s="220" t="s">
+        <v>786</v>
+      </c>
+      <c r="B25" s="221"/>
+      <c r="C25" s="222"/>
+      <c r="D25" s="223"/>
+      <c r="E25" s="220" t="s">
+        <v>787</v>
+      </c>
+      <c r="F25" s="221"/>
+      <c r="G25" s="222"/>
+      <c r="H25" s="223"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B26" s="224" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C26" s="225"/>
       <c r="D26" s="226"/>
       <c r="E26" s="125" t="s">
-        <v>792</v>
-      </c>
-      <c r="F26" s="232" t="s">
-        <v>793</v>
-      </c>
-      <c r="G26" s="233"/>
-      <c r="H26" s="234" t="s">
-        <v>761</v>
+        <v>790</v>
+      </c>
+      <c r="F26" s="227" t="s">
+        <v>791</v>
+      </c>
+      <c r="G26" s="228"/>
+      <c r="H26" s="229" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="137" t="s">
+        <v>792</v>
+      </c>
+      <c r="B27" s="230" t="s">
+        <v>793</v>
+      </c>
+      <c r="C27" s="231"/>
+      <c r="D27" s="232" t="s">
+        <v>623</v>
+      </c>
+      <c r="E27" s="129" t="s">
         <v>794</v>
       </c>
-      <c r="B27" s="227" t="s">
+      <c r="F27" s="224" t="s">
         <v>795</v>
       </c>
-      <c r="C27" s="228"/>
-      <c r="D27" s="230" t="s">
-        <v>623</v>
-      </c>
-      <c r="E27" s="129" t="s">
-        <v>796</v>
-      </c>
-      <c r="F27" s="224" t="s">
-        <v>797</v>
-      </c>
       <c r="G27" s="225"/>
-      <c r="H27" s="231" t="s">
-        <v>763</v>
+      <c r="H27" s="233" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="129" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B28" s="224" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C28" s="225"/>
       <c r="D28" s="226" t="s">
         <v>624</v>
       </c>
       <c r="E28" s="137" t="s">
-        <v>800</v>
-      </c>
-      <c r="F28" s="227" t="s">
-        <v>801</v>
-      </c>
-      <c r="G28" s="228"/>
-      <c r="H28" s="229" t="s">
-        <v>765</v>
+        <v>798</v>
+      </c>
+      <c r="F28" s="230" t="s">
+        <v>799</v>
+      </c>
+      <c r="G28" s="231"/>
+      <c r="H28" s="234" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="137" t="s">
+        <v>800</v>
+      </c>
+      <c r="B29" s="230" t="s">
+        <v>801</v>
+      </c>
+      <c r="C29" s="231"/>
+      <c r="D29" s="232" t="s">
+        <v>625</v>
+      </c>
+      <c r="E29" s="129" t="s">
         <v>802</v>
       </c>
-      <c r="B29" s="227" t="s">
+      <c r="F29" s="224" t="s">
         <v>803</v>
       </c>
-      <c r="C29" s="228"/>
-      <c r="D29" s="230" t="s">
-        <v>625</v>
-      </c>
-      <c r="E29" s="129" t="s">
-        <v>804</v>
-      </c>
-      <c r="F29" s="224" t="s">
-        <v>805</v>
-      </c>
       <c r="G29" s="225"/>
-      <c r="H29" s="231" t="s">
-        <v>767</v>
+      <c r="H29" s="233" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="129" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B30" s="224" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C30" s="225"/>
       <c r="D30" s="226" t="s">
         <v>626</v>
       </c>
       <c r="E30" s="137" t="s">
-        <v>808</v>
-      </c>
-      <c r="F30" s="227" t="s">
-        <v>809</v>
-      </c>
-      <c r="G30" s="228"/>
-      <c r="H30" s="229" t="s">
-        <v>769</v>
+        <v>806</v>
+      </c>
+      <c r="F30" s="230" t="s">
+        <v>807</v>
+      </c>
+      <c r="G30" s="231"/>
+      <c r="H30" s="234" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="137" t="s">
+        <v>808</v>
+      </c>
+      <c r="B31" s="230" t="s">
+        <v>809</v>
+      </c>
+      <c r="C31" s="231"/>
+      <c r="D31" s="232" t="s">
+        <v>627</v>
+      </c>
+      <c r="E31" s="129" t="s">
         <v>810</v>
       </c>
-      <c r="B31" s="227" t="s">
+      <c r="F31" s="224" t="s">
         <v>811</v>
       </c>
-      <c r="C31" s="228"/>
-      <c r="D31" s="230" t="s">
-        <v>627</v>
-      </c>
-      <c r="E31" s="129" t="s">
-        <v>812</v>
-      </c>
-      <c r="F31" s="224" t="s">
-        <v>813</v>
-      </c>
       <c r="G31" s="225"/>
-      <c r="H31" s="231" t="s">
+      <c r="H31" s="233" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="129" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B32" s="224" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C32" s="225"/>
       <c r="D32" s="226" t="s">
         <v>628</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="227"/>
-      <c r="G32" s="228"/>
-      <c r="H32" s="229" t="s">
+      <c r="F32" s="230"/>
+      <c r="G32" s="231"/>
+      <c r="H32" s="234" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18.75" thickBot="1">
       <c r="A33" s="137" t="s">
-        <v>816</v>
-      </c>
-      <c r="B33" s="227" t="s">
-        <v>817</v>
-      </c>
-      <c r="C33" s="228"/>
-      <c r="D33" s="230" t="s">
+        <v>814</v>
+      </c>
+      <c r="B33" s="230" t="s">
+        <v>815</v>
+      </c>
+      <c r="C33" s="231"/>
+      <c r="D33" s="232" t="s">
         <v>622</v>
       </c>
       <c r="E33" s="129"/>
       <c r="F33" s="224"/>
       <c r="G33" s="225"/>
-      <c r="H33" s="231" t="s">
-        <v>761</v>
+      <c r="H33" s="233" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18.75" thickBot="1">
       <c r="A34" s="129" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B34" s="224" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C34" s="225"/>
       <c r="D34" s="226" t="s">
         <v>623</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="227"/>
-      <c r="G34" s="228"/>
-      <c r="H34" s="229" t="s">
-        <v>763</v>
+      <c r="F34" s="230"/>
+      <c r="G34" s="231"/>
+      <c r="H34" s="234" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18.75" thickBot="1">
       <c r="A35" s="137" t="s">
-        <v>820</v>
-      </c>
-      <c r="B35" s="227" t="s">
-        <v>821</v>
-      </c>
-      <c r="C35" s="228"/>
-      <c r="D35" s="230" t="s">
+        <v>818</v>
+      </c>
+      <c r="B35" s="230" t="s">
+        <v>819</v>
+      </c>
+      <c r="C35" s="231"/>
+      <c r="D35" s="232" t="s">
         <v>624</v>
       </c>
       <c r="E35" s="129"/>
       <c r="F35" s="224"/>
       <c r="G35" s="225"/>
-      <c r="H35" s="231" t="s">
-        <v>765</v>
+      <c r="H35" s="233" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18.75" thickBot="1">
       <c r="A36" s="129" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B36" s="224" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C36" s="225"/>
       <c r="D36" s="226" t="s">
         <v>625</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="227"/>
-      <c r="G36" s="228"/>
-      <c r="H36" s="229" t="s">
-        <v>767</v>
+      <c r="F36" s="230"/>
+      <c r="G36" s="231"/>
+      <c r="H36" s="234" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" thickBot="1">
       <c r="A37" s="137" t="s">
-        <v>824</v>
-      </c>
-      <c r="B37" s="227" t="s">
-        <v>825</v>
-      </c>
-      <c r="C37" s="228"/>
-      <c r="D37" s="230" t="s">
+        <v>822</v>
+      </c>
+      <c r="B37" s="230" t="s">
+        <v>823</v>
+      </c>
+      <c r="C37" s="231"/>
+      <c r="D37" s="232" t="s">
         <v>626</v>
       </c>
       <c r="E37" s="129"/>
       <c r="F37" s="224"/>
       <c r="G37" s="225"/>
-      <c r="H37" s="231" t="s">
-        <v>769</v>
+      <c r="H37" s="233" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" thickBot="1">
       <c r="A38" s="129" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B38" s="224" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C38" s="225"/>
       <c r="D38" s="226" t="s">
         <v>627</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="227"/>
-      <c r="G38" s="228"/>
-      <c r="H38" s="229" t="s">
+      <c r="F38" s="230"/>
+      <c r="G38" s="231"/>
+      <c r="H38" s="234" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" thickBot="1">
       <c r="A39" s="137" t="s">
-        <v>828</v>
-      </c>
-      <c r="B39" s="227" t="s">
-        <v>829</v>
-      </c>
-      <c r="C39" s="228"/>
-      <c r="D39" s="230" t="s">
+        <v>826</v>
+      </c>
+      <c r="B39" s="230" t="s">
+        <v>827</v>
+      </c>
+      <c r="C39" s="231"/>
+      <c r="D39" s="232" t="s">
         <v>628</v>
       </c>
       <c r="E39" s="129"/>
       <c r="F39" s="224"/>
       <c r="G39" s="225"/>
-      <c r="H39" s="231" t="s">
+      <c r="H39" s="233" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" thickBot="1">
       <c r="A40" s="129" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B40" s="224" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C40" s="225"/>
       <c r="D40" s="226" t="s">
         <v>628</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="227"/>
-      <c r="G40" s="228"/>
-      <c r="H40" s="229"/>
+      <c r="F40" s="230"/>
+      <c r="G40" s="231"/>
+      <c r="H40" s="234"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
-        <v>831</v>
-      </c>
-      <c r="B41" s="218" t="s">
         <v>829</v>
       </c>
-      <c r="C41" s="219"/>
-      <c r="D41" s="220" t="s">
+      <c r="B41" s="235" t="s">
+        <v>827</v>
+      </c>
+      <c r="C41" s="236"/>
+      <c r="D41" s="237" t="s">
         <v>628</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="221"/>
-      <c r="G41" s="222"/>
-      <c r="H41" s="223"/>
+      <c r="F41" s="238"/>
+      <c r="G41" s="239"/>
+      <c r="H41" s="240"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -16045,6 +15892,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Updated AH64 presets and correcter carrier cycles
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="904">
   <si>
     <t>AWACS</t>
   </si>
@@ -2639,9 +2639,6 @@
     <t>309.80</t>
   </si>
   <si>
-    <t>AH-64D presets  (OPAR) V1.0</t>
-  </si>
-  <si>
     <t>VHF</t>
   </si>
   <si>
@@ -2654,9 +2651,6 @@
     <t>SLATE 1</t>
   </si>
   <si>
-    <t>OLIVE 11</t>
-  </si>
-  <si>
     <t>SLATE 2</t>
   </si>
   <si>
@@ -2733,6 +2727,54 @@
   </si>
   <si>
     <t>HORNET</t>
+  </si>
+  <si>
+    <t>Hatay</t>
+  </si>
+  <si>
+    <t>AH-64</t>
+  </si>
+  <si>
+    <t>GUNSLINGER</t>
+  </si>
+  <si>
+    <t>SABER</t>
+  </si>
+  <si>
+    <t>AWACS check-in</t>
+  </si>
+  <si>
+    <t>AWACS report net</t>
+  </si>
+  <si>
+    <t>WARRIOR secondary</t>
+  </si>
+  <si>
+    <t>SPARTAN secondary</t>
+  </si>
+  <si>
+    <t>HITMAN secondary</t>
+  </si>
+  <si>
+    <t>AWACS alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWACS CSAR </t>
+  </si>
+  <si>
+    <t>WARRIOR primary</t>
+  </si>
+  <si>
+    <t>SPARTAN primary</t>
+  </si>
+  <si>
+    <t>HITMAN primary</t>
+  </si>
+  <si>
+    <t>VHF back-up</t>
+  </si>
+  <si>
+    <t>AH-64D presets  (OPAR) V1.1</t>
   </si>
 </sst>
 </file>
@@ -2742,7 +2784,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2942,6 +2984,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -3703,7 +3751,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -3712,8 +3760,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -3728,7 +3778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4086,33 +4136,15 @@
     <xf numFmtId="0" fontId="19" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -4122,31 +4154,83 @@
     <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="17" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4156,21 +4240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4255,6 +4324,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4273,57 +4393,6 @@
     <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4336,34 +4405,69 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4406,7 +4510,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4892,7 +4996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AJ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
@@ -4944,11 +5048,11 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="186" t="s">
+      <c r="R3" s="185" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="186"/>
-      <c r="T3" s="186"/>
+      <c r="S3" s="185"/>
+      <c r="T3" s="185"/>
       <c r="AA3" s="187" t="s">
         <v>9</v>
       </c>
@@ -4998,7 +5102,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="179" t="s">
+      <c r="R4" s="190" t="s">
         <v>638</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -5007,12 +5111,12 @@
       <c r="T4" s="99" t="s">
         <v>641</v>
       </c>
-      <c r="V4" s="177" t="s">
+      <c r="V4" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="177"/>
-      <c r="X4" s="177"/>
-      <c r="Y4" s="177"/>
+      <c r="W4" s="186"/>
+      <c r="X4" s="186"/>
+      <c r="Y4" s="186"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -5066,7 +5170,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="180"/>
+      <c r="R5" s="191"/>
       <c r="S5" s="31" t="s">
         <v>607</v>
       </c>
@@ -5144,7 +5248,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="181"/>
+      <c r="R6" s="192"/>
       <c r="S6" s="100" t="s">
         <v>640</v>
       </c>
@@ -5220,7 +5324,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="179" t="s">
+      <c r="R7" s="190" t="s">
         <v>644</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5300,7 +5404,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="180"/>
+      <c r="R8" s="191"/>
       <c r="S8" s="31" t="s">
         <v>607</v>
       </c>
@@ -5369,7 +5473,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="181"/>
+      <c r="R9" s="192"/>
       <c r="S9" s="100" t="s">
         <v>640</v>
       </c>
@@ -5496,7 +5600,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="182" t="s">
+      <c r="R11" s="194" t="s">
         <v>645</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5569,7 +5673,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="183"/>
+      <c r="R12" s="195"/>
       <c r="S12" s="97" t="s">
         <v>607</v>
       </c>
@@ -5636,7 +5740,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="184"/>
+      <c r="R13" s="196"/>
       <c r="S13" s="105" t="s">
         <v>640</v>
       </c>
@@ -5710,7 +5814,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="179" t="s">
+      <c r="R14" s="190" t="s">
         <v>648</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5788,7 +5892,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="180"/>
+      <c r="R15" s="191"/>
       <c r="S15" s="97" t="s">
         <v>607</v>
       </c>
@@ -5849,22 +5953,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="181"/>
+      <c r="R16" s="192"/>
       <c r="S16" s="105" t="s">
         <v>640</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="V16" s="177" t="s">
+      <c r="V16" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="177"/>
-      <c r="X16" s="177"/>
-      <c r="Y16" s="177"/>
-      <c r="Z16" s="177"/>
-      <c r="AA16" s="177"/>
-      <c r="AB16" s="177"/>
+      <c r="W16" s="186"/>
+      <c r="X16" s="186"/>
+      <c r="Y16" s="186"/>
+      <c r="Z16" s="186"/>
+      <c r="AA16" s="186"/>
+      <c r="AB16" s="186"/>
       <c r="AD16" s="7" t="s">
         <v>623</v>
       </c>
@@ -6156,11 +6260,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="177" t="s">
+      <c r="R20" s="186" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="177"/>
-      <c r="T20" s="177"/>
+      <c r="S20" s="186"/>
+      <c r="T20" s="186"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>672</v>
@@ -6808,33 +6912,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="177" t="s">
+      <c r="B31" s="186" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="177"/>
-      <c r="D31" s="177"/>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
-      <c r="H31" s="177"/>
-      <c r="J31" s="177" t="s">
+      <c r="C31" s="186"/>
+      <c r="D31" s="186"/>
+      <c r="E31" s="186"/>
+      <c r="F31" s="186"/>
+      <c r="G31" s="186"/>
+      <c r="H31" s="186"/>
+      <c r="J31" s="186" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="177"/>
-      <c r="L31" s="177"/>
-      <c r="M31" s="177"/>
-      <c r="N31" s="177"/>
-      <c r="O31" s="177"/>
-      <c r="P31" s="177"/>
-      <c r="T31" s="177" t="s">
+      <c r="K31" s="186"/>
+      <c r="L31" s="186"/>
+      <c r="M31" s="186"/>
+      <c r="N31" s="186"/>
+      <c r="O31" s="186"/>
+      <c r="P31" s="186"/>
+      <c r="T31" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="177"/>
-      <c r="V31" s="177"/>
-      <c r="W31" s="177"/>
-      <c r="X31" s="177"/>
-      <c r="Y31" s="177"/>
-      <c r="Z31" s="177"/>
+      <c r="U31" s="186"/>
+      <c r="V31" s="186"/>
+      <c r="W31" s="186"/>
+      <c r="X31" s="186"/>
+      <c r="Y31" s="186"/>
+      <c r="Z31" s="186"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -7116,7 +7220,7 @@
       <c r="Z35" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AD35" s="185" t="s">
+      <c r="AD35" s="184" t="s">
         <v>700</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -7202,7 +7306,7 @@
       <c r="Z36" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD36" s="185"/>
+      <c r="AD36" s="184"/>
       <c r="AE36" s="7"/>
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
@@ -7274,7 +7378,7 @@
       <c r="Z37" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD37" s="185"/>
+      <c r="AD37" s="184"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7331,7 +7435,7 @@
       <c r="Z38" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="AD38" s="185"/>
+      <c r="AD38" s="184"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7346,15 +7450,15 @@
       <c r="F39" t="s">
         <v>567</v>
       </c>
-      <c r="J39" s="178" t="s">
+      <c r="J39" s="193" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="178"/>
-      <c r="L39" s="178"/>
-      <c r="M39" s="178"/>
-      <c r="N39" s="178"/>
-      <c r="O39" s="178"/>
-      <c r="P39" s="178"/>
+      <c r="K39" s="193"/>
+      <c r="L39" s="193"/>
+      <c r="M39" s="193"/>
+      <c r="N39" s="193"/>
+      <c r="O39" s="193"/>
+      <c r="P39" s="193"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7580,13 +7684,13 @@
         <v>839</v>
       </c>
       <c r="J48" t="s">
-        <v>880</v>
-      </c>
-      <c r="L48" s="176">
+        <v>878</v>
+      </c>
+      <c r="L48" s="168">
         <v>65.599999999999994</v>
       </c>
       <c r="M48" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
@@ -7604,13 +7708,13 @@
         <v>840</v>
       </c>
       <c r="J49" t="s">
-        <v>880</v>
-      </c>
-      <c r="L49" s="176">
+        <v>878</v>
+      </c>
+      <c r="L49" s="168">
         <v>65.7</v>
       </c>
       <c r="M49" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="T49" s="7" t="s">
         <v>694</v>
@@ -7640,13 +7744,13 @@
         <v>841</v>
       </c>
       <c r="J50" t="s">
-        <v>880</v>
-      </c>
-      <c r="L50" s="176">
+        <v>878</v>
+      </c>
+      <c r="L50" s="168">
         <v>65.8</v>
       </c>
       <c r="M50" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="T50" s="7" t="s">
         <v>695</v>
@@ -7670,13 +7774,13 @@
     </row>
     <row r="51" spans="5:26">
       <c r="J51" t="s">
-        <v>880</v>
-      </c>
-      <c r="L51" s="176">
+        <v>878</v>
+      </c>
+      <c r="L51" s="168">
         <v>65.900000000000006</v>
       </c>
       <c r="M51" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="T51" s="7" t="s">
         <v>696</v>
@@ -7700,13 +7804,13 @@
     </row>
     <row r="52" spans="5:26">
       <c r="J52" t="s">
-        <v>880</v>
-      </c>
-      <c r="L52" s="176">
+        <v>878</v>
+      </c>
+      <c r="L52" s="168">
         <v>66</v>
       </c>
       <c r="M52" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
@@ -7728,61 +7832,68 @@
     </row>
     <row r="53" spans="5:26">
       <c r="J53" t="s">
-        <v>880</v>
-      </c>
-      <c r="L53" s="176">
+        <v>878</v>
+      </c>
+      <c r="L53" s="168">
         <v>66.099999999999994</v>
       </c>
       <c r="M53" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="54" spans="5:26">
       <c r="J54" t="s">
-        <v>880</v>
-      </c>
-      <c r="L54" s="176">
+        <v>878</v>
+      </c>
+      <c r="L54" s="168">
         <v>66.2</v>
       </c>
       <c r="M54" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="55" spans="5:26">
       <c r="J55" t="s">
-        <v>880</v>
-      </c>
-      <c r="L55" s="176">
+        <v>878</v>
+      </c>
+      <c r="L55" s="168">
         <v>66.300000000000097</v>
       </c>
       <c r="M55" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="56" spans="5:26">
       <c r="J56" t="s">
-        <v>880</v>
-      </c>
-      <c r="L56" s="176">
+        <v>878</v>
+      </c>
+      <c r="L56" s="168">
         <v>66.400000000000105</v>
       </c>
       <c r="M56" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="57" spans="5:26">
       <c r="J57" t="s">
-        <v>880</v>
-      </c>
-      <c r="L57" s="176">
+        <v>878</v>
+      </c>
+      <c r="L57" s="168">
         <v>66.500000000000099</v>
       </c>
       <c r="M57" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7792,13 +7903,6 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7825,34 +7929,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="248" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
-      <c r="E1" s="241"/>
-      <c r="F1" s="241"/>
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="242"/>
-      <c r="B2" s="242"/>
-      <c r="C2" s="242"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
+      <c r="A2" s="249"/>
+      <c r="B2" s="249"/>
+      <c r="C2" s="249"/>
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="209" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="202" t="s">
+      <c r="B3" s="210"/>
+      <c r="C3" s="211"/>
+      <c r="D3" s="209" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="203"/>
-      <c r="F3" s="204"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="211"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -8209,14 +8313,14 @@
       <c r="F21" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="N21" s="243" t="s">
+      <c r="N21" s="250" t="s">
         <v>838</v>
       </c>
-      <c r="O21" s="243"/>
-      <c r="P21" s="243"/>
-      <c r="Q21" s="243"/>
-      <c r="R21" s="243"/>
-      <c r="S21" s="243"/>
+      <c r="O21" s="250"/>
+      <c r="P21" s="250"/>
+      <c r="Q21" s="250"/>
+      <c r="R21" s="250"/>
+      <c r="S21" s="250"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1">
       <c r="A22" s="54">
@@ -8237,12 +8341,12 @@
       <c r="F22" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="O22" s="244" t="s">
+      <c r="O22" s="251" t="s">
         <v>363</v>
       </c>
-      <c r="P22" s="244"/>
-      <c r="Q22" s="244"/>
-      <c r="R22" s="244"/>
+      <c r="P22" s="251"/>
+      <c r="Q22" s="251"/>
+      <c r="R22" s="251"/>
     </row>
     <row r="23" spans="1:19" ht="19.5" thickBot="1">
       <c r="A23" s="54">
@@ -8499,22 +8603,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="243" t="s">
+      <c r="A1" s="250" t="s">
         <v>838</v>
       </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="251" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -8637,12 +8741,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" customWidth="1"/>
     <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -8726,7 +8831,7 @@
         <v>729</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -8753,7 +8858,7 @@
         <v>387</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
       <c r="S2" s="66" t="s">
         <v>753</v>
@@ -8805,7 +8910,7 @@
         <v>387</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
       <c r="S3" s="66"/>
       <c r="T3" s="66"/>
@@ -8853,7 +8958,7 @@
         <v>387</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
       <c r="S4" s="66"/>
       <c r="T4" s="66"/>
@@ -8901,7 +9006,7 @@
         <v>387</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
       <c r="S5" s="66"/>
       <c r="T5" s="66"/>
@@ -8917,7 +9022,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="7" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
@@ -8932,7 +9037,7 @@
         <v>729</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
@@ -8959,7 +9064,7 @@
         <v>387</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -8996,7 +9101,7 @@
         <v>387</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -9033,7 +9138,7 @@
         <v>387</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -9070,12 +9175,12 @@
         <v>387</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>729</v>
+        <v>888</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B10" s="7">
         <v>3</v>
@@ -9090,7 +9195,7 @@
         <v>729</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="H10" s="7">
         <v>3</v>
@@ -9335,7 +9440,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="7" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B18" s="7">
         <v>5</v>
@@ -9417,7 +9522,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="7" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B22" s="7">
         <v>6</v>
@@ -9436,6 +9541,21 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
+      <c r="M22" s="155" t="s">
+        <v>734</v>
+      </c>
+      <c r="N22" s="155" t="s">
+        <v>731</v>
+      </c>
+      <c r="O22" s="155" t="s">
+        <v>730</v>
+      </c>
+      <c r="P22" s="155" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q22" s="155" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="7"/>
@@ -9456,6 +9576,21 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
+      <c r="M23" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="N23" s="7">
+        <v>1</v>
+      </c>
+      <c r="O23" s="7">
+        <v>711</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="7"/>
@@ -9476,6 +9611,21 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
+      <c r="M24" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="N24" s="7">
+        <v>1</v>
+      </c>
+      <c r="O24" s="7">
+        <v>712</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="7"/>
@@ -9496,6 +9646,21 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
+      <c r="M25" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="N25" s="7">
+        <v>1</v>
+      </c>
+      <c r="O25" s="7">
+        <v>713</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="7"/>
@@ -9508,6 +9673,21 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
+      <c r="M26" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="N26" s="7">
+        <v>1</v>
+      </c>
+      <c r="O26" s="7">
+        <v>714</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="7"/>
@@ -9520,6 +9700,21 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
+      <c r="M27" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="N27" s="7">
+        <v>2</v>
+      </c>
+      <c r="O27" s="7">
+        <v>721</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="7"/>
@@ -9532,6 +9727,21 @@
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="N28" s="7">
+        <v>2</v>
+      </c>
+      <c r="O28" s="7">
+        <v>722</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="7"/>
@@ -9539,11 +9749,26 @@
       <c r="C29" s="38"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="G29" s="254"/>
-      <c r="H29" s="254"/>
-      <c r="I29" s="254"/>
-      <c r="J29" s="254"/>
-      <c r="K29" s="254"/>
+      <c r="G29" s="169"/>
+      <c r="H29" s="169"/>
+      <c r="I29" s="169"/>
+      <c r="J29" s="169"/>
+      <c r="K29" s="169"/>
+      <c r="M29" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="N29" s="7">
+        <v>2</v>
+      </c>
+      <c r="O29" s="7">
+        <v>723</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="7"/>
@@ -9556,6 +9781,21 @@
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
+      <c r="M30" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="N30" s="7">
+        <v>2</v>
+      </c>
+      <c r="O30" s="7">
+        <v>724</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="7"/>
@@ -9670,7 +9910,7 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="7" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
@@ -9810,7 +10050,7 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="7" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B44" s="7">
         <v>2</v>
@@ -9908,7 +10148,7 @@
       <c r="J47" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="K47" s="254" t="s">
+      <c r="K47" s="169" t="s">
         <v>729</v>
       </c>
     </row>
@@ -10112,10 +10352,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10127,931 +10367,729 @@
     <col min="5" max="5" width="3.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="258" t="s">
+        <v>903</v>
+      </c>
+      <c r="B1" s="259"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
+      <c r="G1" s="259"/>
+      <c r="H1" s="260"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
+      <c r="A2" s="261"/>
+      <c r="B2" s="262"/>
+      <c r="C2" s="262"/>
+      <c r="D2" s="262"/>
+      <c r="E2" s="262"/>
+      <c r="F2" s="262"/>
+      <c r="G2" s="262"/>
+      <c r="H2" s="263"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" thickBot="1">
+      <c r="A3" s="252" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="253"/>
+      <c r="C3" s="253"/>
+      <c r="D3" s="254"/>
+      <c r="E3" s="252" t="s">
         <v>858</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="251"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="252"/>
-      <c r="B2" s="253"/>
-      <c r="C2" s="253"/>
-      <c r="D2" s="253"/>
-      <c r="E2" s="253"/>
-      <c r="F2" s="253"/>
-      <c r="G2" s="253"/>
-      <c r="H2" s="253"/>
-    </row>
-    <row r="3" spans="1:8" ht="20.25">
-      <c r="A3" s="245" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="246"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="246"/>
-      <c r="E3" s="246" t="s">
+      <c r="F3" s="253"/>
+      <c r="G3" s="253"/>
+      <c r="H3" s="254"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A4" s="178">
+        <v>1</v>
+      </c>
+      <c r="B4" s="177" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="179" t="s">
+        <v>479</v>
+      </c>
+      <c r="D4" s="180" t="s">
+        <v>892</v>
+      </c>
+      <c r="E4" s="178">
+        <v>1</v>
+      </c>
+      <c r="F4" s="177" t="s">
+        <v>643</v>
+      </c>
+      <c r="G4" s="179" t="s">
+        <v>640</v>
+      </c>
+      <c r="H4" s="180" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A5" s="178">
+        <v>2</v>
+      </c>
+      <c r="B5" s="177" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="179" t="s">
+        <v>484</v>
+      </c>
+      <c r="D5" s="180" t="s">
+        <v>893</v>
+      </c>
+      <c r="E5" s="178">
+        <v>2</v>
+      </c>
+      <c r="F5" s="177" t="s">
+        <v>642</v>
+      </c>
+      <c r="G5" s="179" t="s">
+        <v>607</v>
+      </c>
+      <c r="H5" s="180" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A6" s="178">
+        <v>3</v>
+      </c>
+      <c r="B6" s="177" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="179" t="s">
+        <v>652</v>
+      </c>
+      <c r="D6" s="180" t="s">
+        <v>894</v>
+      </c>
+      <c r="E6" s="178">
+        <v>3</v>
+      </c>
+      <c r="F6" s="177" t="s">
+        <v>505</v>
+      </c>
+      <c r="G6" s="179" t="s">
+        <v>640</v>
+      </c>
+      <c r="H6" s="180" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A7" s="178">
+        <v>4</v>
+      </c>
+      <c r="B7" s="177" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="179" t="s">
+        <v>653</v>
+      </c>
+      <c r="D7" s="180" t="s">
+        <v>895</v>
+      </c>
+      <c r="E7" s="178">
+        <v>4</v>
+      </c>
+      <c r="F7" s="177" t="s">
+        <v>504</v>
+      </c>
+      <c r="G7" s="179" t="s">
+        <v>607</v>
+      </c>
+      <c r="H7" s="180" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A8" s="178">
+        <v>5</v>
+      </c>
+      <c r="B8" s="177" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="179" t="s">
+        <v>654</v>
+      </c>
+      <c r="D8" s="180" t="s">
+        <v>896</v>
+      </c>
+      <c r="E8" s="178">
+        <v>5</v>
+      </c>
+      <c r="F8" s="177" t="s">
+        <v>651</v>
+      </c>
+      <c r="G8" s="179" t="s">
+        <v>640</v>
+      </c>
+      <c r="H8" s="180" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A9" s="178">
+        <v>6</v>
+      </c>
+      <c r="B9" s="177" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="179" t="s">
+        <v>485</v>
+      </c>
+      <c r="D9" s="180" t="s">
+        <v>897</v>
+      </c>
+      <c r="E9" s="178">
+        <v>6</v>
+      </c>
+      <c r="F9" s="177" t="s">
+        <v>650</v>
+      </c>
+      <c r="G9" s="179" t="s">
+        <v>607</v>
+      </c>
+      <c r="H9" s="180" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A10" s="178">
+        <v>7</v>
+      </c>
+      <c r="B10" s="177" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="179" t="s">
+        <v>487</v>
+      </c>
+      <c r="D10" s="180" t="s">
+        <v>898</v>
+      </c>
+      <c r="E10" s="178">
+        <v>7</v>
+      </c>
+      <c r="F10" s="177" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="179" t="s">
+        <v>378</v>
+      </c>
+      <c r="H10" s="180" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A11" s="178"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="179"/>
+      <c r="D11" s="180"/>
+      <c r="E11" s="178">
+        <v>8</v>
+      </c>
+      <c r="F11" s="177" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="179" t="s">
+        <v>491</v>
+      </c>
+      <c r="H11" s="180" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A12" s="178"/>
+      <c r="B12" s="177"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="178">
+        <v>9</v>
+      </c>
+      <c r="F12" s="177" t="s">
+        <v>257</v>
+      </c>
+      <c r="G12" s="179" t="s">
+        <v>496</v>
+      </c>
+      <c r="H12" s="180" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A13" s="178"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="179"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="178">
+        <v>10</v>
+      </c>
+      <c r="F13" s="177" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="179" t="s">
+        <v>556</v>
+      </c>
+      <c r="H13" s="180" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="181"/>
+      <c r="B14" s="173"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="172"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="182"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="181"/>
+      <c r="B15" s="173"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="172"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="176"/>
+      <c r="H15" s="171"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="181"/>
+      <c r="B16" s="173"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="174"/>
+      <c r="H16" s="170"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="181"/>
+      <c r="B17" s="173"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="175"/>
+      <c r="E17" s="172"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="174"/>
+      <c r="H17" s="170"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="181"/>
+      <c r="B18" s="173"/>
+      <c r="C18" s="174"/>
+      <c r="D18" s="175"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="170"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="181"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="172"/>
+      <c r="F19" s="173"/>
+      <c r="G19" s="174"/>
+      <c r="H19" s="170"/>
+    </row>
+    <row r="20" spans="1:8" ht="78.75" customHeight="1">
+      <c r="A20" s="181"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="174"/>
+      <c r="H20" s="170"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A21" s="181"/>
+      <c r="B21" s="173"/>
+      <c r="C21" s="174"/>
+      <c r="D21" s="175"/>
+      <c r="E21" s="172"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="174"/>
+      <c r="H21" s="170"/>
+    </row>
+    <row r="22" spans="1:8" ht="20.25" thickBot="1">
+      <c r="A22" s="255" t="s">
         <v>859</v>
       </c>
-      <c r="F3" s="246"/>
-      <c r="G3" s="246"/>
-      <c r="H3" s="247"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="164">
+      <c r="B22" s="256"/>
+      <c r="C22" s="256"/>
+      <c r="D22" s="257"/>
+      <c r="E22" s="255" t="s">
+        <v>860</v>
+      </c>
+      <c r="F22" s="256"/>
+      <c r="G22" s="256"/>
+      <c r="H22" s="257"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A23" s="161">
         <v>1</v>
       </c>
-      <c r="B4" s="165" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="160" t="s">
-        <v>479</v>
-      </c>
-      <c r="D4" s="162" t="s">
+      <c r="B23" s="183">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="C23" s="160" t="s">
+        <v>861</v>
+      </c>
+      <c r="D23" s="160" t="s">
+        <v>861</v>
+      </c>
+      <c r="E23" s="161">
+        <v>1</v>
+      </c>
+      <c r="F23" s="165">
+        <v>35.6</v>
+      </c>
+      <c r="G23" s="166" t="s">
+        <v>523</v>
+      </c>
+      <c r="H23" s="167" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A24" s="161">
         <v>2</v>
       </c>
-      <c r="E4" s="81">
-        <v>1</v>
-      </c>
-      <c r="F4" s="165">
-        <v>129.6</v>
-      </c>
-      <c r="G4" s="161" t="s">
-        <v>640</v>
-      </c>
-      <c r="H4" s="162" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="164">
+      <c r="B24" s="162">
+        <v>65.7</v>
+      </c>
+      <c r="C24" s="163" t="s">
+        <v>862</v>
+      </c>
+      <c r="D24" s="163" t="s">
+        <v>862</v>
+      </c>
+      <c r="E24" s="161">
         <v>2</v>
       </c>
-      <c r="B5" s="165" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="162" t="s">
-        <v>484</v>
-      </c>
-      <c r="D5" s="173" t="s">
+      <c r="F24" s="165" t="s">
+        <v>442</v>
+      </c>
+      <c r="G24" s="166" t="s">
+        <v>463</v>
+      </c>
+      <c r="H24" s="167" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A25" s="161">
+        <v>3</v>
+      </c>
+      <c r="B25" s="162">
+        <v>65.8</v>
+      </c>
+      <c r="C25" s="163" t="s">
+        <v>863</v>
+      </c>
+      <c r="D25" s="163" t="s">
+        <v>863</v>
+      </c>
+      <c r="E25" s="161">
+        <v>3</v>
+      </c>
+      <c r="F25" s="165" t="s">
+        <v>443</v>
+      </c>
+      <c r="G25" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="H25" s="167" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A26" s="161">
+        <v>4</v>
+      </c>
+      <c r="B26" s="162">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="C26" s="163" t="s">
+        <v>864</v>
+      </c>
+      <c r="D26" s="163" t="s">
+        <v>864</v>
+      </c>
+      <c r="E26" s="161">
+        <v>4</v>
+      </c>
+      <c r="F26" s="165" t="s">
+        <v>444</v>
+      </c>
+      <c r="G26" s="166" t="s">
+        <v>467</v>
+      </c>
+      <c r="H26" s="167" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A27" s="161">
         <v>5</v>
       </c>
-      <c r="E5" s="81">
-        <v>2</v>
-      </c>
-      <c r="F5" s="165">
-        <v>129.19999999999999</v>
-      </c>
-      <c r="G5" s="161" t="s">
-        <v>607</v>
-      </c>
-      <c r="H5" s="162" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="164">
-        <v>3</v>
-      </c>
-      <c r="B6" s="165" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="160" t="s">
-        <v>480</v>
-      </c>
-      <c r="D6" s="162" t="s">
-        <v>622</v>
-      </c>
-      <c r="E6" s="81">
-        <v>3</v>
-      </c>
-      <c r="F6" s="165">
-        <v>118.4</v>
-      </c>
-      <c r="G6" s="161" t="s">
-        <v>640</v>
-      </c>
-      <c r="H6" s="162" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="164">
-        <v>4</v>
-      </c>
-      <c r="B7" s="165" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="160" t="s">
-        <v>482</v>
-      </c>
-      <c r="D7" s="162" t="s">
-        <v>623</v>
-      </c>
-      <c r="E7" s="81">
-        <v>4</v>
-      </c>
-      <c r="F7" s="165">
-        <v>118.2</v>
-      </c>
-      <c r="G7" s="161" t="s">
-        <v>607</v>
-      </c>
-      <c r="H7" s="162" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A8" s="164">
+      <c r="B27" s="162">
+        <v>66</v>
+      </c>
+      <c r="C27" s="163" t="s">
+        <v>865</v>
+      </c>
+      <c r="D27" s="163" t="s">
+        <v>865</v>
+      </c>
+      <c r="E27" s="161">
         <v>5</v>
       </c>
-      <c r="B8" s="165" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="160" t="s">
-        <v>481</v>
-      </c>
-      <c r="D8" s="162" t="s">
-        <v>624</v>
-      </c>
-      <c r="E8" s="81">
-        <v>5</v>
-      </c>
-      <c r="F8" s="165" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="161" t="s">
-        <v>655</v>
-      </c>
-      <c r="H8" s="162" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="164">
+      <c r="F27" s="165" t="s">
+        <v>271</v>
+      </c>
+      <c r="G27" s="166" t="s">
+        <v>469</v>
+      </c>
+      <c r="H27" s="167" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A28" s="161">
         <v>6</v>
       </c>
-      <c r="B9" s="165" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="160" t="s">
-        <v>483</v>
-      </c>
-      <c r="D9" s="162" t="s">
-        <v>625</v>
-      </c>
-      <c r="E9" s="81">
+      <c r="B28" s="162">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="C28" s="163" t="s">
+        <v>866</v>
+      </c>
+      <c r="D28" s="163" t="s">
+        <v>866</v>
+      </c>
+      <c r="E28" s="161">
         <v>6</v>
       </c>
-      <c r="F9" s="165" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="161" t="s">
-        <v>658</v>
-      </c>
-      <c r="H9" s="162" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="164">
+      <c r="F28" s="165" t="s">
+        <v>272</v>
+      </c>
+      <c r="G28" s="166" t="s">
+        <v>471</v>
+      </c>
+      <c r="H28" s="167" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A29" s="161">
         <v>7</v>
       </c>
-      <c r="B10" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="160" t="s">
-        <v>486</v>
-      </c>
-      <c r="D10" s="162" t="s">
-        <v>626</v>
-      </c>
-      <c r="E10" s="81">
+      <c r="B29" s="162">
+        <v>66.2</v>
+      </c>
+      <c r="C29" s="163" t="s">
+        <v>867</v>
+      </c>
+      <c r="D29" s="163" t="s">
+        <v>867</v>
+      </c>
+      <c r="E29" s="161">
         <v>7</v>
       </c>
-      <c r="F10" s="165" t="s">
-        <v>238</v>
-      </c>
-      <c r="G10" s="161" t="s">
-        <v>659</v>
-      </c>
-      <c r="H10" s="162" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="164">
+      <c r="F29" s="165" t="s">
+        <v>273</v>
+      </c>
+      <c r="G29" s="166" t="s">
+        <v>473</v>
+      </c>
+      <c r="H29" s="167" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A30" s="161">
         <v>8</v>
       </c>
-      <c r="B11" s="165" t="s">
-        <v>230</v>
-      </c>
-      <c r="C11" s="160" t="s">
-        <v>488</v>
-      </c>
-      <c r="D11" s="162" t="s">
-        <v>627</v>
-      </c>
-      <c r="E11" s="81">
+      <c r="B30" s="162">
+        <v>66.300000000000097</v>
+      </c>
+      <c r="C30" s="163" t="s">
+        <v>868</v>
+      </c>
+      <c r="D30" s="163" t="s">
+        <v>868</v>
+      </c>
+      <c r="E30" s="161">
         <v>8</v>
       </c>
-      <c r="F11" s="165" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="161" t="s">
-        <v>660</v>
-      </c>
-      <c r="H11" s="162" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="164">
+      <c r="F30" s="165">
+        <v>36.4</v>
+      </c>
+      <c r="G30" s="166" t="s">
+        <v>714</v>
+      </c>
+      <c r="H30" s="164"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A31" s="161">
         <v>9</v>
       </c>
-      <c r="B12" s="165" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="160" t="s">
-        <v>489</v>
-      </c>
-      <c r="D12" s="162" t="s">
-        <v>628</v>
-      </c>
-      <c r="E12" s="81">
+      <c r="B31" s="162">
+        <v>66.400000000000105</v>
+      </c>
+      <c r="C31" s="164" t="s">
+        <v>869</v>
+      </c>
+      <c r="D31" s="164" t="s">
+        <v>869</v>
+      </c>
+      <c r="E31" s="161">
         <v>9</v>
       </c>
-      <c r="F12" s="165" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="161" t="s">
-        <v>378</v>
-      </c>
-      <c r="H12" s="173" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A13" s="164">
+      <c r="F31" s="165">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="G31" s="166" t="s">
+        <v>473</v>
+      </c>
+      <c r="H31" s="164"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A32" s="267">
         <v>10</v>
       </c>
-      <c r="B13" s="165" t="s">
-        <v>222</v>
-      </c>
-      <c r="C13" s="160" t="s">
-        <v>490</v>
-      </c>
-      <c r="D13" s="162" t="s">
-        <v>629</v>
-      </c>
-      <c r="E13" s="81">
+      <c r="B32" s="162">
+        <v>66.500000000000099</v>
+      </c>
+      <c r="C32" s="164" t="s">
+        <v>870</v>
+      </c>
+      <c r="D32" s="164" t="s">
+        <v>870</v>
+      </c>
+      <c r="E32" s="267">
         <v>10</v>
       </c>
-      <c r="F13" s="165" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="161" t="s">
-        <v>491</v>
-      </c>
-      <c r="H13" s="163" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A14" s="164">
-        <v>11</v>
-      </c>
-      <c r="B14" s="165" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="160" t="s">
-        <v>506</v>
-      </c>
-      <c r="D14" s="162" t="s">
-        <v>631</v>
-      </c>
-      <c r="E14" s="81">
-        <v>11</v>
-      </c>
-      <c r="F14" s="165" t="s">
-        <v>257</v>
-      </c>
-      <c r="G14" s="161" t="s">
-        <v>496</v>
-      </c>
-      <c r="H14" s="163" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A15" s="164">
-        <v>12</v>
-      </c>
-      <c r="B15" s="165" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="160" t="s">
-        <v>507</v>
-      </c>
-      <c r="D15" s="162" t="s">
-        <v>632</v>
-      </c>
-      <c r="E15" s="81">
-        <v>12</v>
-      </c>
-      <c r="F15" s="165" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="161" t="s">
-        <v>556</v>
-      </c>
-      <c r="H15" s="162" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A16" s="164">
-        <v>13</v>
-      </c>
-      <c r="B16" s="165" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="160" t="s">
-        <v>508</v>
-      </c>
-      <c r="D16" s="162" t="s">
-        <v>633</v>
-      </c>
-      <c r="E16" s="81">
-        <v>13</v>
-      </c>
-      <c r="F16" s="165"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A17" s="164">
-        <v>14</v>
-      </c>
-      <c r="B17" s="165" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="160" t="s">
-        <v>652</v>
-      </c>
-      <c r="D17" s="162" t="s">
-        <v>709</v>
-      </c>
-      <c r="E17" s="81">
-        <v>14</v>
-      </c>
-      <c r="F17" s="165"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A18" s="164">
-        <v>15</v>
-      </c>
-      <c r="B18" s="165" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="160" t="s">
-        <v>653</v>
-      </c>
-      <c r="D18" s="162" t="s">
-        <v>710</v>
-      </c>
-      <c r="E18" s="81">
-        <v>15</v>
-      </c>
-      <c r="F18" s="165"/>
-      <c r="G18" s="160"/>
-      <c r="H18" s="160"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A19" s="164">
-        <v>16</v>
-      </c>
-      <c r="B19" s="165" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="160" t="s">
-        <v>654</v>
-      </c>
-      <c r="D19" s="162" t="s">
-        <v>711</v>
-      </c>
-      <c r="E19" s="81">
-        <v>16</v>
-      </c>
-      <c r="F19" s="165"/>
-      <c r="G19" s="160"/>
-      <c r="H19" s="160"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A20" s="164">
-        <v>17</v>
-      </c>
-      <c r="B20" s="165" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="160" t="s">
-        <v>485</v>
-      </c>
-      <c r="D20" s="162" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="81">
-        <v>17</v>
-      </c>
-      <c r="F20" s="165"/>
-      <c r="G20" s="160"/>
-      <c r="H20" s="160"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A21" s="164">
-        <v>18</v>
-      </c>
-      <c r="B21" s="165" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="160" t="s">
-        <v>487</v>
-      </c>
-      <c r="D21" s="162" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="81">
-        <v>18</v>
-      </c>
-      <c r="F21" s="165"/>
-      <c r="G21" s="160"/>
-      <c r="H21" s="160"/>
-    </row>
-    <row r="22" spans="1:8" ht="19.5">
-      <c r="A22" s="248" t="s">
-        <v>860</v>
-      </c>
-      <c r="B22" s="249"/>
-      <c r="C22" s="249"/>
-      <c r="D22" s="249"/>
-      <c r="E22" s="248" t="s">
-        <v>861</v>
-      </c>
-      <c r="F22" s="249"/>
-      <c r="G22" s="249"/>
-      <c r="H22" s="249"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A23" s="164">
-        <v>1</v>
-      </c>
-      <c r="B23" s="166">
-        <v>65.599999999999994</v>
-      </c>
-      <c r="C23" s="167" t="s">
-        <v>862</v>
-      </c>
-      <c r="D23" s="167" t="s">
-        <v>862</v>
-      </c>
-      <c r="E23" s="164">
-        <v>1</v>
-      </c>
-      <c r="F23" s="166">
-        <v>21</v>
-      </c>
-      <c r="G23" s="167" t="s">
-        <v>863</v>
-      </c>
-      <c r="H23" s="174" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A24" s="164">
-        <v>2</v>
-      </c>
-      <c r="B24" s="168">
-        <v>65.7</v>
-      </c>
-      <c r="C24" s="169" t="s">
-        <v>864</v>
-      </c>
-      <c r="D24" s="169" t="s">
-        <v>864</v>
-      </c>
-      <c r="E24" s="164">
-        <v>2</v>
-      </c>
-      <c r="F24" s="168"/>
-      <c r="G24" s="169"/>
-      <c r="H24" s="169"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A25" s="164">
-        <v>3</v>
-      </c>
-      <c r="B25" s="168">
-        <v>65.8</v>
-      </c>
-      <c r="C25" s="169" t="s">
-        <v>865</v>
-      </c>
-      <c r="D25" s="169" t="s">
-        <v>865</v>
-      </c>
-      <c r="E25" s="164">
-        <v>3</v>
-      </c>
-      <c r="F25" s="168"/>
-      <c r="G25" s="169"/>
-      <c r="H25" s="169"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A26" s="164">
-        <v>4</v>
-      </c>
-      <c r="B26" s="168">
-        <v>65.900000000000006</v>
-      </c>
-      <c r="C26" s="169" t="s">
-        <v>866</v>
-      </c>
-      <c r="D26" s="169" t="s">
-        <v>866</v>
-      </c>
-      <c r="E26" s="164">
-        <v>4</v>
-      </c>
-      <c r="F26" s="168"/>
-      <c r="G26" s="169"/>
-      <c r="H26" s="169"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A27" s="164">
-        <v>5</v>
-      </c>
-      <c r="B27" s="168">
-        <v>66</v>
-      </c>
-      <c r="C27" s="169" t="s">
-        <v>867</v>
-      </c>
-      <c r="D27" s="169" t="s">
-        <v>867</v>
-      </c>
-      <c r="E27" s="164">
-        <v>5</v>
-      </c>
-      <c r="F27" s="168"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="169"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A28" s="164">
-        <v>6</v>
-      </c>
-      <c r="B28" s="168">
-        <v>66.099999999999994</v>
-      </c>
-      <c r="C28" s="169" t="s">
-        <v>868</v>
-      </c>
-      <c r="D28" s="169" t="s">
-        <v>868</v>
-      </c>
-      <c r="E28" s="164">
-        <v>6</v>
-      </c>
-      <c r="F28" s="168"/>
-      <c r="G28" s="169"/>
-      <c r="H28" s="169"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A29" s="164">
-        <v>7</v>
-      </c>
-      <c r="B29" s="168">
-        <v>66.2</v>
-      </c>
-      <c r="C29" s="169" t="s">
-        <v>869</v>
-      </c>
-      <c r="D29" s="169" t="s">
-        <v>869</v>
-      </c>
-      <c r="E29" s="164">
-        <v>7</v>
-      </c>
-      <c r="F29" s="168"/>
-      <c r="G29" s="169"/>
-      <c r="H29" s="169"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A30" s="164">
-        <v>8</v>
-      </c>
-      <c r="B30" s="168">
-        <v>66.300000000000097</v>
-      </c>
-      <c r="C30" s="169" t="s">
-        <v>870</v>
-      </c>
-      <c r="D30" s="169" t="s">
-        <v>870</v>
-      </c>
-      <c r="E30" s="164">
-        <v>8</v>
-      </c>
-      <c r="F30" s="168"/>
-      <c r="G30" s="169"/>
-      <c r="H30" s="169"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A31" s="164">
-        <v>9</v>
-      </c>
-      <c r="B31" s="168">
-        <v>66.400000000000105</v>
-      </c>
-      <c r="C31" s="170" t="s">
-        <v>871</v>
-      </c>
-      <c r="D31" s="170" t="s">
-        <v>871</v>
-      </c>
-      <c r="E31" s="164">
-        <v>9</v>
-      </c>
-      <c r="F31" s="168"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="170"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A32" s="164">
-        <v>10</v>
-      </c>
-      <c r="B32" s="168">
-        <v>66.500000000000099</v>
-      </c>
-      <c r="C32" s="170" t="s">
-        <v>872</v>
-      </c>
-      <c r="D32" s="170" t="s">
-        <v>872</v>
-      </c>
-      <c r="E32" s="164">
-        <v>10</v>
-      </c>
-      <c r="F32" s="168"/>
-      <c r="G32" s="170"/>
-      <c r="H32" s="170"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A33" s="164">
-        <v>11</v>
-      </c>
-      <c r="B33" s="171">
-        <v>35.6</v>
-      </c>
-      <c r="C33" s="172" t="s">
-        <v>523</v>
-      </c>
-      <c r="D33" s="175" t="s">
-        <v>873</v>
-      </c>
-      <c r="E33" s="164">
-        <v>11</v>
-      </c>
-      <c r="F33" s="171"/>
-      <c r="G33" s="172"/>
+      <c r="F32" s="165">
+        <v>32.25</v>
+      </c>
+      <c r="G32" s="166" t="s">
+        <v>715</v>
+      </c>
+      <c r="H32" s="164"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75">
+      <c r="A33" s="181"/>
+      <c r="B33" s="264"/>
+      <c r="C33" s="265"/>
+      <c r="D33" s="266"/>
+      <c r="E33" s="172"/>
+      <c r="F33" s="264"/>
+      <c r="G33" s="265"/>
       <c r="H33" s="170"/>
     </row>
-    <row r="34" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A34" s="164">
-        <v>12</v>
-      </c>
-      <c r="B34" s="171" t="s">
-        <v>442</v>
-      </c>
-      <c r="C34" s="172" t="s">
-        <v>463</v>
-      </c>
-      <c r="D34" s="175" t="s">
-        <v>874</v>
-      </c>
-      <c r="E34" s="164">
-        <v>12</v>
-      </c>
-      <c r="F34" s="171"/>
-      <c r="G34" s="172"/>
+    <row r="34" spans="1:8" ht="15.75">
+      <c r="A34" s="181"/>
+      <c r="B34" s="264"/>
+      <c r="C34" s="265"/>
+      <c r="D34" s="266"/>
+      <c r="E34" s="172"/>
+      <c r="F34" s="264"/>
+      <c r="G34" s="265"/>
       <c r="H34" s="170"/>
     </row>
-    <row r="35" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A35" s="164">
-        <v>13</v>
-      </c>
-      <c r="B35" s="171" t="s">
-        <v>443</v>
-      </c>
-      <c r="C35" s="172" t="s">
-        <v>466</v>
-      </c>
-      <c r="D35" s="175" t="s">
-        <v>875</v>
-      </c>
-      <c r="E35" s="164">
-        <v>13</v>
-      </c>
-      <c r="F35" s="171"/>
-      <c r="G35" s="172"/>
+    <row r="35" spans="1:8" ht="15.75">
+      <c r="A35" s="181"/>
+      <c r="B35" s="264"/>
+      <c r="C35" s="265"/>
+      <c r="D35" s="266"/>
+      <c r="E35" s="172"/>
+      <c r="F35" s="264"/>
+      <c r="G35" s="265"/>
       <c r="H35" s="170"/>
     </row>
-    <row r="36" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A36" s="164">
-        <v>14</v>
-      </c>
-      <c r="B36" s="171" t="s">
-        <v>444</v>
-      </c>
-      <c r="C36" s="172" t="s">
-        <v>467</v>
-      </c>
-      <c r="D36" s="175" t="s">
-        <v>876</v>
-      </c>
-      <c r="E36" s="164">
-        <v>14</v>
-      </c>
-      <c r="F36" s="171"/>
-      <c r="G36" s="172"/>
+    <row r="36" spans="1:8" ht="15.75">
+      <c r="A36" s="181"/>
+      <c r="B36" s="264"/>
+      <c r="C36" s="265"/>
+      <c r="D36" s="266"/>
+      <c r="E36" s="172"/>
+      <c r="F36" s="264"/>
+      <c r="G36" s="265"/>
       <c r="H36" s="170"/>
     </row>
-    <row r="37" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A37" s="164">
-        <v>15</v>
-      </c>
-      <c r="B37" s="171" t="s">
-        <v>271</v>
-      </c>
-      <c r="C37" s="172" t="s">
-        <v>469</v>
-      </c>
-      <c r="D37" s="175" t="s">
-        <v>877</v>
-      </c>
-      <c r="E37" s="164">
-        <v>15</v>
-      </c>
-      <c r="F37" s="171"/>
-      <c r="G37" s="172"/>
+    <row r="37" spans="1:8" ht="15.75">
+      <c r="A37" s="181"/>
+      <c r="B37" s="264"/>
+      <c r="C37" s="265"/>
+      <c r="D37" s="266"/>
+      <c r="E37" s="172"/>
+      <c r="F37" s="264"/>
+      <c r="G37" s="265"/>
       <c r="H37" s="170"/>
     </row>
-    <row r="38" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A38" s="164">
-        <v>16</v>
-      </c>
-      <c r="B38" s="171" t="s">
-        <v>272</v>
-      </c>
-      <c r="C38" s="172" t="s">
-        <v>471</v>
-      </c>
-      <c r="D38" s="175" t="s">
-        <v>878</v>
-      </c>
-      <c r="E38" s="164">
-        <v>16</v>
-      </c>
-      <c r="F38" s="171"/>
-      <c r="G38" s="172"/>
+    <row r="38" spans="1:8" ht="15.75">
+      <c r="A38" s="181"/>
+      <c r="B38" s="264"/>
+      <c r="C38" s="265"/>
+      <c r="D38" s="266"/>
+      <c r="E38" s="172"/>
+      <c r="F38" s="264"/>
+      <c r="G38" s="265"/>
       <c r="H38" s="170"/>
     </row>
-    <row r="39" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A39" s="164">
-        <v>17</v>
-      </c>
-      <c r="B39" s="171" t="s">
-        <v>273</v>
-      </c>
-      <c r="C39" s="172" t="s">
-        <v>473</v>
-      </c>
-      <c r="D39" s="175" t="s">
-        <v>879</v>
-      </c>
-      <c r="E39" s="164">
-        <v>17</v>
-      </c>
-      <c r="F39" s="171"/>
-      <c r="G39" s="172"/>
+    <row r="39" spans="1:8" ht="15.75">
+      <c r="A39" s="181"/>
+      <c r="B39" s="264"/>
+      <c r="C39" s="265"/>
+      <c r="D39" s="266"/>
+      <c r="E39" s="172"/>
+      <c r="F39" s="264"/>
+      <c r="G39" s="265"/>
       <c r="H39" s="170"/>
     </row>
-    <row r="40" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A40" s="164">
-        <v>18</v>
-      </c>
-      <c r="B40" s="171">
-        <v>36.4</v>
-      </c>
-      <c r="C40" s="172" t="s">
-        <v>714</v>
-      </c>
-      <c r="D40" s="170"/>
-      <c r="E40" s="164">
-        <v>18</v>
-      </c>
-      <c r="F40" s="171"/>
-      <c r="G40" s="172"/>
+    <row r="40" spans="1:8" ht="15.75">
+      <c r="A40" s="181"/>
+      <c r="B40" s="264"/>
+      <c r="C40" s="265"/>
+      <c r="D40" s="174"/>
+      <c r="E40" s="172"/>
+      <c r="F40" s="264"/>
+      <c r="G40" s="265"/>
       <c r="H40" s="170"/>
     </row>
-    <row r="41" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A41" s="164">
-        <v>19</v>
-      </c>
-      <c r="B41" s="171">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="C41" s="172" t="s">
-        <v>473</v>
-      </c>
-      <c r="D41" s="170"/>
-      <c r="E41" s="164">
-        <v>19</v>
-      </c>
-      <c r="F41" s="171"/>
-      <c r="G41" s="172"/>
+    <row r="41" spans="1:8" ht="15.75">
+      <c r="A41" s="181"/>
+      <c r="B41" s="264"/>
+      <c r="C41" s="265"/>
+      <c r="D41" s="174"/>
+      <c r="E41" s="172"/>
+      <c r="F41" s="264"/>
+      <c r="G41" s="265"/>
       <c r="H41" s="170"/>
     </row>
     <row r="42" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A42" s="164">
-        <v>20</v>
-      </c>
-      <c r="B42" s="171">
-        <v>32.25</v>
-      </c>
-      <c r="C42" s="172" t="s">
-        <v>715</v>
-      </c>
-      <c r="D42" s="170"/>
-      <c r="E42" s="164">
-        <v>20</v>
-      </c>
-      <c r="F42" s="171"/>
-      <c r="G42" s="172"/>
-      <c r="H42" s="170"/>
-    </row>
-    <row r="43" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A43" s="171"/>
-      <c r="B43" s="171"/>
-      <c r="C43" s="171"/>
-      <c r="D43" s="171"/>
-      <c r="E43" s="171"/>
-      <c r="F43" s="171"/>
-      <c r="G43" s="171"/>
-      <c r="H43" s="171"/>
-    </row>
-    <row r="44" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A44" s="171"/>
-      <c r="B44" s="171"/>
-      <c r="C44" s="171"/>
-      <c r="D44" s="171"/>
-      <c r="E44" s="171"/>
-      <c r="F44" s="171"/>
-      <c r="G44" s="171"/>
-      <c r="H44" s="171"/>
-    </row>
-    <row r="45" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A45" s="171"/>
-      <c r="B45" s="171"/>
-      <c r="C45" s="171"/>
-      <c r="D45" s="171"/>
-      <c r="E45" s="171"/>
-      <c r="F45" s="171"/>
-      <c r="G45" s="171"/>
-      <c r="H45" s="171"/>
-    </row>
-    <row r="46" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A46" s="171"/>
-      <c r="B46" s="171"/>
-      <c r="C46" s="171"/>
-      <c r="D46" s="171"/>
-      <c r="E46" s="171"/>
-      <c r="F46" s="171"/>
-      <c r="G46" s="171"/>
-      <c r="H46" s="171"/>
+      <c r="A42" s="268"/>
+      <c r="B42" s="269"/>
+      <c r="C42" s="270"/>
+      <c r="D42" s="271"/>
+      <c r="E42" s="272"/>
+      <c r="F42" s="269"/>
+      <c r="G42" s="270"/>
+      <c r="H42" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11088,40 +11126,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="197" t="s">
         <v>701</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="192"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="199"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="193"/>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="194"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="194"/>
-      <c r="H2" s="195"/>
+      <c r="A2" s="200"/>
+      <c r="B2" s="201"/>
+      <c r="C2" s="201"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="202"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="203" t="s">
         <v>608</v>
       </c>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197" t="s">
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204" t="s">
         <v>609</v>
       </c>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="198"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="205"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="78">
@@ -12154,14 +12192,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="206" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="201"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="208"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -12172,16 +12210,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="209" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="202" t="s">
+      <c r="B3" s="210"/>
+      <c r="C3" s="211"/>
+      <c r="D3" s="209" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="203"/>
-      <c r="F3" s="204"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="211"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -12451,28 +12489,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="215" t="s">
         <v>737</v>
       </c>
-      <c r="B1" s="208"/>
-      <c r="C1" s="208"/>
-      <c r="D1" s="208"/>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
+      <c r="G1" s="215"/>
+      <c r="H1" s="215"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="205" t="s">
+      <c r="A2" s="212" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="206"/>
-      <c r="F2" s="206"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="207"/>
+      <c r="B2" s="213"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="214"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -12747,16 +12785,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="205" t="s">
+      <c r="A15" s="212" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="206"/>
-      <c r="C15" s="206"/>
-      <c r="D15" s="206"/>
-      <c r="E15" s="206"/>
-      <c r="F15" s="206"/>
-      <c r="G15" s="206"/>
-      <c r="H15" s="207"/>
+      <c r="B15" s="213"/>
+      <c r="C15" s="213"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="213"/>
+      <c r="F15" s="213"/>
+      <c r="G15" s="213"/>
+      <c r="H15" s="214"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -13046,16 +13084,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="205" t="s">
+      <c r="A28" s="212" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="206"/>
-      <c r="C28" s="206"/>
-      <c r="D28" s="206"/>
-      <c r="E28" s="206"/>
-      <c r="F28" s="206"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="207"/>
+      <c r="B28" s="213"/>
+      <c r="C28" s="213"/>
+      <c r="D28" s="213"/>
+      <c r="E28" s="213"/>
+      <c r="F28" s="213"/>
+      <c r="G28" s="213"/>
+      <c r="H28" s="214"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -13368,12 +13406,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="216" t="s">
         <v>713</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -13581,28 +13619,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="217" t="s">
         <v>751</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="205" t="s">
+      <c r="A2" s="212" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="206"/>
-      <c r="F2" s="206"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="207"/>
+      <c r="B2" s="213"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="214"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -13893,12 +13931,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="205" t="s">
+      <c r="A15" s="212" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="206"/>
-      <c r="C15" s="206"/>
-      <c r="D15" s="207"/>
+      <c r="B15" s="213"/>
+      <c r="C15" s="213"/>
+      <c r="D15" s="214"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -14066,12 +14104,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="205" t="s">
+      <c r="A28" s="212" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="206"/>
-      <c r="C28" s="206"/>
-      <c r="D28" s="207"/>
+      <c r="B28" s="213"/>
+      <c r="C28" s="213"/>
+      <c r="D28" s="214"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -14275,40 +14313,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="206" t="s">
         <v>832</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="201"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="208"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="211"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="213"/>
+      <c r="A2" s="218"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="220"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="221" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="215"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="214" t="s">
+      <c r="B3" s="222"/>
+      <c r="C3" s="223"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="221" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="215"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="217"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="74">
@@ -15001,40 +15039,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="242" t="s">
         <v>830</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
+      <c r="B1" s="242"/>
+      <c r="C1" s="242"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="242"/>
+      <c r="F1" s="242"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="242"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="219"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="243"/>
+      <c r="C2" s="243"/>
+      <c r="D2" s="243"/>
+      <c r="E2" s="243"/>
+      <c r="F2" s="243"/>
+      <c r="G2" s="243"/>
+      <c r="H2" s="243"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="220" t="s">
+      <c r="A3" s="244" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="221"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="223"/>
-      <c r="E3" s="220" t="s">
+      <c r="B3" s="245"/>
+      <c r="C3" s="246"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="244" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="221"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="223"/>
+      <c r="F3" s="245"/>
+      <c r="G3" s="246"/>
+      <c r="H3" s="247"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -15563,36 +15601,36 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="220" t="s">
+      <c r="A25" s="244" t="s">
         <v>786</v>
       </c>
-      <c r="B25" s="221"/>
-      <c r="C25" s="222"/>
-      <c r="D25" s="223"/>
-      <c r="E25" s="220" t="s">
+      <c r="B25" s="245"/>
+      <c r="C25" s="246"/>
+      <c r="D25" s="247"/>
+      <c r="E25" s="244" t="s">
         <v>787</v>
       </c>
-      <c r="F25" s="221"/>
-      <c r="G25" s="222"/>
-      <c r="H25" s="223"/>
+      <c r="F25" s="245"/>
+      <c r="G25" s="246"/>
+      <c r="H25" s="247"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
         <v>788</v>
       </c>
-      <c r="B26" s="224" t="s">
+      <c r="B26" s="231" t="s">
         <v>789</v>
       </c>
-      <c r="C26" s="225"/>
-      <c r="D26" s="226"/>
+      <c r="C26" s="232"/>
+      <c r="D26" s="233"/>
       <c r="E26" s="125" t="s">
         <v>790</v>
       </c>
-      <c r="F26" s="227" t="s">
+      <c r="F26" s="239" t="s">
         <v>791</v>
       </c>
-      <c r="G26" s="228"/>
-      <c r="H26" s="229" t="s">
+      <c r="G26" s="240"/>
+      <c r="H26" s="241" t="s">
         <v>759</v>
       </c>
     </row>
@@ -15600,21 +15638,21 @@
       <c r="A27" s="137" t="s">
         <v>792</v>
       </c>
-      <c r="B27" s="230" t="s">
+      <c r="B27" s="234" t="s">
         <v>793</v>
       </c>
-      <c r="C27" s="231"/>
-      <c r="D27" s="232" t="s">
+      <c r="C27" s="235"/>
+      <c r="D27" s="237" t="s">
         <v>623</v>
       </c>
       <c r="E27" s="129" t="s">
         <v>794</v>
       </c>
-      <c r="F27" s="224" t="s">
+      <c r="F27" s="231" t="s">
         <v>795</v>
       </c>
-      <c r="G27" s="225"/>
-      <c r="H27" s="233" t="s">
+      <c r="G27" s="232"/>
+      <c r="H27" s="238" t="s">
         <v>761</v>
       </c>
     </row>
@@ -15622,21 +15660,21 @@
       <c r="A28" s="129" t="s">
         <v>796</v>
       </c>
-      <c r="B28" s="224" t="s">
+      <c r="B28" s="231" t="s">
         <v>797</v>
       </c>
-      <c r="C28" s="225"/>
-      <c r="D28" s="226" t="s">
+      <c r="C28" s="232"/>
+      <c r="D28" s="233" t="s">
         <v>624</v>
       </c>
       <c r="E28" s="137" t="s">
         <v>798</v>
       </c>
-      <c r="F28" s="230" t="s">
+      <c r="F28" s="234" t="s">
         <v>799</v>
       </c>
-      <c r="G28" s="231"/>
-      <c r="H28" s="234" t="s">
+      <c r="G28" s="235"/>
+      <c r="H28" s="236" t="s">
         <v>763</v>
       </c>
     </row>
@@ -15644,21 +15682,21 @@
       <c r="A29" s="137" t="s">
         <v>800</v>
       </c>
-      <c r="B29" s="230" t="s">
+      <c r="B29" s="234" t="s">
         <v>801</v>
       </c>
-      <c r="C29" s="231"/>
-      <c r="D29" s="232" t="s">
+      <c r="C29" s="235"/>
+      <c r="D29" s="237" t="s">
         <v>625</v>
       </c>
       <c r="E29" s="129" t="s">
         <v>802</v>
       </c>
-      <c r="F29" s="224" t="s">
+      <c r="F29" s="231" t="s">
         <v>803</v>
       </c>
-      <c r="G29" s="225"/>
-      <c r="H29" s="233" t="s">
+      <c r="G29" s="232"/>
+      <c r="H29" s="238" t="s">
         <v>765</v>
       </c>
     </row>
@@ -15666,21 +15704,21 @@
       <c r="A30" s="129" t="s">
         <v>804</v>
       </c>
-      <c r="B30" s="224" t="s">
+      <c r="B30" s="231" t="s">
         <v>805</v>
       </c>
-      <c r="C30" s="225"/>
-      <c r="D30" s="226" t="s">
+      <c r="C30" s="232"/>
+      <c r="D30" s="233" t="s">
         <v>626</v>
       </c>
       <c r="E30" s="137" t="s">
         <v>806</v>
       </c>
-      <c r="F30" s="230" t="s">
+      <c r="F30" s="234" t="s">
         <v>807</v>
       </c>
-      <c r="G30" s="231"/>
-      <c r="H30" s="234" t="s">
+      <c r="G30" s="235"/>
+      <c r="H30" s="236" t="s">
         <v>767</v>
       </c>
     </row>
@@ -15688,21 +15726,21 @@
       <c r="A31" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="B31" s="230" t="s">
+      <c r="B31" s="234" t="s">
         <v>809</v>
       </c>
-      <c r="C31" s="231"/>
-      <c r="D31" s="232" t="s">
+      <c r="C31" s="235"/>
+      <c r="D31" s="237" t="s">
         <v>627</v>
       </c>
       <c r="E31" s="129" t="s">
         <v>810</v>
       </c>
-      <c r="F31" s="224" t="s">
+      <c r="F31" s="231" t="s">
         <v>811</v>
       </c>
-      <c r="G31" s="225"/>
-      <c r="H31" s="233" t="s">
+      <c r="G31" s="232"/>
+      <c r="H31" s="238" t="s">
         <v>494</v>
       </c>
     </row>
@@ -15710,17 +15748,17 @@
       <c r="A32" s="129" t="s">
         <v>812</v>
       </c>
-      <c r="B32" s="224" t="s">
+      <c r="B32" s="231" t="s">
         <v>813</v>
       </c>
-      <c r="C32" s="225"/>
-      <c r="D32" s="226" t="s">
+      <c r="C32" s="232"/>
+      <c r="D32" s="233" t="s">
         <v>628</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="230"/>
-      <c r="G32" s="231"/>
-      <c r="H32" s="234" t="s">
+      <c r="F32" s="234"/>
+      <c r="G32" s="235"/>
+      <c r="H32" s="236" t="s">
         <v>495</v>
       </c>
     </row>
@@ -15728,17 +15766,17 @@
       <c r="A33" s="137" t="s">
         <v>814</v>
       </c>
-      <c r="B33" s="230" t="s">
+      <c r="B33" s="234" t="s">
         <v>815</v>
       </c>
-      <c r="C33" s="231"/>
-      <c r="D33" s="232" t="s">
+      <c r="C33" s="235"/>
+      <c r="D33" s="237" t="s">
         <v>622</v>
       </c>
       <c r="E33" s="129"/>
-      <c r="F33" s="224"/>
-      <c r="G33" s="225"/>
-      <c r="H33" s="233" t="s">
+      <c r="F33" s="231"/>
+      <c r="G33" s="232"/>
+      <c r="H33" s="238" t="s">
         <v>759</v>
       </c>
     </row>
@@ -15746,17 +15784,17 @@
       <c r="A34" s="129" t="s">
         <v>816</v>
       </c>
-      <c r="B34" s="224" t="s">
+      <c r="B34" s="231" t="s">
         <v>817</v>
       </c>
-      <c r="C34" s="225"/>
-      <c r="D34" s="226" t="s">
+      <c r="C34" s="232"/>
+      <c r="D34" s="233" t="s">
         <v>623</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="230"/>
-      <c r="G34" s="231"/>
-      <c r="H34" s="234" t="s">
+      <c r="F34" s="234"/>
+      <c r="G34" s="235"/>
+      <c r="H34" s="236" t="s">
         <v>761</v>
       </c>
     </row>
@@ -15764,17 +15802,17 @@
       <c r="A35" s="137" t="s">
         <v>818</v>
       </c>
-      <c r="B35" s="230" t="s">
+      <c r="B35" s="234" t="s">
         <v>819</v>
       </c>
-      <c r="C35" s="231"/>
-      <c r="D35" s="232" t="s">
+      <c r="C35" s="235"/>
+      <c r="D35" s="237" t="s">
         <v>624</v>
       </c>
       <c r="E35" s="129"/>
-      <c r="F35" s="224"/>
-      <c r="G35" s="225"/>
-      <c r="H35" s="233" t="s">
+      <c r="F35" s="231"/>
+      <c r="G35" s="232"/>
+      <c r="H35" s="238" t="s">
         <v>763</v>
       </c>
     </row>
@@ -15782,17 +15820,17 @@
       <c r="A36" s="129" t="s">
         <v>820</v>
       </c>
-      <c r="B36" s="224" t="s">
+      <c r="B36" s="231" t="s">
         <v>821</v>
       </c>
-      <c r="C36" s="225"/>
-      <c r="D36" s="226" t="s">
+      <c r="C36" s="232"/>
+      <c r="D36" s="233" t="s">
         <v>625</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="230"/>
-      <c r="G36" s="231"/>
-      <c r="H36" s="234" t="s">
+      <c r="F36" s="234"/>
+      <c r="G36" s="235"/>
+      <c r="H36" s="236" t="s">
         <v>765</v>
       </c>
     </row>
@@ -15800,17 +15838,17 @@
       <c r="A37" s="137" t="s">
         <v>822</v>
       </c>
-      <c r="B37" s="230" t="s">
+      <c r="B37" s="234" t="s">
         <v>823</v>
       </c>
-      <c r="C37" s="231"/>
-      <c r="D37" s="232" t="s">
+      <c r="C37" s="235"/>
+      <c r="D37" s="237" t="s">
         <v>626</v>
       </c>
       <c r="E37" s="129"/>
-      <c r="F37" s="224"/>
-      <c r="G37" s="225"/>
-      <c r="H37" s="233" t="s">
+      <c r="F37" s="231"/>
+      <c r="G37" s="232"/>
+      <c r="H37" s="238" t="s">
         <v>767</v>
       </c>
     </row>
@@ -15818,17 +15856,17 @@
       <c r="A38" s="129" t="s">
         <v>824</v>
       </c>
-      <c r="B38" s="224" t="s">
+      <c r="B38" s="231" t="s">
         <v>825</v>
       </c>
-      <c r="C38" s="225"/>
-      <c r="D38" s="226" t="s">
+      <c r="C38" s="232"/>
+      <c r="D38" s="233" t="s">
         <v>627</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="230"/>
-      <c r="G38" s="231"/>
-      <c r="H38" s="234" t="s">
+      <c r="F38" s="234"/>
+      <c r="G38" s="235"/>
+      <c r="H38" s="236" t="s">
         <v>494</v>
       </c>
     </row>
@@ -15836,17 +15874,17 @@
       <c r="A39" s="137" t="s">
         <v>826</v>
       </c>
-      <c r="B39" s="230" t="s">
+      <c r="B39" s="234" t="s">
         <v>827</v>
       </c>
-      <c r="C39" s="231"/>
-      <c r="D39" s="232" t="s">
+      <c r="C39" s="235"/>
+      <c r="D39" s="237" t="s">
         <v>628</v>
       </c>
       <c r="E39" s="129"/>
-      <c r="F39" s="224"/>
-      <c r="G39" s="225"/>
-      <c r="H39" s="233" t="s">
+      <c r="F39" s="231"/>
+      <c r="G39" s="232"/>
+      <c r="H39" s="238" t="s">
         <v>495</v>
       </c>
     </row>
@@ -15854,36 +15892,65 @@
       <c r="A40" s="129" t="s">
         <v>828</v>
       </c>
-      <c r="B40" s="224" t="s">
+      <c r="B40" s="231" t="s">
         <v>827</v>
       </c>
-      <c r="C40" s="225"/>
-      <c r="D40" s="226" t="s">
+      <c r="C40" s="232"/>
+      <c r="D40" s="233" t="s">
         <v>628</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="230"/>
-      <c r="G40" s="231"/>
-      <c r="H40" s="234"/>
+      <c r="F40" s="234"/>
+      <c r="G40" s="235"/>
+      <c r="H40" s="236"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>829</v>
       </c>
-      <c r="B41" s="235" t="s">
+      <c r="B41" s="225" t="s">
         <v>827</v>
       </c>
-      <c r="C41" s="236"/>
-      <c r="D41" s="237" t="s">
+      <c r="C41" s="226"/>
+      <c r="D41" s="227" t="s">
         <v>628</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="238"/>
-      <c r="G41" s="239"/>
-      <c r="H41" s="240"/>
+      <c r="F41" s="228"/>
+      <c r="G41" s="229"/>
+      <c r="H41" s="230"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -15892,35 +15959,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added prep for D7
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="906">
   <si>
     <t>AWACS</t>
   </si>
@@ -2624,9 +2624,6 @@
     <t>DALLAS</t>
   </si>
   <si>
-    <t>ORANGE 11</t>
-  </si>
-  <si>
     <t xml:space="preserve">COLT </t>
   </si>
   <si>
@@ -2775,6 +2772,15 @@
   </si>
   <si>
     <t>AH-64D presets  (OPAR) V1.1</t>
+  </si>
+  <si>
+    <t>BERLIN (LCC)</t>
+  </si>
+  <si>
+    <t>127.7</t>
+  </si>
+  <si>
+    <t>128.9</t>
   </si>
 </sst>
 </file>
@@ -4201,15 +4207,63 @@
     <xf numFmtId="164" fontId="19" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4219,27 +4273,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4324,6 +4357,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4342,57 +4426,6 @@
     <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4439,33 +4472,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4510,7 +4516,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4996,8 +5002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AJ57"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P48" sqref="P48"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5048,18 +5054,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="185" t="s">
+      <c r="R3" s="202" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="185"/>
-      <c r="T3" s="185"/>
-      <c r="AA3" s="187" t="s">
+      <c r="S3" s="202"/>
+      <c r="T3" s="202"/>
+      <c r="AA3" s="203" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="188"/>
-      <c r="AC3" s="188"/>
-      <c r="AD3" s="188"/>
-      <c r="AE3" s="189"/>
+      <c r="AB3" s="204"/>
+      <c r="AC3" s="204"/>
+      <c r="AD3" s="204"/>
+      <c r="AE3" s="205"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -5102,7 +5108,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="190" t="s">
+      <c r="R4" s="195" t="s">
         <v>638</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -5111,12 +5117,12 @@
       <c r="T4" s="99" t="s">
         <v>641</v>
       </c>
-      <c r="V4" s="186" t="s">
+      <c r="V4" s="193" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="186"/>
-      <c r="X4" s="186"/>
-      <c r="Y4" s="186"/>
+      <c r="W4" s="193"/>
+      <c r="X4" s="193"/>
+      <c r="Y4" s="193"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -5170,7 +5176,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="191"/>
+      <c r="R5" s="196"/>
       <c r="S5" s="31" t="s">
         <v>607</v>
       </c>
@@ -5248,7 +5254,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="192"/>
+      <c r="R6" s="197"/>
       <c r="S6" s="100" t="s">
         <v>640</v>
       </c>
@@ -5324,7 +5330,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="190" t="s">
+      <c r="R7" s="195" t="s">
         <v>644</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -5404,7 +5410,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="191"/>
+      <c r="R8" s="196"/>
       <c r="S8" s="31" t="s">
         <v>607</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="192"/>
+      <c r="R9" s="197"/>
       <c r="S9" s="100" t="s">
         <v>640</v>
       </c>
@@ -5600,7 +5606,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="194" t="s">
+      <c r="R11" s="198" t="s">
         <v>645</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -5673,7 +5679,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="195"/>
+      <c r="R12" s="199"/>
       <c r="S12" s="97" t="s">
         <v>607</v>
       </c>
@@ -5740,7 +5746,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="196"/>
+      <c r="R13" s="200"/>
       <c r="S13" s="105" t="s">
         <v>640</v>
       </c>
@@ -5763,11 +5769,11 @@
       <c r="AA13" s="41" t="s">
         <v>851</v>
       </c>
-      <c r="AD13" s="187" t="s">
+      <c r="AD13" s="203" t="s">
         <v>630</v>
       </c>
-      <c r="AE13" s="188"/>
-      <c r="AF13" s="189"/>
+      <c r="AE13" s="204"/>
+      <c r="AF13" s="205"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -5814,7 +5820,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="190" t="s">
+      <c r="R14" s="195" t="s">
         <v>648</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -5892,7 +5898,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="191"/>
+      <c r="R15" s="196"/>
       <c r="S15" s="97" t="s">
         <v>607</v>
       </c>
@@ -5953,22 +5959,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="192"/>
+      <c r="R16" s="197"/>
       <c r="S16" s="105" t="s">
         <v>640</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="V16" s="186" t="s">
+      <c r="V16" s="193" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="186"/>
-      <c r="X16" s="186"/>
-      <c r="Y16" s="186"/>
-      <c r="Z16" s="186"/>
-      <c r="AA16" s="186"/>
-      <c r="AB16" s="186"/>
+      <c r="W16" s="193"/>
+      <c r="X16" s="193"/>
+      <c r="Y16" s="193"/>
+      <c r="Z16" s="193"/>
+      <c r="AA16" s="193"/>
+      <c r="AB16" s="193"/>
       <c r="AD16" s="7" t="s">
         <v>623</v>
       </c>
@@ -6260,11 +6266,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="186" t="s">
+      <c r="R20" s="193" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="186"/>
-      <c r="T20" s="186"/>
+      <c r="S20" s="193"/>
+      <c r="T20" s="193"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>672</v>
@@ -6435,15 +6441,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="187" t="s">
+      <c r="V22" s="203" t="s">
         <v>663</v>
       </c>
-      <c r="W22" s="188"/>
-      <c r="X22" s="188"/>
-      <c r="Y22" s="188"/>
-      <c r="Z22" s="188"/>
-      <c r="AA22" s="188"/>
-      <c r="AB22" s="189"/>
+      <c r="W22" s="204"/>
+      <c r="X22" s="204"/>
+      <c r="Y22" s="204"/>
+      <c r="Z22" s="204"/>
+      <c r="AA22" s="204"/>
+      <c r="AB22" s="205"/>
       <c r="AD22" s="7" t="s">
         <v>629</v>
       </c>
@@ -6585,11 +6591,8 @@
       <c r="R24" t="s">
         <v>852</v>
       </c>
-      <c r="S24" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="T24" t="s">
-        <v>853</v>
+      <c r="S24" s="94" t="s">
+        <v>904</v>
       </c>
       <c r="V24" s="39" t="s">
         <v>674</v>
@@ -6666,8 +6669,12 @@
       <c r="P25" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="R25" s="96"/>
-      <c r="S25" s="96"/>
+      <c r="R25" s="96" t="s">
+        <v>903</v>
+      </c>
+      <c r="S25" s="96" t="s">
+        <v>905</v>
+      </c>
       <c r="T25" s="96"/>
       <c r="U25" s="41"/>
       <c r="V25" s="7" t="s">
@@ -6912,33 +6919,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="186" t="s">
+      <c r="B31" s="193" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="186"/>
-      <c r="D31" s="186"/>
-      <c r="E31" s="186"/>
-      <c r="F31" s="186"/>
-      <c r="G31" s="186"/>
-      <c r="H31" s="186"/>
-      <c r="J31" s="186" t="s">
+      <c r="C31" s="193"/>
+      <c r="D31" s="193"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
+      <c r="G31" s="193"/>
+      <c r="H31" s="193"/>
+      <c r="J31" s="193" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="186"/>
-      <c r="L31" s="186"/>
-      <c r="M31" s="186"/>
-      <c r="N31" s="186"/>
-      <c r="O31" s="186"/>
-      <c r="P31" s="186"/>
-      <c r="T31" s="186" t="s">
+      <c r="K31" s="193"/>
+      <c r="L31" s="193"/>
+      <c r="M31" s="193"/>
+      <c r="N31" s="193"/>
+      <c r="O31" s="193"/>
+      <c r="P31" s="193"/>
+      <c r="T31" s="193" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="186"/>
-      <c r="V31" s="186"/>
-      <c r="W31" s="186"/>
-      <c r="X31" s="186"/>
-      <c r="Y31" s="186"/>
-      <c r="Z31" s="186"/>
+      <c r="U31" s="193"/>
+      <c r="V31" s="193"/>
+      <c r="W31" s="193"/>
+      <c r="X31" s="193"/>
+      <c r="Y31" s="193"/>
+      <c r="Z31" s="193"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -7153,7 +7160,7 @@
         <v>699</v>
       </c>
       <c r="AJ34" s="158" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="35" spans="2:36">
@@ -7220,7 +7227,7 @@
       <c r="Z35" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AD35" s="184" t="s">
+      <c r="AD35" s="201" t="s">
         <v>700</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -7239,7 +7246,7 @@
         <v>12</v>
       </c>
       <c r="AJ35" s="38" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="36" spans="2:36">
@@ -7306,7 +7313,7 @@
       <c r="Z36" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD36" s="184"/>
+      <c r="AD36" s="201"/>
       <c r="AE36" s="7"/>
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
@@ -7378,7 +7385,7 @@
       <c r="Z37" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD37" s="184"/>
+      <c r="AD37" s="201"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -7435,7 +7442,7 @@
       <c r="Z38" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="AD38" s="184"/>
+      <c r="AD38" s="201"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -7450,15 +7457,15 @@
       <c r="F39" t="s">
         <v>567</v>
       </c>
-      <c r="J39" s="193" t="s">
+      <c r="J39" s="194" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="193"/>
-      <c r="L39" s="193"/>
-      <c r="M39" s="193"/>
-      <c r="N39" s="193"/>
-      <c r="O39" s="193"/>
-      <c r="P39" s="193"/>
+      <c r="K39" s="194"/>
+      <c r="L39" s="194"/>
+      <c r="M39" s="194"/>
+      <c r="N39" s="194"/>
+      <c r="O39" s="194"/>
+      <c r="P39" s="194"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -7684,13 +7691,13 @@
         <v>839</v>
       </c>
       <c r="J48" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L48" s="168">
         <v>65.599999999999994</v>
       </c>
       <c r="M48" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
@@ -7708,13 +7715,13 @@
         <v>840</v>
       </c>
       <c r="J49" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L49" s="168">
         <v>65.7</v>
       </c>
       <c r="M49" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T49" s="7" t="s">
         <v>694</v>
@@ -7744,13 +7751,13 @@
         <v>841</v>
       </c>
       <c r="J50" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L50" s="168">
         <v>65.8</v>
       </c>
       <c r="M50" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="T50" s="7" t="s">
         <v>695</v>
@@ -7774,13 +7781,13 @@
     </row>
     <row r="51" spans="5:26">
       <c r="J51" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L51" s="168">
         <v>65.900000000000006</v>
       </c>
       <c r="M51" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="T51" s="7" t="s">
         <v>696</v>
@@ -7804,13 +7811,13 @@
     </row>
     <row r="52" spans="5:26">
       <c r="J52" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L52" s="168">
         <v>66</v>
       </c>
       <c r="M52" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="T52" s="7"/>
       <c r="U52" s="7"/>
@@ -7832,68 +7839,61 @@
     </row>
     <row r="53" spans="5:26">
       <c r="J53" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L53" s="168">
         <v>66.099999999999994</v>
       </c>
       <c r="M53" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="54" spans="5:26">
       <c r="J54" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L54" s="168">
         <v>66.2</v>
       </c>
       <c r="M54" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="55" spans="5:26">
       <c r="J55" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L55" s="168">
         <v>66.300000000000097</v>
       </c>
       <c r="M55" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="56" spans="5:26">
       <c r="J56" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L56" s="168">
         <v>66.400000000000105</v>
       </c>
       <c r="M56" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="57" spans="5:26">
       <c r="J57" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="L57" s="168">
         <v>66.500000000000099</v>
       </c>
       <c r="M57" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -7903,6 +7903,13 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7929,34 +7936,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="248" t="s">
+      <c r="A1" s="257" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="248"/>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="248"/>
+      <c r="B1" s="257"/>
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="249"/>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
+      <c r="A2" s="258"/>
+      <c r="B2" s="258"/>
+      <c r="C2" s="258"/>
+      <c r="D2" s="258"/>
+      <c r="E2" s="258"/>
+      <c r="F2" s="258"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="218" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="210"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="209" t="s">
+      <c r="B3" s="219"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="218" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="210"/>
-      <c r="F3" s="211"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="220"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -8313,14 +8320,14 @@
       <c r="F21" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="N21" s="250" t="s">
+      <c r="N21" s="259" t="s">
         <v>838</v>
       </c>
-      <c r="O21" s="250"/>
-      <c r="P21" s="250"/>
-      <c r="Q21" s="250"/>
-      <c r="R21" s="250"/>
-      <c r="S21" s="250"/>
+      <c r="O21" s="259"/>
+      <c r="P21" s="259"/>
+      <c r="Q21" s="259"/>
+      <c r="R21" s="259"/>
+      <c r="S21" s="259"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1">
       <c r="A22" s="54">
@@ -8341,12 +8348,12 @@
       <c r="F22" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="O22" s="251" t="s">
+      <c r="O22" s="260" t="s">
         <v>363</v>
       </c>
-      <c r="P22" s="251"/>
-      <c r="Q22" s="251"/>
-      <c r="R22" s="251"/>
+      <c r="P22" s="260"/>
+      <c r="Q22" s="260"/>
+      <c r="R22" s="260"/>
     </row>
     <row r="23" spans="1:19" ht="19.5" thickBot="1">
       <c r="A23" s="54">
@@ -8603,22 +8610,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="259" t="s">
         <v>838</v>
       </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="250"/>
-      <c r="E1" s="250"/>
-      <c r="F1" s="250"/>
+      <c r="B1" s="259"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
+      <c r="E1" s="259"/>
+      <c r="F1" s="259"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="251" t="s">
+      <c r="B2" s="260" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="251"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -8831,7 +8838,7 @@
         <v>729</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -8858,7 +8865,7 @@
         <v>387</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="S2" s="66" t="s">
         <v>753</v>
@@ -8910,7 +8917,7 @@
         <v>387</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="S3" s="66"/>
       <c r="T3" s="66"/>
@@ -8958,7 +8965,7 @@
         <v>387</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="S4" s="66"/>
       <c r="T4" s="66"/>
@@ -9006,7 +9013,7 @@
         <v>387</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="S5" s="66"/>
       <c r="T5" s="66"/>
@@ -9022,7 +9029,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B6" s="7">
         <v>2</v>
@@ -9037,7 +9044,7 @@
         <v>729</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
@@ -9064,7 +9071,7 @@
         <v>387</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -9101,7 +9108,7 @@
         <v>387</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -9138,7 +9145,7 @@
         <v>387</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -9175,12 +9182,12 @@
         <v>387</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B10" s="7">
         <v>3</v>
@@ -9195,7 +9202,7 @@
         <v>729</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="H10" s="7">
         <v>3</v>
@@ -9440,7 +9447,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="7" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B18" s="7">
         <v>5</v>
@@ -9522,7 +9529,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="7" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B22" s="7">
         <v>6</v>
@@ -9577,7 +9584,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="M23" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N23" s="7">
         <v>1</v>
@@ -9586,10 +9593,10 @@
         <v>711</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -9612,7 +9619,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="M24" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N24" s="7">
         <v>1</v>
@@ -9621,10 +9628,10 @@
         <v>712</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -9647,7 +9654,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="M25" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N25" s="7">
         <v>1</v>
@@ -9656,10 +9663,10 @@
         <v>713</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -9674,7 +9681,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="M26" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N26" s="7">
         <v>1</v>
@@ -9683,10 +9690,10 @@
         <v>714</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q26" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -9701,7 +9708,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="M27" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N27" s="7">
         <v>2</v>
@@ -9710,10 +9717,10 @@
         <v>721</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -9728,7 +9735,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="M28" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N28" s="7">
         <v>2</v>
@@ -9737,10 +9744,10 @@
         <v>722</v>
       </c>
       <c r="P28" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -9755,7 +9762,7 @@
       <c r="J29" s="169"/>
       <c r="K29" s="169"/>
       <c r="M29" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N29" s="7">
         <v>2</v>
@@ -9764,10 +9771,10 @@
         <v>723</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -9782,7 +9789,7 @@
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="M30" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N30" s="7">
         <v>2</v>
@@ -9791,10 +9798,10 @@
         <v>724</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="Q30" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -9910,7 +9917,7 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="7" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
@@ -10050,7 +10057,7 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="7" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B44" s="7">
         <v>2</v>
@@ -10201,7 +10208,7 @@
         <v>756</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H50" s="2">
         <v>3</v>
@@ -10213,7 +10220,7 @@
         <v>601</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -10229,7 +10236,7 @@
         <v>756</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2">
@@ -10239,7 +10246,7 @@
         <v>601</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -10259,7 +10266,7 @@
         <v>756</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2">
@@ -10269,7 +10276,7 @@
         <v>601</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -10285,7 +10292,7 @@
         <v>756</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2">
@@ -10295,7 +10302,7 @@
         <v>601</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -10354,7 +10361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -10372,40 +10379,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="258" t="s">
-        <v>903</v>
-      </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="260"/>
+      <c r="A1" s="267" t="s">
+        <v>902</v>
+      </c>
+      <c r="B1" s="268"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="269"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="261"/>
-      <c r="B2" s="262"/>
-      <c r="C2" s="262"/>
-      <c r="D2" s="262"/>
-      <c r="E2" s="262"/>
-      <c r="F2" s="262"/>
-      <c r="G2" s="262"/>
-      <c r="H2" s="263"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="271"/>
+      <c r="C2" s="271"/>
+      <c r="D2" s="271"/>
+      <c r="E2" s="271"/>
+      <c r="F2" s="271"/>
+      <c r="G2" s="271"/>
+      <c r="H2" s="272"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="252" t="s">
+      <c r="A3" s="261" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="254"/>
-      <c r="E3" s="252" t="s">
-        <v>858</v>
-      </c>
-      <c r="F3" s="253"/>
-      <c r="G3" s="253"/>
-      <c r="H3" s="254"/>
+      <c r="B3" s="262"/>
+      <c r="C3" s="262"/>
+      <c r="D3" s="263"/>
+      <c r="E3" s="261" t="s">
+        <v>857</v>
+      </c>
+      <c r="F3" s="262"/>
+      <c r="G3" s="262"/>
+      <c r="H3" s="263"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="178">
@@ -10418,7 +10425,7 @@
         <v>479</v>
       </c>
       <c r="D4" s="180" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E4" s="178">
         <v>1</v>
@@ -10444,7 +10451,7 @@
         <v>484</v>
       </c>
       <c r="D5" s="180" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E5" s="178">
         <v>2</v>
@@ -10470,7 +10477,7 @@
         <v>652</v>
       </c>
       <c r="D6" s="180" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E6" s="178">
         <v>3</v>
@@ -10496,7 +10503,7 @@
         <v>653</v>
       </c>
       <c r="D7" s="180" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E7" s="178">
         <v>4</v>
@@ -10522,7 +10529,7 @@
         <v>654</v>
       </c>
       <c r="D8" s="180" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E8" s="178">
         <v>5</v>
@@ -10548,7 +10555,7 @@
         <v>485</v>
       </c>
       <c r="D9" s="180" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E9" s="178">
         <v>6</v>
@@ -10574,7 +10581,7 @@
         <v>487</v>
       </c>
       <c r="D10" s="180" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E10" s="178">
         <v>7</v>
@@ -10586,7 +10593,7 @@
         <v>378</v>
       </c>
       <c r="H10" s="180" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17.25" thickBot="1">
@@ -10604,7 +10611,7 @@
         <v>491</v>
       </c>
       <c r="H11" s="180" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" thickBot="1">
@@ -10622,7 +10629,7 @@
         <v>496</v>
       </c>
       <c r="H12" s="180" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17.25" thickBot="1">
@@ -10640,7 +10647,7 @@
         <v>556</v>
       </c>
       <c r="H13" s="180" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -10724,18 +10731,18 @@
       <c r="H21" s="170"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="255" t="s">
+      <c r="A22" s="264" t="s">
+        <v>858</v>
+      </c>
+      <c r="B22" s="265"/>
+      <c r="C22" s="265"/>
+      <c r="D22" s="266"/>
+      <c r="E22" s="264" t="s">
         <v>859</v>
       </c>
-      <c r="B22" s="256"/>
-      <c r="C22" s="256"/>
-      <c r="D22" s="257"/>
-      <c r="E22" s="255" t="s">
-        <v>860</v>
-      </c>
-      <c r="F22" s="256"/>
-      <c r="G22" s="256"/>
-      <c r="H22" s="257"/>
+      <c r="F22" s="265"/>
+      <c r="G22" s="265"/>
+      <c r="H22" s="266"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="161">
@@ -10745,10 +10752,10 @@
         <v>65.599999999999994</v>
       </c>
       <c r="C23" s="160" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D23" s="160" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E23" s="161">
         <v>1</v>
@@ -10760,7 +10767,7 @@
         <v>523</v>
       </c>
       <c r="H23" s="167" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1">
@@ -10771,10 +10778,10 @@
         <v>65.7</v>
       </c>
       <c r="C24" s="163" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D24" s="163" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E24" s="161">
         <v>2</v>
@@ -10786,7 +10793,7 @@
         <v>463</v>
       </c>
       <c r="H24" s="167" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16.5" thickBot="1">
@@ -10797,10 +10804,10 @@
         <v>65.8</v>
       </c>
       <c r="C25" s="163" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D25" s="163" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E25" s="161">
         <v>3</v>
@@ -10812,7 +10819,7 @@
         <v>466</v>
       </c>
       <c r="H25" s="167" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="16.5" thickBot="1">
@@ -10823,10 +10830,10 @@
         <v>65.900000000000006</v>
       </c>
       <c r="C26" s="163" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D26" s="163" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E26" s="161">
         <v>4</v>
@@ -10838,7 +10845,7 @@
         <v>467</v>
       </c>
       <c r="H26" s="167" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickBot="1">
@@ -10849,10 +10856,10 @@
         <v>66</v>
       </c>
       <c r="C27" s="163" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D27" s="163" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E27" s="161">
         <v>5</v>
@@ -10864,7 +10871,7 @@
         <v>469</v>
       </c>
       <c r="H27" s="167" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1">
@@ -10875,10 +10882,10 @@
         <v>66.099999999999994</v>
       </c>
       <c r="C28" s="163" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D28" s="163" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E28" s="161">
         <v>6</v>
@@ -10890,7 +10897,7 @@
         <v>471</v>
       </c>
       <c r="H28" s="167" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16.5" thickBot="1">
@@ -10901,10 +10908,10 @@
         <v>66.2</v>
       </c>
       <c r="C29" s="163" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D29" s="163" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E29" s="161">
         <v>7</v>
@@ -10916,7 +10923,7 @@
         <v>473</v>
       </c>
       <c r="H29" s="167" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16.5" thickBot="1">
@@ -10927,10 +10934,10 @@
         <v>66.300000000000097</v>
       </c>
       <c r="C30" s="163" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D30" s="163" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E30" s="161">
         <v>8</v>
@@ -10951,10 +10958,10 @@
         <v>66.400000000000105</v>
       </c>
       <c r="C31" s="164" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D31" s="164" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E31" s="161">
         <v>9</v>
@@ -10968,19 +10975,19 @@
       <c r="H31" s="164"/>
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A32" s="267">
+      <c r="A32" s="187">
         <v>10</v>
       </c>
       <c r="B32" s="162">
         <v>66.500000000000099</v>
       </c>
       <c r="C32" s="164" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D32" s="164" t="s">
-        <v>870</v>
-      </c>
-      <c r="E32" s="267">
+        <v>869</v>
+      </c>
+      <c r="E32" s="187">
         <v>10</v>
       </c>
       <c r="F32" s="165">
@@ -10993,102 +11000,102 @@
     </row>
     <row r="33" spans="1:8" ht="15.75">
       <c r="A33" s="181"/>
-      <c r="B33" s="264"/>
-      <c r="C33" s="265"/>
-      <c r="D33" s="266"/>
+      <c r="B33" s="184"/>
+      <c r="C33" s="185"/>
+      <c r="D33" s="186"/>
       <c r="E33" s="172"/>
-      <c r="F33" s="264"/>
-      <c r="G33" s="265"/>
+      <c r="F33" s="184"/>
+      <c r="G33" s="185"/>
       <c r="H33" s="170"/>
     </row>
     <row r="34" spans="1:8" ht="15.75">
       <c r="A34" s="181"/>
-      <c r="B34" s="264"/>
-      <c r="C34" s="265"/>
-      <c r="D34" s="266"/>
+      <c r="B34" s="184"/>
+      <c r="C34" s="185"/>
+      <c r="D34" s="186"/>
       <c r="E34" s="172"/>
-      <c r="F34" s="264"/>
-      <c r="G34" s="265"/>
+      <c r="F34" s="184"/>
+      <c r="G34" s="185"/>
       <c r="H34" s="170"/>
     </row>
     <row r="35" spans="1:8" ht="15.75">
       <c r="A35" s="181"/>
-      <c r="B35" s="264"/>
-      <c r="C35" s="265"/>
-      <c r="D35" s="266"/>
+      <c r="B35" s="184"/>
+      <c r="C35" s="185"/>
+      <c r="D35" s="186"/>
       <c r="E35" s="172"/>
-      <c r="F35" s="264"/>
-      <c r="G35" s="265"/>
+      <c r="F35" s="184"/>
+      <c r="G35" s="185"/>
       <c r="H35" s="170"/>
     </row>
     <row r="36" spans="1:8" ht="15.75">
       <c r="A36" s="181"/>
-      <c r="B36" s="264"/>
-      <c r="C36" s="265"/>
-      <c r="D36" s="266"/>
+      <c r="B36" s="184"/>
+      <c r="C36" s="185"/>
+      <c r="D36" s="186"/>
       <c r="E36" s="172"/>
-      <c r="F36" s="264"/>
-      <c r="G36" s="265"/>
+      <c r="F36" s="184"/>
+      <c r="G36" s="185"/>
       <c r="H36" s="170"/>
     </row>
     <row r="37" spans="1:8" ht="15.75">
       <c r="A37" s="181"/>
-      <c r="B37" s="264"/>
-      <c r="C37" s="265"/>
-      <c r="D37" s="266"/>
+      <c r="B37" s="184"/>
+      <c r="C37" s="185"/>
+      <c r="D37" s="186"/>
       <c r="E37" s="172"/>
-      <c r="F37" s="264"/>
-      <c r="G37" s="265"/>
+      <c r="F37" s="184"/>
+      <c r="G37" s="185"/>
       <c r="H37" s="170"/>
     </row>
     <row r="38" spans="1:8" ht="15.75">
       <c r="A38" s="181"/>
-      <c r="B38" s="264"/>
-      <c r="C38" s="265"/>
-      <c r="D38" s="266"/>
+      <c r="B38" s="184"/>
+      <c r="C38" s="185"/>
+      <c r="D38" s="186"/>
       <c r="E38" s="172"/>
-      <c r="F38" s="264"/>
-      <c r="G38" s="265"/>
+      <c r="F38" s="184"/>
+      <c r="G38" s="185"/>
       <c r="H38" s="170"/>
     </row>
     <row r="39" spans="1:8" ht="15.75">
       <c r="A39" s="181"/>
-      <c r="B39" s="264"/>
-      <c r="C39" s="265"/>
-      <c r="D39" s="266"/>
+      <c r="B39" s="184"/>
+      <c r="C39" s="185"/>
+      <c r="D39" s="186"/>
       <c r="E39" s="172"/>
-      <c r="F39" s="264"/>
-      <c r="G39" s="265"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="185"/>
       <c r="H39" s="170"/>
     </row>
     <row r="40" spans="1:8" ht="15.75">
       <c r="A40" s="181"/>
-      <c r="B40" s="264"/>
-      <c r="C40" s="265"/>
+      <c r="B40" s="184"/>
+      <c r="C40" s="185"/>
       <c r="D40" s="174"/>
       <c r="E40" s="172"/>
-      <c r="F40" s="264"/>
-      <c r="G40" s="265"/>
+      <c r="F40" s="184"/>
+      <c r="G40" s="185"/>
       <c r="H40" s="170"/>
     </row>
     <row r="41" spans="1:8" ht="15.75">
       <c r="A41" s="181"/>
-      <c r="B41" s="264"/>
-      <c r="C41" s="265"/>
+      <c r="B41" s="184"/>
+      <c r="C41" s="185"/>
       <c r="D41" s="174"/>
       <c r="E41" s="172"/>
-      <c r="F41" s="264"/>
-      <c r="G41" s="265"/>
+      <c r="F41" s="184"/>
+      <c r="G41" s="185"/>
       <c r="H41" s="170"/>
     </row>
     <row r="42" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A42" s="268"/>
-      <c r="B42" s="269"/>
-      <c r="C42" s="270"/>
-      <c r="D42" s="271"/>
-      <c r="E42" s="272"/>
-      <c r="F42" s="269"/>
-      <c r="G42" s="270"/>
+      <c r="A42" s="188"/>
+      <c r="B42" s="189"/>
+      <c r="C42" s="190"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="189"/>
+      <c r="G42" s="190"/>
       <c r="H42" s="160"/>
     </row>
   </sheetData>
@@ -11126,40 +11133,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="206" t="s">
         <v>701</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="199"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="207"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="208"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="200"/>
-      <c r="B2" s="201"/>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="202"/>
+      <c r="A2" s="209"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="211"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="212" t="s">
         <v>608</v>
       </c>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204" t="s">
+      <c r="B3" s="213"/>
+      <c r="C3" s="213"/>
+      <c r="D3" s="213"/>
+      <c r="E3" s="213" t="s">
         <v>609</v>
       </c>
-      <c r="F3" s="204"/>
-      <c r="G3" s="204"/>
-      <c r="H3" s="205"/>
+      <c r="F3" s="213"/>
+      <c r="G3" s="213"/>
+      <c r="H3" s="214"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="78">
@@ -12192,14 +12199,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="215" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="208"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="217"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -12210,16 +12217,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="218" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="210"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="209" t="s">
+      <c r="B3" s="219"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="218" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="210"/>
-      <c r="F3" s="211"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="220"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -12489,28 +12496,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="224" t="s">
         <v>737</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
-      <c r="G1" s="215"/>
-      <c r="H1" s="215"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
+      <c r="G1" s="224"/>
+      <c r="H1" s="224"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="212" t="s">
+      <c r="A2" s="221" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-      <c r="H2" s="214"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -12785,16 +12792,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="212" t="s">
+      <c r="A15" s="221" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="213"/>
-      <c r="C15" s="213"/>
-      <c r="D15" s="213"/>
-      <c r="E15" s="213"/>
-      <c r="F15" s="213"/>
-      <c r="G15" s="213"/>
-      <c r="H15" s="214"/>
+      <c r="B15" s="222"/>
+      <c r="C15" s="222"/>
+      <c r="D15" s="222"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="222"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="223"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -13084,16 +13091,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="212" t="s">
+      <c r="A28" s="221" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="213"/>
-      <c r="C28" s="213"/>
-      <c r="D28" s="213"/>
-      <c r="E28" s="213"/>
-      <c r="F28" s="213"/>
-      <c r="G28" s="213"/>
-      <c r="H28" s="214"/>
+      <c r="B28" s="222"/>
+      <c r="C28" s="222"/>
+      <c r="D28" s="222"/>
+      <c r="E28" s="222"/>
+      <c r="F28" s="222"/>
+      <c r="G28" s="222"/>
+      <c r="H28" s="223"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -13406,12 +13413,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="225" t="s">
         <v>713</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
+      <c r="B1" s="225"/>
+      <c r="C1" s="225"/>
+      <c r="D1" s="225"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -13619,28 +13626,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="217" t="s">
+      <c r="A1" s="226" t="s">
         <v>751</v>
       </c>
-      <c r="B1" s="217"/>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="217"/>
-      <c r="H1" s="217"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="212" t="s">
+      <c r="A2" s="221" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
-      <c r="H2" s="214"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="223"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -13931,12 +13938,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="212" t="s">
+      <c r="A15" s="221" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="213"/>
-      <c r="C15" s="213"/>
-      <c r="D15" s="214"/>
+      <c r="B15" s="222"/>
+      <c r="C15" s="222"/>
+      <c r="D15" s="223"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -14104,12 +14111,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="212" t="s">
+      <c r="A28" s="221" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="213"/>
-      <c r="C28" s="213"/>
-      <c r="D28" s="214"/>
+      <c r="B28" s="222"/>
+      <c r="C28" s="222"/>
+      <c r="D28" s="223"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -14313,40 +14320,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="215" t="s">
         <v>832</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="208"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="217"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="218"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="220"/>
+      <c r="A2" s="227"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="229"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="221" t="s">
+      <c r="A3" s="230" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="222"/>
-      <c r="C3" s="223"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="221" t="s">
+      <c r="B3" s="231"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="230" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="223"/>
-      <c r="H3" s="224"/>
+      <c r="F3" s="231"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="233"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="74">
@@ -15039,40 +15046,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="242" t="s">
+      <c r="A1" s="234" t="s">
         <v>830</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
+      <c r="B1" s="234"/>
+      <c r="C1" s="234"/>
+      <c r="D1" s="234"/>
+      <c r="E1" s="234"/>
+      <c r="F1" s="234"/>
+      <c r="G1" s="234"/>
+      <c r="H1" s="234"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="243"/>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
+      <c r="A2" s="235"/>
+      <c r="B2" s="235"/>
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+      <c r="E2" s="235"/>
+      <c r="F2" s="235"/>
+      <c r="G2" s="235"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="236" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="247"/>
-      <c r="E3" s="244" t="s">
+      <c r="B3" s="237"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="236" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="245"/>
-      <c r="G3" s="246"/>
-      <c r="H3" s="247"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="238"/>
+      <c r="H3" s="239"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -15601,36 +15608,36 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="244" t="s">
+      <c r="A25" s="236" t="s">
         <v>786</v>
       </c>
-      <c r="B25" s="245"/>
-      <c r="C25" s="246"/>
-      <c r="D25" s="247"/>
-      <c r="E25" s="244" t="s">
+      <c r="B25" s="237"/>
+      <c r="C25" s="238"/>
+      <c r="D25" s="239"/>
+      <c r="E25" s="236" t="s">
         <v>787</v>
       </c>
-      <c r="F25" s="245"/>
-      <c r="G25" s="246"/>
-      <c r="H25" s="247"/>
+      <c r="F25" s="237"/>
+      <c r="G25" s="238"/>
+      <c r="H25" s="239"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
         <v>788</v>
       </c>
-      <c r="B26" s="231" t="s">
+      <c r="B26" s="240" t="s">
         <v>789</v>
       </c>
-      <c r="C26" s="232"/>
-      <c r="D26" s="233"/>
+      <c r="C26" s="241"/>
+      <c r="D26" s="242"/>
       <c r="E26" s="125" t="s">
         <v>790</v>
       </c>
-      <c r="F26" s="239" t="s">
+      <c r="F26" s="243" t="s">
         <v>791</v>
       </c>
-      <c r="G26" s="240"/>
-      <c r="H26" s="241" t="s">
+      <c r="G26" s="244"/>
+      <c r="H26" s="245" t="s">
         <v>759</v>
       </c>
     </row>
@@ -15638,21 +15645,21 @@
       <c r="A27" s="137" t="s">
         <v>792</v>
       </c>
-      <c r="B27" s="234" t="s">
+      <c r="B27" s="246" t="s">
         <v>793</v>
       </c>
-      <c r="C27" s="235"/>
-      <c r="D27" s="237" t="s">
+      <c r="C27" s="247"/>
+      <c r="D27" s="248" t="s">
         <v>623</v>
       </c>
       <c r="E27" s="129" t="s">
         <v>794</v>
       </c>
-      <c r="F27" s="231" t="s">
+      <c r="F27" s="240" t="s">
         <v>795</v>
       </c>
-      <c r="G27" s="232"/>
-      <c r="H27" s="238" t="s">
+      <c r="G27" s="241"/>
+      <c r="H27" s="249" t="s">
         <v>761</v>
       </c>
     </row>
@@ -15660,21 +15667,21 @@
       <c r="A28" s="129" t="s">
         <v>796</v>
       </c>
-      <c r="B28" s="231" t="s">
+      <c r="B28" s="240" t="s">
         <v>797</v>
       </c>
-      <c r="C28" s="232"/>
-      <c r="D28" s="233" t="s">
+      <c r="C28" s="241"/>
+      <c r="D28" s="242" t="s">
         <v>624</v>
       </c>
       <c r="E28" s="137" t="s">
         <v>798</v>
       </c>
-      <c r="F28" s="234" t="s">
+      <c r="F28" s="246" t="s">
         <v>799</v>
       </c>
-      <c r="G28" s="235"/>
-      <c r="H28" s="236" t="s">
+      <c r="G28" s="247"/>
+      <c r="H28" s="250" t="s">
         <v>763</v>
       </c>
     </row>
@@ -15682,21 +15689,21 @@
       <c r="A29" s="137" t="s">
         <v>800</v>
       </c>
-      <c r="B29" s="234" t="s">
+      <c r="B29" s="246" t="s">
         <v>801</v>
       </c>
-      <c r="C29" s="235"/>
-      <c r="D29" s="237" t="s">
+      <c r="C29" s="247"/>
+      <c r="D29" s="248" t="s">
         <v>625</v>
       </c>
       <c r="E29" s="129" t="s">
         <v>802</v>
       </c>
-      <c r="F29" s="231" t="s">
+      <c r="F29" s="240" t="s">
         <v>803</v>
       </c>
-      <c r="G29" s="232"/>
-      <c r="H29" s="238" t="s">
+      <c r="G29" s="241"/>
+      <c r="H29" s="249" t="s">
         <v>765</v>
       </c>
     </row>
@@ -15704,21 +15711,21 @@
       <c r="A30" s="129" t="s">
         <v>804</v>
       </c>
-      <c r="B30" s="231" t="s">
+      <c r="B30" s="240" t="s">
         <v>805</v>
       </c>
-      <c r="C30" s="232"/>
-      <c r="D30" s="233" t="s">
+      <c r="C30" s="241"/>
+      <c r="D30" s="242" t="s">
         <v>626</v>
       </c>
       <c r="E30" s="137" t="s">
         <v>806</v>
       </c>
-      <c r="F30" s="234" t="s">
+      <c r="F30" s="246" t="s">
         <v>807</v>
       </c>
-      <c r="G30" s="235"/>
-      <c r="H30" s="236" t="s">
+      <c r="G30" s="247"/>
+      <c r="H30" s="250" t="s">
         <v>767</v>
       </c>
     </row>
@@ -15726,21 +15733,21 @@
       <c r="A31" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="B31" s="234" t="s">
+      <c r="B31" s="246" t="s">
         <v>809</v>
       </c>
-      <c r="C31" s="235"/>
-      <c r="D31" s="237" t="s">
+      <c r="C31" s="247"/>
+      <c r="D31" s="248" t="s">
         <v>627</v>
       </c>
       <c r="E31" s="129" t="s">
         <v>810</v>
       </c>
-      <c r="F31" s="231" t="s">
+      <c r="F31" s="240" t="s">
         <v>811</v>
       </c>
-      <c r="G31" s="232"/>
-      <c r="H31" s="238" t="s">
+      <c r="G31" s="241"/>
+      <c r="H31" s="249" t="s">
         <v>494</v>
       </c>
     </row>
@@ -15748,17 +15755,17 @@
       <c r="A32" s="129" t="s">
         <v>812</v>
       </c>
-      <c r="B32" s="231" t="s">
+      <c r="B32" s="240" t="s">
         <v>813</v>
       </c>
-      <c r="C32" s="232"/>
-      <c r="D32" s="233" t="s">
+      <c r="C32" s="241"/>
+      <c r="D32" s="242" t="s">
         <v>628</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="234"/>
-      <c r="G32" s="235"/>
-      <c r="H32" s="236" t="s">
+      <c r="F32" s="246"/>
+      <c r="G32" s="247"/>
+      <c r="H32" s="250" t="s">
         <v>495</v>
       </c>
     </row>
@@ -15766,17 +15773,17 @@
       <c r="A33" s="137" t="s">
         <v>814</v>
       </c>
-      <c r="B33" s="234" t="s">
+      <c r="B33" s="246" t="s">
         <v>815</v>
       </c>
-      <c r="C33" s="235"/>
-      <c r="D33" s="237" t="s">
+      <c r="C33" s="247"/>
+      <c r="D33" s="248" t="s">
         <v>622</v>
       </c>
       <c r="E33" s="129"/>
-      <c r="F33" s="231"/>
-      <c r="G33" s="232"/>
-      <c r="H33" s="238" t="s">
+      <c r="F33" s="240"/>
+      <c r="G33" s="241"/>
+      <c r="H33" s="249" t="s">
         <v>759</v>
       </c>
     </row>
@@ -15784,17 +15791,17 @@
       <c r="A34" s="129" t="s">
         <v>816</v>
       </c>
-      <c r="B34" s="231" t="s">
+      <c r="B34" s="240" t="s">
         <v>817</v>
       </c>
-      <c r="C34" s="232"/>
-      <c r="D34" s="233" t="s">
+      <c r="C34" s="241"/>
+      <c r="D34" s="242" t="s">
         <v>623</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="234"/>
-      <c r="G34" s="235"/>
-      <c r="H34" s="236" t="s">
+      <c r="F34" s="246"/>
+      <c r="G34" s="247"/>
+      <c r="H34" s="250" t="s">
         <v>761</v>
       </c>
     </row>
@@ -15802,17 +15809,17 @@
       <c r="A35" s="137" t="s">
         <v>818</v>
       </c>
-      <c r="B35" s="234" t="s">
+      <c r="B35" s="246" t="s">
         <v>819</v>
       </c>
-      <c r="C35" s="235"/>
-      <c r="D35" s="237" t="s">
+      <c r="C35" s="247"/>
+      <c r="D35" s="248" t="s">
         <v>624</v>
       </c>
       <c r="E35" s="129"/>
-      <c r="F35" s="231"/>
-      <c r="G35" s="232"/>
-      <c r="H35" s="238" t="s">
+      <c r="F35" s="240"/>
+      <c r="G35" s="241"/>
+      <c r="H35" s="249" t="s">
         <v>763</v>
       </c>
     </row>
@@ -15820,17 +15827,17 @@
       <c r="A36" s="129" t="s">
         <v>820</v>
       </c>
-      <c r="B36" s="231" t="s">
+      <c r="B36" s="240" t="s">
         <v>821</v>
       </c>
-      <c r="C36" s="232"/>
-      <c r="D36" s="233" t="s">
+      <c r="C36" s="241"/>
+      <c r="D36" s="242" t="s">
         <v>625</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="234"/>
-      <c r="G36" s="235"/>
-      <c r="H36" s="236" t="s">
+      <c r="F36" s="246"/>
+      <c r="G36" s="247"/>
+      <c r="H36" s="250" t="s">
         <v>765</v>
       </c>
     </row>
@@ -15838,17 +15845,17 @@
       <c r="A37" s="137" t="s">
         <v>822</v>
       </c>
-      <c r="B37" s="234" t="s">
+      <c r="B37" s="246" t="s">
         <v>823</v>
       </c>
-      <c r="C37" s="235"/>
-      <c r="D37" s="237" t="s">
+      <c r="C37" s="247"/>
+      <c r="D37" s="248" t="s">
         <v>626</v>
       </c>
       <c r="E37" s="129"/>
-      <c r="F37" s="231"/>
-      <c r="G37" s="232"/>
-      <c r="H37" s="238" t="s">
+      <c r="F37" s="240"/>
+      <c r="G37" s="241"/>
+      <c r="H37" s="249" t="s">
         <v>767</v>
       </c>
     </row>
@@ -15856,17 +15863,17 @@
       <c r="A38" s="129" t="s">
         <v>824</v>
       </c>
-      <c r="B38" s="231" t="s">
+      <c r="B38" s="240" t="s">
         <v>825</v>
       </c>
-      <c r="C38" s="232"/>
-      <c r="D38" s="233" t="s">
+      <c r="C38" s="241"/>
+      <c r="D38" s="242" t="s">
         <v>627</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="234"/>
-      <c r="G38" s="235"/>
-      <c r="H38" s="236" t="s">
+      <c r="F38" s="246"/>
+      <c r="G38" s="247"/>
+      <c r="H38" s="250" t="s">
         <v>494</v>
       </c>
     </row>
@@ -15874,17 +15881,17 @@
       <c r="A39" s="137" t="s">
         <v>826</v>
       </c>
-      <c r="B39" s="234" t="s">
+      <c r="B39" s="246" t="s">
         <v>827</v>
       </c>
-      <c r="C39" s="235"/>
-      <c r="D39" s="237" t="s">
+      <c r="C39" s="247"/>
+      <c r="D39" s="248" t="s">
         <v>628</v>
       </c>
       <c r="E39" s="129"/>
-      <c r="F39" s="231"/>
-      <c r="G39" s="232"/>
-      <c r="H39" s="238" t="s">
+      <c r="F39" s="240"/>
+      <c r="G39" s="241"/>
+      <c r="H39" s="249" t="s">
         <v>495</v>
       </c>
     </row>
@@ -15892,65 +15899,36 @@
       <c r="A40" s="129" t="s">
         <v>828</v>
       </c>
-      <c r="B40" s="231" t="s">
+      <c r="B40" s="240" t="s">
         <v>827</v>
       </c>
-      <c r="C40" s="232"/>
-      <c r="D40" s="233" t="s">
+      <c r="C40" s="241"/>
+      <c r="D40" s="242" t="s">
         <v>628</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="234"/>
-      <c r="G40" s="235"/>
-      <c r="H40" s="236"/>
+      <c r="F40" s="246"/>
+      <c r="G40" s="247"/>
+      <c r="H40" s="250"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>829</v>
       </c>
-      <c r="B41" s="225" t="s">
+      <c r="B41" s="251" t="s">
         <v>827</v>
       </c>
-      <c r="C41" s="226"/>
-      <c r="D41" s="227" t="s">
+      <c r="C41" s="252"/>
+      <c r="D41" s="253" t="s">
         <v>628</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="228"/>
-      <c r="G41" s="229"/>
-      <c r="H41" s="230"/>
+      <c r="F41" s="254"/>
+      <c r="G41" s="255"/>
+      <c r="H41" s="256"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -15959,6 +15937,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Add TWR and ATIS freq for Gazintiep
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
+++ b/COMMUNICATIONS/OPAR Frequency and Callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="F-15 Presets " sheetId="17" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="913">
   <si>
     <t>AWACS</t>
   </si>
@@ -2791,6 +2791,18 @@
   </si>
   <si>
     <t>F-15 presets  (OPAR) V1.0</t>
+  </si>
+  <si>
+    <t>Gazientep</t>
+  </si>
+  <si>
+    <t>120.1</t>
+  </si>
+  <si>
+    <t>120.6</t>
+  </si>
+  <si>
+    <t>120.2</t>
   </si>
 </sst>
 </file>
@@ -3151,7 +3163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -3790,11 +3802,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4244,15 +4267,81 @@
     <xf numFmtId="0" fontId="19" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4262,54 +4351,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4367,6 +4408,57 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4385,57 +4477,6 @@
     <xf numFmtId="49" fontId="12" fillId="21" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="21" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="16" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4484,24 +4525,8 @@
     <xf numFmtId="0" fontId="25" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4544,7 +4569,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5030,7 +5055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -5048,40 +5073,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="199" t="s">
         <v>908</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="208"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="201"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="209"/>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="211"/>
+      <c r="A2" s="202"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="204"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="205" t="s">
         <v>907</v>
       </c>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
-      <c r="E3" s="213" t="s">
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206" t="s">
         <v>906</v>
       </c>
-      <c r="F3" s="213"/>
-      <c r="G3" s="213"/>
-      <c r="H3" s="214"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="78">
@@ -5568,228 +5593,228 @@
       <c r="D23" s="88" t="s">
         <v>520</v>
       </c>
-      <c r="E23" s="273">
+      <c r="E23" s="193">
         <v>20</v>
       </c>
-      <c r="F23" s="276"/>
-      <c r="G23" s="277"/>
-      <c r="H23" s="276"/>
+      <c r="F23" s="196"/>
+      <c r="G23" s="197"/>
+      <c r="H23" s="196"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" thickBot="1">
       <c r="A24" s="82"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83"/>
       <c r="D24" s="83"/>
-      <c r="E24" s="275">
+      <c r="E24" s="195">
         <v>21</v>
       </c>
-      <c r="F24" s="274"/>
-      <c r="G24" s="278"/>
-      <c r="H24" s="274"/>
+      <c r="F24" s="194"/>
+      <c r="G24" s="198"/>
+      <c r="H24" s="194"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
       <c r="A25" s="82"/>
       <c r="B25" s="83"/>
       <c r="C25" s="83"/>
       <c r="D25" s="83"/>
-      <c r="E25" s="275">
+      <c r="E25" s="195">
         <v>22</v>
       </c>
-      <c r="F25" s="274"/>
-      <c r="G25" s="278"/>
-      <c r="H25" s="274"/>
+      <c r="F25" s="194"/>
+      <c r="G25" s="198"/>
+      <c r="H25" s="194"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="82"/>
       <c r="B26" s="83"/>
       <c r="C26" s="83"/>
       <c r="D26" s="83"/>
-      <c r="E26" s="275">
+      <c r="E26" s="195">
         <v>23</v>
       </c>
-      <c r="F26" s="274"/>
-      <c r="G26" s="278"/>
-      <c r="H26" s="274"/>
+      <c r="F26" s="194"/>
+      <c r="G26" s="198"/>
+      <c r="H26" s="194"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="82"/>
       <c r="B27" s="83"/>
       <c r="C27" s="83"/>
       <c r="D27" s="83"/>
-      <c r="E27" s="275">
+      <c r="E27" s="195">
         <v>24</v>
       </c>
-      <c r="F27" s="274"/>
-      <c r="G27" s="278"/>
-      <c r="H27" s="274"/>
+      <c r="F27" s="194"/>
+      <c r="G27" s="198"/>
+      <c r="H27" s="194"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="82"/>
       <c r="B28" s="83"/>
       <c r="C28" s="83"/>
       <c r="D28" s="83"/>
-      <c r="E28" s="275">
+      <c r="E28" s="195">
         <v>25</v>
       </c>
-      <c r="F28" s="274"/>
-      <c r="G28" s="278"/>
-      <c r="H28" s="274"/>
+      <c r="F28" s="194"/>
+      <c r="G28" s="198"/>
+      <c r="H28" s="194"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="82"/>
       <c r="B29" s="83"/>
       <c r="C29" s="83"/>
       <c r="D29" s="83"/>
-      <c r="E29" s="275">
+      <c r="E29" s="195">
         <v>26</v>
       </c>
-      <c r="F29" s="274"/>
-      <c r="G29" s="278"/>
-      <c r="H29" s="274"/>
+      <c r="F29" s="194"/>
+      <c r="G29" s="198"/>
+      <c r="H29" s="194"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="82"/>
       <c r="B30" s="83"/>
       <c r="C30" s="83"/>
       <c r="D30" s="83"/>
-      <c r="E30" s="275">
+      <c r="E30" s="195">
         <v>27</v>
       </c>
-      <c r="F30" s="274"/>
-      <c r="G30" s="278"/>
-      <c r="H30" s="274"/>
+      <c r="F30" s="194"/>
+      <c r="G30" s="198"/>
+      <c r="H30" s="194"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="82"/>
       <c r="B31" s="83"/>
       <c r="C31" s="83"/>
       <c r="D31" s="83"/>
-      <c r="E31" s="275">
+      <c r="E31" s="195">
         <v>28</v>
       </c>
-      <c r="F31" s="274"/>
-      <c r="G31" s="278"/>
-      <c r="H31" s="274"/>
+      <c r="F31" s="194"/>
+      <c r="G31" s="198"/>
+      <c r="H31" s="194"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="82"/>
       <c r="B32" s="83"/>
       <c r="C32" s="83"/>
       <c r="D32" s="83"/>
-      <c r="E32" s="275">
+      <c r="E32" s="195">
         <v>29</v>
       </c>
-      <c r="F32" s="274"/>
-      <c r="G32" s="278"/>
-      <c r="H32" s="274"/>
+      <c r="F32" s="194"/>
+      <c r="G32" s="198"/>
+      <c r="H32" s="194"/>
     </row>
     <row r="33" spans="1:8" ht="18.75" thickBot="1">
       <c r="A33" s="82"/>
       <c r="B33" s="83"/>
       <c r="C33" s="83"/>
       <c r="D33" s="83"/>
-      <c r="E33" s="275">
+      <c r="E33" s="195">
         <v>30</v>
       </c>
-      <c r="F33" s="274"/>
-      <c r="G33" s="278"/>
-      <c r="H33" s="274"/>
+      <c r="F33" s="194"/>
+      <c r="G33" s="198"/>
+      <c r="H33" s="194"/>
     </row>
     <row r="34" spans="1:8" ht="18.75" thickBot="1">
       <c r="A34" s="82"/>
       <c r="B34" s="83"/>
       <c r="C34" s="83"/>
       <c r="D34" s="83"/>
-      <c r="E34" s="275">
+      <c r="E34" s="195">
         <v>31</v>
       </c>
-      <c r="F34" s="274"/>
-      <c r="G34" s="278"/>
-      <c r="H34" s="274"/>
+      <c r="F34" s="194"/>
+      <c r="G34" s="198"/>
+      <c r="H34" s="194"/>
     </row>
     <row r="35" spans="1:8" ht="18.75" thickBot="1">
       <c r="A35" s="82"/>
       <c r="B35" s="83"/>
       <c r="C35" s="83"/>
       <c r="D35" s="83"/>
-      <c r="E35" s="275">
+      <c r="E35" s="195">
         <v>32</v>
       </c>
-      <c r="F35" s="274"/>
-      <c r="G35" s="278"/>
-      <c r="H35" s="274"/>
+      <c r="F35" s="194"/>
+      <c r="G35" s="198"/>
+      <c r="H35" s="194"/>
     </row>
     <row r="36" spans="1:8" ht="18.75" thickBot="1">
       <c r="A36" s="82"/>
       <c r="B36" s="83"/>
       <c r="C36" s="83"/>
       <c r="D36" s="83"/>
-      <c r="E36" s="275">
+      <c r="E36" s="195">
         <v>33</v>
       </c>
-      <c r="F36" s="274"/>
-      <c r="G36" s="278"/>
-      <c r="H36" s="274"/>
+      <c r="F36" s="194"/>
+      <c r="G36" s="198"/>
+      <c r="H36" s="194"/>
     </row>
     <row r="37" spans="1:8" ht="18.75" thickBot="1">
       <c r="A37" s="82"/>
       <c r="B37" s="83"/>
       <c r="C37" s="83"/>
       <c r="D37" s="83"/>
-      <c r="E37" s="275">
+      <c r="E37" s="195">
         <v>34</v>
       </c>
-      <c r="F37" s="274"/>
-      <c r="G37" s="278"/>
-      <c r="H37" s="274"/>
+      <c r="F37" s="194"/>
+      <c r="G37" s="198"/>
+      <c r="H37" s="194"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" thickBot="1">
       <c r="A38" s="82"/>
       <c r="B38" s="83"/>
       <c r="C38" s="83"/>
       <c r="D38" s="83"/>
-      <c r="E38" s="275">
+      <c r="E38" s="195">
         <v>35</v>
       </c>
-      <c r="F38" s="274"/>
-      <c r="G38" s="278"/>
-      <c r="H38" s="274"/>
+      <c r="F38" s="194"/>
+      <c r="G38" s="198"/>
+      <c r="H38" s="194"/>
     </row>
     <row r="39" spans="1:8" ht="18.75" thickBot="1">
       <c r="A39" s="82"/>
       <c r="B39" s="83"/>
       <c r="C39" s="83"/>
       <c r="D39" s="83"/>
-      <c r="E39" s="275">
+      <c r="E39" s="195">
         <v>36</v>
       </c>
-      <c r="F39" s="274"/>
-      <c r="G39" s="278"/>
-      <c r="H39" s="274"/>
+      <c r="F39" s="194"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="194"/>
     </row>
     <row r="40" spans="1:8" ht="18.75" thickBot="1">
       <c r="A40" s="82"/>
       <c r="B40" s="83"/>
       <c r="C40" s="83"/>
       <c r="D40" s="83"/>
-      <c r="E40" s="275">
+      <c r="E40" s="195">
         <v>37</v>
       </c>
-      <c r="F40" s="274"/>
-      <c r="G40" s="278"/>
-      <c r="H40" s="274"/>
+      <c r="F40" s="194"/>
+      <c r="G40" s="198"/>
+      <c r="H40" s="194"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="82"/>
       <c r="B41" s="83"/>
       <c r="C41" s="83"/>
       <c r="D41" s="83"/>
-      <c r="E41" s="275">
+      <c r="E41" s="195">
         <v>38</v>
       </c>
-      <c r="F41" s="274"/>
-      <c r="G41" s="278"/>
-      <c r="H41" s="274"/>
+      <c r="F41" s="194"/>
+      <c r="G41" s="198"/>
+      <c r="H41" s="194"/>
     </row>
     <row r="42" spans="1:8" ht="18.75" thickBot="1">
       <c r="A42" s="82"/>
@@ -5808,12 +5833,12 @@
       <c r="B43" s="83"/>
       <c r="C43" s="83"/>
       <c r="D43" s="83"/>
-      <c r="E43" s="275">
+      <c r="E43" s="195">
         <v>40</v>
       </c>
-      <c r="F43" s="274"/>
-      <c r="G43" s="278"/>
-      <c r="H43" s="274"/>
+      <c r="F43" s="194"/>
+      <c r="G43" s="198"/>
+      <c r="H43" s="194"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="82"/>
@@ -5888,40 +5913,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="251" t="s">
+      <c r="A1" s="240" t="s">
         <v>830</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="252"/>
-      <c r="B2" s="252"/>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-      <c r="E2" s="252"/>
-      <c r="F2" s="252"/>
-      <c r="G2" s="252"/>
-      <c r="H2" s="252"/>
+      <c r="A2" s="241"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="241"/>
+      <c r="D2" s="241"/>
+      <c r="E2" s="241"/>
+      <c r="F2" s="241"/>
+      <c r="G2" s="241"/>
+      <c r="H2" s="241"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="253" t="s">
+      <c r="A3" s="242" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="254"/>
-      <c r="C3" s="255"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="253" t="s">
+      <c r="B3" s="243"/>
+      <c r="C3" s="244"/>
+      <c r="D3" s="245"/>
+      <c r="E3" s="242" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="254"/>
-      <c r="G3" s="255"/>
-      <c r="H3" s="256"/>
+      <c r="F3" s="243"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="245"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="125">
@@ -6450,36 +6475,36 @@
       <c r="H24" s="153"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="253" t="s">
+      <c r="A25" s="242" t="s">
         <v>786</v>
       </c>
-      <c r="B25" s="254"/>
-      <c r="C25" s="255"/>
-      <c r="D25" s="256"/>
-      <c r="E25" s="253" t="s">
+      <c r="B25" s="243"/>
+      <c r="C25" s="244"/>
+      <c r="D25" s="245"/>
+      <c r="E25" s="242" t="s">
         <v>787</v>
       </c>
-      <c r="F25" s="254"/>
-      <c r="G25" s="255"/>
-      <c r="H25" s="256"/>
+      <c r="F25" s="243"/>
+      <c r="G25" s="244"/>
+      <c r="H25" s="245"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="129" t="s">
         <v>788</v>
       </c>
-      <c r="B26" s="240" t="s">
+      <c r="B26" s="246" t="s">
         <v>789</v>
       </c>
-      <c r="C26" s="241"/>
-      <c r="D26" s="242"/>
+      <c r="C26" s="247"/>
+      <c r="D26" s="248"/>
       <c r="E26" s="125" t="s">
         <v>790</v>
       </c>
-      <c r="F26" s="248" t="s">
+      <c r="F26" s="249" t="s">
         <v>791</v>
       </c>
-      <c r="G26" s="249"/>
-      <c r="H26" s="250" t="s">
+      <c r="G26" s="250"/>
+      <c r="H26" s="251" t="s">
         <v>759</v>
       </c>
     </row>
@@ -6487,21 +6512,21 @@
       <c r="A27" s="137" t="s">
         <v>792</v>
       </c>
-      <c r="B27" s="243" t="s">
+      <c r="B27" s="252" t="s">
         <v>793</v>
       </c>
-      <c r="C27" s="244"/>
-      <c r="D27" s="246" t="s">
+      <c r="C27" s="253"/>
+      <c r="D27" s="254" t="s">
         <v>623</v>
       </c>
       <c r="E27" s="129" t="s">
         <v>794</v>
       </c>
-      <c r="F27" s="240" t="s">
+      <c r="F27" s="246" t="s">
         <v>795</v>
       </c>
-      <c r="G27" s="241"/>
-      <c r="H27" s="247" t="s">
+      <c r="G27" s="247"/>
+      <c r="H27" s="255" t="s">
         <v>761</v>
       </c>
     </row>
@@ -6509,21 +6534,21 @@
       <c r="A28" s="129" t="s">
         <v>796</v>
       </c>
-      <c r="B28" s="240" t="s">
+      <c r="B28" s="246" t="s">
         <v>797</v>
       </c>
-      <c r="C28" s="241"/>
-      <c r="D28" s="242" t="s">
+      <c r="C28" s="247"/>
+      <c r="D28" s="248" t="s">
         <v>624</v>
       </c>
       <c r="E28" s="137" t="s">
         <v>798</v>
       </c>
-      <c r="F28" s="243" t="s">
+      <c r="F28" s="252" t="s">
         <v>799</v>
       </c>
-      <c r="G28" s="244"/>
-      <c r="H28" s="245" t="s">
+      <c r="G28" s="253"/>
+      <c r="H28" s="256" t="s">
         <v>763</v>
       </c>
     </row>
@@ -6531,21 +6556,21 @@
       <c r="A29" s="137" t="s">
         <v>800</v>
       </c>
-      <c r="B29" s="243" t="s">
+      <c r="B29" s="252" t="s">
         <v>801</v>
       </c>
-      <c r="C29" s="244"/>
-      <c r="D29" s="246" t="s">
+      <c r="C29" s="253"/>
+      <c r="D29" s="254" t="s">
         <v>625</v>
       </c>
       <c r="E29" s="129" t="s">
         <v>802</v>
       </c>
-      <c r="F29" s="240" t="s">
+      <c r="F29" s="246" t="s">
         <v>803</v>
       </c>
-      <c r="G29" s="241"/>
-      <c r="H29" s="247" t="s">
+      <c r="G29" s="247"/>
+      <c r="H29" s="255" t="s">
         <v>765</v>
       </c>
     </row>
@@ -6553,21 +6578,21 @@
       <c r="A30" s="129" t="s">
         <v>804</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="246" t="s">
         <v>805</v>
       </c>
-      <c r="C30" s="241"/>
-      <c r="D30" s="242" t="s">
+      <c r="C30" s="247"/>
+      <c r="D30" s="248" t="s">
         <v>626</v>
       </c>
       <c r="E30" s="137" t="s">
         <v>806</v>
       </c>
-      <c r="F30" s="243" t="s">
+      <c r="F30" s="252" t="s">
         <v>807</v>
       </c>
-      <c r="G30" s="244"/>
-      <c r="H30" s="245" t="s">
+      <c r="G30" s="253"/>
+      <c r="H30" s="256" t="s">
         <v>767</v>
       </c>
     </row>
@@ -6575,21 +6600,21 @@
       <c r="A31" s="137" t="s">
         <v>808</v>
       </c>
-      <c r="B31" s="243" t="s">
+      <c r="B31" s="252" t="s">
         <v>809</v>
       </c>
-      <c r="C31" s="244"/>
-      <c r="D31" s="246" t="s">
+      <c r="C31" s="253"/>
+      <c r="D31" s="254" t="s">
         <v>627</v>
       </c>
       <c r="E31" s="129" t="s">
         <v>810</v>
       </c>
-      <c r="F31" s="240" t="s">
+      <c r="F31" s="246" t="s">
         <v>811</v>
       </c>
-      <c r="G31" s="241"/>
-      <c r="H31" s="247" t="s">
+      <c r="G31" s="247"/>
+      <c r="H31" s="255" t="s">
         <v>494</v>
       </c>
     </row>
@@ -6597,17 +6622,17 @@
       <c r="A32" s="129" t="s">
         <v>812</v>
       </c>
-      <c r="B32" s="240" t="s">
+      <c r="B32" s="246" t="s">
         <v>813</v>
       </c>
-      <c r="C32" s="241"/>
-      <c r="D32" s="242" t="s">
+      <c r="C32" s="247"/>
+      <c r="D32" s="248" t="s">
         <v>628</v>
       </c>
       <c r="E32" s="137"/>
-      <c r="F32" s="243"/>
-      <c r="G32" s="244"/>
-      <c r="H32" s="245" t="s">
+      <c r="F32" s="252"/>
+      <c r="G32" s="253"/>
+      <c r="H32" s="256" t="s">
         <v>495</v>
       </c>
     </row>
@@ -6615,17 +6640,17 @@
       <c r="A33" s="137" t="s">
         <v>814</v>
       </c>
-      <c r="B33" s="243" t="s">
+      <c r="B33" s="252" t="s">
         <v>815</v>
       </c>
-      <c r="C33" s="244"/>
-      <c r="D33" s="246" t="s">
+      <c r="C33" s="253"/>
+      <c r="D33" s="254" t="s">
         <v>622</v>
       </c>
       <c r="E33" s="129"/>
-      <c r="F33" s="240"/>
-      <c r="G33" s="241"/>
-      <c r="H33" s="247" t="s">
+      <c r="F33" s="246"/>
+      <c r="G33" s="247"/>
+      <c r="H33" s="255" t="s">
         <v>759</v>
       </c>
     </row>
@@ -6633,17 +6658,17 @@
       <c r="A34" s="129" t="s">
         <v>816</v>
       </c>
-      <c r="B34" s="240" t="s">
+      <c r="B34" s="246" t="s">
         <v>817</v>
       </c>
-      <c r="C34" s="241"/>
-      <c r="D34" s="242" t="s">
+      <c r="C34" s="247"/>
+      <c r="D34" s="248" t="s">
         <v>623</v>
       </c>
       <c r="E34" s="137"/>
-      <c r="F34" s="243"/>
-      <c r="G34" s="244"/>
-      <c r="H34" s="245" t="s">
+      <c r="F34" s="252"/>
+      <c r="G34" s="253"/>
+      <c r="H34" s="256" t="s">
         <v>761</v>
       </c>
     </row>
@@ -6651,17 +6676,17 @@
       <c r="A35" s="137" t="s">
         <v>818</v>
       </c>
-      <c r="B35" s="243" t="s">
+      <c r="B35" s="252" t="s">
         <v>819</v>
       </c>
-      <c r="C35" s="244"/>
-      <c r="D35" s="246" t="s">
+      <c r="C35" s="253"/>
+      <c r="D35" s="254" t="s">
         <v>624</v>
       </c>
       <c r="E35" s="129"/>
-      <c r="F35" s="240"/>
-      <c r="G35" s="241"/>
-      <c r="H35" s="247" t="s">
+      <c r="F35" s="246"/>
+      <c r="G35" s="247"/>
+      <c r="H35" s="255" t="s">
         <v>763</v>
       </c>
     </row>
@@ -6669,17 +6694,17 @@
       <c r="A36" s="129" t="s">
         <v>820</v>
       </c>
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="246" t="s">
         <v>821</v>
       </c>
-      <c r="C36" s="241"/>
-      <c r="D36" s="242" t="s">
+      <c r="C36" s="247"/>
+      <c r="D36" s="248" t="s">
         <v>625</v>
       </c>
       <c r="E36" s="137"/>
-      <c r="F36" s="243"/>
-      <c r="G36" s="244"/>
-      <c r="H36" s="245" t="s">
+      <c r="F36" s="252"/>
+      <c r="G36" s="253"/>
+      <c r="H36" s="256" t="s">
         <v>765</v>
       </c>
     </row>
@@ -6687,17 +6712,17 @@
       <c r="A37" s="137" t="s">
         <v>822</v>
       </c>
-      <c r="B37" s="243" t="s">
+      <c r="B37" s="252" t="s">
         <v>823</v>
       </c>
-      <c r="C37" s="244"/>
-      <c r="D37" s="246" t="s">
+      <c r="C37" s="253"/>
+      <c r="D37" s="254" t="s">
         <v>626</v>
       </c>
       <c r="E37" s="129"/>
-      <c r="F37" s="240"/>
-      <c r="G37" s="241"/>
-      <c r="H37" s="247" t="s">
+      <c r="F37" s="246"/>
+      <c r="G37" s="247"/>
+      <c r="H37" s="255" t="s">
         <v>767</v>
       </c>
     </row>
@@ -6705,17 +6730,17 @@
       <c r="A38" s="129" t="s">
         <v>824</v>
       </c>
-      <c r="B38" s="240" t="s">
+      <c r="B38" s="246" t="s">
         <v>825</v>
       </c>
-      <c r="C38" s="241"/>
-      <c r="D38" s="242" t="s">
+      <c r="C38" s="247"/>
+      <c r="D38" s="248" t="s">
         <v>627</v>
       </c>
       <c r="E38" s="137"/>
-      <c r="F38" s="243"/>
-      <c r="G38" s="244"/>
-      <c r="H38" s="245" t="s">
+      <c r="F38" s="252"/>
+      <c r="G38" s="253"/>
+      <c r="H38" s="256" t="s">
         <v>494</v>
       </c>
     </row>
@@ -6723,17 +6748,17 @@
       <c r="A39" s="137" t="s">
         <v>826</v>
       </c>
-      <c r="B39" s="243" t="s">
+      <c r="B39" s="252" t="s">
         <v>827</v>
       </c>
-      <c r="C39" s="244"/>
-      <c r="D39" s="246" t="s">
+      <c r="C39" s="253"/>
+      <c r="D39" s="254" t="s">
         <v>628</v>
       </c>
       <c r="E39" s="129"/>
-      <c r="F39" s="240"/>
-      <c r="G39" s="241"/>
-      <c r="H39" s="247" t="s">
+      <c r="F39" s="246"/>
+      <c r="G39" s="247"/>
+      <c r="H39" s="255" t="s">
         <v>495</v>
       </c>
     </row>
@@ -6741,65 +6766,36 @@
       <c r="A40" s="129" t="s">
         <v>828</v>
       </c>
-      <c r="B40" s="240" t="s">
+      <c r="B40" s="246" t="s">
         <v>827</v>
       </c>
-      <c r="C40" s="241"/>
-      <c r="D40" s="242" t="s">
+      <c r="C40" s="247"/>
+      <c r="D40" s="248" t="s">
         <v>628</v>
       </c>
       <c r="E40" s="137"/>
-      <c r="F40" s="243"/>
-      <c r="G40" s="244"/>
-      <c r="H40" s="245"/>
+      <c r="F40" s="252"/>
+      <c r="G40" s="253"/>
+      <c r="H40" s="256"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="149" t="s">
         <v>829</v>
       </c>
-      <c r="B41" s="234" t="s">
+      <c r="B41" s="257" t="s">
         <v>827</v>
       </c>
-      <c r="C41" s="235"/>
-      <c r="D41" s="236" t="s">
+      <c r="C41" s="258"/>
+      <c r="D41" s="259" t="s">
         <v>628</v>
       </c>
       <c r="E41" s="154"/>
-      <c r="F41" s="237"/>
-      <c r="G41" s="238"/>
-      <c r="H41" s="239"/>
+      <c r="F41" s="260"/>
+      <c r="G41" s="261"/>
+      <c r="H41" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -6808,6 +6804,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6833,34 +6858,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="257" t="s">
+      <c r="A1" s="263" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="263"/>
+      <c r="F1" s="263"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="258"/>
-      <c r="B2" s="258"/>
-      <c r="C2" s="258"/>
-      <c r="D2" s="258"/>
-      <c r="E2" s="258"/>
-      <c r="F2" s="258"/>
+      <c r="A2" s="264"/>
+      <c r="B2" s="264"/>
+      <c r="C2" s="264"/>
+      <c r="D2" s="264"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="224" t="s">
         <v>320</v>
       </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="218" t="s">
+      <c r="B3" s="225"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="224" t="s">
         <v>321</v>
       </c>
-      <c r="E3" s="219"/>
-      <c r="F3" s="220"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="226"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1">
       <c r="A4" s="54">
@@ -7217,14 +7242,14 @@
       <c r="F21" s="56" t="s">
         <v>348</v>
       </c>
-      <c r="N21" s="259" t="s">
+      <c r="N21" s="265" t="s">
         <v>838</v>
       </c>
-      <c r="O21" s="259"/>
-      <c r="P21" s="259"/>
-      <c r="Q21" s="259"/>
-      <c r="R21" s="259"/>
-      <c r="S21" s="259"/>
+      <c r="O21" s="265"/>
+      <c r="P21" s="265"/>
+      <c r="Q21" s="265"/>
+      <c r="R21" s="265"/>
+      <c r="S21" s="265"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1">
       <c r="A22" s="54">
@@ -7245,12 +7270,12 @@
       <c r="F22" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="O22" s="260" t="s">
+      <c r="O22" s="266" t="s">
         <v>363</v>
       </c>
-      <c r="P22" s="260"/>
-      <c r="Q22" s="260"/>
-      <c r="R22" s="260"/>
+      <c r="P22" s="266"/>
+      <c r="Q22" s="266"/>
+      <c r="R22" s="266"/>
     </row>
     <row r="23" spans="1:19" ht="19.5" thickBot="1">
       <c r="A23" s="54">
@@ -7507,22 +7532,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="259" t="s">
+      <c r="A1" s="265" t="s">
         <v>838</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
     </row>
     <row r="2" spans="1:6" ht="18.75">
-      <c r="B2" s="260" t="s">
+      <c r="B2" s="266" t="s">
         <v>363</v>
       </c>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
     </row>
     <row r="3" spans="1:6" ht="18.75">
       <c r="B3" s="43"/>
@@ -9276,40 +9301,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="267" t="s">
+      <c r="A1" s="273" t="s">
         <v>902</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="269"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="270"/>
-      <c r="B2" s="271"/>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="272"/>
+      <c r="A2" s="276"/>
+      <c r="B2" s="277"/>
+      <c r="C2" s="277"/>
+      <c r="D2" s="277"/>
+      <c r="E2" s="277"/>
+      <c r="F2" s="277"/>
+      <c r="G2" s="277"/>
+      <c r="H2" s="278"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="261" t="s">
+      <c r="A3" s="267" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="262"/>
-      <c r="C3" s="262"/>
-      <c r="D3" s="263"/>
-      <c r="E3" s="261" t="s">
+      <c r="B3" s="268"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="269"/>
+      <c r="E3" s="267" t="s">
         <v>857</v>
       </c>
-      <c r="F3" s="262"/>
-      <c r="G3" s="262"/>
-      <c r="H3" s="263"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
+      <c r="H3" s="269"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="178">
@@ -9628,18 +9653,18 @@
       <c r="H21" s="170"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="264" t="s">
+      <c r="A22" s="270" t="s">
         <v>858</v>
       </c>
-      <c r="B22" s="265"/>
-      <c r="C22" s="265"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="264" t="s">
+      <c r="B22" s="271"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="272"/>
+      <c r="E22" s="270" t="s">
         <v>859</v>
       </c>
-      <c r="F22" s="265"/>
-      <c r="G22" s="265"/>
-      <c r="H22" s="266"/>
+      <c r="F22" s="271"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="272"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="161">
@@ -10012,8 +10037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AJ57"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -10064,18 +10089,18 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
-      <c r="R3" s="194" t="s">
+      <c r="R3" s="217" t="s">
         <v>282</v>
       </c>
-      <c r="S3" s="194"/>
-      <c r="T3" s="194"/>
-      <c r="AA3" s="196" t="s">
+      <c r="S3" s="217"/>
+      <c r="T3" s="217"/>
+      <c r="AA3" s="218" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="197"/>
-      <c r="AC3" s="197"/>
-      <c r="AD3" s="197"/>
-      <c r="AE3" s="198"/>
+      <c r="AB3" s="219"/>
+      <c r="AC3" s="219"/>
+      <c r="AD3" s="219"/>
+      <c r="AE3" s="220"/>
     </row>
     <row r="4" spans="2:32" ht="15.75">
       <c r="B4" s="57" t="s">
@@ -10118,7 +10143,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="52"/>
-      <c r="R4" s="199" t="s">
+      <c r="R4" s="210" t="s">
         <v>638</v>
       </c>
       <c r="S4" s="98" t="s">
@@ -10127,12 +10152,12 @@
       <c r="T4" s="99" t="s">
         <v>641</v>
       </c>
-      <c r="V4" s="195" t="s">
+      <c r="V4" s="208" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="195"/>
-      <c r="X4" s="195"/>
-      <c r="Y4" s="195"/>
+      <c r="W4" s="208"/>
+      <c r="X4" s="208"/>
+      <c r="Y4" s="208"/>
       <c r="AA4" s="89" t="s">
         <v>290</v>
       </c>
@@ -10186,7 +10211,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="52"/>
-      <c r="R5" s="200"/>
+      <c r="R5" s="211"/>
       <c r="S5" s="31" t="s">
         <v>607</v>
       </c>
@@ -10264,7 +10289,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="201"/>
+      <c r="R6" s="212"/>
       <c r="S6" s="100" t="s">
         <v>640</v>
       </c>
@@ -10340,7 +10365,7 @@
         <v>284</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="199" t="s">
+      <c r="R7" s="210" t="s">
         <v>644</v>
       </c>
       <c r="S7" s="98" t="s">
@@ -10420,7 +10445,7 @@
         <v>285</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="200"/>
+      <c r="R8" s="211"/>
       <c r="S8" s="31" t="s">
         <v>607</v>
       </c>
@@ -10489,7 +10514,7 @@
         <v>286</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="201"/>
+      <c r="R9" s="212"/>
       <c r="S9" s="100" t="s">
         <v>640</v>
       </c>
@@ -10616,7 +10641,7 @@
         <v>9</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="203" t="s">
+      <c r="R11" s="213" t="s">
         <v>645</v>
       </c>
       <c r="S11" s="103" t="s">
@@ -10689,7 +10714,7 @@
       <c r="O12" s="94"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="204"/>
+      <c r="R12" s="214"/>
       <c r="S12" s="97" t="s">
         <v>607</v>
       </c>
@@ -10756,7 +10781,7 @@
       <c r="O13" s="94"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="205"/>
+      <c r="R13" s="215"/>
       <c r="S13" s="105" t="s">
         <v>640</v>
       </c>
@@ -10779,11 +10804,11 @@
       <c r="AA13" s="41" t="s">
         <v>851</v>
       </c>
-      <c r="AD13" s="196" t="s">
+      <c r="AD13" s="218" t="s">
         <v>630</v>
       </c>
-      <c r="AE13" s="197"/>
-      <c r="AF13" s="198"/>
+      <c r="AE13" s="219"/>
+      <c r="AF13" s="220"/>
     </row>
     <row r="14" spans="2:32" ht="15.75">
       <c r="B14" s="57" t="s">
@@ -10830,7 +10855,7 @@
         <v>281</v>
       </c>
       <c r="Q14" s="3"/>
-      <c r="R14" s="199" t="s">
+      <c r="R14" s="210" t="s">
         <v>648</v>
       </c>
       <c r="S14" s="103" t="s">
@@ -10908,7 +10933,7 @@
         <v>294</v>
       </c>
       <c r="Q15" s="3"/>
-      <c r="R15" s="200"/>
+      <c r="R15" s="211"/>
       <c r="S15" s="97" t="s">
         <v>607</v>
       </c>
@@ -10969,22 +10994,22 @@
         <v>293</v>
       </c>
       <c r="Q16" s="3"/>
-      <c r="R16" s="201"/>
+      <c r="R16" s="212"/>
       <c r="S16" s="105" t="s">
         <v>640</v>
       </c>
       <c r="T16" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="V16" s="195" t="s">
+      <c r="V16" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="195"/>
-      <c r="X16" s="195"/>
-      <c r="Y16" s="195"/>
-      <c r="Z16" s="195"/>
-      <c r="AA16" s="195"/>
-      <c r="AB16" s="195"/>
+      <c r="W16" s="208"/>
+      <c r="X16" s="208"/>
+      <c r="Y16" s="208"/>
+      <c r="Z16" s="208"/>
+      <c r="AA16" s="208"/>
+      <c r="AB16" s="208"/>
       <c r="AD16" s="7" t="s">
         <v>623</v>
       </c>
@@ -10995,7 +11020,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="17" spans="2:32">
+    <row r="17" spans="2:32" ht="15.75">
       <c r="B17" s="57" t="s">
         <v>153</v>
       </c>
@@ -11040,6 +11065,15 @@
         <v>297</v>
       </c>
       <c r="Q17" s="3"/>
+      <c r="R17" t="s">
+        <v>909</v>
+      </c>
+      <c r="S17" s="103" t="s">
+        <v>639</v>
+      </c>
+      <c r="T17" s="280" t="s">
+        <v>910</v>
+      </c>
       <c r="V17" s="119" t="s">
         <v>290</v>
       </c>
@@ -11071,7 +11105,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:32" ht="15.75">
       <c r="B18" s="57" t="s">
         <v>165</v>
       </c>
@@ -11117,8 +11151,12 @@
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="96"/>
-      <c r="S18" s="96"/>
-      <c r="T18" s="96"/>
+      <c r="S18" s="97" t="s">
+        <v>607</v>
+      </c>
+      <c r="T18" s="96" t="s">
+        <v>912</v>
+      </c>
       <c r="U18" s="41"/>
       <c r="V18" s="39" t="s">
         <v>670</v>
@@ -11151,7 +11189,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:32" ht="16.5" thickBot="1">
       <c r="B19" s="57" t="s">
         <v>177</v>
       </c>
@@ -11197,8 +11235,12 @@
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="95"/>
-      <c r="S19" s="95"/>
-      <c r="T19" s="95"/>
+      <c r="S19" s="105" t="s">
+        <v>640</v>
+      </c>
+      <c r="T19" s="95" t="s">
+        <v>911</v>
+      </c>
       <c r="U19" s="41"/>
       <c r="V19" s="7" t="s">
         <v>671</v>
@@ -11276,11 +11318,11 @@
         <v>302</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="195" t="s">
+      <c r="R20" s="208" t="s">
         <v>281</v>
       </c>
-      <c r="S20" s="195"/>
-      <c r="T20" s="195"/>
+      <c r="S20" s="208"/>
+      <c r="T20" s="208"/>
       <c r="U20" s="3"/>
       <c r="V20" s="7" t="s">
         <v>672</v>
@@ -11451,15 +11493,15 @@
       <c r="T22" t="s">
         <v>478</v>
       </c>
-      <c r="V22" s="196" t="s">
+      <c r="V22" s="218" t="s">
         <v>663</v>
       </c>
-      <c r="W22" s="197"/>
-      <c r="X22" s="197"/>
-      <c r="Y22" s="197"/>
-      <c r="Z22" s="197"/>
-      <c r="AA22" s="197"/>
-      <c r="AB22" s="198"/>
+      <c r="W22" s="219"/>
+      <c r="X22" s="219"/>
+      <c r="Y22" s="219"/>
+      <c r="Z22" s="219"/>
+      <c r="AA22" s="219"/>
+      <c r="AB22" s="220"/>
       <c r="AD22" s="7" t="s">
         <v>629</v>
       </c>
@@ -11929,33 +11971,33 @@
       </c>
     </row>
     <row r="31" spans="2:32">
-      <c r="B31" s="195" t="s">
+      <c r="B31" s="208" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="195"/>
-      <c r="D31" s="195"/>
-      <c r="E31" s="195"/>
-      <c r="F31" s="195"/>
-      <c r="G31" s="195"/>
-      <c r="H31" s="195"/>
-      <c r="J31" s="195" t="s">
+      <c r="C31" s="208"/>
+      <c r="D31" s="208"/>
+      <c r="E31" s="208"/>
+      <c r="F31" s="208"/>
+      <c r="G31" s="208"/>
+      <c r="H31" s="208"/>
+      <c r="J31" s="208" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="195"/>
-      <c r="L31" s="195"/>
-      <c r="M31" s="195"/>
-      <c r="N31" s="195"/>
-      <c r="O31" s="195"/>
-      <c r="P31" s="195"/>
-      <c r="T31" s="195" t="s">
+      <c r="K31" s="208"/>
+      <c r="L31" s="208"/>
+      <c r="M31" s="208"/>
+      <c r="N31" s="208"/>
+      <c r="O31" s="208"/>
+      <c r="P31" s="208"/>
+      <c r="T31" s="208" t="s">
         <v>283</v>
       </c>
-      <c r="U31" s="195"/>
-      <c r="V31" s="195"/>
-      <c r="W31" s="195"/>
-      <c r="X31" s="195"/>
-      <c r="Y31" s="195"/>
-      <c r="Z31" s="195"/>
+      <c r="U31" s="208"/>
+      <c r="V31" s="208"/>
+      <c r="W31" s="208"/>
+      <c r="X31" s="208"/>
+      <c r="Y31" s="208"/>
+      <c r="Z31" s="208"/>
     </row>
     <row r="32" spans="2:32">
       <c r="B32" s="51" t="s">
@@ -12237,7 +12279,7 @@
       <c r="Z35" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="AD35" s="193" t="s">
+      <c r="AD35" s="216" t="s">
         <v>700</v>
       </c>
       <c r="AE35" s="7" t="s">
@@ -12323,7 +12365,7 @@
       <c r="Z36" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="AD36" s="193"/>
+      <c r="AD36" s="216"/>
       <c r="AE36" s="7"/>
       <c r="AF36" s="7"/>
       <c r="AG36" s="7"/>
@@ -12395,7 +12437,7 @@
       <c r="Z37" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="AD37" s="193"/>
+      <c r="AD37" s="216"/>
       <c r="AE37" s="7"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
@@ -12452,7 +12494,7 @@
       <c r="Z38" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="AD38" s="193"/>
+      <c r="AD38" s="216"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
@@ -12467,15 +12509,15 @@
       <c r="F39" t="s">
         <v>567</v>
       </c>
-      <c r="J39" s="202" t="s">
+      <c r="J39" s="209" t="s">
         <v>475</v>
       </c>
-      <c r="K39" s="202"/>
-      <c r="L39" s="202"/>
-      <c r="M39" s="202"/>
-      <c r="N39" s="202"/>
-      <c r="O39" s="202"/>
-      <c r="P39" s="202"/>
+      <c r="K39" s="209"/>
+      <c r="L39" s="209"/>
+      <c r="M39" s="209"/>
+      <c r="N39" s="209"/>
+      <c r="O39" s="209"/>
+      <c r="P39" s="209"/>
       <c r="S39">
         <v>7</v>
       </c>
@@ -12590,6 +12632,7 @@
       <c r="N42" t="s">
         <v>715</v>
       </c>
+      <c r="Q42" s="279"/>
       <c r="S42">
         <v>10</v>
       </c>
@@ -12904,13 +12947,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="T31:Z31"/>
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="R11:R13"/>
-    <mergeCell ref="R14:R16"/>
     <mergeCell ref="AD35:AD38"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
@@ -12920,6 +12956,13 @@
     <mergeCell ref="AD13:AF13"/>
     <mergeCell ref="R4:R6"/>
     <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="T31:Z31"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="R11:R13"/>
+    <mergeCell ref="R14:R16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12949,40 +12992,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="199" t="s">
         <v>701</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="208"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="201"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="209"/>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
-      <c r="H2" s="211"/>
+      <c r="A2" s="202"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="204"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="205" t="s">
         <v>608</v>
       </c>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
-      <c r="E3" s="213" t="s">
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206" t="s">
         <v>609</v>
       </c>
-      <c r="F3" s="213"/>
-      <c r="G3" s="213"/>
-      <c r="H3" s="214"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="78">
@@ -14015,14 +14058,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="221" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="217"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="223"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="17"/>
@@ -14033,16 +14076,16 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="224" t="s">
         <v>304</v>
       </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="220"/>
-      <c r="D3" s="218" t="s">
+      <c r="B3" s="225"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="224" t="s">
         <v>305</v>
       </c>
-      <c r="E3" s="219"/>
-      <c r="F3" s="220"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="226"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20">
@@ -14312,28 +14355,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="230" t="s">
         <v>737</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="230"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="227" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="223"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="229"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="27"/>
@@ -14608,16 +14651,16 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="221" t="s">
+      <c r="A15" s="227" t="s">
         <v>310</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="C15" s="222"/>
-      <c r="D15" s="222"/>
-      <c r="E15" s="222"/>
-      <c r="F15" s="222"/>
-      <c r="G15" s="222"/>
-      <c r="H15" s="223"/>
+      <c r="B15" s="228"/>
+      <c r="C15" s="228"/>
+      <c r="D15" s="228"/>
+      <c r="E15" s="228"/>
+      <c r="F15" s="228"/>
+      <c r="G15" s="228"/>
+      <c r="H15" s="229"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="32"/>
@@ -14907,16 +14950,16 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="221" t="s">
+      <c r="A28" s="227" t="s">
         <v>311</v>
       </c>
-      <c r="B28" s="222"/>
-      <c r="C28" s="222"/>
-      <c r="D28" s="222"/>
-      <c r="E28" s="222"/>
-      <c r="F28" s="222"/>
-      <c r="G28" s="222"/>
-      <c r="H28" s="223"/>
+      <c r="B28" s="228"/>
+      <c r="C28" s="228"/>
+      <c r="D28" s="228"/>
+      <c r="E28" s="228"/>
+      <c r="F28" s="228"/>
+      <c r="G28" s="228"/>
+      <c r="H28" s="229"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="27"/>
@@ -15229,12 +15272,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="231" t="s">
         <v>713</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
@@ -15442,28 +15485,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="226" t="s">
+      <c r="A1" s="232" t="s">
         <v>751</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
+      <c r="H1" s="232"/>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="227" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
-      <c r="G2" s="222"/>
-      <c r="H2" s="223"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="229"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="33" t="s">
@@ -15754,12 +15797,12 @@
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
-      <c r="A15" s="221" t="s">
+      <c r="A15" s="227" t="s">
         <v>314</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="C15" s="222"/>
-      <c r="D15" s="223"/>
+      <c r="B15" s="228"/>
+      <c r="C15" s="228"/>
+      <c r="D15" s="229"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75">
@@ -15927,12 +15970,12 @@
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="15.75">
-      <c r="A28" s="221" t="s">
+      <c r="A28" s="227" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="222"/>
-      <c r="C28" s="222"/>
-      <c r="D28" s="223"/>
+      <c r="B28" s="228"/>
+      <c r="C28" s="228"/>
+      <c r="D28" s="229"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75">
@@ -16136,40 +16179,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="221" t="s">
         <v>832</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="217"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="223"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="227"/>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="229"/>
+      <c r="A2" s="233"/>
+      <c r="B2" s="234"/>
+      <c r="C2" s="234"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="235"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="236" t="s">
         <v>380</v>
       </c>
-      <c r="B3" s="231"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="233"/>
-      <c r="E3" s="230" t="s">
+      <c r="B3" s="237"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="236" t="s">
         <v>381</v>
       </c>
-      <c r="F3" s="231"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="233"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="238"/>
+      <c r="H3" s="239"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="74">

</xml_diff>